<commit_message>
자동 업데이트: 2025-03-26 00:37:17
</commit_message>
<xml_diff>
--- a/data/daily_report.xlsx
+++ b/data/daily_report.xlsx
@@ -8,14 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c58a53286e4c1d7a/문서/GitHub/Dashboard/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="115" documentId="8_{9DD2A88B-03DA-4864-84CC-4418086E8BD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6144204D-87AA-43BF-A619-25CACCDAE208}"/>
+  <xr:revisionPtr revIDLastSave="117" documentId="8_{9DD2A88B-03DA-4864-84CC-4418086E8BD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E64422EE-AB09-46E1-B207-6C4A715C1D2C}"/>
   <bookViews>
-    <workbookView xWindow="4200" yWindow="3795" windowWidth="21885" windowHeight="15885" xr2:uid="{4AB8DADE-1167-4E84-9D67-55086BA93884}"/>
+    <workbookView xWindow="1290" yWindow="1860" windowWidth="27915" windowHeight="15885" xr2:uid="{4AB8DADE-1167-4E84-9D67-55086BA93884}"/>
   </bookViews>
   <sheets>
     <sheet name="daily_report" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -753,6 +766,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1075,7 +1092,7 @@
   <dimension ref="A1:Q24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O18" sqref="O18"/>
+      <selection activeCell="P25" sqref="P25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1212,7 +1229,7 @@
         <v>6546</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F23" si="0">E3-D3</f>
+        <f t="shared" ref="F3:F24" si="0">E3-D3</f>
         <v>146</v>
       </c>
       <c r="G3" s="2">
@@ -1239,7 +1256,7 @@
         <v>0</v>
       </c>
       <c r="M3">
-        <f t="shared" ref="M3:M23" si="2">L3+E3</f>
+        <f t="shared" ref="M3:M24" si="2">L3+E3</f>
         <v>6546</v>
       </c>
       <c r="N3" s="2">
@@ -1282,11 +1299,11 @@
         <v>144.5</v>
       </c>
       <c r="H4" s="2">
-        <f t="shared" ref="H4:H23" si="3">(E4/D4-1)*100</f>
+        <f t="shared" ref="H4:H24" si="3">(E4/D4-1)*100</f>
         <v>2.1845401772074613</v>
       </c>
       <c r="I4" s="2">
-        <f t="shared" ref="I4:I23" si="4">(POWER((E4/$D$3),1/A4)-1)*100</f>
+        <f t="shared" ref="I4:I24" si="4">(POWER((E4/$D$3),1/A4)-1)*100</f>
         <v>2.2328836529616813</v>
       </c>
       <c r="J4" s="3">
@@ -1294,7 +1311,7 @@
         <v>6567.4815999999983</v>
       </c>
       <c r="K4" s="3">
-        <f t="shared" ref="K4:K23" si="6">E4-J4</f>
+        <f t="shared" ref="K4:K24" si="6">E4-J4</f>
         <v>121.51840000000175</v>
       </c>
       <c r="L4">
@@ -1305,7 +1322,7 @@
         <v>6689</v>
       </c>
       <c r="N4" s="2">
-        <f t="shared" ref="N4:N23" si="7">E4/$D$2*100</f>
+        <f t="shared" ref="N4:N24" si="7">E4/$D$2*100</f>
         <v>104.515625</v>
       </c>
       <c r="O4">
@@ -2510,24 +2527,53 @@
       <c r="D24">
         <v>8925</v>
       </c>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
+      <c r="E24">
+        <v>9113</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="0"/>
+        <v>188</v>
+      </c>
+      <c r="G24" s="2">
+        <f>(E24-$D$2)/A24</f>
+        <v>117.95652173913044</v>
+      </c>
+      <c r="H24" s="2">
+        <f t="shared" si="3"/>
+        <v>2.1064425770308093</v>
+      </c>
+      <c r="I24" s="2">
+        <f t="shared" si="4"/>
+        <v>1.5484044777758443</v>
+      </c>
       <c r="J24" s="3">
         <f t="shared" si="5"/>
         <v>8503.3052957129839</v>
       </c>
-      <c r="K24" s="3"/>
+      <c r="K24" s="3">
+        <f t="shared" si="6"/>
+        <v>609.69470428701607</v>
+      </c>
       <c r="L24">
         <v>0</v>
       </c>
-      <c r="N24" s="2"/>
+      <c r="M24">
+        <f t="shared" si="2"/>
+        <v>9113</v>
+      </c>
+      <c r="N24" s="2">
+        <f t="shared" si="7"/>
+        <v>142.390625</v>
+      </c>
       <c r="O24">
         <v>87921</v>
       </c>
+      <c r="P24">
+        <v>87985.1</v>
+      </c>
       <c r="Q24">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>98.59390250325248</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
자동 업데이트: 2025-03-27 01:01:32
</commit_message>
<xml_diff>
--- a/data/daily_report.xlsx
+++ b/data/daily_report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c58a53286e4c1d7a/문서/GitHub/Dashboard/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="117" documentId="8_{9DD2A88B-03DA-4864-84CC-4418086E8BD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E64422EE-AB09-46E1-B207-6C4A715C1D2C}"/>
+  <xr:revisionPtr revIDLastSave="123" documentId="8_{9DD2A88B-03DA-4864-84CC-4418086E8BD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2B11172D-445D-481C-8CF4-73CC638D0F7D}"/>
   <bookViews>
-    <workbookView xWindow="1290" yWindow="1860" windowWidth="27915" windowHeight="15885" xr2:uid="{4AB8DADE-1167-4E84-9D67-55086BA93884}"/>
+    <workbookView xWindow="990" yWindow="3165" windowWidth="25335" windowHeight="15885" xr2:uid="{4AB8DADE-1167-4E84-9D67-55086BA93884}"/>
   </bookViews>
   <sheets>
     <sheet name="daily_report" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="24">
   <si>
     <t>Index</t>
   </si>
@@ -1089,10 +1089,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48182F73-FFD5-43FF-A3B0-19A54A277A3F}">
-  <dimension ref="A1:Q24"/>
+  <dimension ref="A1:Q25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P25" sqref="P25"/>
+      <selection activeCell="P26" sqref="P26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1307,7 +1307,7 @@
         <v>2.2328836529616813</v>
       </c>
       <c r="J4" s="3">
-        <f t="shared" ref="J4:J24" si="5">J3*1.013</f>
+        <f t="shared" ref="J4:J25" si="5">J3*1.013</f>
         <v>6567.4815999999983</v>
       </c>
       <c r="K4" s="3">
@@ -2574,6 +2574,68 @@
       <c r="Q24">
         <f t="shared" si="8"/>
         <v>98.59390250325248</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" s="1">
+        <v>45742</v>
+      </c>
+      <c r="C25" t="s">
+        <v>19</v>
+      </c>
+      <c r="D25">
+        <v>9113</v>
+      </c>
+      <c r="E25">
+        <v>9163</v>
+      </c>
+      <c r="F25">
+        <f t="shared" ref="F25" si="9">E25-D25</f>
+        <v>50</v>
+      </c>
+      <c r="G25" s="2">
+        <f>(E25-$D$2)/A25</f>
+        <v>115.125</v>
+      </c>
+      <c r="H25" s="2">
+        <f t="shared" ref="H25" si="10">(E25/D25-1)*100</f>
+        <v>0.54866673982223446</v>
+      </c>
+      <c r="I25" s="2">
+        <f t="shared" ref="I25" si="11">(POWER((E25/$D$3),1/A25)-1)*100</f>
+        <v>1.5065509612034012</v>
+      </c>
+      <c r="J25" s="3">
+        <f t="shared" si="5"/>
+        <v>8613.8482645572512</v>
+      </c>
+      <c r="K25" s="3">
+        <f t="shared" ref="K25" si="12">E25-J25</f>
+        <v>549.15173544274876</v>
+      </c>
+      <c r="L25">
+        <v>0</v>
+      </c>
+      <c r="M25">
+        <f t="shared" ref="M25" si="13">L25+E25</f>
+        <v>9163</v>
+      </c>
+      <c r="N25" s="2">
+        <f t="shared" ref="N25" si="14">E25/$D$2*100</f>
+        <v>143.171875</v>
+      </c>
+      <c r="O25">
+        <v>87985.1</v>
+      </c>
+      <c r="P25">
+        <v>86736.1</v>
+      </c>
+      <c r="Q25">
+        <f t="shared" ref="Q25" si="15">P25/$O$2*100</f>
+        <v>97.194304341443697</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
자동 업데이트: 2025-03-28 00:06:12
</commit_message>
<xml_diff>
--- a/data/daily_report.xlsx
+++ b/data/daily_report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c58a53286e4c1d7a/문서/GitHub/Dashboard/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="123" documentId="8_{9DD2A88B-03DA-4864-84CC-4418086E8BD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2B11172D-445D-481C-8CF4-73CC638D0F7D}"/>
+  <xr:revisionPtr revIDLastSave="129" documentId="8_{9DD2A88B-03DA-4864-84CC-4418086E8BD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{977D2A81-1022-4F69-9EA8-7CDCAD076B6D}"/>
   <bookViews>
-    <workbookView xWindow="990" yWindow="3165" windowWidth="25335" windowHeight="15885" xr2:uid="{4AB8DADE-1167-4E84-9D67-55086BA93884}"/>
+    <workbookView xWindow="6060" yWindow="3165" windowWidth="27180" windowHeight="15885" xr2:uid="{4AB8DADE-1167-4E84-9D67-55086BA93884}"/>
   </bookViews>
   <sheets>
     <sheet name="daily_report" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="24">
   <si>
     <t>Index</t>
   </si>
@@ -1089,10 +1089,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48182F73-FFD5-43FF-A3B0-19A54A277A3F}">
-  <dimension ref="A1:Q25"/>
+  <dimension ref="A1:Q26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P26" sqref="P26"/>
+      <selection activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1307,7 +1307,7 @@
         <v>2.2328836529616813</v>
       </c>
       <c r="J4" s="3">
-        <f t="shared" ref="J4:J25" si="5">J3*1.013</f>
+        <f t="shared" ref="J4:J26" si="5">J3*1.013</f>
         <v>6567.4815999999983</v>
       </c>
       <c r="K4" s="3">
@@ -2636,6 +2636,68 @@
       <c r="Q25">
         <f t="shared" ref="Q25" si="15">P25/$O$2*100</f>
         <v>97.194304341443697</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" s="1">
+        <v>45743</v>
+      </c>
+      <c r="C26" t="s">
+        <v>20</v>
+      </c>
+      <c r="D26">
+        <v>9163</v>
+      </c>
+      <c r="E26">
+        <v>9353</v>
+      </c>
+      <c r="F26">
+        <f t="shared" ref="F26" si="16">E26-D26</f>
+        <v>190</v>
+      </c>
+      <c r="G26" s="2">
+        <f>(E26-$D$2)/A26</f>
+        <v>118.12</v>
+      </c>
+      <c r="H26" s="2">
+        <f t="shared" ref="H26" si="17">(E26/D26-1)*100</f>
+        <v>2.0735566954054319</v>
+      </c>
+      <c r="I26" s="2">
+        <f t="shared" ref="I26" si="18">(POWER((E26/$D$3),1/A26)-1)*100</f>
+        <v>1.5291706005972516</v>
+      </c>
+      <c r="J26" s="3">
+        <f t="shared" si="5"/>
+        <v>8725.828291996495</v>
+      </c>
+      <c r="K26" s="3">
+        <f t="shared" ref="K26" si="19">E26-J26</f>
+        <v>627.17170800350505</v>
+      </c>
+      <c r="L26">
+        <v>0</v>
+      </c>
+      <c r="M26">
+        <f t="shared" ref="M26" si="20">L26+E26</f>
+        <v>9353</v>
+      </c>
+      <c r="N26" s="2">
+        <f t="shared" ref="N26" si="21">E26/$D$2*100</f>
+        <v>146.140625</v>
+      </c>
+      <c r="O26">
+        <v>86736.1</v>
+      </c>
+      <c r="P26">
+        <v>87249.1</v>
+      </c>
+      <c r="Q26">
+        <f t="shared" ref="Q26" si="22">P26/$O$2*100</f>
+        <v>97.769159311025689</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
자동 업데이트: 2025-04-03 01:57:23
</commit_message>
<xml_diff>
--- a/data/daily_report.xlsx
+++ b/data/daily_report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c58a53286e4c1d7a/문서/GitHub/Dashboard/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="129" documentId="8_{9DD2A88B-03DA-4864-84CC-4418086E8BD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{977D2A81-1022-4F69-9EA8-7CDCAD076B6D}"/>
+  <xr:revisionPtr revIDLastSave="170" documentId="8_{9DD2A88B-03DA-4864-84CC-4418086E8BD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00C58272-3F59-453C-9024-AB7816EC47F9}"/>
   <bookViews>
-    <workbookView xWindow="6060" yWindow="3165" windowWidth="27180" windowHeight="15885" xr2:uid="{4AB8DADE-1167-4E84-9D67-55086BA93884}"/>
+    <workbookView xWindow="-26220" yWindow="1350" windowWidth="23580" windowHeight="20970" xr2:uid="{4AB8DADE-1167-4E84-9D67-55086BA93884}"/>
   </bookViews>
   <sheets>
     <sheet name="daily_report" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="24">
   <si>
     <t>Index</t>
   </si>
@@ -1089,10 +1089,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48182F73-FFD5-43FF-A3B0-19A54A277A3F}">
-  <dimension ref="A1:Q26"/>
+  <dimension ref="A1:Q32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q14" sqref="Q14"/>
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1307,7 +1307,7 @@
         <v>2.2328836529616813</v>
       </c>
       <c r="J4" s="3">
-        <f t="shared" ref="J4:J26" si="5">J3*1.013</f>
+        <f t="shared" ref="J4:J32" si="5">J3*1.013</f>
         <v>6567.4815999999983</v>
       </c>
       <c r="K4" s="3">
@@ -2698,6 +2698,378 @@
       <c r="Q26">
         <f t="shared" ref="Q26" si="22">P26/$O$2*100</f>
         <v>97.769159311025689</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" s="1">
+        <v>45744</v>
+      </c>
+      <c r="C27" t="s">
+        <v>21</v>
+      </c>
+      <c r="D27">
+        <v>9353</v>
+      </c>
+      <c r="E27">
+        <v>9353</v>
+      </c>
+      <c r="F27">
+        <f t="shared" ref="F27:F32" si="23">E27-D27</f>
+        <v>0</v>
+      </c>
+      <c r="G27" s="2">
+        <f t="shared" ref="G27:G31" si="24">(E27-$D$2)/A27</f>
+        <v>113.57692307692308</v>
+      </c>
+      <c r="H27" s="2">
+        <f t="shared" ref="H27:H32" si="25">(E27/D27-1)*100</f>
+        <v>0</v>
+      </c>
+      <c r="I27" s="2">
+        <f t="shared" ref="I27:I32" si="26">(POWER((E27/$D$3),1/A27)-1)*100</f>
+        <v>1.4699262282590997</v>
+      </c>
+      <c r="J27" s="3">
+        <f t="shared" si="5"/>
+        <v>8839.2640597924492</v>
+      </c>
+      <c r="K27" s="3">
+        <f t="shared" ref="K27:K32" si="27">E27-J27</f>
+        <v>513.73594020755081</v>
+      </c>
+      <c r="L27">
+        <v>0</v>
+      </c>
+      <c r="M27">
+        <f t="shared" ref="M27:M32" si="28">L27+E27</f>
+        <v>9353</v>
+      </c>
+      <c r="N27" s="2">
+        <f t="shared" ref="N27:N32" si="29">E27/$D$2*100</f>
+        <v>146.140625</v>
+      </c>
+      <c r="O27">
+        <v>87249.1</v>
+      </c>
+      <c r="P27">
+        <v>84105.3</v>
+      </c>
+      <c r="Q27">
+        <f t="shared" ref="Q27:Q32" si="30">P27/$O$2*100</f>
+        <v>94.246295659228679</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" s="1">
+        <v>45745</v>
+      </c>
+      <c r="C28" t="s">
+        <v>22</v>
+      </c>
+      <c r="D28">
+        <v>9353</v>
+      </c>
+      <c r="E28">
+        <v>9400</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="23"/>
+        <v>47</v>
+      </c>
+      <c r="G28" s="2">
+        <f t="shared" si="24"/>
+        <v>111.11111111111111</v>
+      </c>
+      <c r="H28" s="2">
+        <f t="shared" si="25"/>
+        <v>0.50251256281406143</v>
+      </c>
+      <c r="I28" s="2">
+        <f t="shared" si="26"/>
+        <v>1.433930583006493</v>
+      </c>
+      <c r="J28" s="3">
+        <f t="shared" si="5"/>
+        <v>8954.1744925697494</v>
+      </c>
+      <c r="K28" s="3">
+        <f t="shared" si="27"/>
+        <v>445.82550743025058</v>
+      </c>
+      <c r="L28">
+        <v>0</v>
+      </c>
+      <c r="M28">
+        <f t="shared" si="28"/>
+        <v>9400</v>
+      </c>
+      <c r="N28" s="2">
+        <f t="shared" si="29"/>
+        <v>146.875</v>
+      </c>
+      <c r="O28">
+        <v>84105.3</v>
+      </c>
+      <c r="P28">
+        <v>82428.800000000003</v>
+      </c>
+      <c r="Q28">
+        <f t="shared" si="30"/>
+        <v>92.367651689434894</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" s="1">
+        <v>45746</v>
+      </c>
+      <c r="C29" t="s">
+        <v>23</v>
+      </c>
+      <c r="D29">
+        <v>9400</v>
+      </c>
+      <c r="E29">
+        <v>9450</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="23"/>
+        <v>50</v>
+      </c>
+      <c r="G29" s="2">
+        <f t="shared" si="24"/>
+        <v>108.92857142857143</v>
+      </c>
+      <c r="H29" s="2">
+        <f t="shared" si="25"/>
+        <v>0.53191489361701372</v>
+      </c>
+      <c r="I29" s="2">
+        <f t="shared" si="26"/>
+        <v>1.4015768054668865</v>
+      </c>
+      <c r="J29" s="3">
+        <f t="shared" si="5"/>
+        <v>9070.578760973156</v>
+      </c>
+      <c r="K29" s="3">
+        <f t="shared" si="27"/>
+        <v>379.42123902684398</v>
+      </c>
+      <c r="L29">
+        <v>0</v>
+      </c>
+      <c r="M29">
+        <f t="shared" si="28"/>
+        <v>9450</v>
+      </c>
+      <c r="N29" s="2">
+        <f t="shared" si="29"/>
+        <v>147.65625</v>
+      </c>
+      <c r="O29">
+        <v>82428.800000000003</v>
+      </c>
+      <c r="P29">
+        <v>82745.100000000006</v>
+      </c>
+      <c r="Q29">
+        <f t="shared" si="30"/>
+        <v>92.72208955859432</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" s="1">
+        <v>45747</v>
+      </c>
+      <c r="C30" t="s">
+        <v>17</v>
+      </c>
+      <c r="D30">
+        <v>9450</v>
+      </c>
+      <c r="E30">
+        <v>9452</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="23"/>
+        <v>2</v>
+      </c>
+      <c r="G30" s="2">
+        <f t="shared" si="24"/>
+        <v>105.24137931034483</v>
+      </c>
+      <c r="H30" s="2">
+        <f t="shared" si="25"/>
+        <v>2.1164021164010727E-2</v>
+      </c>
+      <c r="I30" s="2">
+        <f t="shared" si="26"/>
+        <v>1.3536607182727423</v>
+      </c>
+      <c r="J30" s="3">
+        <f t="shared" si="5"/>
+        <v>9188.496284865807</v>
+      </c>
+      <c r="K30" s="3">
+        <f t="shared" si="27"/>
+        <v>263.50371513419304</v>
+      </c>
+      <c r="L30">
+        <v>0</v>
+      </c>
+      <c r="M30">
+        <f t="shared" si="28"/>
+        <v>9452</v>
+      </c>
+      <c r="N30" s="2">
+        <f t="shared" si="29"/>
+        <v>147.6875</v>
+      </c>
+      <c r="O30">
+        <v>82745.100000000006</v>
+      </c>
+      <c r="P30">
+        <v>83448.100000000006</v>
+      </c>
+      <c r="Q30">
+        <f t="shared" si="30"/>
+        <v>93.509853776169635</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" s="1">
+        <v>45748</v>
+      </c>
+      <c r="C31" t="s">
+        <v>18</v>
+      </c>
+      <c r="D31">
+        <v>9452</v>
+      </c>
+      <c r="E31">
+        <v>9454</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="23"/>
+        <v>2</v>
+      </c>
+      <c r="G31" s="2">
+        <f t="shared" si="24"/>
+        <v>101.8</v>
+      </c>
+      <c r="H31" s="2">
+        <f t="shared" si="25"/>
+        <v>2.1159542953874677E-2</v>
+      </c>
+      <c r="I31" s="2">
+        <f t="shared" si="26"/>
+        <v>1.3089593141764722</v>
+      </c>
+      <c r="J31" s="3">
+        <f t="shared" si="5"/>
+        <v>9307.9467365690616</v>
+      </c>
+      <c r="K31" s="3">
+        <f t="shared" si="27"/>
+        <v>146.05326343093839</v>
+      </c>
+      <c r="L31">
+        <v>0</v>
+      </c>
+      <c r="M31">
+        <f t="shared" si="28"/>
+        <v>9454</v>
+      </c>
+      <c r="N31" s="2">
+        <f t="shared" si="29"/>
+        <v>147.71875</v>
+      </c>
+      <c r="O31">
+        <v>83448.100000000006</v>
+      </c>
+      <c r="P31">
+        <v>84138.9</v>
+      </c>
+      <c r="Q31">
+        <f t="shared" si="30"/>
+        <v>94.2839469788738</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" s="1">
+        <v>45749</v>
+      </c>
+      <c r="C32" t="s">
+        <v>19</v>
+      </c>
+      <c r="D32">
+        <v>9454</v>
+      </c>
+      <c r="E32">
+        <v>9456</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="23"/>
+        <v>2</v>
+      </c>
+      <c r="G32" s="2">
+        <f>(E32-$D$2)/A32</f>
+        <v>98.58064516129032</v>
+      </c>
+      <c r="H32" s="2">
+        <f t="shared" si="25"/>
+        <v>2.1155066638467446E-2</v>
+      </c>
+      <c r="I32" s="2">
+        <f t="shared" si="26"/>
+        <v>1.2671595739860209</v>
+      </c>
+      <c r="J32" s="3">
+        <f t="shared" si="5"/>
+        <v>9428.9500441444579</v>
+      </c>
+      <c r="K32" s="3">
+        <f t="shared" si="27"/>
+        <v>27.049955855542066</v>
+      </c>
+      <c r="L32">
+        <v>0</v>
+      </c>
+      <c r="M32">
+        <f t="shared" si="28"/>
+        <v>9456</v>
+      </c>
+      <c r="N32" s="2">
+        <f t="shared" si="29"/>
+        <v>147.75</v>
+      </c>
+      <c r="O32">
+        <v>84138.9</v>
+      </c>
+      <c r="P32">
+        <v>85827.9</v>
+      </c>
+      <c r="Q32">
+        <f t="shared" si="30"/>
+        <v>96.176598136035565</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
자동 업데이트: 2025-04-12 01:03:43
</commit_message>
<xml_diff>
--- a/data/daily_report.xlsx
+++ b/data/daily_report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c58a53286e4c1d7a/문서/GitHub/Dashboard/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="170" documentId="8_{9DD2A88B-03DA-4864-84CC-4418086E8BD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00C58272-3F59-453C-9024-AB7816EC47F9}"/>
+  <xr:revisionPtr revIDLastSave="207" documentId="8_{9DD2A88B-03DA-4864-84CC-4418086E8BD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{489BD9FD-DBA7-4441-8847-3841177F407E}"/>
   <bookViews>
-    <workbookView xWindow="-26220" yWindow="1350" windowWidth="23580" windowHeight="20970" xr2:uid="{4AB8DADE-1167-4E84-9D67-55086BA93884}"/>
+    <workbookView xWindow="16215" yWindow="300" windowWidth="21975" windowHeight="20970" xr2:uid="{4AB8DADE-1167-4E84-9D67-55086BA93884}"/>
   </bookViews>
   <sheets>
     <sheet name="daily_report" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="24">
   <si>
     <t>Index</t>
   </si>
@@ -1089,10 +1089,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48182F73-FFD5-43FF-A3B0-19A54A277A3F}">
-  <dimension ref="A1:Q32"/>
+  <dimension ref="A1:Q44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M23" sqref="M23"/>
+      <selection activeCell="Q41" sqref="Q41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1189,7 +1189,8 @@
         <f>D2</f>
         <v>6400</v>
       </c>
-      <c r="K2">
+      <c r="K2" s="3">
+        <f t="shared" ref="K2:K36" si="0">M2-J2</f>
         <v>0</v>
       </c>
       <c r="L2">
@@ -1199,7 +1200,8 @@
         <f>L2+E2</f>
         <v>6400</v>
       </c>
-      <c r="N2">
+      <c r="N2" s="2">
+        <f t="shared" ref="N2:N36" si="1">M2/$D$2*100</f>
         <v>100</v>
       </c>
       <c r="O2">
@@ -1229,11 +1231,11 @@
         <v>6546</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F24" si="0">E3-D3</f>
+        <f t="shared" ref="F3:F24" si="2">E3-D3</f>
         <v>146</v>
       </c>
       <c r="G3" s="2">
-        <f t="shared" ref="G3:G22" si="1">(E3-$D$2)/A3</f>
+        <f t="shared" ref="G3:G22" si="3">(E3-$D$2)/A3</f>
         <v>146</v>
       </c>
       <c r="H3" s="2">
@@ -1249,18 +1251,18 @@
         <v>6483.1999999999989</v>
       </c>
       <c r="K3" s="3">
-        <f>E3-J3</f>
+        <f t="shared" si="0"/>
         <v>62.800000000001091</v>
       </c>
       <c r="L3">
         <v>0</v>
       </c>
       <c r="M3">
-        <f t="shared" ref="M3:M24" si="2">L3+E3</f>
+        <f t="shared" ref="M3:M24" si="4">L3+E3</f>
         <v>6546</v>
       </c>
       <c r="N3" s="2">
-        <f>E3/$D$2*100</f>
+        <f t="shared" si="1"/>
         <v>102.28124999999999</v>
       </c>
       <c r="O3">
@@ -1291,38 +1293,38 @@
         <v>6689</v>
       </c>
       <c r="F4">
+        <f t="shared" si="2"/>
+        <v>143</v>
+      </c>
+      <c r="G4" s="2">
+        <f t="shared" si="3"/>
+        <v>144.5</v>
+      </c>
+      <c r="H4" s="2">
+        <f t="shared" ref="H4:H24" si="5">(E4/D4-1)*100</f>
+        <v>2.1845401772074613</v>
+      </c>
+      <c r="I4" s="2">
+        <f t="shared" ref="I4:I24" si="6">(POWER((E4/$D$3),1/A4)-1)*100</f>
+        <v>2.2328836529616813</v>
+      </c>
+      <c r="J4" s="3">
+        <f t="shared" ref="J4:J44" si="7">J3*1.013</f>
+        <v>6567.4815999999983</v>
+      </c>
+      <c r="K4" s="3">
         <f t="shared" si="0"/>
-        <v>143</v>
-      </c>
-      <c r="G4" s="2">
+        <v>121.51840000000175</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <f t="shared" si="4"/>
+        <v>6689</v>
+      </c>
+      <c r="N4" s="2">
         <f t="shared" si="1"/>
-        <v>144.5</v>
-      </c>
-      <c r="H4" s="2">
-        <f t="shared" ref="H4:H24" si="3">(E4/D4-1)*100</f>
-        <v>2.1845401772074613</v>
-      </c>
-      <c r="I4" s="2">
-        <f t="shared" ref="I4:I24" si="4">(POWER((E4/$D$3),1/A4)-1)*100</f>
-        <v>2.2328836529616813</v>
-      </c>
-      <c r="J4" s="3">
-        <f t="shared" ref="J4:J32" si="5">J3*1.013</f>
-        <v>6567.4815999999983</v>
-      </c>
-      <c r="K4" s="3">
-        <f t="shared" ref="K4:K24" si="6">E4-J4</f>
-        <v>121.51840000000175</v>
-      </c>
-      <c r="L4">
-        <v>0</v>
-      </c>
-      <c r="M4">
-        <f t="shared" si="2"/>
-        <v>6689</v>
-      </c>
-      <c r="N4" s="2">
-        <f t="shared" ref="N4:N24" si="7">E4/$D$2*100</f>
         <v>104.515625</v>
       </c>
       <c r="O4">
@@ -1353,38 +1355,38 @@
         <v>6846</v>
       </c>
       <c r="F5">
+        <f t="shared" si="2"/>
+        <v>157</v>
+      </c>
+      <c r="G5" s="2">
+        <f t="shared" si="3"/>
+        <v>148.66666666666666</v>
+      </c>
+      <c r="H5" s="2">
+        <f t="shared" si="5"/>
+        <v>2.3471370907460098</v>
+      </c>
+      <c r="I5" s="2">
+        <f t="shared" si="6"/>
+        <v>2.2709539535396894</v>
+      </c>
+      <c r="J5" s="3">
+        <f t="shared" si="7"/>
+        <v>6652.8588607999973</v>
+      </c>
+      <c r="K5" s="3">
         <f t="shared" si="0"/>
-        <v>157</v>
-      </c>
-      <c r="G5" s="2">
+        <v>193.14113920000273</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="4"/>
+        <v>6846</v>
+      </c>
+      <c r="N5" s="2">
         <f t="shared" si="1"/>
-        <v>148.66666666666666</v>
-      </c>
-      <c r="H5" s="2">
-        <f t="shared" si="3"/>
-        <v>2.3471370907460098</v>
-      </c>
-      <c r="I5" s="2">
-        <f t="shared" si="4"/>
-        <v>2.2709539535396894</v>
-      </c>
-      <c r="J5" s="3">
-        <f t="shared" si="5"/>
-        <v>6652.8588607999973</v>
-      </c>
-      <c r="K5" s="3">
-        <f t="shared" si="6"/>
-        <v>193.14113920000273</v>
-      </c>
-      <c r="L5">
-        <v>0</v>
-      </c>
-      <c r="M5">
-        <f t="shared" si="2"/>
-        <v>6846</v>
-      </c>
-      <c r="N5" s="2">
-        <f t="shared" si="7"/>
         <v>106.96874999999999</v>
       </c>
       <c r="O5">
@@ -1415,38 +1417,38 @@
         <v>7015</v>
       </c>
       <c r="F6">
+        <f t="shared" si="2"/>
+        <v>169</v>
+      </c>
+      <c r="G6" s="2">
+        <f t="shared" si="3"/>
+        <v>153.75</v>
+      </c>
+      <c r="H6" s="2">
+        <f t="shared" si="5"/>
+        <v>2.4685947998831503</v>
+      </c>
+      <c r="I6" s="2">
+        <f t="shared" si="6"/>
+        <v>2.3203283980714806</v>
+      </c>
+      <c r="J6" s="3">
+        <f t="shared" si="7"/>
+        <v>6739.3460259903968</v>
+      </c>
+      <c r="K6" s="3">
         <f t="shared" si="0"/>
-        <v>169</v>
-      </c>
-      <c r="G6" s="2">
+        <v>275.65397400960319</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="4"/>
+        <v>7015</v>
+      </c>
+      <c r="N6" s="2">
         <f t="shared" si="1"/>
-        <v>153.75</v>
-      </c>
-      <c r="H6" s="2">
-        <f t="shared" si="3"/>
-        <v>2.4685947998831503</v>
-      </c>
-      <c r="I6" s="2">
-        <f t="shared" si="4"/>
-        <v>2.3203283980714806</v>
-      </c>
-      <c r="J6" s="3">
-        <f t="shared" si="5"/>
-        <v>6739.3460259903968</v>
-      </c>
-      <c r="K6" s="3">
-        <f t="shared" si="6"/>
-        <v>275.65397400960319</v>
-      </c>
-      <c r="L6">
-        <v>0</v>
-      </c>
-      <c r="M6">
-        <f t="shared" si="2"/>
-        <v>7015</v>
-      </c>
-      <c r="N6" s="2">
-        <f t="shared" si="7"/>
         <v>109.60937500000001</v>
       </c>
       <c r="O6">
@@ -1477,38 +1479,38 @@
         <v>7050</v>
       </c>
       <c r="F7">
+        <f t="shared" si="2"/>
+        <v>35</v>
+      </c>
+      <c r="G7" s="2">
+        <f t="shared" si="3"/>
+        <v>130</v>
+      </c>
+      <c r="H7" s="2">
+        <f t="shared" si="5"/>
+        <v>0.49893086243764095</v>
+      </c>
+      <c r="I7" s="2">
+        <f t="shared" si="6"/>
+        <v>1.9534270313376956</v>
+      </c>
+      <c r="J7" s="3">
+        <f t="shared" si="7"/>
+        <v>6826.9575243282716</v>
+      </c>
+      <c r="K7" s="3">
         <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-      <c r="G7" s="2">
+        <v>223.04247567172843</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="4"/>
+        <v>7050</v>
+      </c>
+      <c r="N7" s="2">
         <f t="shared" si="1"/>
-        <v>130</v>
-      </c>
-      <c r="H7" s="2">
-        <f t="shared" si="3"/>
-        <v>0.49893086243764095</v>
-      </c>
-      <c r="I7" s="2">
-        <f t="shared" si="4"/>
-        <v>1.9534270313376956</v>
-      </c>
-      <c r="J7" s="3">
-        <f t="shared" si="5"/>
-        <v>6826.9575243282716</v>
-      </c>
-      <c r="K7" s="3">
-        <f t="shared" si="6"/>
-        <v>223.04247567172843</v>
-      </c>
-      <c r="L7">
-        <v>0</v>
-      </c>
-      <c r="M7">
-        <f t="shared" si="2"/>
-        <v>7050</v>
-      </c>
-      <c r="N7" s="2">
-        <f t="shared" si="7"/>
         <v>110.15625</v>
       </c>
       <c r="O7">
@@ -1539,38 +1541,38 @@
         <v>6979</v>
       </c>
       <c r="F8">
+        <f t="shared" si="2"/>
+        <v>-71</v>
+      </c>
+      <c r="G8" s="2">
+        <f t="shared" si="3"/>
+        <v>96.5</v>
+      </c>
+      <c r="H8" s="2">
+        <f t="shared" si="5"/>
+        <v>-1.0070921985815606</v>
+      </c>
+      <c r="I8" s="2">
+        <f t="shared" si="6"/>
+        <v>1.4539290311231801</v>
+      </c>
+      <c r="J8" s="3">
+        <f t="shared" si="7"/>
+        <v>6915.7079721445389</v>
+      </c>
+      <c r="K8" s="3">
         <f t="shared" si="0"/>
-        <v>-71</v>
-      </c>
-      <c r="G8" s="2">
+        <v>63.292027855461129</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="4"/>
+        <v>6979</v>
+      </c>
+      <c r="N8" s="2">
         <f t="shared" si="1"/>
-        <v>96.5</v>
-      </c>
-      <c r="H8" s="2">
-        <f t="shared" si="3"/>
-        <v>-1.0070921985815606</v>
-      </c>
-      <c r="I8" s="2">
-        <f t="shared" si="4"/>
-        <v>1.4539290311231801</v>
-      </c>
-      <c r="J8" s="3">
-        <f t="shared" si="5"/>
-        <v>6915.7079721445389</v>
-      </c>
-      <c r="K8" s="3">
-        <f t="shared" si="6"/>
-        <v>63.292027855461129</v>
-      </c>
-      <c r="L8">
-        <v>0</v>
-      </c>
-      <c r="M8">
-        <f t="shared" si="2"/>
-        <v>6979</v>
-      </c>
-      <c r="N8" s="2">
-        <f t="shared" si="7"/>
         <v>109.04687500000001</v>
       </c>
       <c r="O8">
@@ -1601,38 +1603,38 @@
         <v>7170</v>
       </c>
       <c r="F9">
+        <f t="shared" si="2"/>
+        <v>191</v>
+      </c>
+      <c r="G9" s="2">
+        <f t="shared" si="3"/>
+        <v>96.25</v>
+      </c>
+      <c r="H9" s="2">
+        <f t="shared" si="5"/>
+        <v>2.7367817738931155</v>
+      </c>
+      <c r="I9" s="2">
+        <f t="shared" si="6"/>
+        <v>1.4302270645888626</v>
+      </c>
+      <c r="J9" s="3">
+        <f t="shared" si="7"/>
+        <v>7005.6121757824176</v>
+      </c>
+      <c r="K9" s="3">
         <f t="shared" si="0"/>
-        <v>191</v>
-      </c>
-      <c r="G9" s="2">
+        <v>164.38782421758242</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="4"/>
+        <v>7170</v>
+      </c>
+      <c r="N9" s="2">
         <f t="shared" si="1"/>
-        <v>96.25</v>
-      </c>
-      <c r="H9" s="2">
-        <f t="shared" si="3"/>
-        <v>2.7367817738931155</v>
-      </c>
-      <c r="I9" s="2">
-        <f t="shared" si="4"/>
-        <v>1.4302270645888626</v>
-      </c>
-      <c r="J9" s="3">
-        <f t="shared" si="5"/>
-        <v>7005.6121757824176</v>
-      </c>
-      <c r="K9" s="3">
-        <f t="shared" si="6"/>
-        <v>164.38782421758242</v>
-      </c>
-      <c r="L9">
-        <v>0</v>
-      </c>
-      <c r="M9">
-        <f t="shared" si="2"/>
-        <v>7170</v>
-      </c>
-      <c r="N9" s="2">
-        <f t="shared" si="7"/>
         <v>112.03125</v>
       </c>
       <c r="O9">
@@ -1663,38 +1665,38 @@
         <v>7315</v>
       </c>
       <c r="F10">
+        <f t="shared" si="2"/>
+        <v>145</v>
+      </c>
+      <c r="G10" s="2">
+        <f t="shared" si="3"/>
+        <v>101.66666666666667</v>
+      </c>
+      <c r="H10" s="2">
+        <f t="shared" si="5"/>
+        <v>2.0223152022315283</v>
+      </c>
+      <c r="I10" s="2">
+        <f t="shared" si="6"/>
+        <v>1.4958445810377752</v>
+      </c>
+      <c r="J10" s="3">
+        <f t="shared" si="7"/>
+        <v>7096.6851340675885</v>
+      </c>
+      <c r="K10" s="3">
         <f t="shared" si="0"/>
-        <v>145</v>
-      </c>
-      <c r="G10" s="2">
+        <v>218.31486593241152</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="4"/>
+        <v>7315</v>
+      </c>
+      <c r="N10" s="2">
         <f t="shared" si="1"/>
-        <v>101.66666666666667</v>
-      </c>
-      <c r="H10" s="2">
-        <f t="shared" si="3"/>
-        <v>2.0223152022315283</v>
-      </c>
-      <c r="I10" s="2">
-        <f t="shared" si="4"/>
-        <v>1.4958445810377752</v>
-      </c>
-      <c r="J10" s="3">
-        <f t="shared" si="5"/>
-        <v>7096.6851340675885</v>
-      </c>
-      <c r="K10" s="3">
-        <f t="shared" si="6"/>
-        <v>218.31486593241152</v>
-      </c>
-      <c r="L10">
-        <v>0</v>
-      </c>
-      <c r="M10">
-        <f t="shared" si="2"/>
-        <v>7315</v>
-      </c>
-      <c r="N10" s="2">
-        <f t="shared" si="7"/>
         <v>114.29687500000001</v>
       </c>
       <c r="O10">
@@ -1725,38 +1727,38 @@
         <v>6845</v>
       </c>
       <c r="F11">
+        <f t="shared" si="2"/>
+        <v>-470</v>
+      </c>
+      <c r="G11" s="2">
+        <f t="shared" si="3"/>
+        <v>44.5</v>
+      </c>
+      <c r="H11" s="2">
+        <f t="shared" si="5"/>
+        <v>-6.4251537935748448</v>
+      </c>
+      <c r="I11" s="2">
+        <f t="shared" si="6"/>
+        <v>0.67446905031474103</v>
+      </c>
+      <c r="J11" s="3">
+        <f t="shared" si="7"/>
+        <v>7188.9420408104661</v>
+      </c>
+      <c r="K11" s="3">
         <f t="shared" si="0"/>
-        <v>-470</v>
-      </c>
-      <c r="G11" s="2">
+        <v>-343.9420408104661</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="4"/>
+        <v>6845</v>
+      </c>
+      <c r="N11" s="2">
         <f t="shared" si="1"/>
-        <v>44.5</v>
-      </c>
-      <c r="H11" s="2">
-        <f t="shared" si="3"/>
-        <v>-6.4251537935748448</v>
-      </c>
-      <c r="I11" s="2">
-        <f t="shared" si="4"/>
-        <v>0.67446905031474103</v>
-      </c>
-      <c r="J11" s="3">
-        <f t="shared" si="5"/>
-        <v>7188.9420408104661</v>
-      </c>
-      <c r="K11" s="3">
-        <f t="shared" si="6"/>
-        <v>-343.9420408104661</v>
-      </c>
-      <c r="L11">
-        <v>0</v>
-      </c>
-      <c r="M11">
-        <f t="shared" si="2"/>
-        <v>6845</v>
-      </c>
-      <c r="N11" s="2">
-        <f t="shared" si="7"/>
         <v>106.953125</v>
       </c>
       <c r="O11">
@@ -1787,38 +1789,38 @@
         <v>7567</v>
       </c>
       <c r="F12">
+        <f t="shared" si="2"/>
+        <v>722</v>
+      </c>
+      <c r="G12" s="2">
+        <f t="shared" si="3"/>
+        <v>106.09090909090909</v>
+      </c>
+      <c r="H12" s="2">
+        <f t="shared" si="5"/>
+        <v>10.547845142439737</v>
+      </c>
+      <c r="I12" s="2">
+        <f t="shared" si="6"/>
+        <v>1.5343678109079883</v>
+      </c>
+      <c r="J12" s="3">
+        <f t="shared" si="7"/>
+        <v>7282.3982873410014</v>
+      </c>
+      <c r="K12" s="3">
         <f t="shared" si="0"/>
-        <v>722</v>
-      </c>
-      <c r="G12" s="2">
+        <v>284.60171265899862</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="4"/>
+        <v>7567</v>
+      </c>
+      <c r="N12" s="2">
         <f t="shared" si="1"/>
-        <v>106.09090909090909</v>
-      </c>
-      <c r="H12" s="2">
-        <f t="shared" si="3"/>
-        <v>10.547845142439737</v>
-      </c>
-      <c r="I12" s="2">
-        <f t="shared" si="4"/>
-        <v>1.5343678109079883</v>
-      </c>
-      <c r="J12" s="3">
-        <f t="shared" si="5"/>
-        <v>7282.3982873410014</v>
-      </c>
-      <c r="K12" s="3">
-        <f t="shared" si="6"/>
-        <v>284.60171265899862</v>
-      </c>
-      <c r="L12">
-        <v>0</v>
-      </c>
-      <c r="M12">
-        <f t="shared" si="2"/>
-        <v>7567</v>
-      </c>
-      <c r="N12" s="2">
-        <f t="shared" si="7"/>
         <v>118.234375</v>
       </c>
       <c r="O12">
@@ -1849,38 +1851,38 @@
         <v>7763</v>
       </c>
       <c r="F13">
+        <f t="shared" si="2"/>
+        <v>196</v>
+      </c>
+      <c r="G13" s="2">
+        <f t="shared" si="3"/>
+        <v>113.58333333333333</v>
+      </c>
+      <c r="H13" s="2">
+        <f t="shared" si="5"/>
+        <v>2.5901942645698339</v>
+      </c>
+      <c r="I13" s="2">
+        <f t="shared" si="6"/>
+        <v>1.6219367680212704</v>
+      </c>
+      <c r="J13" s="3">
+        <f t="shared" si="7"/>
+        <v>7377.0694650764335</v>
+      </c>
+      <c r="K13" s="3">
         <f t="shared" si="0"/>
-        <v>196</v>
-      </c>
-      <c r="G13" s="2">
+        <v>385.93053492356648</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="4"/>
+        <v>7763</v>
+      </c>
+      <c r="N13" s="2">
         <f t="shared" si="1"/>
-        <v>113.58333333333333</v>
-      </c>
-      <c r="H13" s="2">
-        <f t="shared" si="3"/>
-        <v>2.5901942645698339</v>
-      </c>
-      <c r="I13" s="2">
-        <f t="shared" si="4"/>
-        <v>1.6219367680212704</v>
-      </c>
-      <c r="J13" s="3">
-        <f t="shared" si="5"/>
-        <v>7377.0694650764335</v>
-      </c>
-      <c r="K13" s="3">
-        <f t="shared" si="6"/>
-        <v>385.93053492356648</v>
-      </c>
-      <c r="L13">
-        <v>0</v>
-      </c>
-      <c r="M13">
-        <f t="shared" si="2"/>
-        <v>7763</v>
-      </c>
-      <c r="N13" s="2">
-        <f t="shared" si="7"/>
         <v>121.296875</v>
       </c>
       <c r="O13">
@@ -1911,38 +1913,38 @@
         <v>7845</v>
       </c>
       <c r="F14">
+        <f t="shared" si="2"/>
+        <v>82</v>
+      </c>
+      <c r="G14" s="2">
+        <f t="shared" si="3"/>
+        <v>111.15384615384616</v>
+      </c>
+      <c r="H14" s="2">
+        <f t="shared" si="5"/>
+        <v>1.0562926703594044</v>
+      </c>
+      <c r="I14" s="2">
+        <f t="shared" si="6"/>
+        <v>1.5783135032505946</v>
+      </c>
+      <c r="J14" s="3">
+        <f t="shared" si="7"/>
+        <v>7472.9713681224266</v>
+      </c>
+      <c r="K14" s="3">
         <f t="shared" si="0"/>
-        <v>82</v>
-      </c>
-      <c r="G14" s="2">
+        <v>372.02863187757339</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="4"/>
+        <v>7845</v>
+      </c>
+      <c r="N14" s="2">
         <f t="shared" si="1"/>
-        <v>111.15384615384616</v>
-      </c>
-      <c r="H14" s="2">
-        <f t="shared" si="3"/>
-        <v>1.0562926703594044</v>
-      </c>
-      <c r="I14" s="2">
-        <f t="shared" si="4"/>
-        <v>1.5783135032505946</v>
-      </c>
-      <c r="J14" s="3">
-        <f t="shared" si="5"/>
-        <v>7472.9713681224266</v>
-      </c>
-      <c r="K14" s="3">
-        <f t="shared" si="6"/>
-        <v>372.02863187757339</v>
-      </c>
-      <c r="L14">
-        <v>0</v>
-      </c>
-      <c r="M14">
-        <f t="shared" si="2"/>
-        <v>7845</v>
-      </c>
-      <c r="N14" s="2">
-        <f t="shared" si="7"/>
         <v>122.578125</v>
       </c>
       <c r="O14">
@@ -1973,38 +1975,38 @@
         <v>7879</v>
       </c>
       <c r="F15">
+        <f t="shared" si="2"/>
+        <v>34</v>
+      </c>
+      <c r="G15" s="2">
+        <f t="shared" si="3"/>
+        <v>105.64285714285714</v>
+      </c>
+      <c r="H15" s="2">
+        <f t="shared" si="5"/>
+        <v>0.43339706819629509</v>
+      </c>
+      <c r="I15" s="2">
+        <f t="shared" si="6"/>
+        <v>1.4961026704697122</v>
+      </c>
+      <c r="J15" s="3">
+        <f t="shared" si="7"/>
+        <v>7570.1199959080177</v>
+      </c>
+      <c r="K15" s="3">
         <f t="shared" si="0"/>
-        <v>34</v>
-      </c>
-      <c r="G15" s="2">
+        <v>308.8800040919823</v>
+      </c>
+      <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="4"/>
+        <v>7879</v>
+      </c>
+      <c r="N15" s="2">
         <f t="shared" si="1"/>
-        <v>105.64285714285714</v>
-      </c>
-      <c r="H15" s="2">
-        <f t="shared" si="3"/>
-        <v>0.43339706819629509</v>
-      </c>
-      <c r="I15" s="2">
-        <f t="shared" si="4"/>
-        <v>1.4961026704697122</v>
-      </c>
-      <c r="J15" s="3">
-        <f t="shared" si="5"/>
-        <v>7570.1199959080177</v>
-      </c>
-      <c r="K15" s="3">
-        <f t="shared" si="6"/>
-        <v>308.8800040919823</v>
-      </c>
-      <c r="L15">
-        <v>0</v>
-      </c>
-      <c r="M15">
-        <f t="shared" si="2"/>
-        <v>7879</v>
-      </c>
-      <c r="N15" s="2">
-        <f t="shared" si="7"/>
         <v>123.10937500000001</v>
       </c>
       <c r="O15">
@@ -2035,38 +2037,38 @@
         <v>7952</v>
       </c>
       <c r="F16">
+        <f t="shared" si="2"/>
+        <v>73</v>
+      </c>
+      <c r="G16" s="2">
+        <f t="shared" si="3"/>
+        <v>103.46666666666667</v>
+      </c>
+      <c r="H16" s="2">
+        <f t="shared" si="5"/>
+        <v>0.92651351694377215</v>
+      </c>
+      <c r="I16" s="2">
+        <f t="shared" si="6"/>
+        <v>1.4580302525748934</v>
+      </c>
+      <c r="J16" s="3">
+        <f t="shared" si="7"/>
+        <v>7668.5315558548209</v>
+      </c>
+      <c r="K16" s="3">
         <f t="shared" si="0"/>
-        <v>73</v>
-      </c>
-      <c r="G16" s="2">
+        <v>283.46844414517909</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="4"/>
+        <v>7952</v>
+      </c>
+      <c r="N16" s="2">
         <f t="shared" si="1"/>
-        <v>103.46666666666667</v>
-      </c>
-      <c r="H16" s="2">
-        <f t="shared" si="3"/>
-        <v>0.92651351694377215</v>
-      </c>
-      <c r="I16" s="2">
-        <f t="shared" si="4"/>
-        <v>1.4580302525748934</v>
-      </c>
-      <c r="J16" s="3">
-        <f t="shared" si="5"/>
-        <v>7668.5315558548209</v>
-      </c>
-      <c r="K16" s="3">
-        <f t="shared" si="6"/>
-        <v>283.46844414517909</v>
-      </c>
-      <c r="L16">
-        <v>0</v>
-      </c>
-      <c r="M16">
-        <f t="shared" si="2"/>
-        <v>7952</v>
-      </c>
-      <c r="N16" s="2">
-        <f t="shared" si="7"/>
         <v>124.25</v>
       </c>
       <c r="O16">
@@ -2097,38 +2099,38 @@
         <v>7797</v>
       </c>
       <c r="F17">
+        <f t="shared" si="2"/>
+        <v>-155</v>
+      </c>
+      <c r="G17" s="2">
+        <f t="shared" si="3"/>
+        <v>87.3125</v>
+      </c>
+      <c r="H17" s="2">
+        <f t="shared" si="5"/>
+        <v>-1.9491951710261524</v>
+      </c>
+      <c r="I17" s="2">
+        <f t="shared" si="6"/>
+        <v>1.2416518639221996</v>
+      </c>
+      <c r="J17" s="3">
+        <f t="shared" si="7"/>
+        <v>7768.2224660809325</v>
+      </c>
+      <c r="K17" s="3">
         <f t="shared" si="0"/>
-        <v>-155</v>
-      </c>
-      <c r="G17" s="2">
+        <v>28.777533919067537</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <f t="shared" si="4"/>
+        <v>7797</v>
+      </c>
+      <c r="N17" s="2">
         <f t="shared" si="1"/>
-        <v>87.3125</v>
-      </c>
-      <c r="H17" s="2">
-        <f t="shared" si="3"/>
-        <v>-1.9491951710261524</v>
-      </c>
-      <c r="I17" s="2">
-        <f t="shared" si="4"/>
-        <v>1.2416518639221996</v>
-      </c>
-      <c r="J17" s="3">
-        <f t="shared" si="5"/>
-        <v>7768.2224660809325</v>
-      </c>
-      <c r="K17" s="3">
-        <f t="shared" si="6"/>
-        <v>28.777533919067537</v>
-      </c>
-      <c r="L17">
-        <v>0</v>
-      </c>
-      <c r="M17">
-        <f t="shared" si="2"/>
-        <v>7797</v>
-      </c>
-      <c r="N17" s="2">
-        <f t="shared" si="7"/>
         <v>121.828125</v>
       </c>
       <c r="O17">
@@ -2159,38 +2161,38 @@
         <v>8335</v>
       </c>
       <c r="F18">
+        <f t="shared" si="2"/>
+        <v>538</v>
+      </c>
+      <c r="G18" s="2">
+        <f t="shared" si="3"/>
+        <v>113.82352941176471</v>
+      </c>
+      <c r="H18" s="2">
+        <f t="shared" si="5"/>
+        <v>6.9000897781198001</v>
+      </c>
+      <c r="I18" s="2">
+        <f t="shared" si="6"/>
+        <v>1.5660508945335661</v>
+      </c>
+      <c r="J18" s="3">
+        <f t="shared" si="7"/>
+        <v>7869.209358139984</v>
+      </c>
+      <c r="K18" s="3">
         <f t="shared" si="0"/>
-        <v>538</v>
-      </c>
-      <c r="G18" s="2">
+        <v>465.79064186001597</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <f t="shared" si="4"/>
+        <v>8335</v>
+      </c>
+      <c r="N18" s="2">
         <f t="shared" si="1"/>
-        <v>113.82352941176471</v>
-      </c>
-      <c r="H18" s="2">
-        <f t="shared" si="3"/>
-        <v>6.9000897781198001</v>
-      </c>
-      <c r="I18" s="2">
-        <f t="shared" si="4"/>
-        <v>1.5660508945335661</v>
-      </c>
-      <c r="J18" s="3">
-        <f t="shared" si="5"/>
-        <v>7869.209358139984</v>
-      </c>
-      <c r="K18" s="3">
-        <f t="shared" si="6"/>
-        <v>465.79064186001597</v>
-      </c>
-      <c r="L18">
-        <v>0</v>
-      </c>
-      <c r="M18">
-        <f t="shared" si="2"/>
-        <v>8335</v>
-      </c>
-      <c r="N18" s="2">
-        <f t="shared" si="7"/>
         <v>130.234375</v>
       </c>
       <c r="O18">
@@ -2221,38 +2223,38 @@
         <v>8461</v>
       </c>
       <c r="F19">
+        <f t="shared" si="2"/>
+        <v>126</v>
+      </c>
+      <c r="G19" s="2">
+        <f t="shared" si="3"/>
+        <v>114.5</v>
+      </c>
+      <c r="H19" s="2">
+        <f t="shared" si="5"/>
+        <v>1.5116976604679033</v>
+      </c>
+      <c r="I19" s="2">
+        <f t="shared" si="6"/>
+        <v>1.5630305070633677</v>
+      </c>
+      <c r="J19" s="3">
+        <f t="shared" si="7"/>
+        <v>7971.5090797958028</v>
+      </c>
+      <c r="K19" s="3">
         <f t="shared" si="0"/>
-        <v>126</v>
-      </c>
-      <c r="G19" s="2">
+        <v>489.49092020419721</v>
+      </c>
+      <c r="L19">
+        <v>0</v>
+      </c>
+      <c r="M19">
+        <f t="shared" si="4"/>
+        <v>8461</v>
+      </c>
+      <c r="N19" s="2">
         <f t="shared" si="1"/>
-        <v>114.5</v>
-      </c>
-      <c r="H19" s="2">
-        <f t="shared" si="3"/>
-        <v>1.5116976604679033</v>
-      </c>
-      <c r="I19" s="2">
-        <f t="shared" si="4"/>
-        <v>1.5630305070633677</v>
-      </c>
-      <c r="J19" s="3">
-        <f t="shared" si="5"/>
-        <v>7971.5090797958028</v>
-      </c>
-      <c r="K19" s="3">
-        <f t="shared" si="6"/>
-        <v>489.49092020419721</v>
-      </c>
-      <c r="L19">
-        <v>0</v>
-      </c>
-      <c r="M19">
-        <f t="shared" si="2"/>
-        <v>8461</v>
-      </c>
-      <c r="N19" s="2">
-        <f t="shared" si="7"/>
         <v>132.203125</v>
       </c>
       <c r="O19">
@@ -2283,38 +2285,38 @@
         <v>8330</v>
       </c>
       <c r="F20">
+        <f t="shared" si="2"/>
+        <v>-131</v>
+      </c>
+      <c r="G20" s="2">
+        <f t="shared" si="3"/>
+        <v>101.57894736842105</v>
+      </c>
+      <c r="H20" s="2">
+        <f t="shared" si="5"/>
+        <v>-1.5482803451128735</v>
+      </c>
+      <c r="I20" s="2">
+        <f t="shared" si="6"/>
+        <v>1.3968527401524877</v>
+      </c>
+      <c r="J20" s="3">
+        <f t="shared" si="7"/>
+        <v>8075.1386978331475</v>
+      </c>
+      <c r="K20" s="3">
         <f t="shared" si="0"/>
-        <v>-131</v>
-      </c>
-      <c r="G20" s="2">
+        <v>254.86130216685251</v>
+      </c>
+      <c r="L20">
+        <v>0</v>
+      </c>
+      <c r="M20">
+        <f t="shared" si="4"/>
+        <v>8330</v>
+      </c>
+      <c r="N20" s="2">
         <f t="shared" si="1"/>
-        <v>101.57894736842105</v>
-      </c>
-      <c r="H20" s="2">
-        <f t="shared" si="3"/>
-        <v>-1.5482803451128735</v>
-      </c>
-      <c r="I20" s="2">
-        <f t="shared" si="4"/>
-        <v>1.3968527401524877</v>
-      </c>
-      <c r="J20" s="3">
-        <f t="shared" si="5"/>
-        <v>8075.1386978331475</v>
-      </c>
-      <c r="K20" s="3">
-        <f t="shared" si="6"/>
-        <v>254.86130216685251</v>
-      </c>
-      <c r="L20">
-        <v>0</v>
-      </c>
-      <c r="M20">
-        <f t="shared" si="2"/>
-        <v>8330</v>
-      </c>
-      <c r="N20" s="2">
-        <f t="shared" si="7"/>
         <v>130.15625</v>
       </c>
       <c r="O20">
@@ -2345,38 +2347,38 @@
         <v>8331</v>
       </c>
       <c r="F21">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G21" s="2">
+        <f t="shared" si="3"/>
+        <v>96.55</v>
+      </c>
+      <c r="H21" s="2">
+        <f t="shared" si="5"/>
+        <v>1.2004801920761921E-2</v>
+      </c>
+      <c r="I21" s="2">
+        <f t="shared" si="6"/>
+        <v>1.3271571111354463</v>
+      </c>
+      <c r="J21" s="3">
+        <f t="shared" si="7"/>
+        <v>8180.115500904978</v>
+      </c>
+      <c r="K21" s="3">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="G21" s="2">
+        <v>150.88449909502197</v>
+      </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <f t="shared" si="4"/>
+        <v>8331</v>
+      </c>
+      <c r="N21" s="2">
         <f t="shared" si="1"/>
-        <v>96.55</v>
-      </c>
-      <c r="H21" s="2">
-        <f t="shared" si="3"/>
-        <v>1.2004801920761921E-2</v>
-      </c>
-      <c r="I21" s="2">
-        <f t="shared" si="4"/>
-        <v>1.3271571111354463</v>
-      </c>
-      <c r="J21" s="3">
-        <f t="shared" si="5"/>
-        <v>8180.115500904978</v>
-      </c>
-      <c r="K21" s="3">
-        <f t="shared" si="6"/>
-        <v>150.88449909502197</v>
-      </c>
-      <c r="L21">
-        <v>0</v>
-      </c>
-      <c r="M21">
-        <f t="shared" si="2"/>
-        <v>8331</v>
-      </c>
-      <c r="N21" s="2">
-        <f t="shared" si="7"/>
         <v>130.171875</v>
       </c>
       <c r="O21">
@@ -2407,38 +2409,38 @@
         <v>8590</v>
       </c>
       <c r="F22">
+        <f t="shared" si="2"/>
+        <v>259</v>
+      </c>
+      <c r="G22" s="2">
+        <f t="shared" si="3"/>
+        <v>104.28571428571429</v>
+      </c>
+      <c r="H22" s="2">
+        <f t="shared" si="5"/>
+        <v>3.1088704837354486</v>
+      </c>
+      <c r="I22" s="2">
+        <f t="shared" si="6"/>
+        <v>1.4112982170128241</v>
+      </c>
+      <c r="J22" s="3">
+        <f t="shared" si="7"/>
+        <v>8286.4570024167424</v>
+      </c>
+      <c r="K22" s="3">
         <f t="shared" si="0"/>
-        <v>259</v>
-      </c>
-      <c r="G22" s="2">
+        <v>303.5429975832576</v>
+      </c>
+      <c r="L22">
+        <v>0</v>
+      </c>
+      <c r="M22">
+        <f t="shared" si="4"/>
+        <v>8590</v>
+      </c>
+      <c r="N22" s="2">
         <f t="shared" si="1"/>
-        <v>104.28571428571429</v>
-      </c>
-      <c r="H22" s="2">
-        <f t="shared" si="3"/>
-        <v>3.1088704837354486</v>
-      </c>
-      <c r="I22" s="2">
-        <f t="shared" si="4"/>
-        <v>1.4112982170128241</v>
-      </c>
-      <c r="J22" s="3">
-        <f t="shared" si="5"/>
-        <v>8286.4570024167424</v>
-      </c>
-      <c r="K22" s="3">
-        <f t="shared" si="6"/>
-        <v>303.5429975832576</v>
-      </c>
-      <c r="L22">
-        <v>0</v>
-      </c>
-      <c r="M22">
-        <f t="shared" si="2"/>
-        <v>8590</v>
-      </c>
-      <c r="N22" s="2">
-        <f t="shared" si="7"/>
         <v>134.21875</v>
       </c>
       <c r="O22">
@@ -2469,7 +2471,7 @@
         <v>8925</v>
       </c>
       <c r="F23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>335</v>
       </c>
       <c r="G23" s="2">
@@ -2477,30 +2479,30 @@
         <v>114.77272727272727</v>
       </c>
       <c r="H23" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>3.8998835855646119</v>
       </c>
       <c r="I23" s="2">
+        <f t="shared" si="6"/>
+        <v>1.5231117007673323</v>
+      </c>
+      <c r="J23" s="3">
+        <f t="shared" si="7"/>
+        <v>8394.1809434481584</v>
+      </c>
+      <c r="K23" s="3">
+        <f t="shared" si="0"/>
+        <v>530.81905655184164</v>
+      </c>
+      <c r="L23">
+        <v>0</v>
+      </c>
+      <c r="M23">
         <f t="shared" si="4"/>
-        <v>1.5231117007673323</v>
-      </c>
-      <c r="J23" s="3">
-        <f t="shared" si="5"/>
-        <v>8394.1809434481584</v>
-      </c>
-      <c r="K23" s="3">
-        <f t="shared" si="6"/>
-        <v>530.81905655184164</v>
-      </c>
-      <c r="L23">
-        <v>0</v>
-      </c>
-      <c r="M23">
-        <f t="shared" si="2"/>
         <v>8925</v>
       </c>
       <c r="N23" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="1"/>
         <v>139.453125</v>
       </c>
       <c r="O23">
@@ -2531,7 +2533,7 @@
         <v>9113</v>
       </c>
       <c r="F24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>188</v>
       </c>
       <c r="G24" s="2">
@@ -2539,30 +2541,30 @@
         <v>117.95652173913044</v>
       </c>
       <c r="H24" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2.1064425770308093</v>
       </c>
       <c r="I24" s="2">
+        <f t="shared" si="6"/>
+        <v>1.5484044777758443</v>
+      </c>
+      <c r="J24" s="3">
+        <f t="shared" si="7"/>
+        <v>8503.3052957129839</v>
+      </c>
+      <c r="K24" s="3">
+        <f t="shared" si="0"/>
+        <v>609.69470428701607</v>
+      </c>
+      <c r="L24">
+        <v>0</v>
+      </c>
+      <c r="M24">
         <f t="shared" si="4"/>
-        <v>1.5484044777758443</v>
-      </c>
-      <c r="J24" s="3">
-        <f t="shared" si="5"/>
-        <v>8503.3052957129839</v>
-      </c>
-      <c r="K24" s="3">
-        <f t="shared" si="6"/>
-        <v>609.69470428701607</v>
-      </c>
-      <c r="L24">
-        <v>0</v>
-      </c>
-      <c r="M24">
-        <f t="shared" si="2"/>
         <v>9113</v>
       </c>
       <c r="N24" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="1"/>
         <v>142.390625</v>
       </c>
       <c r="O24">
@@ -2609,22 +2611,22 @@
         <v>1.5065509612034012</v>
       </c>
       <c r="J25" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>8613.8482645572512</v>
       </c>
       <c r="K25" s="3">
-        <f t="shared" ref="K25" si="12">E25-J25</f>
+        <f t="shared" si="0"/>
         <v>549.15173544274876</v>
       </c>
       <c r="L25">
         <v>0</v>
       </c>
       <c r="M25">
-        <f t="shared" ref="M25" si="13">L25+E25</f>
+        <f t="shared" ref="M25" si="12">L25+E25</f>
         <v>9163</v>
       </c>
       <c r="N25" s="2">
-        <f t="shared" ref="N25" si="14">E25/$D$2*100</f>
+        <f t="shared" si="1"/>
         <v>143.171875</v>
       </c>
       <c r="O25">
@@ -2634,7 +2636,7 @@
         <v>86736.1</v>
       </c>
       <c r="Q25">
-        <f t="shared" ref="Q25" si="15">P25/$O$2*100</f>
+        <f t="shared" ref="Q25" si="13">P25/$O$2*100</f>
         <v>97.194304341443697</v>
       </c>
     </row>
@@ -2655,7 +2657,7 @@
         <v>9353</v>
       </c>
       <c r="F26">
-        <f t="shared" ref="F26" si="16">E26-D26</f>
+        <f t="shared" ref="F26" si="14">E26-D26</f>
         <v>190</v>
       </c>
       <c r="G26" s="2">
@@ -2663,30 +2665,30 @@
         <v>118.12</v>
       </c>
       <c r="H26" s="2">
-        <f t="shared" ref="H26" si="17">(E26/D26-1)*100</f>
+        <f t="shared" ref="H26" si="15">(E26/D26-1)*100</f>
         <v>2.0735566954054319</v>
       </c>
       <c r="I26" s="2">
-        <f t="shared" ref="I26" si="18">(POWER((E26/$D$3),1/A26)-1)*100</f>
+        <f t="shared" ref="I26" si="16">(POWER((E26/$D$3),1/A26)-1)*100</f>
         <v>1.5291706005972516</v>
       </c>
       <c r="J26" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>8725.828291996495</v>
       </c>
       <c r="K26" s="3">
-        <f t="shared" ref="K26" si="19">E26-J26</f>
+        <f t="shared" si="0"/>
         <v>627.17170800350505</v>
       </c>
       <c r="L26">
         <v>0</v>
       </c>
       <c r="M26">
-        <f t="shared" ref="M26" si="20">L26+E26</f>
+        <f t="shared" ref="M26" si="17">L26+E26</f>
         <v>9353</v>
       </c>
       <c r="N26" s="2">
-        <f t="shared" ref="N26" si="21">E26/$D$2*100</f>
+        <f t="shared" si="1"/>
         <v>146.140625</v>
       </c>
       <c r="O26">
@@ -2696,7 +2698,7 @@
         <v>87249.1</v>
       </c>
       <c r="Q26">
-        <f t="shared" ref="Q26" si="22">P26/$O$2*100</f>
+        <f t="shared" ref="Q26" si="18">P26/$O$2*100</f>
         <v>97.769159311025689</v>
       </c>
     </row>
@@ -2717,38 +2719,38 @@
         <v>9353</v>
       </c>
       <c r="F27">
-        <f t="shared" ref="F27:F32" si="23">E27-D27</f>
+        <f t="shared" ref="F27:F32" si="19">E27-D27</f>
         <v>0</v>
       </c>
       <c r="G27" s="2">
-        <f t="shared" ref="G27:G31" si="24">(E27-$D$2)/A27</f>
+        <f t="shared" ref="G27:G31" si="20">(E27-$D$2)/A27</f>
         <v>113.57692307692308</v>
       </c>
       <c r="H27" s="2">
-        <f t="shared" ref="H27:H32" si="25">(E27/D27-1)*100</f>
+        <f t="shared" ref="H27:H32" si="21">(E27/D27-1)*100</f>
         <v>0</v>
       </c>
       <c r="I27" s="2">
-        <f t="shared" ref="I27:I32" si="26">(POWER((E27/$D$3),1/A27)-1)*100</f>
+        <f t="shared" ref="I27:I32" si="22">(POWER((E27/$D$3),1/A27)-1)*100</f>
         <v>1.4699262282590997</v>
       </c>
       <c r="J27" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>8839.2640597924492</v>
       </c>
       <c r="K27" s="3">
-        <f t="shared" ref="K27:K32" si="27">E27-J27</f>
+        <f t="shared" si="0"/>
         <v>513.73594020755081</v>
       </c>
       <c r="L27">
         <v>0</v>
       </c>
       <c r="M27">
-        <f t="shared" ref="M27:M32" si="28">L27+E27</f>
+        <f t="shared" ref="M27:M32" si="23">L27+E27</f>
         <v>9353</v>
       </c>
       <c r="N27" s="2">
-        <f t="shared" ref="N27:N32" si="29">E27/$D$2*100</f>
+        <f t="shared" si="1"/>
         <v>146.140625</v>
       </c>
       <c r="O27">
@@ -2758,7 +2760,7 @@
         <v>84105.3</v>
       </c>
       <c r="Q27">
-        <f t="shared" ref="Q27:Q32" si="30">P27/$O$2*100</f>
+        <f t="shared" ref="Q27:Q32" si="24">P27/$O$2*100</f>
         <v>94.246295659228679</v>
       </c>
     </row>
@@ -2779,38 +2781,38 @@
         <v>9400</v>
       </c>
       <c r="F28">
+        <f t="shared" si="19"/>
+        <v>47</v>
+      </c>
+      <c r="G28" s="2">
+        <f t="shared" si="20"/>
+        <v>111.11111111111111</v>
+      </c>
+      <c r="H28" s="2">
+        <f t="shared" si="21"/>
+        <v>0.50251256281406143</v>
+      </c>
+      <c r="I28" s="2">
+        <f t="shared" si="22"/>
+        <v>1.433930583006493</v>
+      </c>
+      <c r="J28" s="3">
+        <f t="shared" si="7"/>
+        <v>8954.1744925697494</v>
+      </c>
+      <c r="K28" s="3">
+        <f t="shared" si="0"/>
+        <v>445.82550743025058</v>
+      </c>
+      <c r="L28">
+        <v>0</v>
+      </c>
+      <c r="M28">
         <f t="shared" si="23"/>
-        <v>47</v>
-      </c>
-      <c r="G28" s="2">
-        <f t="shared" si="24"/>
-        <v>111.11111111111111</v>
-      </c>
-      <c r="H28" s="2">
-        <f t="shared" si="25"/>
-        <v>0.50251256281406143</v>
-      </c>
-      <c r="I28" s="2">
-        <f t="shared" si="26"/>
-        <v>1.433930583006493</v>
-      </c>
-      <c r="J28" s="3">
-        <f t="shared" si="5"/>
-        <v>8954.1744925697494</v>
-      </c>
-      <c r="K28" s="3">
-        <f t="shared" si="27"/>
-        <v>445.82550743025058</v>
-      </c>
-      <c r="L28">
-        <v>0</v>
-      </c>
-      <c r="M28">
-        <f t="shared" si="28"/>
         <v>9400</v>
       </c>
       <c r="N28" s="2">
-        <f t="shared" si="29"/>
+        <f t="shared" si="1"/>
         <v>146.875</v>
       </c>
       <c r="O28">
@@ -2820,7 +2822,7 @@
         <v>82428.800000000003</v>
       </c>
       <c r="Q28">
-        <f t="shared" si="30"/>
+        <f t="shared" si="24"/>
         <v>92.367651689434894</v>
       </c>
     </row>
@@ -2841,38 +2843,38 @@
         <v>9450</v>
       </c>
       <c r="F29">
+        <f t="shared" si="19"/>
+        <v>50</v>
+      </c>
+      <c r="G29" s="2">
+        <f t="shared" si="20"/>
+        <v>108.92857142857143</v>
+      </c>
+      <c r="H29" s="2">
+        <f t="shared" si="21"/>
+        <v>0.53191489361701372</v>
+      </c>
+      <c r="I29" s="2">
+        <f t="shared" si="22"/>
+        <v>1.4015768054668865</v>
+      </c>
+      <c r="J29" s="3">
+        <f t="shared" si="7"/>
+        <v>9070.578760973156</v>
+      </c>
+      <c r="K29" s="3">
+        <f t="shared" si="0"/>
+        <v>379.42123902684398</v>
+      </c>
+      <c r="L29">
+        <v>0</v>
+      </c>
+      <c r="M29">
         <f t="shared" si="23"/>
-        <v>50</v>
-      </c>
-      <c r="G29" s="2">
-        <f t="shared" si="24"/>
-        <v>108.92857142857143</v>
-      </c>
-      <c r="H29" s="2">
-        <f t="shared" si="25"/>
-        <v>0.53191489361701372</v>
-      </c>
-      <c r="I29" s="2">
-        <f t="shared" si="26"/>
-        <v>1.4015768054668865</v>
-      </c>
-      <c r="J29" s="3">
-        <f t="shared" si="5"/>
-        <v>9070.578760973156</v>
-      </c>
-      <c r="K29" s="3">
-        <f t="shared" si="27"/>
-        <v>379.42123902684398</v>
-      </c>
-      <c r="L29">
-        <v>0</v>
-      </c>
-      <c r="M29">
-        <f t="shared" si="28"/>
         <v>9450</v>
       </c>
       <c r="N29" s="2">
-        <f t="shared" si="29"/>
+        <f t="shared" si="1"/>
         <v>147.65625</v>
       </c>
       <c r="O29">
@@ -2882,7 +2884,7 @@
         <v>82745.100000000006</v>
       </c>
       <c r="Q29">
-        <f t="shared" si="30"/>
+        <f t="shared" si="24"/>
         <v>92.72208955859432</v>
       </c>
     </row>
@@ -2903,38 +2905,38 @@
         <v>9452</v>
       </c>
       <c r="F30">
+        <f t="shared" si="19"/>
+        <v>2</v>
+      </c>
+      <c r="G30" s="2">
+        <f t="shared" si="20"/>
+        <v>105.24137931034483</v>
+      </c>
+      <c r="H30" s="2">
+        <f t="shared" si="21"/>
+        <v>2.1164021164010727E-2</v>
+      </c>
+      <c r="I30" s="2">
+        <f t="shared" si="22"/>
+        <v>1.3536607182727423</v>
+      </c>
+      <c r="J30" s="3">
+        <f t="shared" si="7"/>
+        <v>9188.496284865807</v>
+      </c>
+      <c r="K30" s="3">
+        <f t="shared" si="0"/>
+        <v>263.50371513419304</v>
+      </c>
+      <c r="L30">
+        <v>0</v>
+      </c>
+      <c r="M30">
         <f t="shared" si="23"/>
-        <v>2</v>
-      </c>
-      <c r="G30" s="2">
-        <f t="shared" si="24"/>
-        <v>105.24137931034483</v>
-      </c>
-      <c r="H30" s="2">
-        <f t="shared" si="25"/>
-        <v>2.1164021164010727E-2</v>
-      </c>
-      <c r="I30" s="2">
-        <f t="shared" si="26"/>
-        <v>1.3536607182727423</v>
-      </c>
-      <c r="J30" s="3">
-        <f t="shared" si="5"/>
-        <v>9188.496284865807</v>
-      </c>
-      <c r="K30" s="3">
-        <f t="shared" si="27"/>
-        <v>263.50371513419304</v>
-      </c>
-      <c r="L30">
-        <v>0</v>
-      </c>
-      <c r="M30">
-        <f t="shared" si="28"/>
         <v>9452</v>
       </c>
       <c r="N30" s="2">
-        <f t="shared" si="29"/>
+        <f t="shared" si="1"/>
         <v>147.6875</v>
       </c>
       <c r="O30">
@@ -2944,7 +2946,7 @@
         <v>83448.100000000006</v>
       </c>
       <c r="Q30">
-        <f t="shared" si="30"/>
+        <f t="shared" si="24"/>
         <v>93.509853776169635</v>
       </c>
     </row>
@@ -2962,42 +2964,42 @@
         <v>9452</v>
       </c>
       <c r="E31">
-        <v>9454</v>
+        <v>9512</v>
       </c>
       <c r="F31">
+        <f t="shared" si="19"/>
+        <v>60</v>
+      </c>
+      <c r="G31" s="2">
+        <f t="shared" si="20"/>
+        <v>103.73333333333333</v>
+      </c>
+      <c r="H31" s="2">
+        <f t="shared" si="21"/>
+        <v>0.6347862886161737</v>
+      </c>
+      <c r="I31" s="2">
+        <f t="shared" si="22"/>
+        <v>1.3296157062268277</v>
+      </c>
+      <c r="J31" s="3">
+        <f t="shared" si="7"/>
+        <v>9307.9467365690616</v>
+      </c>
+      <c r="K31" s="3">
+        <f t="shared" si="0"/>
+        <v>204.05326343093839</v>
+      </c>
+      <c r="L31">
+        <v>0</v>
+      </c>
+      <c r="M31">
         <f t="shared" si="23"/>
-        <v>2</v>
-      </c>
-      <c r="G31" s="2">
-        <f t="shared" si="24"/>
-        <v>101.8</v>
-      </c>
-      <c r="H31" s="2">
-        <f t="shared" si="25"/>
-        <v>2.1159542953874677E-2</v>
-      </c>
-      <c r="I31" s="2">
-        <f t="shared" si="26"/>
-        <v>1.3089593141764722</v>
-      </c>
-      <c r="J31" s="3">
-        <f t="shared" si="5"/>
-        <v>9307.9467365690616</v>
-      </c>
-      <c r="K31" s="3">
-        <f t="shared" si="27"/>
-        <v>146.05326343093839</v>
-      </c>
-      <c r="L31">
-        <v>0</v>
-      </c>
-      <c r="M31">
-        <f t="shared" si="28"/>
-        <v>9454</v>
+        <v>9512</v>
       </c>
       <c r="N31" s="2">
-        <f t="shared" si="29"/>
-        <v>147.71875</v>
+        <f t="shared" si="1"/>
+        <v>148.625</v>
       </c>
       <c r="O31">
         <v>83448.100000000006</v>
@@ -3006,7 +3008,7 @@
         <v>84138.9</v>
       </c>
       <c r="Q31">
-        <f t="shared" si="30"/>
+        <f t="shared" si="24"/>
         <v>94.2839469788738</v>
       </c>
     </row>
@@ -3021,45 +3023,45 @@
         <v>19</v>
       </c>
       <c r="D32">
-        <v>9454</v>
+        <v>9512</v>
       </c>
       <c r="E32">
-        <v>9456</v>
+        <v>9666</v>
       </c>
       <c r="F32">
-        <f t="shared" si="23"/>
-        <v>2</v>
+        <f t="shared" si="19"/>
+        <v>154</v>
       </c>
       <c r="G32" s="2">
         <f>(E32-$D$2)/A32</f>
-        <v>98.58064516129032</v>
+        <v>105.35483870967742</v>
       </c>
       <c r="H32" s="2">
-        <f t="shared" si="25"/>
-        <v>2.1155066638467446E-2</v>
+        <f t="shared" si="21"/>
+        <v>1.619007569386044</v>
       </c>
       <c r="I32" s="2">
-        <f t="shared" si="26"/>
-        <v>1.2671595739860209</v>
+        <f t="shared" si="22"/>
+        <v>1.3389380513060933</v>
       </c>
       <c r="J32" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>9428.9500441444579</v>
       </c>
       <c r="K32" s="3">
-        <f t="shared" si="27"/>
-        <v>27.049955855542066</v>
+        <f t="shared" si="0"/>
+        <v>237.04995585554207</v>
       </c>
       <c r="L32">
         <v>0</v>
       </c>
       <c r="M32">
-        <f t="shared" si="28"/>
-        <v>9456</v>
+        <f t="shared" si="23"/>
+        <v>9666</v>
       </c>
       <c r="N32" s="2">
-        <f t="shared" si="29"/>
-        <v>147.75</v>
+        <f t="shared" si="1"/>
+        <v>151.03125</v>
       </c>
       <c r="O32">
         <v>84138.9</v>
@@ -3068,9 +3070,594 @@
         <v>85827.9</v>
       </c>
       <c r="Q32">
+        <f t="shared" si="24"/>
+        <v>96.176598136035565</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" s="1">
+        <v>45750</v>
+      </c>
+      <c r="C33" t="s">
+        <v>20</v>
+      </c>
+      <c r="D33">
+        <v>9666</v>
+      </c>
+      <c r="E33">
+        <v>9890</v>
+      </c>
+      <c r="F33">
+        <f t="shared" ref="F33:F44" si="25">E33-D33</f>
+        <v>224</v>
+      </c>
+      <c r="G33" s="2">
+        <f t="shared" ref="G33:G44" si="26">(E33-$D$2)/A33</f>
+        <v>109.0625</v>
+      </c>
+      <c r="H33" s="2">
+        <f t="shared" ref="H33:H44" si="27">(E33/D33-1)*100</f>
+        <v>2.3174012000827693</v>
+      </c>
+      <c r="I33" s="2">
+        <f t="shared" ref="I33:I44" si="28">(POWER((E33/$D$3),1/A33)-1)*100</f>
+        <v>1.3693729216394335</v>
+      </c>
+      <c r="J33" s="3">
+        <f t="shared" si="7"/>
+        <v>9551.5263947183357</v>
+      </c>
+      <c r="K33" s="3">
+        <f t="shared" si="0"/>
+        <v>338.47360528166428</v>
+      </c>
+      <c r="L33">
+        <v>0</v>
+      </c>
+      <c r="M33">
+        <f t="shared" ref="M33:M44" si="29">L33+E33</f>
+        <v>9890</v>
+      </c>
+      <c r="N33" s="2">
+        <f t="shared" si="1"/>
+        <v>154.53125</v>
+      </c>
+      <c r="O33">
+        <v>85827.9</v>
+      </c>
+      <c r="P33">
+        <v>81465.600000000006</v>
+      </c>
+      <c r="Q33">
+        <f t="shared" ref="Q33:Q44" si="30">P33/$O$2*100</f>
+        <v>91.288313859607655</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" s="1">
+        <v>45751</v>
+      </c>
+      <c r="C34" t="s">
+        <v>21</v>
+      </c>
+      <c r="D34">
+        <v>9890</v>
+      </c>
+      <c r="E34">
+        <v>10200</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="25"/>
+        <v>310</v>
+      </c>
+      <c r="G34" s="2">
+        <f t="shared" si="26"/>
+        <v>115.15151515151516</v>
+      </c>
+      <c r="H34" s="2">
+        <f t="shared" si="27"/>
+        <v>3.1344792719919079</v>
+      </c>
+      <c r="I34" s="2">
+        <f t="shared" si="28"/>
+        <v>1.4224145175464553</v>
+      </c>
+      <c r="J34" s="3">
+        <f t="shared" si="7"/>
+        <v>9675.6962378496737</v>
+      </c>
+      <c r="K34" s="3">
+        <f t="shared" si="0"/>
+        <v>524.30376215032629</v>
+      </c>
+      <c r="L34">
+        <v>0</v>
+      </c>
+      <c r="M34">
+        <f t="shared" si="29"/>
+        <v>10200</v>
+      </c>
+      <c r="N34" s="2">
+        <f t="shared" si="1"/>
+        <v>159.375</v>
+      </c>
+      <c r="O34">
+        <v>81465.600000000006</v>
+      </c>
+      <c r="P34">
+        <v>82498</v>
+      </c>
+      <c r="Q34">
         <f t="shared" si="30"/>
-        <v>96.176598136035565</v>
-      </c>
+        <v>92.445195478704036</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" s="1">
+        <v>45752</v>
+      </c>
+      <c r="C35" t="s">
+        <v>22</v>
+      </c>
+      <c r="D35">
+        <v>10200</v>
+      </c>
+      <c r="E35">
+        <v>10565</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="25"/>
+        <v>365</v>
+      </c>
+      <c r="G35" s="2">
+        <f t="shared" si="26"/>
+        <v>122.5</v>
+      </c>
+      <c r="H35" s="2">
+        <f t="shared" si="27"/>
+        <v>3.5784313725490291</v>
+      </c>
+      <c r="I35" s="2">
+        <f t="shared" si="28"/>
+        <v>1.4851815919634914</v>
+      </c>
+      <c r="J35" s="3">
+        <f t="shared" si="7"/>
+        <v>9801.4802889417188</v>
+      </c>
+      <c r="K35" s="3">
+        <f t="shared" si="0"/>
+        <v>763.51971105828125</v>
+      </c>
+      <c r="L35">
+        <v>0</v>
+      </c>
+      <c r="M35">
+        <f t="shared" si="29"/>
+        <v>10565</v>
+      </c>
+      <c r="N35" s="2">
+        <f t="shared" si="1"/>
+        <v>165.078125</v>
+      </c>
+      <c r="O35">
+        <v>82498</v>
+      </c>
+      <c r="P35">
+        <v>82847.899999999994</v>
+      </c>
+      <c r="Q35">
+        <f t="shared" si="30"/>
+        <v>92.837284667508584</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" s="1">
+        <v>45753</v>
+      </c>
+      <c r="C36" t="s">
+        <v>23</v>
+      </c>
+      <c r="D36">
+        <v>10565</v>
+      </c>
+      <c r="E36">
+        <v>10845</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="25"/>
+        <v>280</v>
+      </c>
+      <c r="G36" s="2">
+        <f t="shared" si="26"/>
+        <v>127</v>
+      </c>
+      <c r="H36" s="2">
+        <f t="shared" si="27"/>
+        <v>2.6502602934216801</v>
+      </c>
+      <c r="I36" s="2">
+        <f t="shared" si="28"/>
+        <v>1.5182853250945039</v>
+      </c>
+      <c r="J36" s="3">
+        <f t="shared" si="7"/>
+        <v>9928.8995326979602</v>
+      </c>
+      <c r="K36" s="3">
+        <f t="shared" si="0"/>
+        <v>916.10046730203976</v>
+      </c>
+      <c r="L36">
+        <v>0</v>
+      </c>
+      <c r="M36">
+        <f t="shared" si="29"/>
+        <v>10845</v>
+      </c>
+      <c r="N36" s="2">
+        <f t="shared" si="1"/>
+        <v>169.453125</v>
+      </c>
+      <c r="O36">
+        <v>82847.899999999994</v>
+      </c>
+      <c r="P36">
+        <v>82606.7</v>
+      </c>
+      <c r="Q36">
+        <f t="shared" si="30"/>
+        <v>92.567001980056006</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" s="1">
+        <v>45754</v>
+      </c>
+      <c r="C37" t="s">
+        <v>17</v>
+      </c>
+      <c r="D37">
+        <v>20845</v>
+      </c>
+      <c r="E37">
+        <v>22699</v>
+      </c>
+      <c r="F37">
+        <f t="shared" si="25"/>
+        <v>1854</v>
+      </c>
+      <c r="G37" s="2">
+        <f t="shared" si="26"/>
+        <v>452.75</v>
+      </c>
+      <c r="H37" s="2">
+        <f t="shared" si="27"/>
+        <v>8.8942192372271514</v>
+      </c>
+      <c r="I37" s="2">
+        <f t="shared" si="28"/>
+        <v>3.5792984780890658</v>
+      </c>
+      <c r="J37" s="3">
+        <f t="shared" si="7"/>
+        <v>10057.975226623033</v>
+      </c>
+      <c r="K37" s="3">
+        <f>M37-J37</f>
+        <v>2641.0247733769666</v>
+      </c>
+      <c r="L37">
+        <v>-10000</v>
+      </c>
+      <c r="M37">
+        <f t="shared" si="29"/>
+        <v>12699</v>
+      </c>
+      <c r="N37" s="2">
+        <f>M37/$D$2*100</f>
+        <v>198.421875</v>
+      </c>
+      <c r="O37">
+        <v>82606.7</v>
+      </c>
+      <c r="P37">
+        <v>78951.899999999994</v>
+      </c>
+      <c r="Q37">
+        <f t="shared" si="30"/>
+        <v>88.471524508655889</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" s="1">
+        <v>45755</v>
+      </c>
+      <c r="C38" t="s">
+        <v>18</v>
+      </c>
+      <c r="D38">
+        <v>22699</v>
+      </c>
+      <c r="E38">
+        <v>22955</v>
+      </c>
+      <c r="F38">
+        <f t="shared" si="25"/>
+        <v>256</v>
+      </c>
+      <c r="G38" s="2">
+        <f t="shared" si="26"/>
+        <v>447.43243243243245</v>
+      </c>
+      <c r="H38" s="2">
+        <f t="shared" si="27"/>
+        <v>1.1278029869157269</v>
+      </c>
+      <c r="I38" s="2">
+        <f t="shared" si="28"/>
+        <v>3.5122668721563333</v>
+      </c>
+      <c r="J38" s="3">
+        <f t="shared" si="7"/>
+        <v>10188.728904569132</v>
+      </c>
+      <c r="K38" s="3">
+        <f t="shared" ref="K38:K41" si="31">M38-J38</f>
+        <v>2766.2710954308677</v>
+      </c>
+      <c r="L38">
+        <v>-10000</v>
+      </c>
+      <c r="M38">
+        <f t="shared" si="29"/>
+        <v>12955</v>
+      </c>
+      <c r="N38" s="2">
+        <f t="shared" ref="N38:N41" si="32">M38/$D$2*100</f>
+        <v>202.42187500000003</v>
+      </c>
+      <c r="O38">
+        <v>78951.899999999994</v>
+      </c>
+      <c r="P38">
+        <v>78410.600000000006</v>
+      </c>
+      <c r="Q38">
+        <f t="shared" si="30"/>
+        <v>87.864957266872793</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" s="1">
+        <v>45756</v>
+      </c>
+      <c r="C39" t="s">
+        <v>19</v>
+      </c>
+      <c r="D39">
+        <v>22955</v>
+      </c>
+      <c r="E39">
+        <v>24388</v>
+      </c>
+      <c r="F39">
+        <f t="shared" si="25"/>
+        <v>1433</v>
+      </c>
+      <c r="G39" s="2">
+        <f t="shared" si="26"/>
+        <v>473.36842105263156</v>
+      </c>
+      <c r="H39" s="2">
+        <f t="shared" si="27"/>
+        <v>6.2426486604225673</v>
+      </c>
+      <c r="I39" s="2">
+        <f t="shared" si="28"/>
+        <v>3.5832120312270677</v>
+      </c>
+      <c r="J39" s="3">
+        <f t="shared" si="7"/>
+        <v>10321.18238032853</v>
+      </c>
+      <c r="K39" s="3">
+        <f t="shared" si="31"/>
+        <v>4066.8176196714703</v>
+      </c>
+      <c r="L39">
+        <v>-10000</v>
+      </c>
+      <c r="M39">
+        <f t="shared" si="29"/>
+        <v>14388</v>
+      </c>
+      <c r="N39" s="2">
+        <f t="shared" si="32"/>
+        <v>224.8125</v>
+      </c>
+      <c r="O39">
+        <v>78410.600000000006</v>
+      </c>
+      <c r="P39">
+        <v>76791.100000000006</v>
+      </c>
+      <c r="Q39">
+        <f t="shared" si="30"/>
+        <v>86.050186071477015</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" s="1">
+        <v>45757</v>
+      </c>
+      <c r="C40" t="s">
+        <v>20</v>
+      </c>
+      <c r="D40">
+        <v>24388</v>
+      </c>
+      <c r="E40">
+        <v>24713</v>
+      </c>
+      <c r="F40">
+        <f t="shared" si="25"/>
+        <v>325</v>
+      </c>
+      <c r="G40" s="2">
+        <f t="shared" si="26"/>
+        <v>469.56410256410254</v>
+      </c>
+      <c r="H40" s="2">
+        <f t="shared" si="27"/>
+        <v>1.3326226012793096</v>
+      </c>
+      <c r="I40" s="2">
+        <f t="shared" si="28"/>
+        <v>3.5248848916893172</v>
+      </c>
+      <c r="J40" s="3">
+        <f t="shared" si="7"/>
+        <v>10455.357751272799</v>
+      </c>
+      <c r="K40" s="3">
+        <f t="shared" si="31"/>
+        <v>4257.6422487272011</v>
+      </c>
+      <c r="L40">
+        <v>-10000</v>
+      </c>
+      <c r="M40">
+        <f t="shared" si="29"/>
+        <v>14713</v>
+      </c>
+      <c r="N40" s="2">
+        <f t="shared" si="32"/>
+        <v>229.890625</v>
+      </c>
+      <c r="O40">
+        <v>76791.100000000006</v>
+      </c>
+      <c r="P40">
+        <v>81192.2</v>
+      </c>
+      <c r="Q40">
+        <f t="shared" si="30"/>
+        <v>90.981948657495138</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" s="1">
+        <v>45758</v>
+      </c>
+      <c r="C41" t="s">
+        <v>21</v>
+      </c>
+      <c r="D41">
+        <v>24713</v>
+      </c>
+      <c r="E41">
+        <v>25029</v>
+      </c>
+      <c r="F41">
+        <f t="shared" si="25"/>
+        <v>316</v>
+      </c>
+      <c r="G41" s="2">
+        <f t="shared" si="26"/>
+        <v>465.72500000000002</v>
+      </c>
+      <c r="H41" s="2">
+        <f t="shared" si="27"/>
+        <v>1.2786792376481948</v>
+      </c>
+      <c r="I41" s="2">
+        <f t="shared" si="28"/>
+        <v>3.4681271506401101</v>
+      </c>
+      <c r="J41" s="3">
+        <f t="shared" si="7"/>
+        <v>10591.277402039344</v>
+      </c>
+      <c r="K41" s="3">
+        <f t="shared" si="31"/>
+        <v>4437.7225979606555</v>
+      </c>
+      <c r="L41">
+        <v>-10000</v>
+      </c>
+      <c r="M41">
+        <f t="shared" si="29"/>
+        <v>15029</v>
+      </c>
+      <c r="N41" s="2">
+        <f t="shared" si="32"/>
+        <v>234.828125</v>
+      </c>
+      <c r="O41">
+        <v>81192.2</v>
+      </c>
+      <c r="P41">
+        <v>81812</v>
+      </c>
+      <c r="Q41">
+        <f t="shared" si="30"/>
+        <v>91.67648103594918</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B42" s="1"/>
+      <c r="G42" s="2"/>
+      <c r="H42" s="2"/>
+      <c r="I42" s="2"/>
+      <c r="J42" s="3"/>
+      <c r="K42" s="3"/>
+      <c r="N42" s="2"/>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B43" s="1"/>
+      <c r="G43" s="2"/>
+      <c r="H43" s="2"/>
+      <c r="I43" s="2"/>
+      <c r="J43" s="3"/>
+      <c r="K43" s="3"/>
+      <c r="N43" s="2"/>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B44" s="1"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="2"/>
+      <c r="I44" s="2"/>
+      <c r="J44" s="3"/>
+      <c r="K44" s="3"/>
+      <c r="N44" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>

</xml_diff>

<commit_message>
자동 업데이트: 2025-04-12 01:33:47
</commit_message>
<xml_diff>
--- a/data/daily_report.xlsx
+++ b/data/daily_report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c58a53286e4c1d7a/문서/GitHub/Dashboard/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="207" documentId="8_{9DD2A88B-03DA-4864-84CC-4418086E8BD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{489BD9FD-DBA7-4441-8847-3841177F407E}"/>
+  <xr:revisionPtr revIDLastSave="213" documentId="8_{9DD2A88B-03DA-4864-84CC-4418086E8BD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5E7B59D6-4343-42D8-B7C5-9B9F06A6B00E}"/>
   <bookViews>
-    <workbookView xWindow="16215" yWindow="300" windowWidth="21975" windowHeight="20970" xr2:uid="{4AB8DADE-1167-4E84-9D67-55086BA93884}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{4AB8DADE-1167-4E84-9D67-55086BA93884}"/>
   </bookViews>
   <sheets>
     <sheet name="daily_report" sheetId="1" r:id="rId1"/>
@@ -1092,7 +1092,7 @@
   <dimension ref="A1:Q44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q41" sqref="Q41"/>
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1100,6 +1100,7 @@
     <col min="2" max="2" width="11.125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11" customWidth="1"/>
     <col min="8" max="8" width="8.375" customWidth="1"/>
+    <col min="14" max="14" width="14.25" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1201,8 +1202,8 @@
         <v>6400</v>
       </c>
       <c r="N2" s="2">
-        <f t="shared" ref="N2:N36" si="1">M2/$D$2*100</f>
-        <v>100</v>
+        <f>M2/$D$2*100-100</f>
+        <v>0</v>
       </c>
       <c r="O2">
         <v>89239.9</v>
@@ -1211,7 +1212,7 @@
         <v>89239.9</v>
       </c>
       <c r="Q2">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
@@ -1231,11 +1232,11 @@
         <v>6546</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F24" si="2">E3-D3</f>
+        <f t="shared" ref="F3:F24" si="1">E3-D3</f>
         <v>146</v>
       </c>
       <c r="G3" s="2">
-        <f t="shared" ref="G3:G22" si="3">(E3-$D$2)/A3</f>
+        <f t="shared" ref="G3:G22" si="2">(E3-$D$2)/A3</f>
         <v>146</v>
       </c>
       <c r="H3" s="2">
@@ -1258,12 +1259,12 @@
         <v>0</v>
       </c>
       <c r="M3">
-        <f t="shared" ref="M3:M24" si="4">L3+E3</f>
+        <f t="shared" ref="M3:M24" si="3">L3+E3</f>
         <v>6546</v>
       </c>
       <c r="N3" s="2">
-        <f t="shared" si="1"/>
-        <v>102.28124999999999</v>
+        <f t="shared" ref="N3:N41" si="4">M3/$D$2*100-100</f>
+        <v>2.2812499999999858</v>
       </c>
       <c r="O3">
         <v>89239.9</v>
@@ -1272,8 +1273,8 @@
         <v>83157.100000000006</v>
       </c>
       <c r="Q3">
-        <f>P3/$O$2*100</f>
-        <v>93.183766454243013</v>
+        <f>P3/$O$2*100-100</f>
+        <v>-6.8162335457569867</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
@@ -1293,11 +1294,11 @@
         <v>6689</v>
       </c>
       <c r="F4">
+        <f t="shared" si="1"/>
+        <v>143</v>
+      </c>
+      <c r="G4" s="2">
         <f t="shared" si="2"/>
-        <v>143</v>
-      </c>
-      <c r="G4" s="2">
-        <f t="shared" si="3"/>
         <v>144.5</v>
       </c>
       <c r="H4" s="2">
@@ -1309,7 +1310,7 @@
         <v>2.2328836529616813</v>
       </c>
       <c r="J4" s="3">
-        <f t="shared" ref="J4:J44" si="7">J3*1.013</f>
+        <f t="shared" ref="J4:J41" si="7">J3*1.013</f>
         <v>6567.4815999999983</v>
       </c>
       <c r="K4" s="3">
@@ -1320,12 +1321,12 @@
         <v>0</v>
       </c>
       <c r="M4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>6689</v>
       </c>
       <c r="N4" s="2">
-        <f t="shared" si="1"/>
-        <v>104.515625</v>
+        <f t="shared" si="4"/>
+        <v>4.515625</v>
       </c>
       <c r="O4">
         <v>83157.100000000006</v>
@@ -1334,8 +1335,8 @@
         <v>88477.3</v>
       </c>
       <c r="Q4">
-        <f t="shared" ref="Q4:Q24" si="8">P4/$O$2*100</f>
-        <v>99.145449513054146</v>
+        <f t="shared" ref="Q4:Q41" si="8">P4/$O$2*100-100</f>
+        <v>-0.854550486945854</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
@@ -1355,11 +1356,11 @@
         <v>6846</v>
       </c>
       <c r="F5">
+        <f t="shared" si="1"/>
+        <v>157</v>
+      </c>
+      <c r="G5" s="2">
         <f t="shared" si="2"/>
-        <v>157</v>
-      </c>
-      <c r="G5" s="2">
-        <f t="shared" si="3"/>
         <v>148.66666666666666</v>
       </c>
       <c r="H5" s="2">
@@ -1382,12 +1383,12 @@
         <v>0</v>
       </c>
       <c r="M5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>6846</v>
       </c>
       <c r="N5" s="2">
-        <f t="shared" si="1"/>
-        <v>106.96874999999999</v>
+        <f t="shared" si="4"/>
+        <v>6.9687499999999858</v>
       </c>
       <c r="O5">
         <v>88477.3</v>
@@ -1397,7 +1398,7 @@
       </c>
       <c r="Q5">
         <f t="shared" si="8"/>
-        <v>100.59446503189717</v>
+        <v>0.59446503189717248</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
@@ -1417,11 +1418,11 @@
         <v>7015</v>
       </c>
       <c r="F6">
+        <f t="shared" si="1"/>
+        <v>169</v>
+      </c>
+      <c r="G6" s="2">
         <f t="shared" si="2"/>
-        <v>169</v>
-      </c>
-      <c r="G6" s="2">
-        <f t="shared" si="3"/>
         <v>153.75</v>
       </c>
       <c r="H6" s="2">
@@ -1444,12 +1445,12 @@
         <v>0</v>
       </c>
       <c r="M6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>7015</v>
       </c>
       <c r="N6" s="2">
-        <f t="shared" si="1"/>
-        <v>109.60937500000001</v>
+        <f t="shared" si="4"/>
+        <v>9.6093750000000142</v>
       </c>
       <c r="O6">
         <v>89770.4</v>
@@ -1459,7 +1460,7 @@
       </c>
       <c r="Q6">
         <f t="shared" si="8"/>
-        <v>101.3129777151252</v>
+        <v>1.3129777151252</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
@@ -1479,11 +1480,11 @@
         <v>7050</v>
       </c>
       <c r="F7">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="G7" s="2">
         <f t="shared" si="2"/>
-        <v>35</v>
-      </c>
-      <c r="G7" s="2">
-        <f t="shared" si="3"/>
         <v>130</v>
       </c>
       <c r="H7" s="2">
@@ -1506,12 +1507,12 @@
         <v>0</v>
       </c>
       <c r="M7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>7050</v>
       </c>
       <c r="N7" s="2">
-        <f t="shared" si="1"/>
-        <v>110.15625</v>
+        <f t="shared" si="4"/>
+        <v>10.15625</v>
       </c>
       <c r="O7">
         <v>90411.6</v>
@@ -1521,7 +1522,7 @@
       </c>
       <c r="Q7">
         <f t="shared" si="8"/>
-        <v>96.731730985803438</v>
+        <v>-3.2682690141965622</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
@@ -1541,11 +1542,11 @@
         <v>6979</v>
       </c>
       <c r="F8">
+        <f t="shared" si="1"/>
+        <v>-71</v>
+      </c>
+      <c r="G8" s="2">
         <f t="shared" si="2"/>
-        <v>-71</v>
-      </c>
-      <c r="G8" s="2">
-        <f t="shared" si="3"/>
         <v>96.5</v>
       </c>
       <c r="H8" s="2">
@@ -1568,12 +1569,12 @@
         <v>0</v>
       </c>
       <c r="M8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>6979</v>
       </c>
       <c r="N8" s="2">
-        <f t="shared" si="1"/>
-        <v>109.04687500000001</v>
+        <f t="shared" si="4"/>
+        <v>9.0468750000000142</v>
       </c>
       <c r="O8">
         <v>86323.3</v>
@@ -1583,7 +1584,7 @@
       </c>
       <c r="Q8">
         <f t="shared" si="8"/>
-        <v>93.638607842456125</v>
+        <v>-6.3613921575438752</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
@@ -1603,11 +1604,11 @@
         <v>7170</v>
       </c>
       <c r="F9">
+        <f t="shared" si="1"/>
+        <v>191</v>
+      </c>
+      <c r="G9" s="2">
         <f t="shared" si="2"/>
-        <v>191</v>
-      </c>
-      <c r="G9" s="2">
-        <f t="shared" si="3"/>
         <v>96.25</v>
       </c>
       <c r="H9" s="2">
@@ -1630,12 +1631,12 @@
         <v>0</v>
       </c>
       <c r="M9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>7170</v>
       </c>
       <c r="N9" s="2">
-        <f t="shared" si="1"/>
-        <v>112.03125</v>
+        <f t="shared" si="4"/>
+        <v>12.03125</v>
       </c>
       <c r="O9">
         <v>83563</v>
@@ -1645,7 +1646,7 @@
       </c>
       <c r="Q9">
         <f t="shared" si="8"/>
-        <v>89.437236034554061</v>
+        <v>-10.562763965445939</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
@@ -1665,11 +1666,11 @@
         <v>7315</v>
       </c>
       <c r="F10">
+        <f t="shared" si="1"/>
+        <v>145</v>
+      </c>
+      <c r="G10" s="2">
         <f t="shared" si="2"/>
-        <v>145</v>
-      </c>
-      <c r="G10" s="2">
-        <f t="shared" si="3"/>
         <v>101.66666666666667</v>
       </c>
       <c r="H10" s="2">
@@ -1692,12 +1693,12 @@
         <v>0</v>
       </c>
       <c r="M10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>7315</v>
       </c>
       <c r="N10" s="2">
-        <f t="shared" si="1"/>
-        <v>114.29687500000001</v>
+        <f t="shared" si="4"/>
+        <v>14.296875000000014</v>
       </c>
       <c r="O10">
         <v>79813.7</v>
@@ -1707,7 +1708,7 @@
       </c>
       <c r="Q10">
         <f t="shared" si="8"/>
-        <v>90.335937176083789</v>
+        <v>-9.6640628239162112</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
@@ -1727,11 +1728,11 @@
         <v>6845</v>
       </c>
       <c r="F11">
+        <f t="shared" si="1"/>
+        <v>-470</v>
+      </c>
+      <c r="G11" s="2">
         <f t="shared" si="2"/>
-        <v>-470</v>
-      </c>
-      <c r="G11" s="2">
-        <f t="shared" si="3"/>
         <v>44.5</v>
       </c>
       <c r="H11" s="2">
@@ -1754,12 +1755,12 @@
         <v>0</v>
       </c>
       <c r="M11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>6845</v>
       </c>
       <c r="N11" s="2">
-        <f t="shared" si="1"/>
-        <v>106.953125</v>
+        <f t="shared" si="4"/>
+        <v>6.953125</v>
       </c>
       <c r="O11">
         <v>80615.7</v>
@@ -1769,7 +1770,7 @@
       </c>
       <c r="Q11">
         <f t="shared" si="8"/>
-        <v>91.327870156734832</v>
+        <v>-8.6721298432651679</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.3">
@@ -1789,11 +1790,11 @@
         <v>7567</v>
       </c>
       <c r="F12">
+        <f t="shared" si="1"/>
+        <v>722</v>
+      </c>
+      <c r="G12" s="2">
         <f t="shared" si="2"/>
-        <v>722</v>
-      </c>
-      <c r="G12" s="2">
-        <f t="shared" si="3"/>
         <v>106.09090909090909</v>
       </c>
       <c r="H12" s="2">
@@ -1816,12 +1817,12 @@
         <v>0</v>
       </c>
       <c r="M12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>7567</v>
       </c>
       <c r="N12" s="2">
-        <f t="shared" si="1"/>
-        <v>118.234375</v>
+        <f t="shared" si="4"/>
+        <v>18.234375</v>
       </c>
       <c r="O12">
         <v>81500.899999999994</v>
@@ -1831,7 +1832,7 @@
       </c>
       <c r="Q12">
         <f t="shared" si="8"/>
-        <v>91.849721929316388</v>
+        <v>-8.150278070683612</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.3">
@@ -1851,11 +1852,11 @@
         <v>7763</v>
       </c>
       <c r="F13">
+        <f t="shared" si="1"/>
+        <v>196</v>
+      </c>
+      <c r="G13" s="2">
         <f t="shared" si="2"/>
-        <v>196</v>
-      </c>
-      <c r="G13" s="2">
-        <f t="shared" si="3"/>
         <v>113.58333333333333</v>
       </c>
       <c r="H13" s="2">
@@ -1878,12 +1879,12 @@
         <v>0</v>
       </c>
       <c r="M13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>7763</v>
       </c>
       <c r="N13" s="2">
-        <f t="shared" si="1"/>
-        <v>121.296875</v>
+        <f t="shared" si="4"/>
+        <v>21.296875</v>
       </c>
       <c r="O13">
         <v>81966.600000000006</v>
@@ -1893,7 +1894,7 @@
       </c>
       <c r="Q13">
         <f t="shared" si="8"/>
-        <v>93.563529318163745</v>
+        <v>-6.4364706818362549</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
@@ -1913,11 +1914,11 @@
         <v>7845</v>
       </c>
       <c r="F14">
+        <f t="shared" si="1"/>
+        <v>82</v>
+      </c>
+      <c r="G14" s="2">
         <f t="shared" si="2"/>
-        <v>82</v>
-      </c>
-      <c r="G14" s="2">
-        <f t="shared" si="3"/>
         <v>111.15384615384616</v>
       </c>
       <c r="H14" s="2">
@@ -1940,12 +1941,12 @@
         <v>0</v>
       </c>
       <c r="M14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>7845</v>
       </c>
       <c r="N14" s="2">
-        <f t="shared" si="1"/>
-        <v>122.578125</v>
+        <f t="shared" si="4"/>
+        <v>22.578125</v>
       </c>
       <c r="O14">
         <v>83496</v>
@@ -1955,7 +1956,7 @@
       </c>
       <c r="Q14">
         <f t="shared" si="8"/>
-        <v>94.249769441695918</v>
+        <v>-5.7502305583040823</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.3">
@@ -1975,11 +1976,11 @@
         <v>7879</v>
       </c>
       <c r="F15">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+      <c r="G15" s="2">
         <f t="shared" si="2"/>
-        <v>34</v>
-      </c>
-      <c r="G15" s="2">
-        <f t="shared" si="3"/>
         <v>105.64285714285714</v>
       </c>
       <c r="H15" s="2">
@@ -2002,12 +2003,12 @@
         <v>0</v>
       </c>
       <c r="M15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>7879</v>
       </c>
       <c r="N15" s="2">
-        <f t="shared" si="1"/>
-        <v>123.10937500000001</v>
+        <f t="shared" si="4"/>
+        <v>23.109375000000014</v>
       </c>
       <c r="O15">
         <v>84108.4</v>
@@ -2017,7 +2018,7 @@
       </c>
       <c r="Q15">
         <f t="shared" si="8"/>
-        <v>93.382220284872574</v>
+        <v>-6.6177797151274262</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.3">
@@ -2037,11 +2038,11 @@
         <v>7952</v>
       </c>
       <c r="F16">
+        <f t="shared" si="1"/>
+        <v>73</v>
+      </c>
+      <c r="G16" s="2">
         <f t="shared" si="2"/>
-        <v>73</v>
-      </c>
-      <c r="G16" s="2">
-        <f t="shared" si="3"/>
         <v>103.46666666666667</v>
       </c>
       <c r="H16" s="2">
@@ -2064,12 +2065,12 @@
         <v>0</v>
       </c>
       <c r="M16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>7952</v>
       </c>
       <c r="N16" s="2">
-        <f t="shared" si="1"/>
-        <v>124.25</v>
+        <f t="shared" si="4"/>
+        <v>24.25</v>
       </c>
       <c r="O16">
         <v>83334.2</v>
@@ -2079,7 +2080,7 @@
       </c>
       <c r="Q16">
         <f t="shared" si="8"/>
-        <v>92.865523157242464</v>
+        <v>-7.134476842757536</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.3">
@@ -2099,11 +2100,11 @@
         <v>7797</v>
       </c>
       <c r="F17">
+        <f t="shared" si="1"/>
+        <v>-155</v>
+      </c>
+      <c r="G17" s="2">
         <f t="shared" si="2"/>
-        <v>-155</v>
-      </c>
-      <c r="G17" s="2">
-        <f t="shared" si="3"/>
         <v>87.3125</v>
       </c>
       <c r="H17" s="2">
@@ -2126,12 +2127,12 @@
         <v>0</v>
       </c>
       <c r="M17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>7797</v>
       </c>
       <c r="N17" s="2">
-        <f t="shared" si="1"/>
-        <v>121.828125</v>
+        <f t="shared" si="4"/>
+        <v>21.828125</v>
       </c>
       <c r="O17">
         <v>82873.100000000006</v>
@@ -2141,7 +2142,7 @@
       </c>
       <c r="Q17">
         <f t="shared" si="8"/>
-        <v>91.673679598475573</v>
+        <v>-8.326320401524427</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.3">
@@ -2161,11 +2162,11 @@
         <v>8335</v>
       </c>
       <c r="F18">
+        <f t="shared" si="1"/>
+        <v>538</v>
+      </c>
+      <c r="G18" s="2">
         <f t="shared" si="2"/>
-        <v>538</v>
-      </c>
-      <c r="G18" s="2">
-        <f t="shared" si="3"/>
         <v>113.82352941176471</v>
       </c>
       <c r="H18" s="2">
@@ -2188,12 +2189,12 @@
         <v>0</v>
       </c>
       <c r="M18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>8335</v>
       </c>
       <c r="N18" s="2">
-        <f t="shared" si="1"/>
-        <v>130.234375</v>
+        <f t="shared" si="4"/>
+        <v>30.234375</v>
       </c>
       <c r="O18">
         <v>81809.5</v>
@@ -2203,7 +2204,7 @@
       </c>
       <c r="Q18">
         <f t="shared" si="8"/>
-        <v>94.427940865016652</v>
+        <v>-5.5720591349833484</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.3">
@@ -2223,11 +2224,11 @@
         <v>8461</v>
       </c>
       <c r="F19">
+        <f t="shared" si="1"/>
+        <v>126</v>
+      </c>
+      <c r="G19" s="2">
         <f t="shared" si="2"/>
-        <v>126</v>
-      </c>
-      <c r="G19" s="2">
-        <f t="shared" si="3"/>
         <v>114.5</v>
       </c>
       <c r="H19" s="2">
@@ -2250,12 +2251,12 @@
         <v>0</v>
       </c>
       <c r="M19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>8461</v>
       </c>
       <c r="N19" s="2">
-        <f t="shared" si="1"/>
-        <v>132.203125</v>
+        <f t="shared" si="4"/>
+        <v>32.203125</v>
       </c>
       <c r="O19">
         <v>84267.4</v>
@@ -2265,7 +2266,7 @@
       </c>
       <c r="Q19">
         <f t="shared" si="8"/>
-        <v>96.507952160412572</v>
+        <v>-3.4920478395874284</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.3">
@@ -2285,11 +2286,11 @@
         <v>8330</v>
       </c>
       <c r="F20">
+        <f t="shared" si="1"/>
+        <v>-131</v>
+      </c>
+      <c r="G20" s="2">
         <f t="shared" si="2"/>
-        <v>-131</v>
-      </c>
-      <c r="G20" s="2">
-        <f t="shared" si="3"/>
         <v>101.57894736842105</v>
       </c>
       <c r="H20" s="2">
@@ -2312,12 +2313,12 @@
         <v>0</v>
       </c>
       <c r="M20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>8330</v>
       </c>
       <c r="N20" s="2">
-        <f t="shared" si="1"/>
-        <v>130.15625</v>
+        <f t="shared" si="4"/>
+        <v>30.15625</v>
       </c>
       <c r="O20">
         <v>86123.6</v>
@@ -2327,7 +2328,7 @@
       </c>
       <c r="Q20">
         <f t="shared" si="8"/>
-        <v>94.352414110728503</v>
+        <v>-5.6475858892714967</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.3">
@@ -2347,11 +2348,11 @@
         <v>8331</v>
       </c>
       <c r="F21">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G21" s="2">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="G21" s="2">
-        <f t="shared" si="3"/>
         <v>96.55</v>
       </c>
       <c r="H21" s="2">
@@ -2374,12 +2375,12 @@
         <v>0</v>
       </c>
       <c r="M21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>8331</v>
       </c>
       <c r="N21" s="2">
-        <f t="shared" si="1"/>
-        <v>130.171875</v>
+        <f t="shared" si="4"/>
+        <v>30.171875</v>
       </c>
       <c r="O21">
         <v>84200</v>
@@ -2389,7 +2390,7 @@
       </c>
       <c r="Q21">
         <f t="shared" si="8"/>
-        <v>94.095354208151292</v>
+        <v>-5.9046457918487079</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.3">
@@ -2409,11 +2410,11 @@
         <v>8590</v>
       </c>
       <c r="F22">
+        <f t="shared" si="1"/>
+        <v>259</v>
+      </c>
+      <c r="G22" s="2">
         <f t="shared" si="2"/>
-        <v>259</v>
-      </c>
-      <c r="G22" s="2">
-        <f t="shared" si="3"/>
         <v>104.28571428571429</v>
       </c>
       <c r="H22" s="2">
@@ -2436,12 +2437,12 @@
         <v>0</v>
       </c>
       <c r="M22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>8590</v>
       </c>
       <c r="N22" s="2">
-        <f t="shared" si="1"/>
-        <v>134.21875</v>
+        <f t="shared" si="4"/>
+        <v>34.21875</v>
       </c>
       <c r="O22">
         <v>83970.6</v>
@@ -2451,7 +2452,7 @@
       </c>
       <c r="Q22">
         <f t="shared" si="8"/>
-        <v>95.094234753736842</v>
+        <v>-4.905765246263158</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.3">
@@ -2471,7 +2472,7 @@
         <v>8925</v>
       </c>
       <c r="F23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>335</v>
       </c>
       <c r="G23" s="2">
@@ -2498,12 +2499,12 @@
         <v>0</v>
       </c>
       <c r="M23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>8925</v>
       </c>
       <c r="N23" s="2">
-        <f t="shared" si="1"/>
-        <v>139.453125</v>
+        <f t="shared" si="4"/>
+        <v>39.453125</v>
       </c>
       <c r="O23">
         <v>84862</v>
@@ -2513,7 +2514,7 @@
       </c>
       <c r="Q23">
         <f t="shared" si="8"/>
-        <v>98.522073646429462</v>
+        <v>-1.4779263535705383</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.3">
@@ -2533,7 +2534,7 @@
         <v>9113</v>
       </c>
       <c r="F24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>188</v>
       </c>
       <c r="G24" s="2">
@@ -2560,12 +2561,12 @@
         <v>0</v>
       </c>
       <c r="M24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>9113</v>
       </c>
       <c r="N24" s="2">
-        <f t="shared" si="1"/>
-        <v>142.390625</v>
+        <f t="shared" si="4"/>
+        <v>42.390625</v>
       </c>
       <c r="O24">
         <v>87921</v>
@@ -2575,7 +2576,7 @@
       </c>
       <c r="Q24">
         <f t="shared" si="8"/>
-        <v>98.59390250325248</v>
+        <v>-1.4060974967475204</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.3">
@@ -2626,8 +2627,8 @@
         <v>9163</v>
       </c>
       <c r="N25" s="2">
-        <f t="shared" si="1"/>
-        <v>143.171875</v>
+        <f t="shared" si="4"/>
+        <v>43.171875</v>
       </c>
       <c r="O25">
         <v>87985.1</v>
@@ -2636,8 +2637,8 @@
         <v>86736.1</v>
       </c>
       <c r="Q25">
-        <f t="shared" ref="Q25" si="13">P25/$O$2*100</f>
-        <v>97.194304341443697</v>
+        <f t="shared" si="8"/>
+        <v>-2.8056956585563029</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.3">
@@ -2657,7 +2658,7 @@
         <v>9353</v>
       </c>
       <c r="F26">
-        <f t="shared" ref="F26" si="14">E26-D26</f>
+        <f t="shared" ref="F26" si="13">E26-D26</f>
         <v>190</v>
       </c>
       <c r="G26" s="2">
@@ -2665,11 +2666,11 @@
         <v>118.12</v>
       </c>
       <c r="H26" s="2">
-        <f t="shared" ref="H26" si="15">(E26/D26-1)*100</f>
+        <f t="shared" ref="H26" si="14">(E26/D26-1)*100</f>
         <v>2.0735566954054319</v>
       </c>
       <c r="I26" s="2">
-        <f t="shared" ref="I26" si="16">(POWER((E26/$D$3),1/A26)-1)*100</f>
+        <f t="shared" ref="I26" si="15">(POWER((E26/$D$3),1/A26)-1)*100</f>
         <v>1.5291706005972516</v>
       </c>
       <c r="J26" s="3">
@@ -2684,12 +2685,12 @@
         <v>0</v>
       </c>
       <c r="M26">
-        <f t="shared" ref="M26" si="17">L26+E26</f>
+        <f t="shared" ref="M26" si="16">L26+E26</f>
         <v>9353</v>
       </c>
       <c r="N26" s="2">
-        <f t="shared" si="1"/>
-        <v>146.140625</v>
+        <f t="shared" si="4"/>
+        <v>46.140625</v>
       </c>
       <c r="O26">
         <v>86736.1</v>
@@ -2698,8 +2699,8 @@
         <v>87249.1</v>
       </c>
       <c r="Q26">
-        <f t="shared" ref="Q26" si="18">P26/$O$2*100</f>
-        <v>97.769159311025689</v>
+        <f t="shared" si="8"/>
+        <v>-2.2308406889743111</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.3">
@@ -2719,19 +2720,19 @@
         <v>9353</v>
       </c>
       <c r="F27">
-        <f t="shared" ref="F27:F32" si="19">E27-D27</f>
+        <f t="shared" ref="F27:F32" si="17">E27-D27</f>
         <v>0</v>
       </c>
       <c r="G27" s="2">
-        <f t="shared" ref="G27:G31" si="20">(E27-$D$2)/A27</f>
+        <f t="shared" ref="G27:G31" si="18">(E27-$D$2)/A27</f>
         <v>113.57692307692308</v>
       </c>
       <c r="H27" s="2">
-        <f t="shared" ref="H27:H32" si="21">(E27/D27-1)*100</f>
+        <f t="shared" ref="H27:H32" si="19">(E27/D27-1)*100</f>
         <v>0</v>
       </c>
       <c r="I27" s="2">
-        <f t="shared" ref="I27:I32" si="22">(POWER((E27/$D$3),1/A27)-1)*100</f>
+        <f t="shared" ref="I27:I32" si="20">(POWER((E27/$D$3),1/A27)-1)*100</f>
         <v>1.4699262282590997</v>
       </c>
       <c r="J27" s="3">
@@ -2746,12 +2747,12 @@
         <v>0</v>
       </c>
       <c r="M27">
-        <f t="shared" ref="M27:M32" si="23">L27+E27</f>
+        <f t="shared" ref="M27:M32" si="21">L27+E27</f>
         <v>9353</v>
       </c>
       <c r="N27" s="2">
-        <f t="shared" si="1"/>
-        <v>146.140625</v>
+        <f t="shared" si="4"/>
+        <v>46.140625</v>
       </c>
       <c r="O27">
         <v>87249.1</v>
@@ -2760,8 +2761,8 @@
         <v>84105.3</v>
       </c>
       <c r="Q27">
-        <f t="shared" ref="Q27:Q32" si="24">P27/$O$2*100</f>
-        <v>94.246295659228679</v>
+        <f t="shared" si="8"/>
+        <v>-5.7537043407713213</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.3">
@@ -2781,19 +2782,19 @@
         <v>9400</v>
       </c>
       <c r="F28">
+        <f t="shared" si="17"/>
+        <v>47</v>
+      </c>
+      <c r="G28" s="2">
+        <f t="shared" si="18"/>
+        <v>111.11111111111111</v>
+      </c>
+      <c r="H28" s="2">
         <f t="shared" si="19"/>
-        <v>47</v>
-      </c>
-      <c r="G28" s="2">
+        <v>0.50251256281406143</v>
+      </c>
+      <c r="I28" s="2">
         <f t="shared" si="20"/>
-        <v>111.11111111111111</v>
-      </c>
-      <c r="H28" s="2">
-        <f t="shared" si="21"/>
-        <v>0.50251256281406143</v>
-      </c>
-      <c r="I28" s="2">
-        <f t="shared" si="22"/>
         <v>1.433930583006493</v>
       </c>
       <c r="J28" s="3">
@@ -2808,12 +2809,12 @@
         <v>0</v>
       </c>
       <c r="M28">
-        <f t="shared" si="23"/>
+        <f t="shared" si="21"/>
         <v>9400</v>
       </c>
       <c r="N28" s="2">
-        <f t="shared" si="1"/>
-        <v>146.875</v>
+        <f t="shared" si="4"/>
+        <v>46.875</v>
       </c>
       <c r="O28">
         <v>84105.3</v>
@@ -2822,8 +2823,8 @@
         <v>82428.800000000003</v>
       </c>
       <c r="Q28">
-        <f t="shared" si="24"/>
-        <v>92.367651689434894</v>
+        <f t="shared" si="8"/>
+        <v>-7.6323483105651064</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.3">
@@ -2843,19 +2844,19 @@
         <v>9450</v>
       </c>
       <c r="F29">
+        <f t="shared" si="17"/>
+        <v>50</v>
+      </c>
+      <c r="G29" s="2">
+        <f t="shared" si="18"/>
+        <v>108.92857142857143</v>
+      </c>
+      <c r="H29" s="2">
         <f t="shared" si="19"/>
-        <v>50</v>
-      </c>
-      <c r="G29" s="2">
+        <v>0.53191489361701372</v>
+      </c>
+      <c r="I29" s="2">
         <f t="shared" si="20"/>
-        <v>108.92857142857143</v>
-      </c>
-      <c r="H29" s="2">
-        <f t="shared" si="21"/>
-        <v>0.53191489361701372</v>
-      </c>
-      <c r="I29" s="2">
-        <f t="shared" si="22"/>
         <v>1.4015768054668865</v>
       </c>
       <c r="J29" s="3">
@@ -2870,12 +2871,12 @@
         <v>0</v>
       </c>
       <c r="M29">
-        <f t="shared" si="23"/>
+        <f t="shared" si="21"/>
         <v>9450</v>
       </c>
       <c r="N29" s="2">
-        <f t="shared" si="1"/>
-        <v>147.65625</v>
+        <f t="shared" si="4"/>
+        <v>47.65625</v>
       </c>
       <c r="O29">
         <v>82428.800000000003</v>
@@ -2884,8 +2885,8 @@
         <v>82745.100000000006</v>
       </c>
       <c r="Q29">
-        <f t="shared" si="24"/>
-        <v>92.72208955859432</v>
+        <f t="shared" si="8"/>
+        <v>-7.2779104414056803</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.3">
@@ -2905,19 +2906,19 @@
         <v>9452</v>
       </c>
       <c r="F30">
+        <f t="shared" si="17"/>
+        <v>2</v>
+      </c>
+      <c r="G30" s="2">
+        <f t="shared" si="18"/>
+        <v>105.24137931034483</v>
+      </c>
+      <c r="H30" s="2">
         <f t="shared" si="19"/>
-        <v>2</v>
-      </c>
-      <c r="G30" s="2">
+        <v>2.1164021164010727E-2</v>
+      </c>
+      <c r="I30" s="2">
         <f t="shared" si="20"/>
-        <v>105.24137931034483</v>
-      </c>
-      <c r="H30" s="2">
-        <f t="shared" si="21"/>
-        <v>2.1164021164010727E-2</v>
-      </c>
-      <c r="I30" s="2">
-        <f t="shared" si="22"/>
         <v>1.3536607182727423</v>
       </c>
       <c r="J30" s="3">
@@ -2932,12 +2933,12 @@
         <v>0</v>
       </c>
       <c r="M30">
-        <f t="shared" si="23"/>
+        <f t="shared" si="21"/>
         <v>9452</v>
       </c>
       <c r="N30" s="2">
-        <f t="shared" si="1"/>
-        <v>147.6875</v>
+        <f t="shared" si="4"/>
+        <v>47.6875</v>
       </c>
       <c r="O30">
         <v>82745.100000000006</v>
@@ -2946,8 +2947,8 @@
         <v>83448.100000000006</v>
       </c>
       <c r="Q30">
-        <f t="shared" si="24"/>
-        <v>93.509853776169635</v>
+        <f t="shared" si="8"/>
+        <v>-6.4901462238303651</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.3">
@@ -2967,19 +2968,19 @@
         <v>9512</v>
       </c>
       <c r="F31">
+        <f t="shared" si="17"/>
+        <v>60</v>
+      </c>
+      <c r="G31" s="2">
+        <f t="shared" si="18"/>
+        <v>103.73333333333333</v>
+      </c>
+      <c r="H31" s="2">
         <f t="shared" si="19"/>
-        <v>60</v>
-      </c>
-      <c r="G31" s="2">
+        <v>0.6347862886161737</v>
+      </c>
+      <c r="I31" s="2">
         <f t="shared" si="20"/>
-        <v>103.73333333333333</v>
-      </c>
-      <c r="H31" s="2">
-        <f t="shared" si="21"/>
-        <v>0.6347862886161737</v>
-      </c>
-      <c r="I31" s="2">
-        <f t="shared" si="22"/>
         <v>1.3296157062268277</v>
       </c>
       <c r="J31" s="3">
@@ -2994,12 +2995,12 @@
         <v>0</v>
       </c>
       <c r="M31">
-        <f t="shared" si="23"/>
+        <f t="shared" si="21"/>
         <v>9512</v>
       </c>
       <c r="N31" s="2">
-        <f t="shared" si="1"/>
-        <v>148.625</v>
+        <f t="shared" si="4"/>
+        <v>48.625</v>
       </c>
       <c r="O31">
         <v>83448.100000000006</v>
@@ -3008,8 +3009,8 @@
         <v>84138.9</v>
       </c>
       <c r="Q31">
-        <f t="shared" si="24"/>
-        <v>94.2839469788738</v>
+        <f t="shared" si="8"/>
+        <v>-5.7160530211262</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.3">
@@ -3029,7 +3030,7 @@
         <v>9666</v>
       </c>
       <c r="F32">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>154</v>
       </c>
       <c r="G32" s="2">
@@ -3037,11 +3038,11 @@
         <v>105.35483870967742</v>
       </c>
       <c r="H32" s="2">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>1.619007569386044</v>
       </c>
       <c r="I32" s="2">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>1.3389380513060933</v>
       </c>
       <c r="J32" s="3">
@@ -3056,12 +3057,12 @@
         <v>0</v>
       </c>
       <c r="M32">
-        <f t="shared" si="23"/>
+        <f t="shared" si="21"/>
         <v>9666</v>
       </c>
       <c r="N32" s="2">
-        <f t="shared" si="1"/>
-        <v>151.03125</v>
+        <f t="shared" si="4"/>
+        <v>51.03125</v>
       </c>
       <c r="O32">
         <v>84138.9</v>
@@ -3070,8 +3071,8 @@
         <v>85827.9</v>
       </c>
       <c r="Q32">
-        <f t="shared" si="24"/>
-        <v>96.176598136035565</v>
+        <f t="shared" si="8"/>
+        <v>-3.8234018639644347</v>
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.3">
@@ -3091,19 +3092,19 @@
         <v>9890</v>
       </c>
       <c r="F33">
-        <f t="shared" ref="F33:F44" si="25">E33-D33</f>
+        <f t="shared" ref="F33:F41" si="22">E33-D33</f>
         <v>224</v>
       </c>
       <c r="G33" s="2">
-        <f t="shared" ref="G33:G44" si="26">(E33-$D$2)/A33</f>
+        <f t="shared" ref="G33:G41" si="23">(E33-$D$2)/A33</f>
         <v>109.0625</v>
       </c>
       <c r="H33" s="2">
-        <f t="shared" ref="H33:H44" si="27">(E33/D33-1)*100</f>
+        <f t="shared" ref="H33:H41" si="24">(E33/D33-1)*100</f>
         <v>2.3174012000827693</v>
       </c>
       <c r="I33" s="2">
-        <f t="shared" ref="I33:I44" si="28">(POWER((E33/$D$3),1/A33)-1)*100</f>
+        <f t="shared" ref="I33:I41" si="25">(POWER((E33/$D$3),1/A33)-1)*100</f>
         <v>1.3693729216394335</v>
       </c>
       <c r="J33" s="3">
@@ -3118,12 +3119,12 @@
         <v>0</v>
       </c>
       <c r="M33">
-        <f t="shared" ref="M33:M44" si="29">L33+E33</f>
+        <f t="shared" ref="M33:M41" si="26">L33+E33</f>
         <v>9890</v>
       </c>
       <c r="N33" s="2">
-        <f t="shared" si="1"/>
-        <v>154.53125</v>
+        <f t="shared" si="4"/>
+        <v>54.53125</v>
       </c>
       <c r="O33">
         <v>85827.9</v>
@@ -3132,8 +3133,8 @@
         <v>81465.600000000006</v>
       </c>
       <c r="Q33">
-        <f t="shared" ref="Q33:Q44" si="30">P33/$O$2*100</f>
-        <v>91.288313859607655</v>
+        <f t="shared" si="8"/>
+        <v>-8.7116861403923451</v>
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.3">
@@ -3153,19 +3154,19 @@
         <v>10200</v>
       </c>
       <c r="F34">
+        <f t="shared" si="22"/>
+        <v>310</v>
+      </c>
+      <c r="G34" s="2">
+        <f t="shared" si="23"/>
+        <v>115.15151515151516</v>
+      </c>
+      <c r="H34" s="2">
+        <f t="shared" si="24"/>
+        <v>3.1344792719919079</v>
+      </c>
+      <c r="I34" s="2">
         <f t="shared" si="25"/>
-        <v>310</v>
-      </c>
-      <c r="G34" s="2">
-        <f t="shared" si="26"/>
-        <v>115.15151515151516</v>
-      </c>
-      <c r="H34" s="2">
-        <f t="shared" si="27"/>
-        <v>3.1344792719919079</v>
-      </c>
-      <c r="I34" s="2">
-        <f t="shared" si="28"/>
         <v>1.4224145175464553</v>
       </c>
       <c r="J34" s="3">
@@ -3180,12 +3181,12 @@
         <v>0</v>
       </c>
       <c r="M34">
-        <f t="shared" si="29"/>
+        <f t="shared" si="26"/>
         <v>10200</v>
       </c>
       <c r="N34" s="2">
-        <f t="shared" si="1"/>
-        <v>159.375</v>
+        <f t="shared" si="4"/>
+        <v>59.375</v>
       </c>
       <c r="O34">
         <v>81465.600000000006</v>
@@ -3194,8 +3195,8 @@
         <v>82498</v>
       </c>
       <c r="Q34">
-        <f t="shared" si="30"/>
-        <v>92.445195478704036</v>
+        <f t="shared" si="8"/>
+        <v>-7.5548045212959636</v>
       </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.3">
@@ -3215,19 +3216,19 @@
         <v>10565</v>
       </c>
       <c r="F35">
+        <f t="shared" si="22"/>
+        <v>365</v>
+      </c>
+      <c r="G35" s="2">
+        <f t="shared" si="23"/>
+        <v>122.5</v>
+      </c>
+      <c r="H35" s="2">
+        <f t="shared" si="24"/>
+        <v>3.5784313725490291</v>
+      </c>
+      <c r="I35" s="2">
         <f t="shared" si="25"/>
-        <v>365</v>
-      </c>
-      <c r="G35" s="2">
-        <f t="shared" si="26"/>
-        <v>122.5</v>
-      </c>
-      <c r="H35" s="2">
-        <f t="shared" si="27"/>
-        <v>3.5784313725490291</v>
-      </c>
-      <c r="I35" s="2">
-        <f t="shared" si="28"/>
         <v>1.4851815919634914</v>
       </c>
       <c r="J35" s="3">
@@ -3242,12 +3243,12 @@
         <v>0</v>
       </c>
       <c r="M35">
-        <f t="shared" si="29"/>
+        <f t="shared" si="26"/>
         <v>10565</v>
       </c>
       <c r="N35" s="2">
-        <f t="shared" si="1"/>
-        <v>165.078125</v>
+        <f t="shared" si="4"/>
+        <v>65.078125</v>
       </c>
       <c r="O35">
         <v>82498</v>
@@ -3256,8 +3257,8 @@
         <v>82847.899999999994</v>
       </c>
       <c r="Q35">
-        <f t="shared" si="30"/>
-        <v>92.837284667508584</v>
+        <f t="shared" si="8"/>
+        <v>-7.1627153324914161</v>
       </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.3">
@@ -3277,19 +3278,19 @@
         <v>10845</v>
       </c>
       <c r="F36">
+        <f t="shared" si="22"/>
+        <v>280</v>
+      </c>
+      <c r="G36" s="2">
+        <f t="shared" si="23"/>
+        <v>127</v>
+      </c>
+      <c r="H36" s="2">
+        <f t="shared" si="24"/>
+        <v>2.6502602934216801</v>
+      </c>
+      <c r="I36" s="2">
         <f t="shared" si="25"/>
-        <v>280</v>
-      </c>
-      <c r="G36" s="2">
-        <f t="shared" si="26"/>
-        <v>127</v>
-      </c>
-      <c r="H36" s="2">
-        <f t="shared" si="27"/>
-        <v>2.6502602934216801</v>
-      </c>
-      <c r="I36" s="2">
-        <f t="shared" si="28"/>
         <v>1.5182853250945039</v>
       </c>
       <c r="J36" s="3">
@@ -3304,12 +3305,12 @@
         <v>0</v>
       </c>
       <c r="M36">
-        <f t="shared" si="29"/>
+        <f t="shared" si="26"/>
         <v>10845</v>
       </c>
       <c r="N36" s="2">
-        <f t="shared" si="1"/>
-        <v>169.453125</v>
+        <f t="shared" si="4"/>
+        <v>69.453125</v>
       </c>
       <c r="O36">
         <v>82847.899999999994</v>
@@ -3318,8 +3319,8 @@
         <v>82606.7</v>
       </c>
       <c r="Q36">
-        <f t="shared" si="30"/>
-        <v>92.567001980056006</v>
+        <f t="shared" si="8"/>
+        <v>-7.4329980199439944</v>
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.3">
@@ -3339,19 +3340,19 @@
         <v>22699</v>
       </c>
       <c r="F37">
+        <f t="shared" si="22"/>
+        <v>1854</v>
+      </c>
+      <c r="G37" s="2">
+        <f t="shared" si="23"/>
+        <v>452.75</v>
+      </c>
+      <c r="H37" s="2">
+        <f t="shared" si="24"/>
+        <v>8.8942192372271514</v>
+      </c>
+      <c r="I37" s="2">
         <f t="shared" si="25"/>
-        <v>1854</v>
-      </c>
-      <c r="G37" s="2">
-        <f t="shared" si="26"/>
-        <v>452.75</v>
-      </c>
-      <c r="H37" s="2">
-        <f t="shared" si="27"/>
-        <v>8.8942192372271514</v>
-      </c>
-      <c r="I37" s="2">
-        <f t="shared" si="28"/>
         <v>3.5792984780890658</v>
       </c>
       <c r="J37" s="3">
@@ -3366,12 +3367,12 @@
         <v>-10000</v>
       </c>
       <c r="M37">
-        <f t="shared" si="29"/>
+        <f t="shared" si="26"/>
         <v>12699</v>
       </c>
       <c r="N37" s="2">
-        <f>M37/$D$2*100</f>
-        <v>198.421875</v>
+        <f t="shared" si="4"/>
+        <v>98.421875</v>
       </c>
       <c r="O37">
         <v>82606.7</v>
@@ -3380,8 +3381,8 @@
         <v>78951.899999999994</v>
       </c>
       <c r="Q37">
-        <f t="shared" si="30"/>
-        <v>88.471524508655889</v>
+        <f t="shared" si="8"/>
+        <v>-11.528475491344111</v>
       </c>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.3">
@@ -3401,19 +3402,19 @@
         <v>22955</v>
       </c>
       <c r="F38">
+        <f t="shared" si="22"/>
+        <v>256</v>
+      </c>
+      <c r="G38" s="2">
+        <f t="shared" si="23"/>
+        <v>447.43243243243245</v>
+      </c>
+      <c r="H38" s="2">
+        <f t="shared" si="24"/>
+        <v>1.1278029869157269</v>
+      </c>
+      <c r="I38" s="2">
         <f t="shared" si="25"/>
-        <v>256</v>
-      </c>
-      <c r="G38" s="2">
-        <f t="shared" si="26"/>
-        <v>447.43243243243245</v>
-      </c>
-      <c r="H38" s="2">
-        <f t="shared" si="27"/>
-        <v>1.1278029869157269</v>
-      </c>
-      <c r="I38" s="2">
-        <f t="shared" si="28"/>
         <v>3.5122668721563333</v>
       </c>
       <c r="J38" s="3">
@@ -3421,19 +3422,19 @@
         <v>10188.728904569132</v>
       </c>
       <c r="K38" s="3">
-        <f t="shared" ref="K38:K41" si="31">M38-J38</f>
+        <f t="shared" ref="K38:K41" si="27">M38-J38</f>
         <v>2766.2710954308677</v>
       </c>
       <c r="L38">
         <v>-10000</v>
       </c>
       <c r="M38">
-        <f t="shared" si="29"/>
+        <f t="shared" si="26"/>
         <v>12955</v>
       </c>
       <c r="N38" s="2">
-        <f t="shared" ref="N38:N41" si="32">M38/$D$2*100</f>
-        <v>202.42187500000003</v>
+        <f t="shared" si="4"/>
+        <v>102.42187500000003</v>
       </c>
       <c r="O38">
         <v>78951.899999999994</v>
@@ -3442,8 +3443,8 @@
         <v>78410.600000000006</v>
       </c>
       <c r="Q38">
-        <f t="shared" si="30"/>
-        <v>87.864957266872793</v>
+        <f t="shared" si="8"/>
+        <v>-12.135042733127207</v>
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.3">
@@ -3463,19 +3464,19 @@
         <v>24388</v>
       </c>
       <c r="F39">
+        <f t="shared" si="22"/>
+        <v>1433</v>
+      </c>
+      <c r="G39" s="2">
+        <f t="shared" si="23"/>
+        <v>473.36842105263156</v>
+      </c>
+      <c r="H39" s="2">
+        <f t="shared" si="24"/>
+        <v>6.2426486604225673</v>
+      </c>
+      <c r="I39" s="2">
         <f t="shared" si="25"/>
-        <v>1433</v>
-      </c>
-      <c r="G39" s="2">
-        <f t="shared" si="26"/>
-        <v>473.36842105263156</v>
-      </c>
-      <c r="H39" s="2">
-        <f t="shared" si="27"/>
-        <v>6.2426486604225673</v>
-      </c>
-      <c r="I39" s="2">
-        <f t="shared" si="28"/>
         <v>3.5832120312270677</v>
       </c>
       <c r="J39" s="3">
@@ -3483,19 +3484,19 @@
         <v>10321.18238032853</v>
       </c>
       <c r="K39" s="3">
-        <f t="shared" si="31"/>
+        <f t="shared" si="27"/>
         <v>4066.8176196714703</v>
       </c>
       <c r="L39">
         <v>-10000</v>
       </c>
       <c r="M39">
-        <f t="shared" si="29"/>
+        <f t="shared" si="26"/>
         <v>14388</v>
       </c>
       <c r="N39" s="2">
-        <f t="shared" si="32"/>
-        <v>224.8125</v>
+        <f t="shared" si="4"/>
+        <v>124.8125</v>
       </c>
       <c r="O39">
         <v>78410.600000000006</v>
@@ -3504,8 +3505,8 @@
         <v>76791.100000000006</v>
       </c>
       <c r="Q39">
-        <f t="shared" si="30"/>
-        <v>86.050186071477015</v>
+        <f t="shared" si="8"/>
+        <v>-13.949813928522985</v>
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.3">
@@ -3525,19 +3526,19 @@
         <v>24713</v>
       </c>
       <c r="F40">
+        <f t="shared" si="22"/>
+        <v>325</v>
+      </c>
+      <c r="G40" s="2">
+        <f t="shared" si="23"/>
+        <v>469.56410256410254</v>
+      </c>
+      <c r="H40" s="2">
+        <f t="shared" si="24"/>
+        <v>1.3326226012793096</v>
+      </c>
+      <c r="I40" s="2">
         <f t="shared" si="25"/>
-        <v>325</v>
-      </c>
-      <c r="G40" s="2">
-        <f t="shared" si="26"/>
-        <v>469.56410256410254</v>
-      </c>
-      <c r="H40" s="2">
-        <f t="shared" si="27"/>
-        <v>1.3326226012793096</v>
-      </c>
-      <c r="I40" s="2">
-        <f t="shared" si="28"/>
         <v>3.5248848916893172</v>
       </c>
       <c r="J40" s="3">
@@ -3545,19 +3546,19 @@
         <v>10455.357751272799</v>
       </c>
       <c r="K40" s="3">
-        <f t="shared" si="31"/>
+        <f t="shared" si="27"/>
         <v>4257.6422487272011</v>
       </c>
       <c r="L40">
         <v>-10000</v>
       </c>
       <c r="M40">
-        <f t="shared" si="29"/>
+        <f t="shared" si="26"/>
         <v>14713</v>
       </c>
       <c r="N40" s="2">
-        <f t="shared" si="32"/>
-        <v>229.890625</v>
+        <f t="shared" si="4"/>
+        <v>129.890625</v>
       </c>
       <c r="O40">
         <v>76791.100000000006</v>
@@ -3566,8 +3567,8 @@
         <v>81192.2</v>
       </c>
       <c r="Q40">
-        <f t="shared" si="30"/>
-        <v>90.981948657495138</v>
+        <f t="shared" si="8"/>
+        <v>-9.0180513425048616</v>
       </c>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.3">
@@ -3587,19 +3588,19 @@
         <v>25029</v>
       </c>
       <c r="F41">
+        <f t="shared" si="22"/>
+        <v>316</v>
+      </c>
+      <c r="G41" s="2">
+        <f t="shared" si="23"/>
+        <v>465.72500000000002</v>
+      </c>
+      <c r="H41" s="2">
+        <f t="shared" si="24"/>
+        <v>1.2786792376481948</v>
+      </c>
+      <c r="I41" s="2">
         <f t="shared" si="25"/>
-        <v>316</v>
-      </c>
-      <c r="G41" s="2">
-        <f t="shared" si="26"/>
-        <v>465.72500000000002</v>
-      </c>
-      <c r="H41" s="2">
-        <f t="shared" si="27"/>
-        <v>1.2786792376481948</v>
-      </c>
-      <c r="I41" s="2">
-        <f t="shared" si="28"/>
         <v>3.4681271506401101</v>
       </c>
       <c r="J41" s="3">
@@ -3607,19 +3608,19 @@
         <v>10591.277402039344</v>
       </c>
       <c r="K41" s="3">
-        <f t="shared" si="31"/>
+        <f t="shared" si="27"/>
         <v>4437.7225979606555</v>
       </c>
       <c r="L41">
         <v>-10000</v>
       </c>
       <c r="M41">
-        <f t="shared" si="29"/>
+        <f t="shared" si="26"/>
         <v>15029</v>
       </c>
       <c r="N41" s="2">
-        <f t="shared" si="32"/>
-        <v>234.828125</v>
+        <f t="shared" si="4"/>
+        <v>134.828125</v>
       </c>
       <c r="O41">
         <v>81192.2</v>
@@ -3628,8 +3629,8 @@
         <v>81812</v>
       </c>
       <c r="Q41">
-        <f t="shared" si="30"/>
-        <v>91.67648103594918</v>
+        <f t="shared" si="8"/>
+        <v>-8.3235189640508196</v>
       </c>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
자동 업데이트: 2025-04-12 12:45:01
</commit_message>
<xml_diff>
--- a/data/daily_report.xlsx
+++ b/data/daily_report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c58a53286e4c1d7a/문서/GitHub/Dashboard/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="213" documentId="8_{9DD2A88B-03DA-4864-84CC-4418086E8BD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5E7B59D6-4343-42D8-B7C5-9B9F06A6B00E}"/>
+  <xr:revisionPtr revIDLastSave="218" documentId="8_{9DD2A88B-03DA-4864-84CC-4418086E8BD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{52BC68C4-853E-42DA-9F03-2D4DFFB9A1EC}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{4AB8DADE-1167-4E84-9D67-55086BA93884}"/>
   </bookViews>
@@ -1092,7 +1092,7 @@
   <dimension ref="A1:Q44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+      <selection activeCell="Q3" sqref="Q3:Q41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1202,8 +1202,8 @@
         <v>6400</v>
       </c>
       <c r="N2" s="2">
-        <f>M2/$D$2*100-100</f>
-        <v>0</v>
+        <f>M2/$D$2*100</f>
+        <v>100</v>
       </c>
       <c r="O2">
         <v>89239.9</v>
@@ -1212,7 +1212,7 @@
         <v>89239.9</v>
       </c>
       <c r="Q2">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
@@ -1263,8 +1263,8 @@
         <v>6546</v>
       </c>
       <c r="N3" s="2">
-        <f t="shared" ref="N3:N41" si="4">M3/$D$2*100-100</f>
-        <v>2.2812499999999858</v>
+        <f t="shared" ref="N3:N41" si="4">M3/$D$2*100</f>
+        <v>102.28124999999999</v>
       </c>
       <c r="O3">
         <v>89239.9</v>
@@ -1273,8 +1273,8 @@
         <v>83157.100000000006</v>
       </c>
       <c r="Q3">
-        <f>P3/$O$2*100-100</f>
-        <v>-6.8162335457569867</v>
+        <f>P3/$O$2*100</f>
+        <v>93.183766454243013</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
@@ -1326,7 +1326,7 @@
       </c>
       <c r="N4" s="2">
         <f t="shared" si="4"/>
-        <v>4.515625</v>
+        <v>104.515625</v>
       </c>
       <c r="O4">
         <v>83157.100000000006</v>
@@ -1335,8 +1335,8 @@
         <v>88477.3</v>
       </c>
       <c r="Q4">
-        <f t="shared" ref="Q4:Q41" si="8">P4/$O$2*100-100</f>
-        <v>-0.854550486945854</v>
+        <f t="shared" ref="Q4:Q41" si="8">P4/$O$2*100</f>
+        <v>99.145449513054146</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
@@ -1388,7 +1388,7 @@
       </c>
       <c r="N5" s="2">
         <f t="shared" si="4"/>
-        <v>6.9687499999999858</v>
+        <v>106.96874999999999</v>
       </c>
       <c r="O5">
         <v>88477.3</v>
@@ -1398,7 +1398,7 @@
       </c>
       <c r="Q5">
         <f t="shared" si="8"/>
-        <v>0.59446503189717248</v>
+        <v>100.59446503189717</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
@@ -1450,7 +1450,7 @@
       </c>
       <c r="N6" s="2">
         <f t="shared" si="4"/>
-        <v>9.6093750000000142</v>
+        <v>109.60937500000001</v>
       </c>
       <c r="O6">
         <v>89770.4</v>
@@ -1460,7 +1460,7 @@
       </c>
       <c r="Q6">
         <f t="shared" si="8"/>
-        <v>1.3129777151252</v>
+        <v>101.3129777151252</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
@@ -1512,7 +1512,7 @@
       </c>
       <c r="N7" s="2">
         <f t="shared" si="4"/>
-        <v>10.15625</v>
+        <v>110.15625</v>
       </c>
       <c r="O7">
         <v>90411.6</v>
@@ -1522,7 +1522,7 @@
       </c>
       <c r="Q7">
         <f t="shared" si="8"/>
-        <v>-3.2682690141965622</v>
+        <v>96.731730985803438</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
@@ -1574,7 +1574,7 @@
       </c>
       <c r="N8" s="2">
         <f t="shared" si="4"/>
-        <v>9.0468750000000142</v>
+        <v>109.04687500000001</v>
       </c>
       <c r="O8">
         <v>86323.3</v>
@@ -1584,7 +1584,7 @@
       </c>
       <c r="Q8">
         <f t="shared" si="8"/>
-        <v>-6.3613921575438752</v>
+        <v>93.638607842456125</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
@@ -1636,7 +1636,7 @@
       </c>
       <c r="N9" s="2">
         <f t="shared" si="4"/>
-        <v>12.03125</v>
+        <v>112.03125</v>
       </c>
       <c r="O9">
         <v>83563</v>
@@ -1646,7 +1646,7 @@
       </c>
       <c r="Q9">
         <f t="shared" si="8"/>
-        <v>-10.562763965445939</v>
+        <v>89.437236034554061</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
@@ -1698,7 +1698,7 @@
       </c>
       <c r="N10" s="2">
         <f t="shared" si="4"/>
-        <v>14.296875000000014</v>
+        <v>114.29687500000001</v>
       </c>
       <c r="O10">
         <v>79813.7</v>
@@ -1708,7 +1708,7 @@
       </c>
       <c r="Q10">
         <f t="shared" si="8"/>
-        <v>-9.6640628239162112</v>
+        <v>90.335937176083789</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
@@ -1760,7 +1760,7 @@
       </c>
       <c r="N11" s="2">
         <f t="shared" si="4"/>
-        <v>6.953125</v>
+        <v>106.953125</v>
       </c>
       <c r="O11">
         <v>80615.7</v>
@@ -1770,7 +1770,7 @@
       </c>
       <c r="Q11">
         <f t="shared" si="8"/>
-        <v>-8.6721298432651679</v>
+        <v>91.327870156734832</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.3">
@@ -1822,7 +1822,7 @@
       </c>
       <c r="N12" s="2">
         <f t="shared" si="4"/>
-        <v>18.234375</v>
+        <v>118.234375</v>
       </c>
       <c r="O12">
         <v>81500.899999999994</v>
@@ -1832,7 +1832,7 @@
       </c>
       <c r="Q12">
         <f t="shared" si="8"/>
-        <v>-8.150278070683612</v>
+        <v>91.849721929316388</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.3">
@@ -1884,7 +1884,7 @@
       </c>
       <c r="N13" s="2">
         <f t="shared" si="4"/>
-        <v>21.296875</v>
+        <v>121.296875</v>
       </c>
       <c r="O13">
         <v>81966.600000000006</v>
@@ -1894,7 +1894,7 @@
       </c>
       <c r="Q13">
         <f t="shared" si="8"/>
-        <v>-6.4364706818362549</v>
+        <v>93.563529318163745</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
@@ -1946,7 +1946,7 @@
       </c>
       <c r="N14" s="2">
         <f t="shared" si="4"/>
-        <v>22.578125</v>
+        <v>122.578125</v>
       </c>
       <c r="O14">
         <v>83496</v>
@@ -1956,7 +1956,7 @@
       </c>
       <c r="Q14">
         <f t="shared" si="8"/>
-        <v>-5.7502305583040823</v>
+        <v>94.249769441695918</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.3">
@@ -2008,7 +2008,7 @@
       </c>
       <c r="N15" s="2">
         <f t="shared" si="4"/>
-        <v>23.109375000000014</v>
+        <v>123.10937500000001</v>
       </c>
       <c r="O15">
         <v>84108.4</v>
@@ -2018,7 +2018,7 @@
       </c>
       <c r="Q15">
         <f t="shared" si="8"/>
-        <v>-6.6177797151274262</v>
+        <v>93.382220284872574</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.3">
@@ -2070,7 +2070,7 @@
       </c>
       <c r="N16" s="2">
         <f t="shared" si="4"/>
-        <v>24.25</v>
+        <v>124.25</v>
       </c>
       <c r="O16">
         <v>83334.2</v>
@@ -2080,7 +2080,7 @@
       </c>
       <c r="Q16">
         <f t="shared" si="8"/>
-        <v>-7.134476842757536</v>
+        <v>92.865523157242464</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.3">
@@ -2132,7 +2132,7 @@
       </c>
       <c r="N17" s="2">
         <f t="shared" si="4"/>
-        <v>21.828125</v>
+        <v>121.828125</v>
       </c>
       <c r="O17">
         <v>82873.100000000006</v>
@@ -2142,7 +2142,7 @@
       </c>
       <c r="Q17">
         <f t="shared" si="8"/>
-        <v>-8.326320401524427</v>
+        <v>91.673679598475573</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.3">
@@ -2194,7 +2194,7 @@
       </c>
       <c r="N18" s="2">
         <f t="shared" si="4"/>
-        <v>30.234375</v>
+        <v>130.234375</v>
       </c>
       <c r="O18">
         <v>81809.5</v>
@@ -2204,7 +2204,7 @@
       </c>
       <c r="Q18">
         <f t="shared" si="8"/>
-        <v>-5.5720591349833484</v>
+        <v>94.427940865016652</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.3">
@@ -2256,7 +2256,7 @@
       </c>
       <c r="N19" s="2">
         <f t="shared" si="4"/>
-        <v>32.203125</v>
+        <v>132.203125</v>
       </c>
       <c r="O19">
         <v>84267.4</v>
@@ -2266,7 +2266,7 @@
       </c>
       <c r="Q19">
         <f t="shared" si="8"/>
-        <v>-3.4920478395874284</v>
+        <v>96.507952160412572</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.3">
@@ -2318,7 +2318,7 @@
       </c>
       <c r="N20" s="2">
         <f t="shared" si="4"/>
-        <v>30.15625</v>
+        <v>130.15625</v>
       </c>
       <c r="O20">
         <v>86123.6</v>
@@ -2328,7 +2328,7 @@
       </c>
       <c r="Q20">
         <f t="shared" si="8"/>
-        <v>-5.6475858892714967</v>
+        <v>94.352414110728503</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.3">
@@ -2380,7 +2380,7 @@
       </c>
       <c r="N21" s="2">
         <f t="shared" si="4"/>
-        <v>30.171875</v>
+        <v>130.171875</v>
       </c>
       <c r="O21">
         <v>84200</v>
@@ -2390,7 +2390,7 @@
       </c>
       <c r="Q21">
         <f t="shared" si="8"/>
-        <v>-5.9046457918487079</v>
+        <v>94.095354208151292</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.3">
@@ -2442,7 +2442,7 @@
       </c>
       <c r="N22" s="2">
         <f t="shared" si="4"/>
-        <v>34.21875</v>
+        <v>134.21875</v>
       </c>
       <c r="O22">
         <v>83970.6</v>
@@ -2452,7 +2452,7 @@
       </c>
       <c r="Q22">
         <f t="shared" si="8"/>
-        <v>-4.905765246263158</v>
+        <v>95.094234753736842</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.3">
@@ -2504,7 +2504,7 @@
       </c>
       <c r="N23" s="2">
         <f t="shared" si="4"/>
-        <v>39.453125</v>
+        <v>139.453125</v>
       </c>
       <c r="O23">
         <v>84862</v>
@@ -2514,7 +2514,7 @@
       </c>
       <c r="Q23">
         <f t="shared" si="8"/>
-        <v>-1.4779263535705383</v>
+        <v>98.522073646429462</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.3">
@@ -2566,7 +2566,7 @@
       </c>
       <c r="N24" s="2">
         <f t="shared" si="4"/>
-        <v>42.390625</v>
+        <v>142.390625</v>
       </c>
       <c r="O24">
         <v>87921</v>
@@ -2576,7 +2576,7 @@
       </c>
       <c r="Q24">
         <f t="shared" si="8"/>
-        <v>-1.4060974967475204</v>
+        <v>98.59390250325248</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.3">
@@ -2628,7 +2628,7 @@
       </c>
       <c r="N25" s="2">
         <f t="shared" si="4"/>
-        <v>43.171875</v>
+        <v>143.171875</v>
       </c>
       <c r="O25">
         <v>87985.1</v>
@@ -2638,7 +2638,7 @@
       </c>
       <c r="Q25">
         <f t="shared" si="8"/>
-        <v>-2.8056956585563029</v>
+        <v>97.194304341443697</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.3">
@@ -2690,7 +2690,7 @@
       </c>
       <c r="N26" s="2">
         <f t="shared" si="4"/>
-        <v>46.140625</v>
+        <v>146.140625</v>
       </c>
       <c r="O26">
         <v>86736.1</v>
@@ -2700,7 +2700,7 @@
       </c>
       <c r="Q26">
         <f t="shared" si="8"/>
-        <v>-2.2308406889743111</v>
+        <v>97.769159311025689</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.3">
@@ -2752,7 +2752,7 @@
       </c>
       <c r="N27" s="2">
         <f t="shared" si="4"/>
-        <v>46.140625</v>
+        <v>146.140625</v>
       </c>
       <c r="O27">
         <v>87249.1</v>
@@ -2762,7 +2762,7 @@
       </c>
       <c r="Q27">
         <f t="shared" si="8"/>
-        <v>-5.7537043407713213</v>
+        <v>94.246295659228679</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.3">
@@ -2814,7 +2814,7 @@
       </c>
       <c r="N28" s="2">
         <f t="shared" si="4"/>
-        <v>46.875</v>
+        <v>146.875</v>
       </c>
       <c r="O28">
         <v>84105.3</v>
@@ -2824,7 +2824,7 @@
       </c>
       <c r="Q28">
         <f t="shared" si="8"/>
-        <v>-7.6323483105651064</v>
+        <v>92.367651689434894</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.3">
@@ -2876,7 +2876,7 @@
       </c>
       <c r="N29" s="2">
         <f t="shared" si="4"/>
-        <v>47.65625</v>
+        <v>147.65625</v>
       </c>
       <c r="O29">
         <v>82428.800000000003</v>
@@ -2886,7 +2886,7 @@
       </c>
       <c r="Q29">
         <f t="shared" si="8"/>
-        <v>-7.2779104414056803</v>
+        <v>92.72208955859432</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.3">
@@ -2938,7 +2938,7 @@
       </c>
       <c r="N30" s="2">
         <f t="shared" si="4"/>
-        <v>47.6875</v>
+        <v>147.6875</v>
       </c>
       <c r="O30">
         <v>82745.100000000006</v>
@@ -2948,7 +2948,7 @@
       </c>
       <c r="Q30">
         <f t="shared" si="8"/>
-        <v>-6.4901462238303651</v>
+        <v>93.509853776169635</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.3">
@@ -3000,7 +3000,7 @@
       </c>
       <c r="N31" s="2">
         <f t="shared" si="4"/>
-        <v>48.625</v>
+        <v>148.625</v>
       </c>
       <c r="O31">
         <v>83448.100000000006</v>
@@ -3010,7 +3010,7 @@
       </c>
       <c r="Q31">
         <f t="shared" si="8"/>
-        <v>-5.7160530211262</v>
+        <v>94.2839469788738</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.3">
@@ -3062,7 +3062,7 @@
       </c>
       <c r="N32" s="2">
         <f t="shared" si="4"/>
-        <v>51.03125</v>
+        <v>151.03125</v>
       </c>
       <c r="O32">
         <v>84138.9</v>
@@ -3072,7 +3072,7 @@
       </c>
       <c r="Q32">
         <f t="shared" si="8"/>
-        <v>-3.8234018639644347</v>
+        <v>96.176598136035565</v>
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.3">
@@ -3124,7 +3124,7 @@
       </c>
       <c r="N33" s="2">
         <f t="shared" si="4"/>
-        <v>54.53125</v>
+        <v>154.53125</v>
       </c>
       <c r="O33">
         <v>85827.9</v>
@@ -3134,7 +3134,7 @@
       </c>
       <c r="Q33">
         <f t="shared" si="8"/>
-        <v>-8.7116861403923451</v>
+        <v>91.288313859607655</v>
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.3">
@@ -3186,7 +3186,7 @@
       </c>
       <c r="N34" s="2">
         <f t="shared" si="4"/>
-        <v>59.375</v>
+        <v>159.375</v>
       </c>
       <c r="O34">
         <v>81465.600000000006</v>
@@ -3196,7 +3196,7 @@
       </c>
       <c r="Q34">
         <f t="shared" si="8"/>
-        <v>-7.5548045212959636</v>
+        <v>92.445195478704036</v>
       </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.3">
@@ -3248,7 +3248,7 @@
       </c>
       <c r="N35" s="2">
         <f t="shared" si="4"/>
-        <v>65.078125</v>
+        <v>165.078125</v>
       </c>
       <c r="O35">
         <v>82498</v>
@@ -3258,7 +3258,7 @@
       </c>
       <c r="Q35">
         <f t="shared" si="8"/>
-        <v>-7.1627153324914161</v>
+        <v>92.837284667508584</v>
       </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.3">
@@ -3310,7 +3310,7 @@
       </c>
       <c r="N36" s="2">
         <f t="shared" si="4"/>
-        <v>69.453125</v>
+        <v>169.453125</v>
       </c>
       <c r="O36">
         <v>82847.899999999994</v>
@@ -3320,7 +3320,7 @@
       </c>
       <c r="Q36">
         <f t="shared" si="8"/>
-        <v>-7.4329980199439944</v>
+        <v>92.567001980056006</v>
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.3">
@@ -3372,7 +3372,7 @@
       </c>
       <c r="N37" s="2">
         <f t="shared" si="4"/>
-        <v>98.421875</v>
+        <v>198.421875</v>
       </c>
       <c r="O37">
         <v>82606.7</v>
@@ -3382,7 +3382,7 @@
       </c>
       <c r="Q37">
         <f t="shared" si="8"/>
-        <v>-11.528475491344111</v>
+        <v>88.471524508655889</v>
       </c>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.3">
@@ -3434,7 +3434,7 @@
       </c>
       <c r="N38" s="2">
         <f t="shared" si="4"/>
-        <v>102.42187500000003</v>
+        <v>202.42187500000003</v>
       </c>
       <c r="O38">
         <v>78951.899999999994</v>
@@ -3444,7 +3444,7 @@
       </c>
       <c r="Q38">
         <f t="shared" si="8"/>
-        <v>-12.135042733127207</v>
+        <v>87.864957266872793</v>
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.3">
@@ -3496,7 +3496,7 @@
       </c>
       <c r="N39" s="2">
         <f t="shared" si="4"/>
-        <v>124.8125</v>
+        <v>224.8125</v>
       </c>
       <c r="O39">
         <v>78410.600000000006</v>
@@ -3506,7 +3506,7 @@
       </c>
       <c r="Q39">
         <f t="shared" si="8"/>
-        <v>-13.949813928522985</v>
+        <v>86.050186071477015</v>
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.3">
@@ -3558,7 +3558,7 @@
       </c>
       <c r="N40" s="2">
         <f t="shared" si="4"/>
-        <v>129.890625</v>
+        <v>229.890625</v>
       </c>
       <c r="O40">
         <v>76791.100000000006</v>
@@ -3568,7 +3568,7 @@
       </c>
       <c r="Q40">
         <f t="shared" si="8"/>
-        <v>-9.0180513425048616</v>
+        <v>90.981948657495138</v>
       </c>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.3">
@@ -3620,7 +3620,7 @@
       </c>
       <c r="N41" s="2">
         <f t="shared" si="4"/>
-        <v>134.828125</v>
+        <v>234.828125</v>
       </c>
       <c r="O41">
         <v>81192.2</v>
@@ -3630,7 +3630,7 @@
       </c>
       <c r="Q41">
         <f t="shared" si="8"/>
-        <v>-8.3235189640508196</v>
+        <v>91.67648103594918</v>
       </c>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
자동 업데이트: 2025-04-17 00:59:41
</commit_message>
<xml_diff>
--- a/data/daily_report.xlsx
+++ b/data/daily_report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c58a53286e4c1d7a/문서/GitHub/Dashboard/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="218" documentId="8_{9DD2A88B-03DA-4864-84CC-4418086E8BD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{52BC68C4-853E-42DA-9F03-2D4DFFB9A1EC}"/>
+  <xr:revisionPtr revIDLastSave="233" documentId="8_{9DD2A88B-03DA-4864-84CC-4418086E8BD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D384F2B2-8A84-4D14-93B1-C02DFC413388}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{4AB8DADE-1167-4E84-9D67-55086BA93884}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24660" windowHeight="21000" xr2:uid="{4AB8DADE-1167-4E84-9D67-55086BA93884}"/>
   </bookViews>
   <sheets>
     <sheet name="daily_report" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="24">
   <si>
     <t>Index</t>
   </si>
@@ -1089,10 +1089,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48182F73-FFD5-43FF-A3B0-19A54A277A3F}">
-  <dimension ref="A1:Q44"/>
+  <dimension ref="A1:Q47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3:Q41"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N33" sqref="N33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1310,7 +1310,7 @@
         <v>2.2328836529616813</v>
       </c>
       <c r="J4" s="3">
-        <f t="shared" ref="J4:J41" si="7">J3*1.013</f>
+        <f t="shared" ref="J4:J47" si="7">J3*1.013</f>
         <v>6567.4815999999983</v>
       </c>
       <c r="K4" s="3">
@@ -3634,31 +3634,323 @@
       </c>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B42" s="1"/>
-      <c r="G42" s="2"/>
-      <c r="H42" s="2"/>
-      <c r="I42" s="2"/>
-      <c r="J42" s="3"/>
-      <c r="K42" s="3"/>
-      <c r="N42" s="2"/>
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" s="1">
+        <v>45759</v>
+      </c>
+      <c r="C42" t="s">
+        <v>22</v>
+      </c>
+      <c r="D42">
+        <v>25029</v>
+      </c>
+      <c r="E42">
+        <v>25088</v>
+      </c>
+      <c r="F42">
+        <f t="shared" ref="F42:F47" si="28">E42-D42</f>
+        <v>59</v>
+      </c>
+      <c r="G42" s="2">
+        <f t="shared" ref="G42:G47" si="29">(E42-$D$2)/A42</f>
+        <v>455.80487804878049</v>
+      </c>
+      <c r="H42" s="2">
+        <f t="shared" ref="H42:H47" si="30">(E42/D42-1)*100</f>
+        <v>0.23572655719366065</v>
+      </c>
+      <c r="I42" s="2">
+        <f t="shared" ref="I42:I47" si="31">(POWER((E42/$D$3),1/A42)-1)*100</f>
+        <v>3.3880613542311755</v>
+      </c>
+      <c r="J42" s="3">
+        <f t="shared" si="7"/>
+        <v>10728.964008265855</v>
+      </c>
+      <c r="K42" s="3">
+        <f t="shared" ref="K42:K47" si="32">M42-J42</f>
+        <v>4359.0359917341448</v>
+      </c>
+      <c r="L42">
+        <v>-10000</v>
+      </c>
+      <c r="M42">
+        <f t="shared" ref="M42:M47" si="33">L42+E42</f>
+        <v>15088</v>
+      </c>
+      <c r="N42" s="2">
+        <f t="shared" ref="N42:N47" si="34">M42/$D$2*100</f>
+        <v>235.75</v>
+      </c>
+      <c r="O42">
+        <v>81812</v>
+      </c>
+      <c r="P42">
+        <v>84763.1</v>
+      </c>
+      <c r="Q42">
+        <f t="shared" ref="Q42:Q47" si="35">P42/$O$2*100</f>
+        <v>94.983409887281383</v>
+      </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B43" s="1"/>
-      <c r="G43" s="2"/>
-      <c r="H43" s="2"/>
-      <c r="I43" s="2"/>
-      <c r="J43" s="3"/>
-      <c r="K43" s="3"/>
-      <c r="N43" s="2"/>
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" s="1">
+        <v>45760</v>
+      </c>
+      <c r="C43" t="s">
+        <v>23</v>
+      </c>
+      <c r="D43">
+        <v>25088</v>
+      </c>
+      <c r="E43">
+        <v>25195</v>
+      </c>
+      <c r="F43">
+        <f t="shared" si="28"/>
+        <v>107</v>
+      </c>
+      <c r="G43" s="2">
+        <f t="shared" si="29"/>
+        <v>447.5</v>
+      </c>
+      <c r="H43" s="2">
+        <f t="shared" si="30"/>
+        <v>0.42649872448978776</v>
+      </c>
+      <c r="I43" s="2">
+        <f t="shared" si="31"/>
+        <v>3.3165430633898429</v>
+      </c>
+      <c r="J43" s="3">
+        <f t="shared" si="7"/>
+        <v>10868.440540373311</v>
+      </c>
+      <c r="K43" s="3">
+        <f t="shared" si="32"/>
+        <v>4326.5594596266892</v>
+      </c>
+      <c r="L43">
+        <v>-10000</v>
+      </c>
+      <c r="M43">
+        <f t="shared" si="33"/>
+        <v>15195</v>
+      </c>
+      <c r="N43" s="2">
+        <f t="shared" si="34"/>
+        <v>237.42187499999997</v>
+      </c>
+      <c r="O43">
+        <v>84763.1</v>
+      </c>
+      <c r="P43">
+        <v>84024</v>
+      </c>
+      <c r="Q43">
+        <f t="shared" si="35"/>
+        <v>94.15519291258731</v>
+      </c>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B44" s="1"/>
-      <c r="G44" s="2"/>
-      <c r="H44" s="2"/>
-      <c r="I44" s="2"/>
-      <c r="J44" s="3"/>
-      <c r="K44" s="3"/>
-      <c r="N44" s="2"/>
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" s="1">
+        <v>45761</v>
+      </c>
+      <c r="C44" t="s">
+        <v>17</v>
+      </c>
+      <c r="D44">
+        <v>25195</v>
+      </c>
+      <c r="E44">
+        <v>25835</v>
+      </c>
+      <c r="F44">
+        <f t="shared" si="28"/>
+        <v>640</v>
+      </c>
+      <c r="G44" s="2">
+        <f t="shared" si="29"/>
+        <v>451.97674418604652</v>
+      </c>
+      <c r="H44" s="2">
+        <f t="shared" si="30"/>
+        <v>2.5401865449493854</v>
+      </c>
+      <c r="I44" s="2">
+        <f t="shared" si="31"/>
+        <v>3.2984216732465654</v>
+      </c>
+      <c r="J44" s="3">
+        <f t="shared" si="7"/>
+        <v>11009.730267398163</v>
+      </c>
+      <c r="K44" s="3">
+        <f t="shared" si="32"/>
+        <v>4825.2697326018369</v>
+      </c>
+      <c r="L44">
+        <v>-10000</v>
+      </c>
+      <c r="M44">
+        <f t="shared" si="33"/>
+        <v>15835</v>
+      </c>
+      <c r="N44" s="2">
+        <f t="shared" si="34"/>
+        <v>247.421875</v>
+      </c>
+      <c r="O44">
+        <v>84024</v>
+      </c>
+      <c r="P44">
+        <v>85364.7</v>
+      </c>
+      <c r="Q44">
+        <f t="shared" si="35"/>
+        <v>95.657547800927617</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" s="1">
+        <v>45762</v>
+      </c>
+      <c r="C45" t="s">
+        <v>18</v>
+      </c>
+      <c r="D45">
+        <v>25835</v>
+      </c>
+      <c r="E45">
+        <v>25600</v>
+      </c>
+      <c r="F45">
+        <f t="shared" si="28"/>
+        <v>-235</v>
+      </c>
+      <c r="G45" s="2">
+        <f t="shared" si="29"/>
+        <v>436.36363636363637</v>
+      </c>
+      <c r="H45" s="2">
+        <f t="shared" si="30"/>
+        <v>-0.90961873427520823</v>
+      </c>
+      <c r="I45" s="2">
+        <f t="shared" si="31"/>
+        <v>3.200827973420961</v>
+      </c>
+      <c r="J45" s="3">
+        <f t="shared" si="7"/>
+        <v>11152.856760874338</v>
+      </c>
+      <c r="K45" s="3">
+        <f t="shared" si="32"/>
+        <v>4447.1432391256621</v>
+      </c>
+      <c r="L45">
+        <v>-10000</v>
+      </c>
+      <c r="M45">
+        <f t="shared" si="33"/>
+        <v>15600</v>
+      </c>
+      <c r="N45" s="2">
+        <f t="shared" si="34"/>
+        <v>243.75</v>
+      </c>
+      <c r="O45">
+        <v>85364.7</v>
+      </c>
+      <c r="P45">
+        <v>85100.2</v>
+      </c>
+      <c r="Q45">
+        <f t="shared" si="35"/>
+        <v>95.36115571622112</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46" s="1">
+        <v>45763</v>
+      </c>
+      <c r="C46" t="s">
+        <v>19</v>
+      </c>
+      <c r="D46">
+        <v>25600</v>
+      </c>
+      <c r="E46">
+        <v>26102</v>
+      </c>
+      <c r="F46">
+        <f t="shared" si="28"/>
+        <v>502</v>
+      </c>
+      <c r="G46" s="2">
+        <f t="shared" si="29"/>
+        <v>437.82222222222219</v>
+      </c>
+      <c r="H46" s="2">
+        <f t="shared" si="30"/>
+        <v>1.9609374999999929</v>
+      </c>
+      <c r="I46" s="2">
+        <f t="shared" si="31"/>
+        <v>3.1731117201337034</v>
+      </c>
+      <c r="J46" s="3">
+        <f t="shared" si="7"/>
+        <v>11297.843898765703</v>
+      </c>
+      <c r="K46" s="3">
+        <f t="shared" si="32"/>
+        <v>4804.1561012342972</v>
+      </c>
+      <c r="L46">
+        <v>-10000</v>
+      </c>
+      <c r="M46">
+        <f t="shared" si="33"/>
+        <v>16102</v>
+      </c>
+      <c r="N46" s="2">
+        <f t="shared" si="34"/>
+        <v>251.59375000000003</v>
+      </c>
+      <c r="O46">
+        <v>85100.2</v>
+      </c>
+      <c r="P46">
+        <v>84562.7</v>
+      </c>
+      <c r="Q46">
+        <f t="shared" si="35"/>
+        <v>94.758846659397875</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B47" s="1"/>
+      <c r="G47" s="2"/>
+      <c r="H47" s="2"/>
+      <c r="I47" s="2"/>
+      <c r="J47" s="3"/>
+      <c r="K47" s="3"/>
+      <c r="N47" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>

</xml_diff>

<commit_message>
자동 업데이트: 2025-05-03 21:52:32
</commit_message>
<xml_diff>
--- a/data/daily_report.xlsx
+++ b/data/daily_report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c58a53286e4c1d7a/문서/GitHub/Dashboard/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="233" documentId="8_{9DD2A88B-03DA-4864-84CC-4418086E8BD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D384F2B2-8A84-4D14-93B1-C02DFC413388}"/>
+  <xr:revisionPtr revIDLastSave="261" documentId="8_{9DD2A88B-03DA-4864-84CC-4418086E8BD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{39634E84-8401-4522-A891-14A66D1080C4}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24660" windowHeight="21000" xr2:uid="{4AB8DADE-1167-4E84-9D67-55086BA93884}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25050" windowHeight="21000" xr2:uid="{4AB8DADE-1167-4E84-9D67-55086BA93884}"/>
   </bookViews>
   <sheets>
     <sheet name="daily_report" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="24">
   <si>
     <t>Index</t>
   </si>
@@ -111,6 +111,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+  </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -569,7 +572,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
@@ -696,8 +699,11 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -710,8 +716,11 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="42" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - 강조색1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - 강조색2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - 강조색3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -743,6 +752,7 @@
     <cellStyle name="보통" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="설명 텍스트" xfId="16" builtinId="53" customBuiltin="1"/>
     <cellStyle name="셀 확인" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="쉼표 [0]" xfId="42" builtinId="6"/>
     <cellStyle name="연결된 셀" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="요약" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="입력" xfId="9" builtinId="20" customBuiltin="1"/>
@@ -766,10 +776,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1089,17 +1095,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48182F73-FFD5-43FF-A3B0-19A54A277A3F}">
-  <dimension ref="A1:Q47"/>
+  <dimension ref="A1:Q62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N33" sqref="N33"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M35" sqref="M35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9" style="4"/>
     <col min="7" max="7" width="11" customWidth="1"/>
     <col min="8" max="8" width="8.375" customWidth="1"/>
+    <col min="13" max="13" width="9" style="4"/>
     <col min="14" max="14" width="14.25" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="13.5" customWidth="1"/>
   </cols>
@@ -1114,10 +1122,10 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
       <c r="F1" t="s">
@@ -1141,7 +1149,7 @@
       <c r="L1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="4" t="s">
         <v>12</v>
       </c>
       <c r="N1" t="s">
@@ -1167,10 +1175,10 @@
       <c r="C2" t="s">
         <v>17</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="4">
         <v>6400</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="4">
         <v>6400</v>
       </c>
       <c r="F2">
@@ -1197,7 +1205,7 @@
       <c r="L2">
         <v>0</v>
       </c>
-      <c r="M2">
+      <c r="M2" s="4">
         <f>L2+E2</f>
         <v>6400</v>
       </c>
@@ -1225,10 +1233,10 @@
       <c r="C3" t="s">
         <v>18</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="4">
         <v>6400</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="4">
         <v>6546</v>
       </c>
       <c r="F3">
@@ -1258,7 +1266,7 @@
       <c r="L3">
         <v>0</v>
       </c>
-      <c r="M3">
+      <c r="M3" s="4">
         <f t="shared" ref="M3:M24" si="3">L3+E3</f>
         <v>6546</v>
       </c>
@@ -1287,10 +1295,10 @@
       <c r="C4" t="s">
         <v>19</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="4">
         <v>6546</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="4">
         <v>6689</v>
       </c>
       <c r="F4">
@@ -1310,7 +1318,7 @@
         <v>2.2328836529616813</v>
       </c>
       <c r="J4" s="3">
-        <f t="shared" ref="J4:J47" si="7">J3*1.013</f>
+        <f t="shared" ref="J4:J62" si="7">J3*1.013</f>
         <v>6567.4815999999983</v>
       </c>
       <c r="K4" s="3">
@@ -1320,7 +1328,7 @@
       <c r="L4">
         <v>0</v>
       </c>
-      <c r="M4">
+      <c r="M4" s="4">
         <f t="shared" si="3"/>
         <v>6689</v>
       </c>
@@ -1349,10 +1357,10 @@
       <c r="C5" t="s">
         <v>20</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="4">
         <v>6689</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="4">
         <v>6846</v>
       </c>
       <c r="F5">
@@ -1382,7 +1390,7 @@
       <c r="L5">
         <v>0</v>
       </c>
-      <c r="M5">
+      <c r="M5" s="4">
         <f t="shared" si="3"/>
         <v>6846</v>
       </c>
@@ -1411,10 +1419,10 @@
       <c r="C6" t="s">
         <v>21</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="4">
         <v>6846</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="4">
         <v>7015</v>
       </c>
       <c r="F6">
@@ -1444,7 +1452,7 @@
       <c r="L6">
         <v>0</v>
       </c>
-      <c r="M6">
+      <c r="M6" s="4">
         <f t="shared" si="3"/>
         <v>7015</v>
       </c>
@@ -1473,10 +1481,10 @@
       <c r="C7" t="s">
         <v>22</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="4">
         <v>7015</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="4">
         <v>7050</v>
       </c>
       <c r="F7">
@@ -1506,7 +1514,7 @@
       <c r="L7">
         <v>0</v>
       </c>
-      <c r="M7">
+      <c r="M7" s="4">
         <f t="shared" si="3"/>
         <v>7050</v>
       </c>
@@ -1535,10 +1543,10 @@
       <c r="C8" t="s">
         <v>23</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="4">
         <v>7050</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="4">
         <v>6979</v>
       </c>
       <c r="F8">
@@ -1568,7 +1576,7 @@
       <c r="L8">
         <v>0</v>
       </c>
-      <c r="M8">
+      <c r="M8" s="4">
         <f t="shared" si="3"/>
         <v>6979</v>
       </c>
@@ -1597,10 +1605,10 @@
       <c r="C9" t="s">
         <v>17</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="4">
         <v>6979</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="4">
         <v>7170</v>
       </c>
       <c r="F9">
@@ -1630,7 +1638,7 @@
       <c r="L9">
         <v>0</v>
       </c>
-      <c r="M9">
+      <c r="M9" s="4">
         <f t="shared" si="3"/>
         <v>7170</v>
       </c>
@@ -1659,10 +1667,10 @@
       <c r="C10" t="s">
         <v>18</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="4">
         <v>7170</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="4">
         <v>7315</v>
       </c>
       <c r="F10">
@@ -1692,7 +1700,7 @@
       <c r="L10">
         <v>0</v>
       </c>
-      <c r="M10">
+      <c r="M10" s="4">
         <f t="shared" si="3"/>
         <v>7315</v>
       </c>
@@ -1721,10 +1729,10 @@
       <c r="C11" t="s">
         <v>19</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="4">
         <v>7315</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="4">
         <v>6845</v>
       </c>
       <c r="F11">
@@ -1754,7 +1762,7 @@
       <c r="L11">
         <v>0</v>
       </c>
-      <c r="M11">
+      <c r="M11" s="4">
         <f t="shared" si="3"/>
         <v>6845</v>
       </c>
@@ -1783,10 +1791,10 @@
       <c r="C12" t="s">
         <v>20</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="4">
         <v>6845</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="4">
         <v>7567</v>
       </c>
       <c r="F12">
@@ -1816,7 +1824,7 @@
       <c r="L12">
         <v>0</v>
       </c>
-      <c r="M12">
+      <c r="M12" s="4">
         <f t="shared" si="3"/>
         <v>7567</v>
       </c>
@@ -1845,10 +1853,10 @@
       <c r="C13" t="s">
         <v>21</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="4">
         <v>7567</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="4">
         <v>7763</v>
       </c>
       <c r="F13">
@@ -1878,7 +1886,7 @@
       <c r="L13">
         <v>0</v>
       </c>
-      <c r="M13">
+      <c r="M13" s="4">
         <f t="shared" si="3"/>
         <v>7763</v>
       </c>
@@ -1907,10 +1915,10 @@
       <c r="C14" t="s">
         <v>22</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="4">
         <v>7763</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="4">
         <v>7845</v>
       </c>
       <c r="F14">
@@ -1940,7 +1948,7 @@
       <c r="L14">
         <v>0</v>
       </c>
-      <c r="M14">
+      <c r="M14" s="4">
         <f t="shared" si="3"/>
         <v>7845</v>
       </c>
@@ -1969,10 +1977,10 @@
       <c r="C15" t="s">
         <v>23</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="4">
         <v>7845</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="4">
         <v>7879</v>
       </c>
       <c r="F15">
@@ -2002,7 +2010,7 @@
       <c r="L15">
         <v>0</v>
       </c>
-      <c r="M15">
+      <c r="M15" s="4">
         <f t="shared" si="3"/>
         <v>7879</v>
       </c>
@@ -2031,10 +2039,10 @@
       <c r="C16" t="s">
         <v>17</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="4">
         <v>7879</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="4">
         <v>7952</v>
       </c>
       <c r="F16">
@@ -2064,7 +2072,7 @@
       <c r="L16">
         <v>0</v>
       </c>
-      <c r="M16">
+      <c r="M16" s="4">
         <f t="shared" si="3"/>
         <v>7952</v>
       </c>
@@ -2093,10 +2101,10 @@
       <c r="C17" t="s">
         <v>18</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="4">
         <v>7952</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="4">
         <v>7797</v>
       </c>
       <c r="F17">
@@ -2126,7 +2134,7 @@
       <c r="L17">
         <v>0</v>
       </c>
-      <c r="M17">
+      <c r="M17" s="4">
         <f t="shared" si="3"/>
         <v>7797</v>
       </c>
@@ -2155,10 +2163,10 @@
       <c r="C18" t="s">
         <v>19</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="4">
         <v>7797</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="4">
         <v>8335</v>
       </c>
       <c r="F18">
@@ -2188,7 +2196,7 @@
       <c r="L18">
         <v>0</v>
       </c>
-      <c r="M18">
+      <c r="M18" s="4">
         <f t="shared" si="3"/>
         <v>8335</v>
       </c>
@@ -2217,10 +2225,10 @@
       <c r="C19" t="s">
         <v>20</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="4">
         <v>8335</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="4">
         <v>8461</v>
       </c>
       <c r="F19">
@@ -2250,7 +2258,7 @@
       <c r="L19">
         <v>0</v>
       </c>
-      <c r="M19">
+      <c r="M19" s="4">
         <f t="shared" si="3"/>
         <v>8461</v>
       </c>
@@ -2279,10 +2287,10 @@
       <c r="C20" t="s">
         <v>21</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="4">
         <v>8461</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="4">
         <v>8330</v>
       </c>
       <c r="F20">
@@ -2312,7 +2320,7 @@
       <c r="L20">
         <v>0</v>
       </c>
-      <c r="M20">
+      <c r="M20" s="4">
         <f t="shared" si="3"/>
         <v>8330</v>
       </c>
@@ -2341,10 +2349,10 @@
       <c r="C21" t="s">
         <v>22</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="4">
         <v>8330</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="4">
         <v>8331</v>
       </c>
       <c r="F21">
@@ -2374,7 +2382,7 @@
       <c r="L21">
         <v>0</v>
       </c>
-      <c r="M21">
+      <c r="M21" s="4">
         <f t="shared" si="3"/>
         <v>8331</v>
       </c>
@@ -2403,10 +2411,10 @@
       <c r="C22" t="s">
         <v>23</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="4">
         <v>8331</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="4">
         <v>8590</v>
       </c>
       <c r="F22">
@@ -2436,7 +2444,7 @@
       <c r="L22">
         <v>0</v>
       </c>
-      <c r="M22">
+      <c r="M22" s="4">
         <f t="shared" si="3"/>
         <v>8590</v>
       </c>
@@ -2465,10 +2473,10 @@
       <c r="C23" t="s">
         <v>17</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="4">
         <v>8590</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="4">
         <v>8925</v>
       </c>
       <c r="F23">
@@ -2498,7 +2506,7 @@
       <c r="L23">
         <v>0</v>
       </c>
-      <c r="M23">
+      <c r="M23" s="4">
         <f t="shared" si="3"/>
         <v>8925</v>
       </c>
@@ -2527,10 +2535,10 @@
       <c r="C24" t="s">
         <v>18</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="4">
         <v>8925</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="4">
         <v>9113</v>
       </c>
       <c r="F24">
@@ -2560,7 +2568,7 @@
       <c r="L24">
         <v>0</v>
       </c>
-      <c r="M24">
+      <c r="M24" s="4">
         <f t="shared" si="3"/>
         <v>9113</v>
       </c>
@@ -2589,10 +2597,10 @@
       <c r="C25" t="s">
         <v>19</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="4">
         <v>9113</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="4">
         <v>9163</v>
       </c>
       <c r="F25">
@@ -2622,7 +2630,7 @@
       <c r="L25">
         <v>0</v>
       </c>
-      <c r="M25">
+      <c r="M25" s="4">
         <f t="shared" ref="M25" si="12">L25+E25</f>
         <v>9163</v>
       </c>
@@ -2651,10 +2659,10 @@
       <c r="C26" t="s">
         <v>20</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="4">
         <v>9163</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="4">
         <v>9353</v>
       </c>
       <c r="F26">
@@ -2684,7 +2692,7 @@
       <c r="L26">
         <v>0</v>
       </c>
-      <c r="M26">
+      <c r="M26" s="4">
         <f t="shared" ref="M26" si="16">L26+E26</f>
         <v>9353</v>
       </c>
@@ -2713,10 +2721,10 @@
       <c r="C27" t="s">
         <v>21</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="4">
         <v>9353</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="4">
         <v>9353</v>
       </c>
       <c r="F27">
@@ -2746,7 +2754,7 @@
       <c r="L27">
         <v>0</v>
       </c>
-      <c r="M27">
+      <c r="M27" s="4">
         <f t="shared" ref="M27:M32" si="21">L27+E27</f>
         <v>9353</v>
       </c>
@@ -2775,10 +2783,10 @@
       <c r="C28" t="s">
         <v>22</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="4">
         <v>9353</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="4">
         <v>9400</v>
       </c>
       <c r="F28">
@@ -2808,7 +2816,7 @@
       <c r="L28">
         <v>0</v>
       </c>
-      <c r="M28">
+      <c r="M28" s="4">
         <f t="shared" si="21"/>
         <v>9400</v>
       </c>
@@ -2837,10 +2845,10 @@
       <c r="C29" t="s">
         <v>23</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="4">
         <v>9400</v>
       </c>
-      <c r="E29">
+      <c r="E29" s="4">
         <v>9450</v>
       </c>
       <c r="F29">
@@ -2870,7 +2878,7 @@
       <c r="L29">
         <v>0</v>
       </c>
-      <c r="M29">
+      <c r="M29" s="4">
         <f t="shared" si="21"/>
         <v>9450</v>
       </c>
@@ -2899,10 +2907,10 @@
       <c r="C30" t="s">
         <v>17</v>
       </c>
-      <c r="D30">
+      <c r="D30" s="4">
         <v>9450</v>
       </c>
-      <c r="E30">
+      <c r="E30" s="4">
         <v>9452</v>
       </c>
       <c r="F30">
@@ -2932,7 +2940,7 @@
       <c r="L30">
         <v>0</v>
       </c>
-      <c r="M30">
+      <c r="M30" s="4">
         <f t="shared" si="21"/>
         <v>9452</v>
       </c>
@@ -2961,10 +2969,10 @@
       <c r="C31" t="s">
         <v>18</v>
       </c>
-      <c r="D31">
+      <c r="D31" s="4">
         <v>9452</v>
       </c>
-      <c r="E31">
+      <c r="E31" s="4">
         <v>9512</v>
       </c>
       <c r="F31">
@@ -2994,7 +3002,7 @@
       <c r="L31">
         <v>0</v>
       </c>
-      <c r="M31">
+      <c r="M31" s="4">
         <f t="shared" si="21"/>
         <v>9512</v>
       </c>
@@ -3023,10 +3031,10 @@
       <c r="C32" t="s">
         <v>19</v>
       </c>
-      <c r="D32">
+      <c r="D32" s="4">
         <v>9512</v>
       </c>
-      <c r="E32">
+      <c r="E32" s="4">
         <v>9666</v>
       </c>
       <c r="F32">
@@ -3056,7 +3064,7 @@
       <c r="L32">
         <v>0</v>
       </c>
-      <c r="M32">
+      <c r="M32" s="4">
         <f t="shared" si="21"/>
         <v>9666</v>
       </c>
@@ -3085,10 +3093,10 @@
       <c r="C33" t="s">
         <v>20</v>
       </c>
-      <c r="D33">
+      <c r="D33" s="4">
         <v>9666</v>
       </c>
-      <c r="E33">
+      <c r="E33" s="4">
         <v>9890</v>
       </c>
       <c r="F33">
@@ -3118,7 +3126,7 @@
       <c r="L33">
         <v>0</v>
       </c>
-      <c r="M33">
+      <c r="M33" s="4">
         <f t="shared" ref="M33:M41" si="26">L33+E33</f>
         <v>9890</v>
       </c>
@@ -3147,10 +3155,10 @@
       <c r="C34" t="s">
         <v>21</v>
       </c>
-      <c r="D34">
+      <c r="D34" s="4">
         <v>9890</v>
       </c>
-      <c r="E34">
+      <c r="E34" s="4">
         <v>10200</v>
       </c>
       <c r="F34">
@@ -3180,7 +3188,7 @@
       <c r="L34">
         <v>0</v>
       </c>
-      <c r="M34">
+      <c r="M34" s="4">
         <f t="shared" si="26"/>
         <v>10200</v>
       </c>
@@ -3209,10 +3217,10 @@
       <c r="C35" t="s">
         <v>22</v>
       </c>
-      <c r="D35">
+      <c r="D35" s="4">
         <v>10200</v>
       </c>
-      <c r="E35">
+      <c r="E35" s="4">
         <v>10565</v>
       </c>
       <c r="F35">
@@ -3242,7 +3250,7 @@
       <c r="L35">
         <v>0</v>
       </c>
-      <c r="M35">
+      <c r="M35" s="4">
         <f t="shared" si="26"/>
         <v>10565</v>
       </c>
@@ -3271,10 +3279,10 @@
       <c r="C36" t="s">
         <v>23</v>
       </c>
-      <c r="D36">
+      <c r="D36" s="4">
         <v>10565</v>
       </c>
-      <c r="E36">
+      <c r="E36" s="4">
         <v>10845</v>
       </c>
       <c r="F36">
@@ -3304,7 +3312,7 @@
       <c r="L36">
         <v>0</v>
       </c>
-      <c r="M36">
+      <c r="M36" s="4">
         <f t="shared" si="26"/>
         <v>10845</v>
       </c>
@@ -3333,10 +3341,10 @@
       <c r="C37" t="s">
         <v>17</v>
       </c>
-      <c r="D37">
+      <c r="D37" s="4">
         <v>20845</v>
       </c>
-      <c r="E37">
+      <c r="E37" s="4">
         <v>22699</v>
       </c>
       <c r="F37">
@@ -3366,7 +3374,7 @@
       <c r="L37">
         <v>-10000</v>
       </c>
-      <c r="M37">
+      <c r="M37" s="4">
         <f t="shared" si="26"/>
         <v>12699</v>
       </c>
@@ -3395,10 +3403,10 @@
       <c r="C38" t="s">
         <v>18</v>
       </c>
-      <c r="D38">
+      <c r="D38" s="4">
         <v>22699</v>
       </c>
-      <c r="E38">
+      <c r="E38" s="4">
         <v>22955</v>
       </c>
       <c r="F38">
@@ -3428,7 +3436,7 @@
       <c r="L38">
         <v>-10000</v>
       </c>
-      <c r="M38">
+      <c r="M38" s="4">
         <f t="shared" si="26"/>
         <v>12955</v>
       </c>
@@ -3457,10 +3465,10 @@
       <c r="C39" t="s">
         <v>19</v>
       </c>
-      <c r="D39">
+      <c r="D39" s="4">
         <v>22955</v>
       </c>
-      <c r="E39">
+      <c r="E39" s="4">
         <v>24388</v>
       </c>
       <c r="F39">
@@ -3490,7 +3498,7 @@
       <c r="L39">
         <v>-10000</v>
       </c>
-      <c r="M39">
+      <c r="M39" s="4">
         <f t="shared" si="26"/>
         <v>14388</v>
       </c>
@@ -3519,10 +3527,10 @@
       <c r="C40" t="s">
         <v>20</v>
       </c>
-      <c r="D40">
+      <c r="D40" s="4">
         <v>24388</v>
       </c>
-      <c r="E40">
+      <c r="E40" s="4">
         <v>24713</v>
       </c>
       <c r="F40">
@@ -3552,7 +3560,7 @@
       <c r="L40">
         <v>-10000</v>
       </c>
-      <c r="M40">
+      <c r="M40" s="4">
         <f t="shared" si="26"/>
         <v>14713</v>
       </c>
@@ -3581,10 +3589,10 @@
       <c r="C41" t="s">
         <v>21</v>
       </c>
-      <c r="D41">
+      <c r="D41" s="4">
         <v>24713</v>
       </c>
-      <c r="E41">
+      <c r="E41" s="4">
         <v>25029</v>
       </c>
       <c r="F41">
@@ -3614,7 +3622,7 @@
       <c r="L41">
         <v>-10000</v>
       </c>
-      <c r="M41">
+      <c r="M41" s="4">
         <f t="shared" si="26"/>
         <v>15029</v>
       </c>
@@ -3643,26 +3651,26 @@
       <c r="C42" t="s">
         <v>22</v>
       </c>
-      <c r="D42">
+      <c r="D42" s="4">
         <v>25029</v>
       </c>
-      <c r="E42">
+      <c r="E42" s="4">
         <v>25088</v>
       </c>
       <c r="F42">
-        <f t="shared" ref="F42:F47" si="28">E42-D42</f>
+        <f t="shared" ref="F42:F46" si="28">E42-D42</f>
         <v>59</v>
       </c>
       <c r="G42" s="2">
-        <f t="shared" ref="G42:G47" si="29">(E42-$D$2)/A42</f>
+        <f t="shared" ref="G42:G46" si="29">(E42-$D$2)/A42</f>
         <v>455.80487804878049</v>
       </c>
       <c r="H42" s="2">
-        <f t="shared" ref="H42:H47" si="30">(E42/D42-1)*100</f>
+        <f t="shared" ref="H42:H46" si="30">(E42/D42-1)*100</f>
         <v>0.23572655719366065</v>
       </c>
       <c r="I42" s="2">
-        <f t="shared" ref="I42:I47" si="31">(POWER((E42/$D$3),1/A42)-1)*100</f>
+        <f t="shared" ref="I42:I46" si="31">(POWER((E42/$D$3),1/A42)-1)*100</f>
         <v>3.3880613542311755</v>
       </c>
       <c r="J42" s="3">
@@ -3670,18 +3678,18 @@
         <v>10728.964008265855</v>
       </c>
       <c r="K42" s="3">
-        <f t="shared" ref="K42:K47" si="32">M42-J42</f>
+        <f t="shared" ref="K42:K46" si="32">M42-J42</f>
         <v>4359.0359917341448</v>
       </c>
       <c r="L42">
         <v>-10000</v>
       </c>
-      <c r="M42">
-        <f t="shared" ref="M42:M47" si="33">L42+E42</f>
+      <c r="M42" s="4">
+        <f t="shared" ref="M42:M46" si="33">L42+E42</f>
         <v>15088</v>
       </c>
       <c r="N42" s="2">
-        <f t="shared" ref="N42:N47" si="34">M42/$D$2*100</f>
+        <f t="shared" ref="N42:N46" si="34">M42/$D$2*100</f>
         <v>235.75</v>
       </c>
       <c r="O42">
@@ -3691,7 +3699,7 @@
         <v>84763.1</v>
       </c>
       <c r="Q42">
-        <f t="shared" ref="Q42:Q47" si="35">P42/$O$2*100</f>
+        <f t="shared" ref="Q42:Q46" si="35">P42/$O$2*100</f>
         <v>94.983409887281383</v>
       </c>
     </row>
@@ -3705,10 +3713,10 @@
       <c r="C43" t="s">
         <v>23</v>
       </c>
-      <c r="D43">
+      <c r="D43" s="4">
         <v>25088</v>
       </c>
-      <c r="E43">
+      <c r="E43" s="4">
         <v>25195</v>
       </c>
       <c r="F43">
@@ -3738,7 +3746,7 @@
       <c r="L43">
         <v>-10000</v>
       </c>
-      <c r="M43">
+      <c r="M43" s="4">
         <f t="shared" si="33"/>
         <v>15195</v>
       </c>
@@ -3767,10 +3775,10 @@
       <c r="C44" t="s">
         <v>17</v>
       </c>
-      <c r="D44">
+      <c r="D44" s="4">
         <v>25195</v>
       </c>
-      <c r="E44">
+      <c r="E44" s="4">
         <v>25835</v>
       </c>
       <c r="F44">
@@ -3800,7 +3808,7 @@
       <c r="L44">
         <v>-10000</v>
       </c>
-      <c r="M44">
+      <c r="M44" s="4">
         <f t="shared" si="33"/>
         <v>15835</v>
       </c>
@@ -3829,10 +3837,10 @@
       <c r="C45" t="s">
         <v>18</v>
       </c>
-      <c r="D45">
+      <c r="D45" s="4">
         <v>25835</v>
       </c>
-      <c r="E45">
+      <c r="E45" s="4">
         <v>25600</v>
       </c>
       <c r="F45">
@@ -3862,7 +3870,7 @@
       <c r="L45">
         <v>-10000</v>
       </c>
-      <c r="M45">
+      <c r="M45" s="4">
         <f t="shared" si="33"/>
         <v>15600</v>
       </c>
@@ -3891,10 +3899,10 @@
       <c r="C46" t="s">
         <v>19</v>
       </c>
-      <c r="D46">
+      <c r="D46" s="4">
         <v>25600</v>
       </c>
-      <c r="E46">
+      <c r="E46" s="4">
         <v>26102</v>
       </c>
       <c r="F46">
@@ -3924,7 +3932,7 @@
       <c r="L46">
         <v>-10000</v>
       </c>
-      <c r="M46">
+      <c r="M46" s="4">
         <f t="shared" si="33"/>
         <v>16102</v>
       </c>
@@ -3944,13 +3952,1012 @@
       </c>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B47" s="1"/>
-      <c r="G47" s="2"/>
-      <c r="H47" s="2"/>
-      <c r="I47" s="2"/>
-      <c r="J47" s="3"/>
-      <c r="K47" s="3"/>
-      <c r="N47" s="2"/>
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" s="1">
+        <v>45764</v>
+      </c>
+      <c r="C47" t="s">
+        <v>20</v>
+      </c>
+      <c r="D47" s="4">
+        <v>46802</v>
+      </c>
+      <c r="E47" s="4">
+        <v>47035</v>
+      </c>
+      <c r="F47">
+        <f t="shared" ref="F47:F62" si="36">E47-D47</f>
+        <v>233</v>
+      </c>
+      <c r="G47" s="2">
+        <f t="shared" ref="G47:G62" si="37">(E47-$D$2)/A47</f>
+        <v>883.36956521739125</v>
+      </c>
+      <c r="H47" s="2">
+        <f t="shared" ref="H47:H62" si="38">(E47/D47-1)*100</f>
+        <v>0.49784197256528273</v>
+      </c>
+      <c r="I47" s="2">
+        <f t="shared" ref="I47:I62" si="39">(POWER((E47/$D$3),1/A47)-1)*100</f>
+        <v>4.4314552374297156</v>
+      </c>
+      <c r="J47" s="3">
+        <f t="shared" si="7"/>
+        <v>11444.715869449656</v>
+      </c>
+      <c r="K47" s="3">
+        <f t="shared" ref="K47:K62" si="40">M47-J47</f>
+        <v>4891.2841305503443</v>
+      </c>
+      <c r="L47">
+        <f>-9999-20700</f>
+        <v>-30699</v>
+      </c>
+      <c r="M47" s="4">
+        <f t="shared" ref="M47:M62" si="41">L47+E47</f>
+        <v>16336</v>
+      </c>
+      <c r="N47" s="2">
+        <f t="shared" ref="N47:N62" si="42">M47/$D$2*100</f>
+        <v>255.25000000000003</v>
+      </c>
+      <c r="O47">
+        <v>84562.7</v>
+      </c>
+      <c r="P47">
+        <v>84046</v>
+      </c>
+      <c r="Q47">
+        <f t="shared" ref="Q47:Q62" si="43">P47/$O$2*100</f>
+        <v>94.179845562354956</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" s="1">
+        <v>45765</v>
+      </c>
+      <c r="C48" t="s">
+        <v>21</v>
+      </c>
+      <c r="D48" s="4">
+        <v>47035</v>
+      </c>
+      <c r="E48" s="4">
+        <v>47070</v>
+      </c>
+      <c r="F48">
+        <f t="shared" si="36"/>
+        <v>35</v>
+      </c>
+      <c r="G48" s="2">
+        <f t="shared" si="37"/>
+        <v>865.31914893617022</v>
+      </c>
+      <c r="H48" s="2">
+        <f t="shared" si="38"/>
+        <v>7.4412671414902931E-2</v>
+      </c>
+      <c r="I48" s="2">
+        <f t="shared" si="39"/>
+        <v>4.3368057343146749</v>
+      </c>
+      <c r="J48" s="3">
+        <f t="shared" si="7"/>
+        <v>11593.4971757525</v>
+      </c>
+      <c r="K48" s="3">
+        <f t="shared" si="40"/>
+        <v>4777.5028242475</v>
+      </c>
+      <c r="L48">
+        <f>L47</f>
+        <v>-30699</v>
+      </c>
+      <c r="M48" s="4">
+        <f t="shared" si="41"/>
+        <v>16371</v>
+      </c>
+      <c r="N48" s="2">
+        <f t="shared" si="42"/>
+        <v>255.796875</v>
+      </c>
+      <c r="O48">
+        <v>84046</v>
+      </c>
+      <c r="P48">
+        <v>84534</v>
+      </c>
+      <c r="Q48">
+        <f t="shared" si="43"/>
+        <v>94.726686157200987</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" s="1">
+        <v>45766</v>
+      </c>
+      <c r="C49" t="s">
+        <v>22</v>
+      </c>
+      <c r="D49" s="4">
+        <v>47070</v>
+      </c>
+      <c r="E49" s="4">
+        <v>47160</v>
+      </c>
+      <c r="F49">
+        <f t="shared" si="36"/>
+        <v>90</v>
+      </c>
+      <c r="G49" s="2">
+        <f t="shared" si="37"/>
+        <v>849.16666666666663</v>
+      </c>
+      <c r="H49" s="2">
+        <f t="shared" si="38"/>
+        <v>0.19120458891013214</v>
+      </c>
+      <c r="I49" s="2">
+        <f t="shared" si="39"/>
+        <v>4.2487136066875042</v>
+      </c>
+      <c r="J49" s="3">
+        <f t="shared" si="7"/>
+        <v>11744.212639037281</v>
+      </c>
+      <c r="K49" s="3">
+        <f t="shared" si="40"/>
+        <v>4716.7873609627186</v>
+      </c>
+      <c r="L49">
+        <f t="shared" ref="L49:L62" si="44">L48</f>
+        <v>-30699</v>
+      </c>
+      <c r="M49" s="4">
+        <f t="shared" si="41"/>
+        <v>16461</v>
+      </c>
+      <c r="N49" s="2">
+        <f t="shared" si="42"/>
+        <v>257.203125</v>
+      </c>
+      <c r="O49">
+        <v>84534</v>
+      </c>
+      <c r="P49">
+        <v>85355</v>
+      </c>
+      <c r="Q49">
+        <f t="shared" si="43"/>
+        <v>95.646678223530074</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50" s="1">
+        <v>45767</v>
+      </c>
+      <c r="C50" t="s">
+        <v>23</v>
+      </c>
+      <c r="D50" s="4">
+        <v>47160</v>
+      </c>
+      <c r="E50" s="4">
+        <v>47420</v>
+      </c>
+      <c r="F50">
+        <f t="shared" si="36"/>
+        <v>260</v>
+      </c>
+      <c r="G50" s="2">
+        <f t="shared" si="37"/>
+        <v>837.14285714285711</v>
+      </c>
+      <c r="H50" s="2">
+        <f t="shared" si="38"/>
+        <v>0.55131467345208574</v>
+      </c>
+      <c r="I50" s="2">
+        <f t="shared" si="39"/>
+        <v>4.1719141601861187</v>
+      </c>
+      <c r="J50" s="3">
+        <f t="shared" si="7"/>
+        <v>11896.887403344765</v>
+      </c>
+      <c r="K50" s="3">
+        <f t="shared" si="40"/>
+        <v>4824.1125966552354</v>
+      </c>
+      <c r="L50">
+        <f t="shared" si="44"/>
+        <v>-30699</v>
+      </c>
+      <c r="M50" s="4">
+        <f t="shared" si="41"/>
+        <v>16721</v>
+      </c>
+      <c r="N50" s="2">
+        <f t="shared" si="42"/>
+        <v>261.265625</v>
+      </c>
+      <c r="O50">
+        <v>85355</v>
+      </c>
+      <c r="P50">
+        <v>84585</v>
+      </c>
+      <c r="Q50">
+        <f t="shared" si="43"/>
+        <v>94.783835481662365</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" s="1">
+        <v>45768</v>
+      </c>
+      <c r="C51" t="s">
+        <v>17</v>
+      </c>
+      <c r="D51" s="4">
+        <v>47420</v>
+      </c>
+      <c r="E51" s="4">
+        <v>47910</v>
+      </c>
+      <c r="F51">
+        <f t="shared" si="36"/>
+        <v>490</v>
+      </c>
+      <c r="G51" s="2">
+        <f t="shared" si="37"/>
+        <v>830.2</v>
+      </c>
+      <c r="H51" s="2">
+        <f t="shared" si="38"/>
+        <v>1.03331927456769</v>
+      </c>
+      <c r="I51" s="2">
+        <f t="shared" si="39"/>
+        <v>4.1081966963260053</v>
+      </c>
+      <c r="J51" s="3">
+        <f t="shared" si="7"/>
+        <v>12051.546939588245</v>
+      </c>
+      <c r="K51" s="3">
+        <f t="shared" si="40"/>
+        <v>5159.4530604117554</v>
+      </c>
+      <c r="L51">
+        <f t="shared" si="44"/>
+        <v>-30699</v>
+      </c>
+      <c r="M51" s="4">
+        <f t="shared" si="41"/>
+        <v>17211</v>
+      </c>
+      <c r="N51" s="2">
+        <f t="shared" si="42"/>
+        <v>268.921875</v>
+      </c>
+      <c r="O51">
+        <v>84585</v>
+      </c>
+      <c r="P51">
+        <v>88165</v>
+      </c>
+      <c r="Q51">
+        <f t="shared" si="43"/>
+        <v>98.795493943852478</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" s="1">
+        <v>45769</v>
+      </c>
+      <c r="C52" t="s">
+        <v>18</v>
+      </c>
+      <c r="D52" s="4">
+        <v>47910</v>
+      </c>
+      <c r="E52" s="4">
+        <v>49488</v>
+      </c>
+      <c r="F52">
+        <f t="shared" si="36"/>
+        <v>1578</v>
+      </c>
+      <c r="G52" s="2">
+        <f t="shared" si="37"/>
+        <v>844.86274509803923</v>
+      </c>
+      <c r="H52" s="2">
+        <f t="shared" si="38"/>
+        <v>3.2936756418284308</v>
+      </c>
+      <c r="I52" s="2">
+        <f t="shared" si="39"/>
+        <v>4.0921641251811192</v>
+      </c>
+      <c r="J52" s="3">
+        <f t="shared" si="7"/>
+        <v>12208.21704980289</v>
+      </c>
+      <c r="K52" s="3">
+        <f t="shared" si="40"/>
+        <v>6580.78295019711</v>
+      </c>
+      <c r="L52">
+        <f t="shared" si="44"/>
+        <v>-30699</v>
+      </c>
+      <c r="M52" s="4">
+        <f t="shared" si="41"/>
+        <v>18789</v>
+      </c>
+      <c r="N52" s="2">
+        <f t="shared" si="42"/>
+        <v>293.578125</v>
+      </c>
+      <c r="O52">
+        <v>88165</v>
+      </c>
+      <c r="P52">
+        <v>91407</v>
+      </c>
+      <c r="Q52">
+        <f t="shared" si="43"/>
+        <v>102.42839805961235</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" s="1">
+        <v>45770</v>
+      </c>
+      <c r="C53" t="s">
+        <v>19</v>
+      </c>
+      <c r="D53" s="4">
+        <v>49488</v>
+      </c>
+      <c r="E53" s="4">
+        <v>50094</v>
+      </c>
+      <c r="F53">
+        <f t="shared" si="36"/>
+        <v>606</v>
+      </c>
+      <c r="G53" s="2">
+        <f t="shared" si="37"/>
+        <v>840.26923076923072</v>
+      </c>
+      <c r="H53" s="2">
+        <f t="shared" si="38"/>
+        <v>1.2245392822502366</v>
+      </c>
+      <c r="I53" s="2">
+        <f t="shared" si="39"/>
+        <v>4.0362586513626564</v>
+      </c>
+      <c r="J53" s="3">
+        <f t="shared" si="7"/>
+        <v>12366.923871450326</v>
+      </c>
+      <c r="K53" s="3">
+        <f t="shared" si="40"/>
+        <v>7028.0761285496737</v>
+      </c>
+      <c r="L53">
+        <f t="shared" si="44"/>
+        <v>-30699</v>
+      </c>
+      <c r="M53" s="4">
+        <f t="shared" si="41"/>
+        <v>19395</v>
+      </c>
+      <c r="N53" s="2">
+        <f t="shared" si="42"/>
+        <v>303.046875</v>
+      </c>
+      <c r="O53">
+        <v>91407</v>
+      </c>
+      <c r="P53">
+        <v>92926</v>
+      </c>
+      <c r="Q53">
+        <f t="shared" si="43"/>
+        <v>104.13055146856955</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" s="1">
+        <v>45771</v>
+      </c>
+      <c r="C54" t="s">
+        <v>20</v>
+      </c>
+      <c r="D54" s="4">
+        <v>50094</v>
+      </c>
+      <c r="E54" s="4">
+        <v>50900</v>
+      </c>
+      <c r="F54">
+        <f t="shared" si="36"/>
+        <v>806</v>
+      </c>
+      <c r="G54" s="2">
+        <f t="shared" si="37"/>
+        <v>839.62264150943395</v>
+      </c>
+      <c r="H54" s="2">
+        <f t="shared" si="38"/>
+        <v>1.6089751267616803</v>
+      </c>
+      <c r="I54" s="2">
+        <f t="shared" si="39"/>
+        <v>3.9899284528173595</v>
+      </c>
+      <c r="J54" s="3">
+        <f t="shared" si="7"/>
+        <v>12527.69388177918</v>
+      </c>
+      <c r="K54" s="3">
+        <f t="shared" si="40"/>
+        <v>7673.3061182208203</v>
+      </c>
+      <c r="L54">
+        <f t="shared" si="44"/>
+        <v>-30699</v>
+      </c>
+      <c r="M54" s="4">
+        <f t="shared" si="41"/>
+        <v>20201</v>
+      </c>
+      <c r="N54" s="2">
+        <f t="shared" si="42"/>
+        <v>315.640625</v>
+      </c>
+      <c r="O54">
+        <v>92926</v>
+      </c>
+      <c r="P54">
+        <v>93092</v>
+      </c>
+      <c r="Q54">
+        <f t="shared" si="43"/>
+        <v>104.31656691681637</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" s="1">
+        <v>45772</v>
+      </c>
+      <c r="C55" t="s">
+        <v>21</v>
+      </c>
+      <c r="D55" s="4">
+        <v>50900</v>
+      </c>
+      <c r="E55" s="4">
+        <v>51087.55</v>
+      </c>
+      <c r="F55">
+        <f t="shared" si="36"/>
+        <v>187.55000000000291</v>
+      </c>
+      <c r="G55" s="2">
+        <f t="shared" si="37"/>
+        <v>827.54722222222233</v>
+      </c>
+      <c r="H55" s="2">
+        <f t="shared" si="38"/>
+        <v>0.36846758349706743</v>
+      </c>
+      <c r="I55" s="2">
+        <f t="shared" si="39"/>
+        <v>3.9216911636315688</v>
+      </c>
+      <c r="J55" s="3">
+        <f t="shared" si="7"/>
+        <v>12690.553902242307</v>
+      </c>
+      <c r="K55" s="3">
+        <f t="shared" si="40"/>
+        <v>7697.9960977576957</v>
+      </c>
+      <c r="L55">
+        <f t="shared" si="44"/>
+        <v>-30699</v>
+      </c>
+      <c r="M55" s="4">
+        <f t="shared" si="41"/>
+        <v>20388.550000000003</v>
+      </c>
+      <c r="N55" s="2">
+        <f t="shared" si="42"/>
+        <v>318.57109375000005</v>
+      </c>
+      <c r="O55">
+        <v>93092</v>
+      </c>
+      <c r="P55">
+        <v>95419</v>
+      </c>
+      <c r="Q55">
+        <f t="shared" si="43"/>
+        <v>106.92414491723994</v>
+      </c>
+    </row>
+    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" s="1">
+        <v>45773</v>
+      </c>
+      <c r="C56" t="s">
+        <v>22</v>
+      </c>
+      <c r="D56" s="4">
+        <v>51087.55</v>
+      </c>
+      <c r="E56" s="4">
+        <v>51166.85</v>
+      </c>
+      <c r="F56">
+        <f t="shared" si="36"/>
+        <v>79.299999999995634</v>
+      </c>
+      <c r="G56" s="2">
+        <f t="shared" si="37"/>
+        <v>813.94272727272721</v>
+      </c>
+      <c r="H56" s="2">
+        <f t="shared" si="38"/>
+        <v>0.15522372867753376</v>
+      </c>
+      <c r="I56" s="2">
+        <f t="shared" si="39"/>
+        <v>3.8519615234979154</v>
+      </c>
+      <c r="J56" s="3">
+        <f t="shared" si="7"/>
+        <v>12855.531102971456</v>
+      </c>
+      <c r="K56" s="3">
+        <f t="shared" si="40"/>
+        <v>7612.3188970285428</v>
+      </c>
+      <c r="L56">
+        <f t="shared" si="44"/>
+        <v>-30699</v>
+      </c>
+      <c r="M56" s="4">
+        <f t="shared" si="41"/>
+        <v>20467.849999999999</v>
+      </c>
+      <c r="N56" s="2">
+        <f t="shared" si="42"/>
+        <v>319.81015624999998</v>
+      </c>
+      <c r="O56">
+        <v>95419</v>
+      </c>
+      <c r="P56">
+        <v>94232</v>
+      </c>
+      <c r="Q56">
+        <f t="shared" si="43"/>
+        <v>105.59402240477635</v>
+      </c>
+    </row>
+    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" s="1">
+        <v>45774</v>
+      </c>
+      <c r="C57" t="s">
+        <v>23</v>
+      </c>
+      <c r="D57" s="4">
+        <v>51166.85</v>
+      </c>
+      <c r="E57" s="4">
+        <v>51225</v>
+      </c>
+      <c r="F57">
+        <f t="shared" si="36"/>
+        <v>58.150000000001455</v>
+      </c>
+      <c r="G57" s="2">
+        <f t="shared" si="37"/>
+        <v>800.44642857142856</v>
+      </c>
+      <c r="H57" s="2">
+        <f t="shared" si="38"/>
+        <v>0.11364780126195129</v>
+      </c>
+      <c r="I57" s="2">
+        <f t="shared" si="39"/>
+        <v>3.7839970496518882</v>
+      </c>
+      <c r="J57" s="3">
+        <f t="shared" si="7"/>
+        <v>13022.653007310084</v>
+      </c>
+      <c r="K57" s="3">
+        <f t="shared" si="40"/>
+        <v>7503.3469926899161</v>
+      </c>
+      <c r="L57">
+        <f t="shared" si="44"/>
+        <v>-30699</v>
+      </c>
+      <c r="M57" s="4">
+        <f t="shared" si="41"/>
+        <v>20526</v>
+      </c>
+      <c r="N57" s="2">
+        <f t="shared" si="42"/>
+        <v>320.71875</v>
+      </c>
+      <c r="O57">
+        <v>94232</v>
+      </c>
+      <c r="P57">
+        <v>94047</v>
+      </c>
+      <c r="Q57">
+        <f t="shared" si="43"/>
+        <v>105.3867160317302</v>
+      </c>
+    </row>
+    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" s="1">
+        <v>45775</v>
+      </c>
+      <c r="C58" t="s">
+        <v>17</v>
+      </c>
+      <c r="D58" s="4">
+        <v>51225</v>
+      </c>
+      <c r="E58" s="4">
+        <v>51915</v>
+      </c>
+      <c r="F58">
+        <f t="shared" si="36"/>
+        <v>690</v>
+      </c>
+      <c r="G58" s="2">
+        <f t="shared" si="37"/>
+        <v>798.50877192982455</v>
+      </c>
+      <c r="H58" s="2">
+        <f t="shared" si="38"/>
+        <v>1.3469985358711467</v>
+      </c>
+      <c r="I58" s="2">
+        <f t="shared" si="39"/>
+        <v>3.7407417401673415</v>
+      </c>
+      <c r="J58" s="3">
+        <f t="shared" si="7"/>
+        <v>13191.947496405113</v>
+      </c>
+      <c r="K58" s="3">
+        <f t="shared" si="40"/>
+        <v>8024.0525035948867</v>
+      </c>
+      <c r="L58">
+        <f t="shared" si="44"/>
+        <v>-30699</v>
+      </c>
+      <c r="M58" s="4">
+        <f t="shared" si="41"/>
+        <v>21216</v>
+      </c>
+      <c r="N58" s="2">
+        <f t="shared" si="42"/>
+        <v>331.5</v>
+      </c>
+      <c r="O58">
+        <v>94047</v>
+      </c>
+      <c r="P58">
+        <v>94415</v>
+      </c>
+      <c r="Q58">
+        <f t="shared" si="43"/>
+        <v>105.7990876278436</v>
+      </c>
+    </row>
+    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" s="1">
+        <v>45776</v>
+      </c>
+      <c r="C59" t="s">
+        <v>18</v>
+      </c>
+      <c r="D59" s="4">
+        <v>51915</v>
+      </c>
+      <c r="E59" s="4">
+        <v>52670</v>
+      </c>
+      <c r="F59">
+        <f t="shared" si="36"/>
+        <v>755</v>
+      </c>
+      <c r="G59" s="2">
+        <f t="shared" si="37"/>
+        <v>797.75862068965512</v>
+      </c>
+      <c r="H59" s="2">
+        <f t="shared" si="38"/>
+        <v>1.45430029856497</v>
+      </c>
+      <c r="I59" s="2">
+        <f t="shared" si="39"/>
+        <v>3.7008870800216309</v>
+      </c>
+      <c r="J59" s="3">
+        <f t="shared" si="7"/>
+        <v>13363.442813858379</v>
+      </c>
+      <c r="K59" s="3">
+        <f t="shared" si="40"/>
+        <v>8607.5571861416211</v>
+      </c>
+      <c r="L59">
+        <f t="shared" si="44"/>
+        <v>-30699</v>
+      </c>
+      <c r="M59" s="4">
+        <f t="shared" si="41"/>
+        <v>21971</v>
+      </c>
+      <c r="N59" s="2">
+        <f t="shared" si="42"/>
+        <v>343.296875</v>
+      </c>
+      <c r="O59">
+        <v>94415</v>
+      </c>
+      <c r="P59">
+        <v>95022</v>
+      </c>
+      <c r="Q59">
+        <f t="shared" si="43"/>
+        <v>106.47927664643282</v>
+      </c>
+    </row>
+    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" s="1">
+        <v>45777</v>
+      </c>
+      <c r="C60" t="s">
+        <v>19</v>
+      </c>
+      <c r="D60" s="4">
+        <v>52670</v>
+      </c>
+      <c r="E60" s="4">
+        <v>53561.74</v>
+      </c>
+      <c r="F60">
+        <f t="shared" si="36"/>
+        <v>891.73999999999796</v>
+      </c>
+      <c r="G60" s="2">
+        <f t="shared" si="37"/>
+        <v>799.35152542372873</v>
+      </c>
+      <c r="H60" s="2">
+        <f t="shared" si="38"/>
+        <v>1.693070058857038</v>
+      </c>
+      <c r="I60" s="2">
+        <f t="shared" si="39"/>
+        <v>3.6665282155353252</v>
+      </c>
+      <c r="J60" s="3">
+        <f t="shared" si="7"/>
+        <v>13537.167570438536</v>
+      </c>
+      <c r="K60" s="3">
+        <f t="shared" si="40"/>
+        <v>9325.5724295614618</v>
+      </c>
+      <c r="L60">
+        <f t="shared" si="44"/>
+        <v>-30699</v>
+      </c>
+      <c r="M60" s="4">
+        <f t="shared" si="41"/>
+        <v>22862.739999999998</v>
+      </c>
+      <c r="N60" s="2">
+        <f t="shared" si="42"/>
+        <v>357.23031249999997</v>
+      </c>
+      <c r="O60">
+        <v>95022</v>
+      </c>
+      <c r="P60">
+        <v>93681</v>
+      </c>
+      <c r="Q60">
+        <f t="shared" si="43"/>
+        <v>104.97658558559569</v>
+      </c>
+    </row>
+    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61" s="1">
+        <v>45778</v>
+      </c>
+      <c r="C61" t="s">
+        <v>20</v>
+      </c>
+      <c r="D61" s="4">
+        <v>53561.74</v>
+      </c>
+      <c r="E61" s="4">
+        <v>54386</v>
+      </c>
+      <c r="F61">
+        <f t="shared" si="36"/>
+        <v>824.26000000000204</v>
+      </c>
+      <c r="G61" s="2">
+        <f t="shared" si="37"/>
+        <v>799.76666666666665</v>
+      </c>
+      <c r="H61" s="2">
+        <f t="shared" si="38"/>
+        <v>1.5388969813153963</v>
+      </c>
+      <c r="I61" s="2">
+        <f t="shared" si="39"/>
+        <v>3.6307049367540145</v>
+      </c>
+      <c r="J61" s="3">
+        <f t="shared" si="7"/>
+        <v>13713.150748854236</v>
+      </c>
+      <c r="K61" s="3">
+        <f t="shared" si="40"/>
+        <v>9973.8492511457644</v>
+      </c>
+      <c r="L61">
+        <f t="shared" si="44"/>
+        <v>-30699</v>
+      </c>
+      <c r="M61" s="4">
+        <f t="shared" si="41"/>
+        <v>23687</v>
+      </c>
+      <c r="N61" s="2">
+        <f t="shared" si="42"/>
+        <v>370.109375</v>
+      </c>
+      <c r="O61">
+        <v>93681</v>
+      </c>
+      <c r="P61">
+        <v>96814</v>
+      </c>
+      <c r="Q61">
+        <f t="shared" si="43"/>
+        <v>108.48734702750676</v>
+      </c>
+    </row>
+    <row r="62" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62" s="1">
+        <v>45779</v>
+      </c>
+      <c r="C62" t="s">
+        <v>21</v>
+      </c>
+      <c r="D62" s="4">
+        <v>54386</v>
+      </c>
+      <c r="E62" s="4">
+        <v>55327</v>
+      </c>
+      <c r="F62">
+        <f t="shared" si="36"/>
+        <v>941</v>
+      </c>
+      <c r="G62" s="2">
+        <f t="shared" si="37"/>
+        <v>802.08196721311481</v>
+      </c>
+      <c r="H62" s="2">
+        <f t="shared" si="38"/>
+        <v>1.7302246901776286</v>
+      </c>
+      <c r="I62" s="2">
+        <f t="shared" si="39"/>
+        <v>3.5992650724708364</v>
+      </c>
+      <c r="J62" s="3">
+        <f t="shared" si="7"/>
+        <v>13891.42170858934</v>
+      </c>
+      <c r="K62" s="3">
+        <f t="shared" si="40"/>
+        <v>10736.57829141066</v>
+      </c>
+      <c r="L62">
+        <f t="shared" si="44"/>
+        <v>-30699</v>
+      </c>
+      <c r="M62" s="4">
+        <f t="shared" si="41"/>
+        <v>24628</v>
+      </c>
+      <c r="N62" s="2">
+        <f t="shared" si="42"/>
+        <v>384.8125</v>
+      </c>
+      <c r="O62">
+        <v>96814</v>
+      </c>
+      <c r="P62">
+        <v>97711</v>
+      </c>
+      <c r="Q62">
+        <f t="shared" si="43"/>
+        <v>109.49250279303317</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>

</xml_diff>

<commit_message>
자동 업데이트: 2025-05-03 21:58:42
</commit_message>
<xml_diff>
--- a/data/daily_report.xlsx
+++ b/data/daily_report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c58a53286e4c1d7a/문서/GitHub/Dashboard/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="261" documentId="8_{9DD2A88B-03DA-4864-84CC-4418086E8BD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{39634E84-8401-4522-A891-14A66D1080C4}"/>
+  <xr:revisionPtr revIDLastSave="268" documentId="8_{9DD2A88B-03DA-4864-84CC-4418086E8BD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{609DDF66-286E-4FB3-A43E-C479D7D175DA}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25050" windowHeight="21000" xr2:uid="{4AB8DADE-1167-4E84-9D67-55086BA93884}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="27300" windowHeight="17325" xr2:uid="{4AB8DADE-1167-4E84-9D67-55086BA93884}"/>
   </bookViews>
   <sheets>
     <sheet name="daily_report" sheetId="1" r:id="rId1"/>
@@ -44,12 +44,6 @@
     <t>Day(Start)</t>
   </si>
   <si>
-    <t>Start(USDT)</t>
-  </si>
-  <si>
-    <t>End(USDT)</t>
-  </si>
-  <si>
     <t>Delta(USDT)</t>
   </si>
   <si>
@@ -69,9 +63,6 @@
   </si>
   <si>
     <t>Withdrawl(USDT)</t>
-  </si>
-  <si>
-    <t>Sum(USDT)</t>
   </si>
   <si>
     <t>Percentage(%)</t>
@@ -105,6 +96,18 @@
   </si>
   <si>
     <t>Sun</t>
+  </si>
+  <si>
+    <t>Start(USDT)</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>End(USDT)</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sum(USDT)</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -703,7 +706,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -717,6 +720,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="42" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -776,6 +782,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1097,8 +1107,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48182F73-FFD5-43FF-A3B0-19A54A277A3F}">
   <dimension ref="A1:Q62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M35" sqref="M35"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1107,7 +1117,7 @@
     <col min="4" max="5" width="9" style="4"/>
     <col min="7" max="7" width="11" customWidth="1"/>
     <col min="8" max="8" width="8.375" customWidth="1"/>
-    <col min="13" max="13" width="9" style="4"/>
+    <col min="13" max="13" width="9.25" style="4" customWidth="1"/>
     <col min="14" max="14" width="14.25" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="13.5" customWidth="1"/>
   </cols>
@@ -1122,47 +1132,47 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="N1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="P1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="Q1" t="s">
         <v>13</v>
-      </c>
-      <c r="O1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
@@ -1173,7 +1183,7 @@
         <v>45719</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D2" s="4">
         <v>6400</v>
@@ -1231,7 +1241,7 @@
         <v>45720</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D3" s="4">
         <v>6400</v>
@@ -1293,7 +1303,7 @@
         <v>45721</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D4" s="4">
         <v>6546</v>
@@ -1355,7 +1365,7 @@
         <v>45722</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D5" s="4">
         <v>6689</v>
@@ -1417,7 +1427,7 @@
         <v>45723</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D6" s="4">
         <v>6846</v>
@@ -1479,7 +1489,7 @@
         <v>45724</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D7" s="4">
         <v>7015</v>
@@ -1541,7 +1551,7 @@
         <v>45725</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D8" s="4">
         <v>7050</v>
@@ -1603,7 +1613,7 @@
         <v>45726</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D9" s="4">
         <v>6979</v>
@@ -1665,7 +1675,7 @@
         <v>45727</v>
       </c>
       <c r="C10" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D10" s="4">
         <v>7170</v>
@@ -1727,7 +1737,7 @@
         <v>45728</v>
       </c>
       <c r="C11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D11" s="4">
         <v>7315</v>
@@ -1789,7 +1799,7 @@
         <v>45729</v>
       </c>
       <c r="C12" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D12" s="4">
         <v>6845</v>
@@ -1851,7 +1861,7 @@
         <v>45730</v>
       </c>
       <c r="C13" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D13" s="4">
         <v>7567</v>
@@ -1913,7 +1923,7 @@
         <v>45731</v>
       </c>
       <c r="C14" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D14" s="4">
         <v>7763</v>
@@ -1975,7 +1985,7 @@
         <v>45732</v>
       </c>
       <c r="C15" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D15" s="4">
         <v>7845</v>
@@ -2037,7 +2047,7 @@
         <v>45733</v>
       </c>
       <c r="C16" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D16" s="4">
         <v>7879</v>
@@ -2099,7 +2109,7 @@
         <v>45734</v>
       </c>
       <c r="C17" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D17" s="4">
         <v>7952</v>
@@ -2161,7 +2171,7 @@
         <v>45735</v>
       </c>
       <c r="C18" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D18" s="4">
         <v>7797</v>
@@ -2223,7 +2233,7 @@
         <v>45736</v>
       </c>
       <c r="C19" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D19" s="4">
         <v>8335</v>
@@ -2285,7 +2295,7 @@
         <v>45737</v>
       </c>
       <c r="C20" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D20" s="4">
         <v>8461</v>
@@ -2347,7 +2357,7 @@
         <v>45738</v>
       </c>
       <c r="C21" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D21" s="4">
         <v>8330</v>
@@ -2409,7 +2419,7 @@
         <v>45739</v>
       </c>
       <c r="C22" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D22" s="4">
         <v>8331</v>
@@ -2471,7 +2481,7 @@
         <v>45740</v>
       </c>
       <c r="C23" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D23" s="4">
         <v>8590</v>
@@ -2533,7 +2543,7 @@
         <v>45741</v>
       </c>
       <c r="C24" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D24" s="4">
         <v>8925</v>
@@ -2595,7 +2605,7 @@
         <v>45742</v>
       </c>
       <c r="C25" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D25" s="4">
         <v>9113</v>
@@ -2657,7 +2667,7 @@
         <v>45743</v>
       </c>
       <c r="C26" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D26" s="4">
         <v>9163</v>
@@ -2719,7 +2729,7 @@
         <v>45744</v>
       </c>
       <c r="C27" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D27" s="4">
         <v>9353</v>
@@ -2781,7 +2791,7 @@
         <v>45745</v>
       </c>
       <c r="C28" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D28" s="4">
         <v>9353</v>
@@ -2843,7 +2853,7 @@
         <v>45746</v>
       </c>
       <c r="C29" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D29" s="4">
         <v>9400</v>
@@ -2905,7 +2915,7 @@
         <v>45747</v>
       </c>
       <c r="C30" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D30" s="4">
         <v>9450</v>
@@ -2967,7 +2977,7 @@
         <v>45748</v>
       </c>
       <c r="C31" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D31" s="4">
         <v>9452</v>
@@ -3029,7 +3039,7 @@
         <v>45749</v>
       </c>
       <c r="C32" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D32" s="4">
         <v>9512</v>
@@ -3091,7 +3101,7 @@
         <v>45750</v>
       </c>
       <c r="C33" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D33" s="4">
         <v>9666</v>
@@ -3153,7 +3163,7 @@
         <v>45751</v>
       </c>
       <c r="C34" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D34" s="4">
         <v>9890</v>
@@ -3215,7 +3225,7 @@
         <v>45752</v>
       </c>
       <c r="C35" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D35" s="4">
         <v>10200</v>
@@ -3277,7 +3287,7 @@
         <v>45753</v>
       </c>
       <c r="C36" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D36" s="4">
         <v>10565</v>
@@ -3339,7 +3349,7 @@
         <v>45754</v>
       </c>
       <c r="C37" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D37" s="4">
         <v>20845</v>
@@ -3401,7 +3411,7 @@
         <v>45755</v>
       </c>
       <c r="C38" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D38" s="4">
         <v>22699</v>
@@ -3463,7 +3473,7 @@
         <v>45756</v>
       </c>
       <c r="C39" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D39" s="4">
         <v>22955</v>
@@ -3525,7 +3535,7 @@
         <v>45757</v>
       </c>
       <c r="C40" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D40" s="4">
         <v>24388</v>
@@ -3587,7 +3597,7 @@
         <v>45758</v>
       </c>
       <c r="C41" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D41" s="4">
         <v>24713</v>
@@ -3649,7 +3659,7 @@
         <v>45759</v>
       </c>
       <c r="C42" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D42" s="4">
         <v>25029</v>
@@ -3711,7 +3721,7 @@
         <v>45760</v>
       </c>
       <c r="C43" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D43" s="4">
         <v>25088</v>
@@ -3773,7 +3783,7 @@
         <v>45761</v>
       </c>
       <c r="C44" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D44" s="4">
         <v>25195</v>
@@ -3835,7 +3845,7 @@
         <v>45762</v>
       </c>
       <c r="C45" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D45" s="4">
         <v>25835</v>
@@ -3897,7 +3907,7 @@
         <v>45763</v>
       </c>
       <c r="C46" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D46" s="4">
         <v>25600</v>
@@ -3959,7 +3969,7 @@
         <v>45764</v>
       </c>
       <c r="C47" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D47" s="4">
         <v>46802</v>
@@ -4022,7 +4032,7 @@
         <v>45765</v>
       </c>
       <c r="C48" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D48" s="4">
         <v>47035</v>
@@ -4085,7 +4095,7 @@
         <v>45766</v>
       </c>
       <c r="C49" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D49" s="4">
         <v>47070</v>
@@ -4148,7 +4158,7 @@
         <v>45767</v>
       </c>
       <c r="C50" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D50" s="4">
         <v>47160</v>
@@ -4211,7 +4221,7 @@
         <v>45768</v>
       </c>
       <c r="C51" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D51" s="4">
         <v>47420</v>
@@ -4274,7 +4284,7 @@
         <v>45769</v>
       </c>
       <c r="C52" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D52" s="4">
         <v>47910</v>
@@ -4337,7 +4347,7 @@
         <v>45770</v>
       </c>
       <c r="C53" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D53" s="4">
         <v>49488</v>
@@ -4400,7 +4410,7 @@
         <v>45771</v>
       </c>
       <c r="C54" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D54" s="4">
         <v>50094</v>
@@ -4463,7 +4473,7 @@
         <v>45772</v>
       </c>
       <c r="C55" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D55" s="4">
         <v>50900</v>
@@ -4526,7 +4536,7 @@
         <v>45773</v>
       </c>
       <c r="C56" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D56" s="4">
         <v>51087.55</v>
@@ -4589,7 +4599,7 @@
         <v>45774</v>
       </c>
       <c r="C57" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D57" s="4">
         <v>51166.85</v>
@@ -4652,7 +4662,7 @@
         <v>45775</v>
       </c>
       <c r="C58" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D58" s="4">
         <v>51225</v>
@@ -4715,7 +4725,7 @@
         <v>45776</v>
       </c>
       <c r="C59" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D59" s="4">
         <v>51915</v>
@@ -4778,7 +4788,7 @@
         <v>45777</v>
       </c>
       <c r="C60" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D60" s="4">
         <v>52670</v>
@@ -4841,7 +4851,7 @@
         <v>45778</v>
       </c>
       <c r="C61" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D61" s="4">
         <v>53561.74</v>
@@ -4904,7 +4914,7 @@
         <v>45779</v>
       </c>
       <c r="C62" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D62" s="4">
         <v>54386</v>

</xml_diff>

<commit_message>
자동 업데이트: 2025-05-03 22:02:12
</commit_message>
<xml_diff>
--- a/data/daily_report.xlsx
+++ b/data/daily_report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c58a53286e4c1d7a/문서/GitHub/Dashboard/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="268" documentId="8_{9DD2A88B-03DA-4864-84CC-4418086E8BD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{609DDF66-286E-4FB3-A43E-C479D7D175DA}"/>
+  <xr:revisionPtr revIDLastSave="269" documentId="8_{9DD2A88B-03DA-4864-84CC-4418086E8BD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{159E1548-2E6F-4CD8-A09F-13D356E11DC7}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="27300" windowHeight="17325" xr2:uid="{4AB8DADE-1167-4E84-9D67-55086BA93884}"/>
+    <workbookView xWindow="4290" yWindow="4275" windowWidth="27300" windowHeight="17325" xr2:uid="{4AB8DADE-1167-4E84-9D67-55086BA93884}"/>
   </bookViews>
   <sheets>
     <sheet name="daily_report" sheetId="1" r:id="rId1"/>
@@ -706,23 +706,17 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="42" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1108,100 +1102,100 @@
   <dimension ref="A1:Q62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="11.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="9" style="4"/>
+    <col min="4" max="5" width="9" style="1"/>
     <col min="7" max="7" width="11" customWidth="1"/>
     <col min="8" max="8" width="8.375" customWidth="1"/>
-    <col min="13" max="13" width="9.25" style="4" customWidth="1"/>
+    <col min="13" max="13" width="9.25" style="1" customWidth="1"/>
     <col min="14" max="14" width="14.25" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A2">
+      <c r="A2" s="3">
         <v>0</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="3">
         <v>45719</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="2">
         <v>6400</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="2">
         <v>6400</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="3">
         <f>E2-D2</f>
         <v>0</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="3">
         <v>0</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="3">
         <v>0</v>
       </c>
-      <c r="I2" s="2">
+      <c r="I2" s="3">
         <v>0</v>
       </c>
       <c r="J2" s="3">
@@ -1212,56 +1206,56 @@
         <f t="shared" ref="K2:K36" si="0">M2-J2</f>
         <v>0</v>
       </c>
-      <c r="L2">
+      <c r="L2" s="3">
         <v>0</v>
       </c>
-      <c r="M2" s="4">
+      <c r="M2" s="2">
         <f>L2+E2</f>
         <v>6400</v>
       </c>
-      <c r="N2" s="2">
+      <c r="N2" s="3">
         <f>M2/$D$2*100</f>
         <v>100</v>
       </c>
-      <c r="O2">
+      <c r="O2" s="3">
         <v>89239.9</v>
       </c>
-      <c r="P2">
+      <c r="P2" s="3">
         <v>89239.9</v>
       </c>
-      <c r="Q2">
+      <c r="Q2" s="3">
         <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A3">
+      <c r="A3" s="3">
         <v>1</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="3">
         <v>45720</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="2">
         <v>6400</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="2">
         <v>6546</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="3">
         <f t="shared" ref="F3:F24" si="1">E3-D3</f>
         <v>146</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3" s="3">
         <f t="shared" ref="G3:G22" si="2">(E3-$D$2)/A3</f>
         <v>146</v>
       </c>
-      <c r="H3" s="2">
+      <c r="H3" s="3">
         <f>(E3/D3-1)*100</f>
         <v>2.2812499999999902</v>
       </c>
-      <c r="I3" s="2">
+      <c r="I3" s="3">
         <f>(POWER((E3/$D$3),1/A3)-1)*100</f>
         <v>2.2812499999999902</v>
       </c>
@@ -1273,57 +1267,57 @@
         <f t="shared" si="0"/>
         <v>62.800000000001091</v>
       </c>
-      <c r="L3">
+      <c r="L3" s="3">
         <v>0</v>
       </c>
-      <c r="M3" s="4">
+      <c r="M3" s="2">
         <f t="shared" ref="M3:M24" si="3">L3+E3</f>
         <v>6546</v>
       </c>
-      <c r="N3" s="2">
+      <c r="N3" s="3">
         <f t="shared" ref="N3:N41" si="4">M3/$D$2*100</f>
         <v>102.28124999999999</v>
       </c>
-      <c r="O3">
+      <c r="O3" s="3">
         <v>89239.9</v>
       </c>
-      <c r="P3">
+      <c r="P3" s="3">
         <v>83157.100000000006</v>
       </c>
-      <c r="Q3">
+      <c r="Q3" s="3">
         <f>P3/$O$2*100</f>
         <v>93.183766454243013</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A4">
+      <c r="A4" s="3">
         <v>2</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="3">
         <v>45721</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="2">
         <v>6546</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="2">
         <v>6689</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="3">
         <f t="shared" si="1"/>
         <v>143</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="3">
         <f t="shared" si="2"/>
         <v>144.5</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4" s="3">
         <f t="shared" ref="H4:H24" si="5">(E4/D4-1)*100</f>
         <v>2.1845401772074613</v>
       </c>
-      <c r="I4" s="2">
+      <c r="I4" s="3">
         <f t="shared" ref="I4:I24" si="6">(POWER((E4/$D$3),1/A4)-1)*100</f>
         <v>2.2328836529616813</v>
       </c>
@@ -1335,57 +1329,57 @@
         <f t="shared" si="0"/>
         <v>121.51840000000175</v>
       </c>
-      <c r="L4">
+      <c r="L4" s="3">
         <v>0</v>
       </c>
-      <c r="M4" s="4">
+      <c r="M4" s="2">
         <f t="shared" si="3"/>
         <v>6689</v>
       </c>
-      <c r="N4" s="2">
+      <c r="N4" s="3">
         <f t="shared" si="4"/>
         <v>104.515625</v>
       </c>
-      <c r="O4">
+      <c r="O4" s="3">
         <v>83157.100000000006</v>
       </c>
-      <c r="P4">
+      <c r="P4" s="3">
         <v>88477.3</v>
       </c>
-      <c r="Q4">
+      <c r="Q4" s="3">
         <f t="shared" ref="Q4:Q41" si="8">P4/$O$2*100</f>
         <v>99.145449513054146</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A5">
+      <c r="A5" s="3">
         <v>3</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="3">
         <v>45722</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="2">
         <v>6689</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="2">
         <v>6846</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="3">
         <f t="shared" si="1"/>
         <v>157</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="3">
         <f t="shared" si="2"/>
         <v>148.66666666666666</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5" s="3">
         <f t="shared" si="5"/>
         <v>2.3471370907460098</v>
       </c>
-      <c r="I5" s="2">
+      <c r="I5" s="3">
         <f t="shared" si="6"/>
         <v>2.2709539535396894</v>
       </c>
@@ -1397,57 +1391,57 @@
         <f t="shared" si="0"/>
         <v>193.14113920000273</v>
       </c>
-      <c r="L5">
+      <c r="L5" s="3">
         <v>0</v>
       </c>
-      <c r="M5" s="4">
+      <c r="M5" s="2">
         <f t="shared" si="3"/>
         <v>6846</v>
       </c>
-      <c r="N5" s="2">
+      <c r="N5" s="3">
         <f t="shared" si="4"/>
         <v>106.96874999999999</v>
       </c>
-      <c r="O5">
+      <c r="O5" s="3">
         <v>88477.3</v>
       </c>
-      <c r="P5">
+      <c r="P5" s="3">
         <v>89770.4</v>
       </c>
-      <c r="Q5">
+      <c r="Q5" s="3">
         <f t="shared" si="8"/>
         <v>100.59446503189717</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A6">
+      <c r="A6" s="3">
         <v>4</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="3">
         <v>45723</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="2">
         <v>6846</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="2">
         <v>7015</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="3">
         <f t="shared" si="1"/>
         <v>169</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" s="3">
         <f t="shared" si="2"/>
         <v>153.75</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H6" s="3">
         <f t="shared" si="5"/>
         <v>2.4685947998831503</v>
       </c>
-      <c r="I6" s="2">
+      <c r="I6" s="3">
         <f t="shared" si="6"/>
         <v>2.3203283980714806</v>
       </c>
@@ -1459,57 +1453,57 @@
         <f t="shared" si="0"/>
         <v>275.65397400960319</v>
       </c>
-      <c r="L6">
+      <c r="L6" s="3">
         <v>0</v>
       </c>
-      <c r="M6" s="4">
+      <c r="M6" s="2">
         <f t="shared" si="3"/>
         <v>7015</v>
       </c>
-      <c r="N6" s="2">
+      <c r="N6" s="3">
         <f t="shared" si="4"/>
         <v>109.60937500000001</v>
       </c>
-      <c r="O6">
+      <c r="O6" s="3">
         <v>89770.4</v>
       </c>
-      <c r="P6">
+      <c r="P6" s="3">
         <v>90411.6</v>
       </c>
-      <c r="Q6">
+      <c r="Q6" s="3">
         <f t="shared" si="8"/>
         <v>101.3129777151252</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A7">
+      <c r="A7" s="3">
         <v>5</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="3">
         <v>45724</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="2">
         <v>7015</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="2">
         <v>7050</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="3">
         <f t="shared" si="1"/>
         <v>35</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7" s="3">
         <f t="shared" si="2"/>
         <v>130</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H7" s="3">
         <f t="shared" si="5"/>
         <v>0.49893086243764095</v>
       </c>
-      <c r="I7" s="2">
+      <c r="I7" s="3">
         <f t="shared" si="6"/>
         <v>1.9534270313376956</v>
       </c>
@@ -1521,57 +1515,57 @@
         <f t="shared" si="0"/>
         <v>223.04247567172843</v>
       </c>
-      <c r="L7">
+      <c r="L7" s="3">
         <v>0</v>
       </c>
-      <c r="M7" s="4">
+      <c r="M7" s="2">
         <f t="shared" si="3"/>
         <v>7050</v>
       </c>
-      <c r="N7" s="2">
+      <c r="N7" s="3">
         <f t="shared" si="4"/>
         <v>110.15625</v>
       </c>
-      <c r="O7">
+      <c r="O7" s="3">
         <v>90411.6</v>
       </c>
-      <c r="P7">
+      <c r="P7" s="3">
         <v>86323.3</v>
       </c>
-      <c r="Q7">
+      <c r="Q7" s="3">
         <f t="shared" si="8"/>
         <v>96.731730985803438</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A8">
+      <c r="A8" s="3">
         <v>6</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="3">
         <v>45725</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="2">
         <v>7050</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="2">
         <v>6979</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="3">
         <f t="shared" si="1"/>
         <v>-71</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G8" s="3">
         <f t="shared" si="2"/>
         <v>96.5</v>
       </c>
-      <c r="H8" s="2">
+      <c r="H8" s="3">
         <f t="shared" si="5"/>
         <v>-1.0070921985815606</v>
       </c>
-      <c r="I8" s="2">
+      <c r="I8" s="3">
         <f t="shared" si="6"/>
         <v>1.4539290311231801</v>
       </c>
@@ -1583,57 +1577,57 @@
         <f t="shared" si="0"/>
         <v>63.292027855461129</v>
       </c>
-      <c r="L8">
+      <c r="L8" s="3">
         <v>0</v>
       </c>
-      <c r="M8" s="4">
+      <c r="M8" s="2">
         <f t="shared" si="3"/>
         <v>6979</v>
       </c>
-      <c r="N8" s="2">
+      <c r="N8" s="3">
         <f t="shared" si="4"/>
         <v>109.04687500000001</v>
       </c>
-      <c r="O8">
+      <c r="O8" s="3">
         <v>86323.3</v>
       </c>
-      <c r="P8">
+      <c r="P8" s="3">
         <v>83563</v>
       </c>
-      <c r="Q8">
+      <c r="Q8" s="3">
         <f t="shared" si="8"/>
         <v>93.638607842456125</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A9">
+      <c r="A9" s="3">
         <v>8</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" s="3">
         <v>45726</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="2">
         <v>6979</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="2">
         <v>7170</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="3">
         <f t="shared" si="1"/>
         <v>191</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G9" s="3">
         <f t="shared" si="2"/>
         <v>96.25</v>
       </c>
-      <c r="H9" s="2">
+      <c r="H9" s="3">
         <f t="shared" si="5"/>
         <v>2.7367817738931155</v>
       </c>
-      <c r="I9" s="2">
+      <c r="I9" s="3">
         <f t="shared" si="6"/>
         <v>1.4302270645888626</v>
       </c>
@@ -1645,57 +1639,57 @@
         <f t="shared" si="0"/>
         <v>164.38782421758242</v>
       </c>
-      <c r="L9">
+      <c r="L9" s="3">
         <v>0</v>
       </c>
-      <c r="M9" s="4">
+      <c r="M9" s="2">
         <f t="shared" si="3"/>
         <v>7170</v>
       </c>
-      <c r="N9" s="2">
+      <c r="N9" s="3">
         <f t="shared" si="4"/>
         <v>112.03125</v>
       </c>
-      <c r="O9">
+      <c r="O9" s="3">
         <v>83563</v>
       </c>
-      <c r="P9">
+      <c r="P9" s="3">
         <v>79813.7</v>
       </c>
-      <c r="Q9">
+      <c r="Q9" s="3">
         <f t="shared" si="8"/>
         <v>89.437236034554061</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A10">
+      <c r="A10" s="3">
         <v>9</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="3">
         <v>45727</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="2">
         <v>7170</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="2">
         <v>7315</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="3">
         <f t="shared" si="1"/>
         <v>145</v>
       </c>
-      <c r="G10" s="2">
+      <c r="G10" s="3">
         <f t="shared" si="2"/>
         <v>101.66666666666667</v>
       </c>
-      <c r="H10" s="2">
+      <c r="H10" s="3">
         <f t="shared" si="5"/>
         <v>2.0223152022315283</v>
       </c>
-      <c r="I10" s="2">
+      <c r="I10" s="3">
         <f t="shared" si="6"/>
         <v>1.4958445810377752</v>
       </c>
@@ -1707,57 +1701,57 @@
         <f t="shared" si="0"/>
         <v>218.31486593241152</v>
       </c>
-      <c r="L10">
+      <c r="L10" s="3">
         <v>0</v>
       </c>
-      <c r="M10" s="4">
+      <c r="M10" s="2">
         <f t="shared" si="3"/>
         <v>7315</v>
       </c>
-      <c r="N10" s="2">
+      <c r="N10" s="3">
         <f t="shared" si="4"/>
         <v>114.29687500000001</v>
       </c>
-      <c r="O10">
+      <c r="O10" s="3">
         <v>79813.7</v>
       </c>
-      <c r="P10">
+      <c r="P10" s="3">
         <v>80615.7</v>
       </c>
-      <c r="Q10">
+      <c r="Q10" s="3">
         <f t="shared" si="8"/>
         <v>90.335937176083789</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A11">
+      <c r="A11" s="3">
         <v>10</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11" s="3">
         <v>45728</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="2">
         <v>7315</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="2">
         <v>6845</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="3">
         <f t="shared" si="1"/>
         <v>-470</v>
       </c>
-      <c r="G11" s="2">
+      <c r="G11" s="3">
         <f t="shared" si="2"/>
         <v>44.5</v>
       </c>
-      <c r="H11" s="2">
+      <c r="H11" s="3">
         <f t="shared" si="5"/>
         <v>-6.4251537935748448</v>
       </c>
-      <c r="I11" s="2">
+      <c r="I11" s="3">
         <f t="shared" si="6"/>
         <v>0.67446905031474103</v>
       </c>
@@ -1769,57 +1763,57 @@
         <f t="shared" si="0"/>
         <v>-343.9420408104661</v>
       </c>
-      <c r="L11">
+      <c r="L11" s="3">
         <v>0</v>
       </c>
-      <c r="M11" s="4">
+      <c r="M11" s="2">
         <f t="shared" si="3"/>
         <v>6845</v>
       </c>
-      <c r="N11" s="2">
+      <c r="N11" s="3">
         <f t="shared" si="4"/>
         <v>106.953125</v>
       </c>
-      <c r="O11">
+      <c r="O11" s="3">
         <v>80615.7</v>
       </c>
-      <c r="P11">
+      <c r="P11" s="3">
         <v>81500.899999999994</v>
       </c>
-      <c r="Q11">
+      <c r="Q11" s="3">
         <f t="shared" si="8"/>
         <v>91.327870156734832</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A12">
+      <c r="A12" s="3">
         <v>11</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12" s="3">
         <v>45729</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="2">
         <v>6845</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="2">
         <v>7567</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="3">
         <f t="shared" si="1"/>
         <v>722</v>
       </c>
-      <c r="G12" s="2">
+      <c r="G12" s="3">
         <f t="shared" si="2"/>
         <v>106.09090909090909</v>
       </c>
-      <c r="H12" s="2">
+      <c r="H12" s="3">
         <f t="shared" si="5"/>
         <v>10.547845142439737</v>
       </c>
-      <c r="I12" s="2">
+      <c r="I12" s="3">
         <f t="shared" si="6"/>
         <v>1.5343678109079883</v>
       </c>
@@ -1831,57 +1825,57 @@
         <f t="shared" si="0"/>
         <v>284.60171265899862</v>
       </c>
-      <c r="L12">
+      <c r="L12" s="3">
         <v>0</v>
       </c>
-      <c r="M12" s="4">
+      <c r="M12" s="2">
         <f t="shared" si="3"/>
         <v>7567</v>
       </c>
-      <c r="N12" s="2">
+      <c r="N12" s="3">
         <f t="shared" si="4"/>
         <v>118.234375</v>
       </c>
-      <c r="O12">
+      <c r="O12" s="3">
         <v>81500.899999999994</v>
       </c>
-      <c r="P12">
+      <c r="P12" s="3">
         <v>81966.600000000006</v>
       </c>
-      <c r="Q12">
+      <c r="Q12" s="3">
         <f t="shared" si="8"/>
         <v>91.849721929316388</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A13">
+      <c r="A13" s="3">
         <v>12</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13" s="3">
         <v>45730</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="4">
+      <c r="D13" s="2">
         <v>7567</v>
       </c>
-      <c r="E13" s="4">
+      <c r="E13" s="2">
         <v>7763</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="3">
         <f t="shared" si="1"/>
         <v>196</v>
       </c>
-      <c r="G13" s="2">
+      <c r="G13" s="3">
         <f t="shared" si="2"/>
         <v>113.58333333333333</v>
       </c>
-      <c r="H13" s="2">
+      <c r="H13" s="3">
         <f t="shared" si="5"/>
         <v>2.5901942645698339</v>
       </c>
-      <c r="I13" s="2">
+      <c r="I13" s="3">
         <f t="shared" si="6"/>
         <v>1.6219367680212704</v>
       </c>
@@ -1893,57 +1887,57 @@
         <f t="shared" si="0"/>
         <v>385.93053492356648</v>
       </c>
-      <c r="L13">
+      <c r="L13" s="3">
         <v>0</v>
       </c>
-      <c r="M13" s="4">
+      <c r="M13" s="2">
         <f t="shared" si="3"/>
         <v>7763</v>
       </c>
-      <c r="N13" s="2">
+      <c r="N13" s="3">
         <f t="shared" si="4"/>
         <v>121.296875</v>
       </c>
-      <c r="O13">
+      <c r="O13" s="3">
         <v>81966.600000000006</v>
       </c>
-      <c r="P13">
+      <c r="P13" s="3">
         <v>83496</v>
       </c>
-      <c r="Q13">
+      <c r="Q13" s="3">
         <f t="shared" si="8"/>
         <v>93.563529318163745</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A14">
+      <c r="A14" s="3">
         <v>13</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14" s="3">
         <v>45731</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="4">
+      <c r="D14" s="2">
         <v>7763</v>
       </c>
-      <c r="E14" s="4">
+      <c r="E14" s="2">
         <v>7845</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="3">
         <f t="shared" si="1"/>
         <v>82</v>
       </c>
-      <c r="G14" s="2">
+      <c r="G14" s="3">
         <f t="shared" si="2"/>
         <v>111.15384615384616</v>
       </c>
-      <c r="H14" s="2">
+      <c r="H14" s="3">
         <f t="shared" si="5"/>
         <v>1.0562926703594044</v>
       </c>
-      <c r="I14" s="2">
+      <c r="I14" s="3">
         <f t="shared" si="6"/>
         <v>1.5783135032505946</v>
       </c>
@@ -1955,57 +1949,57 @@
         <f t="shared" si="0"/>
         <v>372.02863187757339</v>
       </c>
-      <c r="L14">
+      <c r="L14" s="3">
         <v>0</v>
       </c>
-      <c r="M14" s="4">
+      <c r="M14" s="2">
         <f t="shared" si="3"/>
         <v>7845</v>
       </c>
-      <c r="N14" s="2">
+      <c r="N14" s="3">
         <f t="shared" si="4"/>
         <v>122.578125</v>
       </c>
-      <c r="O14">
+      <c r="O14" s="3">
         <v>83496</v>
       </c>
-      <c r="P14">
+      <c r="P14" s="3">
         <v>84108.4</v>
       </c>
-      <c r="Q14">
+      <c r="Q14" s="3">
         <f t="shared" si="8"/>
         <v>94.249769441695918</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A15">
+      <c r="A15" s="3">
         <v>14</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15" s="3">
         <v>45732</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D15" s="4">
+      <c r="D15" s="2">
         <v>7845</v>
       </c>
-      <c r="E15" s="4">
+      <c r="E15" s="2">
         <v>7879</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="3">
         <f t="shared" si="1"/>
         <v>34</v>
       </c>
-      <c r="G15" s="2">
+      <c r="G15" s="3">
         <f t="shared" si="2"/>
         <v>105.64285714285714</v>
       </c>
-      <c r="H15" s="2">
+      <c r="H15" s="3">
         <f t="shared" si="5"/>
         <v>0.43339706819629509</v>
       </c>
-      <c r="I15" s="2">
+      <c r="I15" s="3">
         <f t="shared" si="6"/>
         <v>1.4961026704697122</v>
       </c>
@@ -2017,57 +2011,57 @@
         <f t="shared" si="0"/>
         <v>308.8800040919823</v>
       </c>
-      <c r="L15">
+      <c r="L15" s="3">
         <v>0</v>
       </c>
-      <c r="M15" s="4">
+      <c r="M15" s="2">
         <f t="shared" si="3"/>
         <v>7879</v>
       </c>
-      <c r="N15" s="2">
+      <c r="N15" s="3">
         <f t="shared" si="4"/>
         <v>123.10937500000001</v>
       </c>
-      <c r="O15">
+      <c r="O15" s="3">
         <v>84108.4</v>
       </c>
-      <c r="P15">
+      <c r="P15" s="3">
         <v>83334.2</v>
       </c>
-      <c r="Q15">
+      <c r="Q15" s="3">
         <f t="shared" si="8"/>
         <v>93.382220284872574</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A16">
+      <c r="A16" s="3">
         <v>15</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16" s="3">
         <v>45733</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="4">
+      <c r="D16" s="2">
         <v>7879</v>
       </c>
-      <c r="E16" s="4">
+      <c r="E16" s="2">
         <v>7952</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="3">
         <f t="shared" si="1"/>
         <v>73</v>
       </c>
-      <c r="G16" s="2">
+      <c r="G16" s="3">
         <f t="shared" si="2"/>
         <v>103.46666666666667</v>
       </c>
-      <c r="H16" s="2">
+      <c r="H16" s="3">
         <f t="shared" si="5"/>
         <v>0.92651351694377215</v>
       </c>
-      <c r="I16" s="2">
+      <c r="I16" s="3">
         <f t="shared" si="6"/>
         <v>1.4580302525748934</v>
       </c>
@@ -2079,57 +2073,57 @@
         <f t="shared" si="0"/>
         <v>283.46844414517909</v>
       </c>
-      <c r="L16">
+      <c r="L16" s="3">
         <v>0</v>
       </c>
-      <c r="M16" s="4">
+      <c r="M16" s="2">
         <f t="shared" si="3"/>
         <v>7952</v>
       </c>
-      <c r="N16" s="2">
+      <c r="N16" s="3">
         <f t="shared" si="4"/>
         <v>124.25</v>
       </c>
-      <c r="O16">
+      <c r="O16" s="3">
         <v>83334.2</v>
       </c>
-      <c r="P16">
+      <c r="P16" s="3">
         <v>82873.100000000006</v>
       </c>
-      <c r="Q16">
+      <c r="Q16" s="3">
         <f t="shared" si="8"/>
         <v>92.865523157242464</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A17">
+      <c r="A17" s="3">
         <v>16</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B17" s="3">
         <v>45734</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="4">
+      <c r="D17" s="2">
         <v>7952</v>
       </c>
-      <c r="E17" s="4">
+      <c r="E17" s="2">
         <v>7797</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="3">
         <f t="shared" si="1"/>
         <v>-155</v>
       </c>
-      <c r="G17" s="2">
+      <c r="G17" s="3">
         <f t="shared" si="2"/>
         <v>87.3125</v>
       </c>
-      <c r="H17" s="2">
+      <c r="H17" s="3">
         <f t="shared" si="5"/>
         <v>-1.9491951710261524</v>
       </c>
-      <c r="I17" s="2">
+      <c r="I17" s="3">
         <f t="shared" si="6"/>
         <v>1.2416518639221996</v>
       </c>
@@ -2141,57 +2135,57 @@
         <f t="shared" si="0"/>
         <v>28.777533919067537</v>
       </c>
-      <c r="L17">
+      <c r="L17" s="3">
         <v>0</v>
       </c>
-      <c r="M17" s="4">
+      <c r="M17" s="2">
         <f t="shared" si="3"/>
         <v>7797</v>
       </c>
-      <c r="N17" s="2">
+      <c r="N17" s="3">
         <f t="shared" si="4"/>
         <v>121.828125</v>
       </c>
-      <c r="O17">
+      <c r="O17" s="3">
         <v>82873.100000000006</v>
       </c>
-      <c r="P17">
+      <c r="P17" s="3">
         <v>81809.5</v>
       </c>
-      <c r="Q17">
+      <c r="Q17" s="3">
         <f t="shared" si="8"/>
         <v>91.673679598475573</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A18">
+      <c r="A18" s="3">
         <v>17</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B18" s="3">
         <v>45735</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D18" s="4">
+      <c r="D18" s="2">
         <v>7797</v>
       </c>
-      <c r="E18" s="4">
+      <c r="E18" s="2">
         <v>8335</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="3">
         <f t="shared" si="1"/>
         <v>538</v>
       </c>
-      <c r="G18" s="2">
+      <c r="G18" s="3">
         <f t="shared" si="2"/>
         <v>113.82352941176471</v>
       </c>
-      <c r="H18" s="2">
+      <c r="H18" s="3">
         <f t="shared" si="5"/>
         <v>6.9000897781198001</v>
       </c>
-      <c r="I18" s="2">
+      <c r="I18" s="3">
         <f t="shared" si="6"/>
         <v>1.5660508945335661</v>
       </c>
@@ -2203,57 +2197,57 @@
         <f t="shared" si="0"/>
         <v>465.79064186001597</v>
       </c>
-      <c r="L18">
+      <c r="L18" s="3">
         <v>0</v>
       </c>
-      <c r="M18" s="4">
+      <c r="M18" s="2">
         <f t="shared" si="3"/>
         <v>8335</v>
       </c>
-      <c r="N18" s="2">
+      <c r="N18" s="3">
         <f t="shared" si="4"/>
         <v>130.234375</v>
       </c>
-      <c r="O18">
+      <c r="O18" s="3">
         <v>81809.5</v>
       </c>
-      <c r="P18">
+      <c r="P18" s="3">
         <v>84267.4</v>
       </c>
-      <c r="Q18">
+      <c r="Q18" s="3">
         <f t="shared" si="8"/>
         <v>94.427940865016652</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A19">
+      <c r="A19" s="3">
         <v>18</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B19" s="3">
         <v>45736</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D19" s="4">
+      <c r="D19" s="2">
         <v>8335</v>
       </c>
-      <c r="E19" s="4">
+      <c r="E19" s="2">
         <v>8461</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="3">
         <f t="shared" si="1"/>
         <v>126</v>
       </c>
-      <c r="G19" s="2">
+      <c r="G19" s="3">
         <f t="shared" si="2"/>
         <v>114.5</v>
       </c>
-      <c r="H19" s="2">
+      <c r="H19" s="3">
         <f t="shared" si="5"/>
         <v>1.5116976604679033</v>
       </c>
-      <c r="I19" s="2">
+      <c r="I19" s="3">
         <f t="shared" si="6"/>
         <v>1.5630305070633677</v>
       </c>
@@ -2265,57 +2259,57 @@
         <f t="shared" si="0"/>
         <v>489.49092020419721</v>
       </c>
-      <c r="L19">
+      <c r="L19" s="3">
         <v>0</v>
       </c>
-      <c r="M19" s="4">
+      <c r="M19" s="2">
         <f t="shared" si="3"/>
         <v>8461</v>
       </c>
-      <c r="N19" s="2">
+      <c r="N19" s="3">
         <f t="shared" si="4"/>
         <v>132.203125</v>
       </c>
-      <c r="O19">
+      <c r="O19" s="3">
         <v>84267.4</v>
       </c>
-      <c r="P19">
+      <c r="P19" s="3">
         <v>86123.6</v>
       </c>
-      <c r="Q19">
+      <c r="Q19" s="3">
         <f t="shared" si="8"/>
         <v>96.507952160412572</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A20">
+      <c r="A20" s="3">
         <v>19</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B20" s="3">
         <v>45737</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D20" s="4">
+      <c r="D20" s="2">
         <v>8461</v>
       </c>
-      <c r="E20" s="4">
+      <c r="E20" s="2">
         <v>8330</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="3">
         <f t="shared" si="1"/>
         <v>-131</v>
       </c>
-      <c r="G20" s="2">
+      <c r="G20" s="3">
         <f t="shared" si="2"/>
         <v>101.57894736842105</v>
       </c>
-      <c r="H20" s="2">
+      <c r="H20" s="3">
         <f t="shared" si="5"/>
         <v>-1.5482803451128735</v>
       </c>
-      <c r="I20" s="2">
+      <c r="I20" s="3">
         <f t="shared" si="6"/>
         <v>1.3968527401524877</v>
       </c>
@@ -2327,57 +2321,57 @@
         <f t="shared" si="0"/>
         <v>254.86130216685251</v>
       </c>
-      <c r="L20">
+      <c r="L20" s="3">
         <v>0</v>
       </c>
-      <c r="M20" s="4">
+      <c r="M20" s="2">
         <f t="shared" si="3"/>
         <v>8330</v>
       </c>
-      <c r="N20" s="2">
+      <c r="N20" s="3">
         <f t="shared" si="4"/>
         <v>130.15625</v>
       </c>
-      <c r="O20">
+      <c r="O20" s="3">
         <v>86123.6</v>
       </c>
-      <c r="P20">
+      <c r="P20" s="3">
         <v>84200</v>
       </c>
-      <c r="Q20">
+      <c r="Q20" s="3">
         <f t="shared" si="8"/>
         <v>94.352414110728503</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A21">
+      <c r="A21" s="3">
         <v>20</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B21" s="3">
         <v>45738</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D21" s="4">
+      <c r="D21" s="2">
         <v>8330</v>
       </c>
-      <c r="E21" s="4">
+      <c r="E21" s="2">
         <v>8331</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="3">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="G21" s="2">
+      <c r="G21" s="3">
         <f t="shared" si="2"/>
         <v>96.55</v>
       </c>
-      <c r="H21" s="2">
+      <c r="H21" s="3">
         <f t="shared" si="5"/>
         <v>1.2004801920761921E-2</v>
       </c>
-      <c r="I21" s="2">
+      <c r="I21" s="3">
         <f t="shared" si="6"/>
         <v>1.3271571111354463</v>
       </c>
@@ -2389,57 +2383,57 @@
         <f t="shared" si="0"/>
         <v>150.88449909502197</v>
       </c>
-      <c r="L21">
+      <c r="L21" s="3">
         <v>0</v>
       </c>
-      <c r="M21" s="4">
+      <c r="M21" s="2">
         <f t="shared" si="3"/>
         <v>8331</v>
       </c>
-      <c r="N21" s="2">
+      <c r="N21" s="3">
         <f t="shared" si="4"/>
         <v>130.171875</v>
       </c>
-      <c r="O21">
+      <c r="O21" s="3">
         <v>84200</v>
       </c>
-      <c r="P21">
+      <c r="P21" s="3">
         <v>83970.6</v>
       </c>
-      <c r="Q21">
+      <c r="Q21" s="3">
         <f t="shared" si="8"/>
         <v>94.095354208151292</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A22">
+      <c r="A22" s="3">
         <v>21</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B22" s="3">
         <v>45739</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D22" s="4">
+      <c r="D22" s="2">
         <v>8331</v>
       </c>
-      <c r="E22" s="4">
+      <c r="E22" s="2">
         <v>8590</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="3">
         <f t="shared" si="1"/>
         <v>259</v>
       </c>
-      <c r="G22" s="2">
+      <c r="G22" s="3">
         <f t="shared" si="2"/>
         <v>104.28571428571429</v>
       </c>
-      <c r="H22" s="2">
+      <c r="H22" s="3">
         <f t="shared" si="5"/>
         <v>3.1088704837354486</v>
       </c>
-      <c r="I22" s="2">
+      <c r="I22" s="3">
         <f t="shared" si="6"/>
         <v>1.4112982170128241</v>
       </c>
@@ -2451,57 +2445,57 @@
         <f t="shared" si="0"/>
         <v>303.5429975832576</v>
       </c>
-      <c r="L22">
+      <c r="L22" s="3">
         <v>0</v>
       </c>
-      <c r="M22" s="4">
+      <c r="M22" s="2">
         <f t="shared" si="3"/>
         <v>8590</v>
       </c>
-      <c r="N22" s="2">
+      <c r="N22" s="3">
         <f t="shared" si="4"/>
         <v>134.21875</v>
       </c>
-      <c r="O22">
+      <c r="O22" s="3">
         <v>83970.6</v>
       </c>
-      <c r="P22">
+      <c r="P22" s="3">
         <v>84862</v>
       </c>
-      <c r="Q22">
+      <c r="Q22" s="3">
         <f t="shared" si="8"/>
         <v>95.094234753736842</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A23">
+      <c r="A23" s="3">
         <v>22</v>
       </c>
-      <c r="B23" s="1">
+      <c r="B23" s="3">
         <v>45740</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D23" s="4">
+      <c r="D23" s="2">
         <v>8590</v>
       </c>
-      <c r="E23" s="4">
+      <c r="E23" s="2">
         <v>8925</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="3">
         <f t="shared" si="1"/>
         <v>335</v>
       </c>
-      <c r="G23" s="2">
+      <c r="G23" s="3">
         <f>(E23-$D$2)/A23</f>
         <v>114.77272727272727</v>
       </c>
-      <c r="H23" s="2">
+      <c r="H23" s="3">
         <f t="shared" si="5"/>
         <v>3.8998835855646119</v>
       </c>
-      <c r="I23" s="2">
+      <c r="I23" s="3">
         <f t="shared" si="6"/>
         <v>1.5231117007673323</v>
       </c>
@@ -2513,57 +2507,57 @@
         <f t="shared" si="0"/>
         <v>530.81905655184164</v>
       </c>
-      <c r="L23">
+      <c r="L23" s="3">
         <v>0</v>
       </c>
-      <c r="M23" s="4">
+      <c r="M23" s="2">
         <f t="shared" si="3"/>
         <v>8925</v>
       </c>
-      <c r="N23" s="2">
+      <c r="N23" s="3">
         <f t="shared" si="4"/>
         <v>139.453125</v>
       </c>
-      <c r="O23">
+      <c r="O23" s="3">
         <v>84862</v>
       </c>
-      <c r="P23">
+      <c r="P23" s="3">
         <v>87921</v>
       </c>
-      <c r="Q23">
+      <c r="Q23" s="3">
         <f t="shared" si="8"/>
         <v>98.522073646429462</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A24">
+      <c r="A24" s="3">
         <v>23</v>
       </c>
-      <c r="B24" s="1">
+      <c r="B24" s="3">
         <v>45741</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D24" s="4">
+      <c r="D24" s="2">
         <v>8925</v>
       </c>
-      <c r="E24" s="4">
+      <c r="E24" s="2">
         <v>9113</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="3">
         <f t="shared" si="1"/>
         <v>188</v>
       </c>
-      <c r="G24" s="2">
+      <c r="G24" s="3">
         <f>(E24-$D$2)/A24</f>
         <v>117.95652173913044</v>
       </c>
-      <c r="H24" s="2">
+      <c r="H24" s="3">
         <f t="shared" si="5"/>
         <v>2.1064425770308093</v>
       </c>
-      <c r="I24" s="2">
+      <c r="I24" s="3">
         <f t="shared" si="6"/>
         <v>1.5484044777758443</v>
       </c>
@@ -2575,57 +2569,57 @@
         <f t="shared" si="0"/>
         <v>609.69470428701607</v>
       </c>
-      <c r="L24">
+      <c r="L24" s="3">
         <v>0</v>
       </c>
-      <c r="M24" s="4">
+      <c r="M24" s="2">
         <f t="shared" si="3"/>
         <v>9113</v>
       </c>
-      <c r="N24" s="2">
+      <c r="N24" s="3">
         <f t="shared" si="4"/>
         <v>142.390625</v>
       </c>
-      <c r="O24">
+      <c r="O24" s="3">
         <v>87921</v>
       </c>
-      <c r="P24">
+      <c r="P24" s="3">
         <v>87985.1</v>
       </c>
-      <c r="Q24">
+      <c r="Q24" s="3">
         <f t="shared" si="8"/>
         <v>98.59390250325248</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A25">
+      <c r="A25" s="3">
         <v>24</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B25" s="3">
         <v>45742</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D25" s="4">
+      <c r="D25" s="2">
         <v>9113</v>
       </c>
-      <c r="E25" s="4">
+      <c r="E25" s="2">
         <v>9163</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="3">
         <f t="shared" ref="F25" si="9">E25-D25</f>
         <v>50</v>
       </c>
-      <c r="G25" s="2">
+      <c r="G25" s="3">
         <f>(E25-$D$2)/A25</f>
         <v>115.125</v>
       </c>
-      <c r="H25" s="2">
+      <c r="H25" s="3">
         <f t="shared" ref="H25" si="10">(E25/D25-1)*100</f>
         <v>0.54866673982223446</v>
       </c>
-      <c r="I25" s="2">
+      <c r="I25" s="3">
         <f t="shared" ref="I25" si="11">(POWER((E25/$D$3),1/A25)-1)*100</f>
         <v>1.5065509612034012</v>
       </c>
@@ -2637,57 +2631,57 @@
         <f t="shared" si="0"/>
         <v>549.15173544274876</v>
       </c>
-      <c r="L25">
+      <c r="L25" s="3">
         <v>0</v>
       </c>
-      <c r="M25" s="4">
+      <c r="M25" s="2">
         <f t="shared" ref="M25" si="12">L25+E25</f>
         <v>9163</v>
       </c>
-      <c r="N25" s="2">
+      <c r="N25" s="3">
         <f t="shared" si="4"/>
         <v>143.171875</v>
       </c>
-      <c r="O25">
+      <c r="O25" s="3">
         <v>87985.1</v>
       </c>
-      <c r="P25">
+      <c r="P25" s="3">
         <v>86736.1</v>
       </c>
-      <c r="Q25">
+      <c r="Q25" s="3">
         <f t="shared" si="8"/>
         <v>97.194304341443697</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A26">
+      <c r="A26" s="3">
         <v>25</v>
       </c>
-      <c r="B26" s="1">
+      <c r="B26" s="3">
         <v>45743</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D26" s="4">
+      <c r="D26" s="2">
         <v>9163</v>
       </c>
-      <c r="E26" s="4">
+      <c r="E26" s="2">
         <v>9353</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="3">
         <f t="shared" ref="F26" si="13">E26-D26</f>
         <v>190</v>
       </c>
-      <c r="G26" s="2">
+      <c r="G26" s="3">
         <f>(E26-$D$2)/A26</f>
         <v>118.12</v>
       </c>
-      <c r="H26" s="2">
+      <c r="H26" s="3">
         <f t="shared" ref="H26" si="14">(E26/D26-1)*100</f>
         <v>2.0735566954054319</v>
       </c>
-      <c r="I26" s="2">
+      <c r="I26" s="3">
         <f t="shared" ref="I26" si="15">(POWER((E26/$D$3),1/A26)-1)*100</f>
         <v>1.5291706005972516</v>
       </c>
@@ -2699,57 +2693,57 @@
         <f t="shared" si="0"/>
         <v>627.17170800350505</v>
       </c>
-      <c r="L26">
+      <c r="L26" s="3">
         <v>0</v>
       </c>
-      <c r="M26" s="4">
+      <c r="M26" s="2">
         <f t="shared" ref="M26" si="16">L26+E26</f>
         <v>9353</v>
       </c>
-      <c r="N26" s="2">
+      <c r="N26" s="3">
         <f t="shared" si="4"/>
         <v>146.140625</v>
       </c>
-      <c r="O26">
+      <c r="O26" s="3">
         <v>86736.1</v>
       </c>
-      <c r="P26">
+      <c r="P26" s="3">
         <v>87249.1</v>
       </c>
-      <c r="Q26">
+      <c r="Q26" s="3">
         <f t="shared" si="8"/>
         <v>97.769159311025689</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A27">
+      <c r="A27" s="3">
         <v>26</v>
       </c>
-      <c r="B27" s="1">
+      <c r="B27" s="3">
         <v>45744</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D27" s="4">
+      <c r="D27" s="2">
         <v>9353</v>
       </c>
-      <c r="E27" s="4">
+      <c r="E27" s="2">
         <v>9353</v>
       </c>
-      <c r="F27">
+      <c r="F27" s="3">
         <f t="shared" ref="F27:F32" si="17">E27-D27</f>
         <v>0</v>
       </c>
-      <c r="G27" s="2">
+      <c r="G27" s="3">
         <f t="shared" ref="G27:G31" si="18">(E27-$D$2)/A27</f>
         <v>113.57692307692308</v>
       </c>
-      <c r="H27" s="2">
+      <c r="H27" s="3">
         <f t="shared" ref="H27:H32" si="19">(E27/D27-1)*100</f>
         <v>0</v>
       </c>
-      <c r="I27" s="2">
+      <c r="I27" s="3">
         <f t="shared" ref="I27:I32" si="20">(POWER((E27/$D$3),1/A27)-1)*100</f>
         <v>1.4699262282590997</v>
       </c>
@@ -2761,57 +2755,57 @@
         <f t="shared" si="0"/>
         <v>513.73594020755081</v>
       </c>
-      <c r="L27">
+      <c r="L27" s="3">
         <v>0</v>
       </c>
-      <c r="M27" s="4">
+      <c r="M27" s="2">
         <f t="shared" ref="M27:M32" si="21">L27+E27</f>
         <v>9353</v>
       </c>
-      <c r="N27" s="2">
+      <c r="N27" s="3">
         <f t="shared" si="4"/>
         <v>146.140625</v>
       </c>
-      <c r="O27">
+      <c r="O27" s="3">
         <v>87249.1</v>
       </c>
-      <c r="P27">
+      <c r="P27" s="3">
         <v>84105.3</v>
       </c>
-      <c r="Q27">
+      <c r="Q27" s="3">
         <f t="shared" si="8"/>
         <v>94.246295659228679</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A28">
+      <c r="A28" s="3">
         <v>27</v>
       </c>
-      <c r="B28" s="1">
+      <c r="B28" s="3">
         <v>45745</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D28" s="4">
+      <c r="D28" s="2">
         <v>9353</v>
       </c>
-      <c r="E28" s="4">
+      <c r="E28" s="2">
         <v>9400</v>
       </c>
-      <c r="F28">
+      <c r="F28" s="3">
         <f t="shared" si="17"/>
         <v>47</v>
       </c>
-      <c r="G28" s="2">
+      <c r="G28" s="3">
         <f t="shared" si="18"/>
         <v>111.11111111111111</v>
       </c>
-      <c r="H28" s="2">
+      <c r="H28" s="3">
         <f t="shared" si="19"/>
         <v>0.50251256281406143</v>
       </c>
-      <c r="I28" s="2">
+      <c r="I28" s="3">
         <f t="shared" si="20"/>
         <v>1.433930583006493</v>
       </c>
@@ -2823,57 +2817,57 @@
         <f t="shared" si="0"/>
         <v>445.82550743025058</v>
       </c>
-      <c r="L28">
+      <c r="L28" s="3">
         <v>0</v>
       </c>
-      <c r="M28" s="4">
+      <c r="M28" s="2">
         <f t="shared" si="21"/>
         <v>9400</v>
       </c>
-      <c r="N28" s="2">
+      <c r="N28" s="3">
         <f t="shared" si="4"/>
         <v>146.875</v>
       </c>
-      <c r="O28">
+      <c r="O28" s="3">
         <v>84105.3</v>
       </c>
-      <c r="P28">
+      <c r="P28" s="3">
         <v>82428.800000000003</v>
       </c>
-      <c r="Q28">
+      <c r="Q28" s="3">
         <f t="shared" si="8"/>
         <v>92.367651689434894</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A29">
+      <c r="A29" s="3">
         <v>28</v>
       </c>
-      <c r="B29" s="1">
+      <c r="B29" s="3">
         <v>45746</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D29" s="4">
+      <c r="D29" s="2">
         <v>9400</v>
       </c>
-      <c r="E29" s="4">
+      <c r="E29" s="2">
         <v>9450</v>
       </c>
-      <c r="F29">
+      <c r="F29" s="3">
         <f t="shared" si="17"/>
         <v>50</v>
       </c>
-      <c r="G29" s="2">
+      <c r="G29" s="3">
         <f t="shared" si="18"/>
         <v>108.92857142857143</v>
       </c>
-      <c r="H29" s="2">
+      <c r="H29" s="3">
         <f t="shared" si="19"/>
         <v>0.53191489361701372</v>
       </c>
-      <c r="I29" s="2">
+      <c r="I29" s="3">
         <f t="shared" si="20"/>
         <v>1.4015768054668865</v>
       </c>
@@ -2885,57 +2879,57 @@
         <f t="shared" si="0"/>
         <v>379.42123902684398</v>
       </c>
-      <c r="L29">
+      <c r="L29" s="3">
         <v>0</v>
       </c>
-      <c r="M29" s="4">
+      <c r="M29" s="2">
         <f t="shared" si="21"/>
         <v>9450</v>
       </c>
-      <c r="N29" s="2">
+      <c r="N29" s="3">
         <f t="shared" si="4"/>
         <v>147.65625</v>
       </c>
-      <c r="O29">
+      <c r="O29" s="3">
         <v>82428.800000000003</v>
       </c>
-      <c r="P29">
+      <c r="P29" s="3">
         <v>82745.100000000006</v>
       </c>
-      <c r="Q29">
+      <c r="Q29" s="3">
         <f t="shared" si="8"/>
         <v>92.72208955859432</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A30">
+      <c r="A30" s="3">
         <v>29</v>
       </c>
-      <c r="B30" s="1">
+      <c r="B30" s="3">
         <v>45747</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D30" s="4">
+      <c r="D30" s="2">
         <v>9450</v>
       </c>
-      <c r="E30" s="4">
+      <c r="E30" s="2">
         <v>9452</v>
       </c>
-      <c r="F30">
+      <c r="F30" s="3">
         <f t="shared" si="17"/>
         <v>2</v>
       </c>
-      <c r="G30" s="2">
+      <c r="G30" s="3">
         <f t="shared" si="18"/>
         <v>105.24137931034483</v>
       </c>
-      <c r="H30" s="2">
+      <c r="H30" s="3">
         <f t="shared" si="19"/>
         <v>2.1164021164010727E-2</v>
       </c>
-      <c r="I30" s="2">
+      <c r="I30" s="3">
         <f t="shared" si="20"/>
         <v>1.3536607182727423</v>
       </c>
@@ -2947,57 +2941,57 @@
         <f t="shared" si="0"/>
         <v>263.50371513419304</v>
       </c>
-      <c r="L30">
+      <c r="L30" s="3">
         <v>0</v>
       </c>
-      <c r="M30" s="4">
+      <c r="M30" s="2">
         <f t="shared" si="21"/>
         <v>9452</v>
       </c>
-      <c r="N30" s="2">
+      <c r="N30" s="3">
         <f t="shared" si="4"/>
         <v>147.6875</v>
       </c>
-      <c r="O30">
+      <c r="O30" s="3">
         <v>82745.100000000006</v>
       </c>
-      <c r="P30">
+      <c r="P30" s="3">
         <v>83448.100000000006</v>
       </c>
-      <c r="Q30">
+      <c r="Q30" s="3">
         <f t="shared" si="8"/>
         <v>93.509853776169635</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A31">
+      <c r="A31" s="3">
         <v>30</v>
       </c>
-      <c r="B31" s="1">
+      <c r="B31" s="3">
         <v>45748</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D31" s="4">
+      <c r="D31" s="2">
         <v>9452</v>
       </c>
-      <c r="E31" s="4">
+      <c r="E31" s="2">
         <v>9512</v>
       </c>
-      <c r="F31">
+      <c r="F31" s="3">
         <f t="shared" si="17"/>
         <v>60</v>
       </c>
-      <c r="G31" s="2">
+      <c r="G31" s="3">
         <f t="shared" si="18"/>
         <v>103.73333333333333</v>
       </c>
-      <c r="H31" s="2">
+      <c r="H31" s="3">
         <f t="shared" si="19"/>
         <v>0.6347862886161737</v>
       </c>
-      <c r="I31" s="2">
+      <c r="I31" s="3">
         <f t="shared" si="20"/>
         <v>1.3296157062268277</v>
       </c>
@@ -3009,57 +3003,57 @@
         <f t="shared" si="0"/>
         <v>204.05326343093839</v>
       </c>
-      <c r="L31">
+      <c r="L31" s="3">
         <v>0</v>
       </c>
-      <c r="M31" s="4">
+      <c r="M31" s="2">
         <f t="shared" si="21"/>
         <v>9512</v>
       </c>
-      <c r="N31" s="2">
+      <c r="N31" s="3">
         <f t="shared" si="4"/>
         <v>148.625</v>
       </c>
-      <c r="O31">
+      <c r="O31" s="3">
         <v>83448.100000000006</v>
       </c>
-      <c r="P31">
+      <c r="P31" s="3">
         <v>84138.9</v>
       </c>
-      <c r="Q31">
+      <c r="Q31" s="3">
         <f t="shared" si="8"/>
         <v>94.2839469788738</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A32">
+      <c r="A32" s="3">
         <v>31</v>
       </c>
-      <c r="B32" s="1">
+      <c r="B32" s="3">
         <v>45749</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D32" s="4">
+      <c r="D32" s="2">
         <v>9512</v>
       </c>
-      <c r="E32" s="4">
+      <c r="E32" s="2">
         <v>9666</v>
       </c>
-      <c r="F32">
+      <c r="F32" s="3">
         <f t="shared" si="17"/>
         <v>154</v>
       </c>
-      <c r="G32" s="2">
+      <c r="G32" s="3">
         <f>(E32-$D$2)/A32</f>
         <v>105.35483870967742</v>
       </c>
-      <c r="H32" s="2">
+      <c r="H32" s="3">
         <f t="shared" si="19"/>
         <v>1.619007569386044</v>
       </c>
-      <c r="I32" s="2">
+      <c r="I32" s="3">
         <f t="shared" si="20"/>
         <v>1.3389380513060933</v>
       </c>
@@ -3071,57 +3065,57 @@
         <f t="shared" si="0"/>
         <v>237.04995585554207</v>
       </c>
-      <c r="L32">
+      <c r="L32" s="3">
         <v>0</v>
       </c>
-      <c r="M32" s="4">
+      <c r="M32" s="2">
         <f t="shared" si="21"/>
         <v>9666</v>
       </c>
-      <c r="N32" s="2">
+      <c r="N32" s="3">
         <f t="shared" si="4"/>
         <v>151.03125</v>
       </c>
-      <c r="O32">
+      <c r="O32" s="3">
         <v>84138.9</v>
       </c>
-      <c r="P32">
+      <c r="P32" s="3">
         <v>85827.9</v>
       </c>
-      <c r="Q32">
+      <c r="Q32" s="3">
         <f t="shared" si="8"/>
         <v>96.176598136035565</v>
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A33">
+      <c r="A33" s="3">
         <v>32</v>
       </c>
-      <c r="B33" s="1">
+      <c r="B33" s="3">
         <v>45750</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D33" s="4">
+      <c r="D33" s="2">
         <v>9666</v>
       </c>
-      <c r="E33" s="4">
+      <c r="E33" s="2">
         <v>9890</v>
       </c>
-      <c r="F33">
+      <c r="F33" s="3">
         <f t="shared" ref="F33:F41" si="22">E33-D33</f>
         <v>224</v>
       </c>
-      <c r="G33" s="2">
+      <c r="G33" s="3">
         <f t="shared" ref="G33:G41" si="23">(E33-$D$2)/A33</f>
         <v>109.0625</v>
       </c>
-      <c r="H33" s="2">
+      <c r="H33" s="3">
         <f t="shared" ref="H33:H41" si="24">(E33/D33-1)*100</f>
         <v>2.3174012000827693</v>
       </c>
-      <c r="I33" s="2">
+      <c r="I33" s="3">
         <f t="shared" ref="I33:I41" si="25">(POWER((E33/$D$3),1/A33)-1)*100</f>
         <v>1.3693729216394335</v>
       </c>
@@ -3133,57 +3127,57 @@
         <f t="shared" si="0"/>
         <v>338.47360528166428</v>
       </c>
-      <c r="L33">
+      <c r="L33" s="3">
         <v>0</v>
       </c>
-      <c r="M33" s="4">
+      <c r="M33" s="2">
         <f t="shared" ref="M33:M41" si="26">L33+E33</f>
         <v>9890</v>
       </c>
-      <c r="N33" s="2">
+      <c r="N33" s="3">
         <f t="shared" si="4"/>
         <v>154.53125</v>
       </c>
-      <c r="O33">
+      <c r="O33" s="3">
         <v>85827.9</v>
       </c>
-      <c r="P33">
+      <c r="P33" s="3">
         <v>81465.600000000006</v>
       </c>
-      <c r="Q33">
+      <c r="Q33" s="3">
         <f t="shared" si="8"/>
         <v>91.288313859607655</v>
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A34">
+      <c r="A34" s="3">
         <v>33</v>
       </c>
-      <c r="B34" s="1">
+      <c r="B34" s="3">
         <v>45751</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D34" s="4">
+      <c r="D34" s="2">
         <v>9890</v>
       </c>
-      <c r="E34" s="4">
+      <c r="E34" s="2">
         <v>10200</v>
       </c>
-      <c r="F34">
+      <c r="F34" s="3">
         <f t="shared" si="22"/>
         <v>310</v>
       </c>
-      <c r="G34" s="2">
+      <c r="G34" s="3">
         <f t="shared" si="23"/>
         <v>115.15151515151516</v>
       </c>
-      <c r="H34" s="2">
+      <c r="H34" s="3">
         <f t="shared" si="24"/>
         <v>3.1344792719919079</v>
       </c>
-      <c r="I34" s="2">
+      <c r="I34" s="3">
         <f t="shared" si="25"/>
         <v>1.4224145175464553</v>
       </c>
@@ -3195,57 +3189,57 @@
         <f t="shared" si="0"/>
         <v>524.30376215032629</v>
       </c>
-      <c r="L34">
+      <c r="L34" s="3">
         <v>0</v>
       </c>
-      <c r="M34" s="4">
+      <c r="M34" s="2">
         <f t="shared" si="26"/>
         <v>10200</v>
       </c>
-      <c r="N34" s="2">
+      <c r="N34" s="3">
         <f t="shared" si="4"/>
         <v>159.375</v>
       </c>
-      <c r="O34">
+      <c r="O34" s="3">
         <v>81465.600000000006</v>
       </c>
-      <c r="P34">
+      <c r="P34" s="3">
         <v>82498</v>
       </c>
-      <c r="Q34">
+      <c r="Q34" s="3">
         <f t="shared" si="8"/>
         <v>92.445195478704036</v>
       </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A35">
+      <c r="A35" s="3">
         <v>34</v>
       </c>
-      <c r="B35" s="1">
+      <c r="B35" s="3">
         <v>45752</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D35" s="4">
+      <c r="D35" s="2">
         <v>10200</v>
       </c>
-      <c r="E35" s="4">
+      <c r="E35" s="2">
         <v>10565</v>
       </c>
-      <c r="F35">
+      <c r="F35" s="3">
         <f t="shared" si="22"/>
         <v>365</v>
       </c>
-      <c r="G35" s="2">
+      <c r="G35" s="3">
         <f t="shared" si="23"/>
         <v>122.5</v>
       </c>
-      <c r="H35" s="2">
+      <c r="H35" s="3">
         <f t="shared" si="24"/>
         <v>3.5784313725490291</v>
       </c>
-      <c r="I35" s="2">
+      <c r="I35" s="3">
         <f t="shared" si="25"/>
         <v>1.4851815919634914</v>
       </c>
@@ -3257,57 +3251,57 @@
         <f t="shared" si="0"/>
         <v>763.51971105828125</v>
       </c>
-      <c r="L35">
+      <c r="L35" s="3">
         <v>0</v>
       </c>
-      <c r="M35" s="4">
+      <c r="M35" s="2">
         <f t="shared" si="26"/>
         <v>10565</v>
       </c>
-      <c r="N35" s="2">
+      <c r="N35" s="3">
         <f t="shared" si="4"/>
         <v>165.078125</v>
       </c>
-      <c r="O35">
+      <c r="O35" s="3">
         <v>82498</v>
       </c>
-      <c r="P35">
+      <c r="P35" s="3">
         <v>82847.899999999994</v>
       </c>
-      <c r="Q35">
+      <c r="Q35" s="3">
         <f t="shared" si="8"/>
         <v>92.837284667508584</v>
       </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A36">
+      <c r="A36" s="3">
         <v>35</v>
       </c>
-      <c r="B36" s="1">
+      <c r="B36" s="3">
         <v>45753</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D36" s="4">
+      <c r="D36" s="2">
         <v>10565</v>
       </c>
-      <c r="E36" s="4">
+      <c r="E36" s="2">
         <v>10845</v>
       </c>
-      <c r="F36">
+      <c r="F36" s="3">
         <f t="shared" si="22"/>
         <v>280</v>
       </c>
-      <c r="G36" s="2">
+      <c r="G36" s="3">
         <f t="shared" si="23"/>
         <v>127</v>
       </c>
-      <c r="H36" s="2">
+      <c r="H36" s="3">
         <f t="shared" si="24"/>
         <v>2.6502602934216801</v>
       </c>
-      <c r="I36" s="2">
+      <c r="I36" s="3">
         <f t="shared" si="25"/>
         <v>1.5182853250945039</v>
       </c>
@@ -3319,57 +3313,57 @@
         <f t="shared" si="0"/>
         <v>916.10046730203976</v>
       </c>
-      <c r="L36">
+      <c r="L36" s="3">
         <v>0</v>
       </c>
-      <c r="M36" s="4">
+      <c r="M36" s="2">
         <f t="shared" si="26"/>
         <v>10845</v>
       </c>
-      <c r="N36" s="2">
+      <c r="N36" s="3">
         <f t="shared" si="4"/>
         <v>169.453125</v>
       </c>
-      <c r="O36">
+      <c r="O36" s="3">
         <v>82847.899999999994</v>
       </c>
-      <c r="P36">
+      <c r="P36" s="3">
         <v>82606.7</v>
       </c>
-      <c r="Q36">
+      <c r="Q36" s="3">
         <f t="shared" si="8"/>
         <v>92.567001980056006</v>
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A37">
+      <c r="A37" s="3">
         <v>36</v>
       </c>
-      <c r="B37" s="1">
+      <c r="B37" s="3">
         <v>45754</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D37" s="4">
+      <c r="D37" s="2">
         <v>20845</v>
       </c>
-      <c r="E37" s="4">
+      <c r="E37" s="2">
         <v>22699</v>
       </c>
-      <c r="F37">
+      <c r="F37" s="3">
         <f t="shared" si="22"/>
         <v>1854</v>
       </c>
-      <c r="G37" s="2">
+      <c r="G37" s="3">
         <f t="shared" si="23"/>
         <v>452.75</v>
       </c>
-      <c r="H37" s="2">
+      <c r="H37" s="3">
         <f t="shared" si="24"/>
         <v>8.8942192372271514</v>
       </c>
-      <c r="I37" s="2">
+      <c r="I37" s="3">
         <f t="shared" si="25"/>
         <v>3.5792984780890658</v>
       </c>
@@ -3381,57 +3375,57 @@
         <f>M37-J37</f>
         <v>2641.0247733769666</v>
       </c>
-      <c r="L37">
+      <c r="L37" s="3">
         <v>-10000</v>
       </c>
-      <c r="M37" s="4">
+      <c r="M37" s="2">
         <f t="shared" si="26"/>
         <v>12699</v>
       </c>
-      <c r="N37" s="2">
+      <c r="N37" s="3">
         <f t="shared" si="4"/>
         <v>198.421875</v>
       </c>
-      <c r="O37">
+      <c r="O37" s="3">
         <v>82606.7</v>
       </c>
-      <c r="P37">
+      <c r="P37" s="3">
         <v>78951.899999999994</v>
       </c>
-      <c r="Q37">
+      <c r="Q37" s="3">
         <f t="shared" si="8"/>
         <v>88.471524508655889</v>
       </c>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A38">
+      <c r="A38" s="3">
         <v>37</v>
       </c>
-      <c r="B38" s="1">
+      <c r="B38" s="3">
         <v>45755</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D38" s="4">
+      <c r="D38" s="2">
         <v>22699</v>
       </c>
-      <c r="E38" s="4">
+      <c r="E38" s="2">
         <v>22955</v>
       </c>
-      <c r="F38">
+      <c r="F38" s="3">
         <f t="shared" si="22"/>
         <v>256</v>
       </c>
-      <c r="G38" s="2">
+      <c r="G38" s="3">
         <f t="shared" si="23"/>
         <v>447.43243243243245</v>
       </c>
-      <c r="H38" s="2">
+      <c r="H38" s="3">
         <f t="shared" si="24"/>
         <v>1.1278029869157269</v>
       </c>
-      <c r="I38" s="2">
+      <c r="I38" s="3">
         <f t="shared" si="25"/>
         <v>3.5122668721563333</v>
       </c>
@@ -3443,57 +3437,57 @@
         <f t="shared" ref="K38:K41" si="27">M38-J38</f>
         <v>2766.2710954308677</v>
       </c>
-      <c r="L38">
+      <c r="L38" s="3">
         <v>-10000</v>
       </c>
-      <c r="M38" s="4">
+      <c r="M38" s="2">
         <f t="shared" si="26"/>
         <v>12955</v>
       </c>
-      <c r="N38" s="2">
+      <c r="N38" s="3">
         <f t="shared" si="4"/>
         <v>202.42187500000003</v>
       </c>
-      <c r="O38">
+      <c r="O38" s="3">
         <v>78951.899999999994</v>
       </c>
-      <c r="P38">
+      <c r="P38" s="3">
         <v>78410.600000000006</v>
       </c>
-      <c r="Q38">
+      <c r="Q38" s="3">
         <f t="shared" si="8"/>
         <v>87.864957266872793</v>
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A39">
+      <c r="A39" s="3">
         <v>38</v>
       </c>
-      <c r="B39" s="1">
+      <c r="B39" s="3">
         <v>45756</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C39" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D39" s="4">
+      <c r="D39" s="2">
         <v>22955</v>
       </c>
-      <c r="E39" s="4">
+      <c r="E39" s="2">
         <v>24388</v>
       </c>
-      <c r="F39">
+      <c r="F39" s="3">
         <f t="shared" si="22"/>
         <v>1433</v>
       </c>
-      <c r="G39" s="2">
+      <c r="G39" s="3">
         <f t="shared" si="23"/>
         <v>473.36842105263156</v>
       </c>
-      <c r="H39" s="2">
+      <c r="H39" s="3">
         <f t="shared" si="24"/>
         <v>6.2426486604225673</v>
       </c>
-      <c r="I39" s="2">
+      <c r="I39" s="3">
         <f t="shared" si="25"/>
         <v>3.5832120312270677</v>
       </c>
@@ -3505,57 +3499,57 @@
         <f t="shared" si="27"/>
         <v>4066.8176196714703</v>
       </c>
-      <c r="L39">
+      <c r="L39" s="3">
         <v>-10000</v>
       </c>
-      <c r="M39" s="4">
+      <c r="M39" s="2">
         <f t="shared" si="26"/>
         <v>14388</v>
       </c>
-      <c r="N39" s="2">
+      <c r="N39" s="3">
         <f t="shared" si="4"/>
         <v>224.8125</v>
       </c>
-      <c r="O39">
+      <c r="O39" s="3">
         <v>78410.600000000006</v>
       </c>
-      <c r="P39">
+      <c r="P39" s="3">
         <v>76791.100000000006</v>
       </c>
-      <c r="Q39">
+      <c r="Q39" s="3">
         <f t="shared" si="8"/>
         <v>86.050186071477015</v>
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A40">
+      <c r="A40" s="3">
         <v>39</v>
       </c>
-      <c r="B40" s="1">
+      <c r="B40" s="3">
         <v>45757</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C40" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D40" s="4">
+      <c r="D40" s="2">
         <v>24388</v>
       </c>
-      <c r="E40" s="4">
+      <c r="E40" s="2">
         <v>24713</v>
       </c>
-      <c r="F40">
+      <c r="F40" s="3">
         <f t="shared" si="22"/>
         <v>325</v>
       </c>
-      <c r="G40" s="2">
+      <c r="G40" s="3">
         <f t="shared" si="23"/>
         <v>469.56410256410254</v>
       </c>
-      <c r="H40" s="2">
+      <c r="H40" s="3">
         <f t="shared" si="24"/>
         <v>1.3326226012793096</v>
       </c>
-      <c r="I40" s="2">
+      <c r="I40" s="3">
         <f t="shared" si="25"/>
         <v>3.5248848916893172</v>
       </c>
@@ -3567,57 +3561,57 @@
         <f t="shared" si="27"/>
         <v>4257.6422487272011</v>
       </c>
-      <c r="L40">
+      <c r="L40" s="3">
         <v>-10000</v>
       </c>
-      <c r="M40" s="4">
+      <c r="M40" s="2">
         <f t="shared" si="26"/>
         <v>14713</v>
       </c>
-      <c r="N40" s="2">
+      <c r="N40" s="3">
         <f t="shared" si="4"/>
         <v>229.890625</v>
       </c>
-      <c r="O40">
+      <c r="O40" s="3">
         <v>76791.100000000006</v>
       </c>
-      <c r="P40">
+      <c r="P40" s="3">
         <v>81192.2</v>
       </c>
-      <c r="Q40">
+      <c r="Q40" s="3">
         <f t="shared" si="8"/>
         <v>90.981948657495138</v>
       </c>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A41">
+      <c r="A41" s="3">
         <v>40</v>
       </c>
-      <c r="B41" s="1">
+      <c r="B41" s="3">
         <v>45758</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C41" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D41" s="4">
+      <c r="D41" s="2">
         <v>24713</v>
       </c>
-      <c r="E41" s="4">
+      <c r="E41" s="2">
         <v>25029</v>
       </c>
-      <c r="F41">
+      <c r="F41" s="3">
         <f t="shared" si="22"/>
         <v>316</v>
       </c>
-      <c r="G41" s="2">
+      <c r="G41" s="3">
         <f t="shared" si="23"/>
         <v>465.72500000000002</v>
       </c>
-      <c r="H41" s="2">
+      <c r="H41" s="3">
         <f t="shared" si="24"/>
         <v>1.2786792376481948</v>
       </c>
-      <c r="I41" s="2">
+      <c r="I41" s="3">
         <f t="shared" si="25"/>
         <v>3.4681271506401101</v>
       </c>
@@ -3629,57 +3623,57 @@
         <f t="shared" si="27"/>
         <v>4437.7225979606555</v>
       </c>
-      <c r="L41">
+      <c r="L41" s="3">
         <v>-10000</v>
       </c>
-      <c r="M41" s="4">
+      <c r="M41" s="2">
         <f t="shared" si="26"/>
         <v>15029</v>
       </c>
-      <c r="N41" s="2">
+      <c r="N41" s="3">
         <f t="shared" si="4"/>
         <v>234.828125</v>
       </c>
-      <c r="O41">
+      <c r="O41" s="3">
         <v>81192.2</v>
       </c>
-      <c r="P41">
+      <c r="P41" s="3">
         <v>81812</v>
       </c>
-      <c r="Q41">
+      <c r="Q41" s="3">
         <f t="shared" si="8"/>
         <v>91.67648103594918</v>
       </c>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A42">
+      <c r="A42" s="3">
         <v>41</v>
       </c>
-      <c r="B42" s="1">
+      <c r="B42" s="3">
         <v>45759</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C42" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D42" s="4">
+      <c r="D42" s="2">
         <v>25029</v>
       </c>
-      <c r="E42" s="4">
+      <c r="E42" s="2">
         <v>25088</v>
       </c>
-      <c r="F42">
+      <c r="F42" s="3">
         <f t="shared" ref="F42:F46" si="28">E42-D42</f>
         <v>59</v>
       </c>
-      <c r="G42" s="2">
+      <c r="G42" s="3">
         <f t="shared" ref="G42:G46" si="29">(E42-$D$2)/A42</f>
         <v>455.80487804878049</v>
       </c>
-      <c r="H42" s="2">
+      <c r="H42" s="3">
         <f t="shared" ref="H42:H46" si="30">(E42/D42-1)*100</f>
         <v>0.23572655719366065</v>
       </c>
-      <c r="I42" s="2">
+      <c r="I42" s="3">
         <f t="shared" ref="I42:I46" si="31">(POWER((E42/$D$3),1/A42)-1)*100</f>
         <v>3.3880613542311755</v>
       </c>
@@ -3691,57 +3685,57 @@
         <f t="shared" ref="K42:K46" si="32">M42-J42</f>
         <v>4359.0359917341448</v>
       </c>
-      <c r="L42">
+      <c r="L42" s="3">
         <v>-10000</v>
       </c>
-      <c r="M42" s="4">
+      <c r="M42" s="2">
         <f t="shared" ref="M42:M46" si="33">L42+E42</f>
         <v>15088</v>
       </c>
-      <c r="N42" s="2">
+      <c r="N42" s="3">
         <f t="shared" ref="N42:N46" si="34">M42/$D$2*100</f>
         <v>235.75</v>
       </c>
-      <c r="O42">
+      <c r="O42" s="3">
         <v>81812</v>
       </c>
-      <c r="P42">
+      <c r="P42" s="3">
         <v>84763.1</v>
       </c>
-      <c r="Q42">
+      <c r="Q42" s="3">
         <f t="shared" ref="Q42:Q46" si="35">P42/$O$2*100</f>
         <v>94.983409887281383</v>
       </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A43">
+      <c r="A43" s="3">
         <v>42</v>
       </c>
-      <c r="B43" s="1">
+      <c r="B43" s="3">
         <v>45760</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C43" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D43" s="4">
+      <c r="D43" s="2">
         <v>25088</v>
       </c>
-      <c r="E43" s="4">
+      <c r="E43" s="2">
         <v>25195</v>
       </c>
-      <c r="F43">
+      <c r="F43" s="3">
         <f t="shared" si="28"/>
         <v>107</v>
       </c>
-      <c r="G43" s="2">
+      <c r="G43" s="3">
         <f t="shared" si="29"/>
         <v>447.5</v>
       </c>
-      <c r="H43" s="2">
+      <c r="H43" s="3">
         <f t="shared" si="30"/>
         <v>0.42649872448978776</v>
       </c>
-      <c r="I43" s="2">
+      <c r="I43" s="3">
         <f t="shared" si="31"/>
         <v>3.3165430633898429</v>
       </c>
@@ -3753,57 +3747,57 @@
         <f t="shared" si="32"/>
         <v>4326.5594596266892</v>
       </c>
-      <c r="L43">
+      <c r="L43" s="3">
         <v>-10000</v>
       </c>
-      <c r="M43" s="4">
+      <c r="M43" s="2">
         <f t="shared" si="33"/>
         <v>15195</v>
       </c>
-      <c r="N43" s="2">
+      <c r="N43" s="3">
         <f t="shared" si="34"/>
         <v>237.42187499999997</v>
       </c>
-      <c r="O43">
+      <c r="O43" s="3">
         <v>84763.1</v>
       </c>
-      <c r="P43">
+      <c r="P43" s="3">
         <v>84024</v>
       </c>
-      <c r="Q43">
+      <c r="Q43" s="3">
         <f t="shared" si="35"/>
         <v>94.15519291258731</v>
       </c>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A44">
+      <c r="A44" s="3">
         <v>43</v>
       </c>
-      <c r="B44" s="1">
+      <c r="B44" s="3">
         <v>45761</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C44" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D44" s="4">
+      <c r="D44" s="2">
         <v>25195</v>
       </c>
-      <c r="E44" s="4">
+      <c r="E44" s="2">
         <v>25835</v>
       </c>
-      <c r="F44">
+      <c r="F44" s="3">
         <f t="shared" si="28"/>
         <v>640</v>
       </c>
-      <c r="G44" s="2">
+      <c r="G44" s="3">
         <f t="shared" si="29"/>
         <v>451.97674418604652</v>
       </c>
-      <c r="H44" s="2">
+      <c r="H44" s="3">
         <f t="shared" si="30"/>
         <v>2.5401865449493854</v>
       </c>
-      <c r="I44" s="2">
+      <c r="I44" s="3">
         <f t="shared" si="31"/>
         <v>3.2984216732465654</v>
       </c>
@@ -3815,57 +3809,57 @@
         <f t="shared" si="32"/>
         <v>4825.2697326018369</v>
       </c>
-      <c r="L44">
+      <c r="L44" s="3">
         <v>-10000</v>
       </c>
-      <c r="M44" s="4">
+      <c r="M44" s="2">
         <f t="shared" si="33"/>
         <v>15835</v>
       </c>
-      <c r="N44" s="2">
+      <c r="N44" s="3">
         <f t="shared" si="34"/>
         <v>247.421875</v>
       </c>
-      <c r="O44">
+      <c r="O44" s="3">
         <v>84024</v>
       </c>
-      <c r="P44">
+      <c r="P44" s="3">
         <v>85364.7</v>
       </c>
-      <c r="Q44">
+      <c r="Q44" s="3">
         <f t="shared" si="35"/>
         <v>95.657547800927617</v>
       </c>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A45">
+      <c r="A45" s="3">
         <v>44</v>
       </c>
-      <c r="B45" s="1">
+      <c r="B45" s="3">
         <v>45762</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C45" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D45" s="4">
+      <c r="D45" s="2">
         <v>25835</v>
       </c>
-      <c r="E45" s="4">
+      <c r="E45" s="2">
         <v>25600</v>
       </c>
-      <c r="F45">
+      <c r="F45" s="3">
         <f t="shared" si="28"/>
         <v>-235</v>
       </c>
-      <c r="G45" s="2">
+      <c r="G45" s="3">
         <f t="shared" si="29"/>
         <v>436.36363636363637</v>
       </c>
-      <c r="H45" s="2">
+      <c r="H45" s="3">
         <f t="shared" si="30"/>
         <v>-0.90961873427520823</v>
       </c>
-      <c r="I45" s="2">
+      <c r="I45" s="3">
         <f t="shared" si="31"/>
         <v>3.200827973420961</v>
       </c>
@@ -3877,57 +3871,57 @@
         <f t="shared" si="32"/>
         <v>4447.1432391256621</v>
       </c>
-      <c r="L45">
+      <c r="L45" s="3">
         <v>-10000</v>
       </c>
-      <c r="M45" s="4">
+      <c r="M45" s="2">
         <f t="shared" si="33"/>
         <v>15600</v>
       </c>
-      <c r="N45" s="2">
+      <c r="N45" s="3">
         <f t="shared" si="34"/>
         <v>243.75</v>
       </c>
-      <c r="O45">
+      <c r="O45" s="3">
         <v>85364.7</v>
       </c>
-      <c r="P45">
+      <c r="P45" s="3">
         <v>85100.2</v>
       </c>
-      <c r="Q45">
+      <c r="Q45" s="3">
         <f t="shared" si="35"/>
         <v>95.36115571622112</v>
       </c>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A46">
+      <c r="A46" s="3">
         <v>45</v>
       </c>
-      <c r="B46" s="1">
+      <c r="B46" s="3">
         <v>45763</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C46" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D46" s="4">
+      <c r="D46" s="2">
         <v>25600</v>
       </c>
-      <c r="E46" s="4">
+      <c r="E46" s="2">
         <v>26102</v>
       </c>
-      <c r="F46">
+      <c r="F46" s="3">
         <f t="shared" si="28"/>
         <v>502</v>
       </c>
-      <c r="G46" s="2">
+      <c r="G46" s="3">
         <f t="shared" si="29"/>
         <v>437.82222222222219</v>
       </c>
-      <c r="H46" s="2">
+      <c r="H46" s="3">
         <f t="shared" si="30"/>
         <v>1.9609374999999929</v>
       </c>
-      <c r="I46" s="2">
+      <c r="I46" s="3">
         <f t="shared" si="31"/>
         <v>3.1731117201337034</v>
       </c>
@@ -3939,57 +3933,57 @@
         <f t="shared" si="32"/>
         <v>4804.1561012342972</v>
       </c>
-      <c r="L46">
+      <c r="L46" s="3">
         <v>-10000</v>
       </c>
-      <c r="M46" s="4">
+      <c r="M46" s="2">
         <f t="shared" si="33"/>
         <v>16102</v>
       </c>
-      <c r="N46" s="2">
+      <c r="N46" s="3">
         <f t="shared" si="34"/>
         <v>251.59375000000003</v>
       </c>
-      <c r="O46">
+      <c r="O46" s="3">
         <v>85100.2</v>
       </c>
-      <c r="P46">
+      <c r="P46" s="3">
         <v>84562.7</v>
       </c>
-      <c r="Q46">
+      <c r="Q46" s="3">
         <f t="shared" si="35"/>
         <v>94.758846659397875</v>
       </c>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A47">
+      <c r="A47" s="3">
         <v>46</v>
       </c>
-      <c r="B47" s="1">
+      <c r="B47" s="3">
         <v>45764</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C47" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D47" s="4">
+      <c r="D47" s="2">
         <v>46802</v>
       </c>
-      <c r="E47" s="4">
+      <c r="E47" s="2">
         <v>47035</v>
       </c>
-      <c r="F47">
+      <c r="F47" s="3">
         <f t="shared" ref="F47:F62" si="36">E47-D47</f>
         <v>233</v>
       </c>
-      <c r="G47" s="2">
+      <c r="G47" s="3">
         <f t="shared" ref="G47:G62" si="37">(E47-$D$2)/A47</f>
         <v>883.36956521739125</v>
       </c>
-      <c r="H47" s="2">
+      <c r="H47" s="3">
         <f t="shared" ref="H47:H62" si="38">(E47/D47-1)*100</f>
         <v>0.49784197256528273</v>
       </c>
-      <c r="I47" s="2">
+      <c r="I47" s="3">
         <f t="shared" ref="I47:I62" si="39">(POWER((E47/$D$3),1/A47)-1)*100</f>
         <v>4.4314552374297156</v>
       </c>
@@ -4001,58 +3995,58 @@
         <f t="shared" ref="K47:K62" si="40">M47-J47</f>
         <v>4891.2841305503443</v>
       </c>
-      <c r="L47">
+      <c r="L47" s="3">
         <f>-9999-20700</f>
         <v>-30699</v>
       </c>
-      <c r="M47" s="4">
+      <c r="M47" s="2">
         <f t="shared" ref="M47:M62" si="41">L47+E47</f>
         <v>16336</v>
       </c>
-      <c r="N47" s="2">
+      <c r="N47" s="3">
         <f t="shared" ref="N47:N62" si="42">M47/$D$2*100</f>
         <v>255.25000000000003</v>
       </c>
-      <c r="O47">
+      <c r="O47" s="3">
         <v>84562.7</v>
       </c>
-      <c r="P47">
+      <c r="P47" s="3">
         <v>84046</v>
       </c>
-      <c r="Q47">
+      <c r="Q47" s="3">
         <f t="shared" ref="Q47:Q62" si="43">P47/$O$2*100</f>
         <v>94.179845562354956</v>
       </c>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A48">
+      <c r="A48" s="3">
         <v>47</v>
       </c>
-      <c r="B48" s="1">
+      <c r="B48" s="3">
         <v>45765</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C48" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D48" s="4">
+      <c r="D48" s="2">
         <v>47035</v>
       </c>
-      <c r="E48" s="4">
+      <c r="E48" s="2">
         <v>47070</v>
       </c>
-      <c r="F48">
+      <c r="F48" s="3">
         <f t="shared" si="36"/>
         <v>35</v>
       </c>
-      <c r="G48" s="2">
+      <c r="G48" s="3">
         <f t="shared" si="37"/>
         <v>865.31914893617022</v>
       </c>
-      <c r="H48" s="2">
+      <c r="H48" s="3">
         <f t="shared" si="38"/>
         <v>7.4412671414902931E-2</v>
       </c>
-      <c r="I48" s="2">
+      <c r="I48" s="3">
         <f t="shared" si="39"/>
         <v>4.3368057343146749</v>
       </c>
@@ -4064,58 +4058,58 @@
         <f t="shared" si="40"/>
         <v>4777.5028242475</v>
       </c>
-      <c r="L48">
+      <c r="L48" s="3">
         <f>L47</f>
         <v>-30699</v>
       </c>
-      <c r="M48" s="4">
+      <c r="M48" s="2">
         <f t="shared" si="41"/>
         <v>16371</v>
       </c>
-      <c r="N48" s="2">
+      <c r="N48" s="3">
         <f t="shared" si="42"/>
         <v>255.796875</v>
       </c>
-      <c r="O48">
+      <c r="O48" s="3">
         <v>84046</v>
       </c>
-      <c r="P48">
+      <c r="P48" s="3">
         <v>84534</v>
       </c>
-      <c r="Q48">
+      <c r="Q48" s="3">
         <f t="shared" si="43"/>
         <v>94.726686157200987</v>
       </c>
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A49">
+      <c r="A49" s="3">
         <v>48</v>
       </c>
-      <c r="B49" s="1">
+      <c r="B49" s="3">
         <v>45766</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C49" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D49" s="4">
+      <c r="D49" s="2">
         <v>47070</v>
       </c>
-      <c r="E49" s="4">
+      <c r="E49" s="2">
         <v>47160</v>
       </c>
-      <c r="F49">
+      <c r="F49" s="3">
         <f t="shared" si="36"/>
         <v>90</v>
       </c>
-      <c r="G49" s="2">
+      <c r="G49" s="3">
         <f t="shared" si="37"/>
         <v>849.16666666666663</v>
       </c>
-      <c r="H49" s="2">
+      <c r="H49" s="3">
         <f t="shared" si="38"/>
         <v>0.19120458891013214</v>
       </c>
-      <c r="I49" s="2">
+      <c r="I49" s="3">
         <f t="shared" si="39"/>
         <v>4.2487136066875042</v>
       </c>
@@ -4127,58 +4121,58 @@
         <f t="shared" si="40"/>
         <v>4716.7873609627186</v>
       </c>
-      <c r="L49">
+      <c r="L49" s="3">
         <f t="shared" ref="L49:L62" si="44">L48</f>
         <v>-30699</v>
       </c>
-      <c r="M49" s="4">
+      <c r="M49" s="2">
         <f t="shared" si="41"/>
         <v>16461</v>
       </c>
-      <c r="N49" s="2">
+      <c r="N49" s="3">
         <f t="shared" si="42"/>
         <v>257.203125</v>
       </c>
-      <c r="O49">
+      <c r="O49" s="3">
         <v>84534</v>
       </c>
-      <c r="P49">
+      <c r="P49" s="3">
         <v>85355</v>
       </c>
-      <c r="Q49">
+      <c r="Q49" s="3">
         <f t="shared" si="43"/>
         <v>95.646678223530074</v>
       </c>
     </row>
     <row r="50" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A50">
+      <c r="A50" s="3">
         <v>49</v>
       </c>
-      <c r="B50" s="1">
+      <c r="B50" s="3">
         <v>45767</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C50" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D50" s="4">
+      <c r="D50" s="2">
         <v>47160</v>
       </c>
-      <c r="E50" s="4">
+      <c r="E50" s="2">
         <v>47420</v>
       </c>
-      <c r="F50">
+      <c r="F50" s="3">
         <f t="shared" si="36"/>
         <v>260</v>
       </c>
-      <c r="G50" s="2">
+      <c r="G50" s="3">
         <f t="shared" si="37"/>
         <v>837.14285714285711</v>
       </c>
-      <c r="H50" s="2">
+      <c r="H50" s="3">
         <f t="shared" si="38"/>
         <v>0.55131467345208574</v>
       </c>
-      <c r="I50" s="2">
+      <c r="I50" s="3">
         <f t="shared" si="39"/>
         <v>4.1719141601861187</v>
       </c>
@@ -4190,58 +4184,58 @@
         <f t="shared" si="40"/>
         <v>4824.1125966552354</v>
       </c>
-      <c r="L50">
+      <c r="L50" s="3">
         <f t="shared" si="44"/>
         <v>-30699</v>
       </c>
-      <c r="M50" s="4">
+      <c r="M50" s="2">
         <f t="shared" si="41"/>
         <v>16721</v>
       </c>
-      <c r="N50" s="2">
+      <c r="N50" s="3">
         <f t="shared" si="42"/>
         <v>261.265625</v>
       </c>
-      <c r="O50">
+      <c r="O50" s="3">
         <v>85355</v>
       </c>
-      <c r="P50">
+      <c r="P50" s="3">
         <v>84585</v>
       </c>
-      <c r="Q50">
+      <c r="Q50" s="3">
         <f t="shared" si="43"/>
         <v>94.783835481662365</v>
       </c>
     </row>
     <row r="51" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A51">
+      <c r="A51" s="3">
         <v>50</v>
       </c>
-      <c r="B51" s="1">
+      <c r="B51" s="3">
         <v>45768</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C51" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D51" s="4">
+      <c r="D51" s="2">
         <v>47420</v>
       </c>
-      <c r="E51" s="4">
+      <c r="E51" s="2">
         <v>47910</v>
       </c>
-      <c r="F51">
+      <c r="F51" s="3">
         <f t="shared" si="36"/>
         <v>490</v>
       </c>
-      <c r="G51" s="2">
+      <c r="G51" s="3">
         <f t="shared" si="37"/>
         <v>830.2</v>
       </c>
-      <c r="H51" s="2">
+      <c r="H51" s="3">
         <f t="shared" si="38"/>
         <v>1.03331927456769</v>
       </c>
-      <c r="I51" s="2">
+      <c r="I51" s="3">
         <f t="shared" si="39"/>
         <v>4.1081966963260053</v>
       </c>
@@ -4253,58 +4247,58 @@
         <f t="shared" si="40"/>
         <v>5159.4530604117554</v>
       </c>
-      <c r="L51">
+      <c r="L51" s="3">
         <f t="shared" si="44"/>
         <v>-30699</v>
       </c>
-      <c r="M51" s="4">
+      <c r="M51" s="2">
         <f t="shared" si="41"/>
         <v>17211</v>
       </c>
-      <c r="N51" s="2">
+      <c r="N51" s="3">
         <f t="shared" si="42"/>
         <v>268.921875</v>
       </c>
-      <c r="O51">
+      <c r="O51" s="3">
         <v>84585</v>
       </c>
-      <c r="P51">
+      <c r="P51" s="3">
         <v>88165</v>
       </c>
-      <c r="Q51">
+      <c r="Q51" s="3">
         <f t="shared" si="43"/>
         <v>98.795493943852478</v>
       </c>
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A52">
+      <c r="A52" s="3">
         <v>51</v>
       </c>
-      <c r="B52" s="1">
+      <c r="B52" s="3">
         <v>45769</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C52" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D52" s="4">
+      <c r="D52" s="2">
         <v>47910</v>
       </c>
-      <c r="E52" s="4">
+      <c r="E52" s="2">
         <v>49488</v>
       </c>
-      <c r="F52">
+      <c r="F52" s="3">
         <f t="shared" si="36"/>
         <v>1578</v>
       </c>
-      <c r="G52" s="2">
+      <c r="G52" s="3">
         <f t="shared" si="37"/>
         <v>844.86274509803923</v>
       </c>
-      <c r="H52" s="2">
+      <c r="H52" s="3">
         <f t="shared" si="38"/>
         <v>3.2936756418284308</v>
       </c>
-      <c r="I52" s="2">
+      <c r="I52" s="3">
         <f t="shared" si="39"/>
         <v>4.0921641251811192</v>
       </c>
@@ -4316,58 +4310,58 @@
         <f t="shared" si="40"/>
         <v>6580.78295019711</v>
       </c>
-      <c r="L52">
+      <c r="L52" s="3">
         <f t="shared" si="44"/>
         <v>-30699</v>
       </c>
-      <c r="M52" s="4">
+      <c r="M52" s="2">
         <f t="shared" si="41"/>
         <v>18789</v>
       </c>
-      <c r="N52" s="2">
+      <c r="N52" s="3">
         <f t="shared" si="42"/>
         <v>293.578125</v>
       </c>
-      <c r="O52">
+      <c r="O52" s="3">
         <v>88165</v>
       </c>
-      <c r="P52">
+      <c r="P52" s="3">
         <v>91407</v>
       </c>
-      <c r="Q52">
+      <c r="Q52" s="3">
         <f t="shared" si="43"/>
         <v>102.42839805961235</v>
       </c>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A53">
+      <c r="A53" s="3">
         <v>52</v>
       </c>
-      <c r="B53" s="1">
+      <c r="B53" s="3">
         <v>45770</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C53" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D53" s="4">
+      <c r="D53" s="2">
         <v>49488</v>
       </c>
-      <c r="E53" s="4">
+      <c r="E53" s="2">
         <v>50094</v>
       </c>
-      <c r="F53">
+      <c r="F53" s="3">
         <f t="shared" si="36"/>
         <v>606</v>
       </c>
-      <c r="G53" s="2">
+      <c r="G53" s="3">
         <f t="shared" si="37"/>
         <v>840.26923076923072</v>
       </c>
-      <c r="H53" s="2">
+      <c r="H53" s="3">
         <f t="shared" si="38"/>
         <v>1.2245392822502366</v>
       </c>
-      <c r="I53" s="2">
+      <c r="I53" s="3">
         <f t="shared" si="39"/>
         <v>4.0362586513626564</v>
       </c>
@@ -4379,58 +4373,58 @@
         <f t="shared" si="40"/>
         <v>7028.0761285496737</v>
       </c>
-      <c r="L53">
+      <c r="L53" s="3">
         <f t="shared" si="44"/>
         <v>-30699</v>
       </c>
-      <c r="M53" s="4">
+      <c r="M53" s="2">
         <f t="shared" si="41"/>
         <v>19395</v>
       </c>
-      <c r="N53" s="2">
+      <c r="N53" s="3">
         <f t="shared" si="42"/>
         <v>303.046875</v>
       </c>
-      <c r="O53">
+      <c r="O53" s="3">
         <v>91407</v>
       </c>
-      <c r="P53">
+      <c r="P53" s="3">
         <v>92926</v>
       </c>
-      <c r="Q53">
+      <c r="Q53" s="3">
         <f t="shared" si="43"/>
         <v>104.13055146856955</v>
       </c>
     </row>
     <row r="54" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A54">
+      <c r="A54" s="3">
         <v>53</v>
       </c>
-      <c r="B54" s="1">
+      <c r="B54" s="3">
         <v>45771</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C54" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D54" s="4">
+      <c r="D54" s="2">
         <v>50094</v>
       </c>
-      <c r="E54" s="4">
+      <c r="E54" s="2">
         <v>50900</v>
       </c>
-      <c r="F54">
+      <c r="F54" s="3">
         <f t="shared" si="36"/>
         <v>806</v>
       </c>
-      <c r="G54" s="2">
+      <c r="G54" s="3">
         <f t="shared" si="37"/>
         <v>839.62264150943395</v>
       </c>
-      <c r="H54" s="2">
+      <c r="H54" s="3">
         <f t="shared" si="38"/>
         <v>1.6089751267616803</v>
       </c>
-      <c r="I54" s="2">
+      <c r="I54" s="3">
         <f t="shared" si="39"/>
         <v>3.9899284528173595</v>
       </c>
@@ -4442,58 +4436,58 @@
         <f t="shared" si="40"/>
         <v>7673.3061182208203</v>
       </c>
-      <c r="L54">
+      <c r="L54" s="3">
         <f t="shared" si="44"/>
         <v>-30699</v>
       </c>
-      <c r="M54" s="4">
+      <c r="M54" s="2">
         <f t="shared" si="41"/>
         <v>20201</v>
       </c>
-      <c r="N54" s="2">
+      <c r="N54" s="3">
         <f t="shared" si="42"/>
         <v>315.640625</v>
       </c>
-      <c r="O54">
+      <c r="O54" s="3">
         <v>92926</v>
       </c>
-      <c r="P54">
+      <c r="P54" s="3">
         <v>93092</v>
       </c>
-      <c r="Q54">
+      <c r="Q54" s="3">
         <f t="shared" si="43"/>
         <v>104.31656691681637</v>
       </c>
     </row>
     <row r="55" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A55">
+      <c r="A55" s="3">
         <v>54</v>
       </c>
-      <c r="B55" s="1">
+      <c r="B55" s="3">
         <v>45772</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C55" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D55" s="4">
+      <c r="D55" s="2">
         <v>50900</v>
       </c>
-      <c r="E55" s="4">
+      <c r="E55" s="2">
         <v>51087.55</v>
       </c>
-      <c r="F55">
+      <c r="F55" s="3">
         <f t="shared" si="36"/>
         <v>187.55000000000291</v>
       </c>
-      <c r="G55" s="2">
+      <c r="G55" s="3">
         <f t="shared" si="37"/>
         <v>827.54722222222233</v>
       </c>
-      <c r="H55" s="2">
+      <c r="H55" s="3">
         <f t="shared" si="38"/>
         <v>0.36846758349706743</v>
       </c>
-      <c r="I55" s="2">
+      <c r="I55" s="3">
         <f t="shared" si="39"/>
         <v>3.9216911636315688</v>
       </c>
@@ -4505,58 +4499,58 @@
         <f t="shared" si="40"/>
         <v>7697.9960977576957</v>
       </c>
-      <c r="L55">
+      <c r="L55" s="3">
         <f t="shared" si="44"/>
         <v>-30699</v>
       </c>
-      <c r="M55" s="4">
+      <c r="M55" s="2">
         <f t="shared" si="41"/>
         <v>20388.550000000003</v>
       </c>
-      <c r="N55" s="2">
+      <c r="N55" s="3">
         <f t="shared" si="42"/>
         <v>318.57109375000005</v>
       </c>
-      <c r="O55">
+      <c r="O55" s="3">
         <v>93092</v>
       </c>
-      <c r="P55">
+      <c r="P55" s="3">
         <v>95419</v>
       </c>
-      <c r="Q55">
+      <c r="Q55" s="3">
         <f t="shared" si="43"/>
         <v>106.92414491723994</v>
       </c>
     </row>
     <row r="56" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A56">
+      <c r="A56" s="3">
         <v>55</v>
       </c>
-      <c r="B56" s="1">
+      <c r="B56" s="3">
         <v>45773</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C56" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D56" s="4">
+      <c r="D56" s="2">
         <v>51087.55</v>
       </c>
-      <c r="E56" s="4">
+      <c r="E56" s="2">
         <v>51166.85</v>
       </c>
-      <c r="F56">
+      <c r="F56" s="3">
         <f t="shared" si="36"/>
         <v>79.299999999995634</v>
       </c>
-      <c r="G56" s="2">
+      <c r="G56" s="3">
         <f t="shared" si="37"/>
         <v>813.94272727272721</v>
       </c>
-      <c r="H56" s="2">
+      <c r="H56" s="3">
         <f t="shared" si="38"/>
         <v>0.15522372867753376</v>
       </c>
-      <c r="I56" s="2">
+      <c r="I56" s="3">
         <f t="shared" si="39"/>
         <v>3.8519615234979154</v>
       </c>
@@ -4568,58 +4562,58 @@
         <f t="shared" si="40"/>
         <v>7612.3188970285428</v>
       </c>
-      <c r="L56">
+      <c r="L56" s="3">
         <f t="shared" si="44"/>
         <v>-30699</v>
       </c>
-      <c r="M56" s="4">
+      <c r="M56" s="2">
         <f t="shared" si="41"/>
         <v>20467.849999999999</v>
       </c>
-      <c r="N56" s="2">
+      <c r="N56" s="3">
         <f t="shared" si="42"/>
         <v>319.81015624999998</v>
       </c>
-      <c r="O56">
+      <c r="O56" s="3">
         <v>95419</v>
       </c>
-      <c r="P56">
+      <c r="P56" s="3">
         <v>94232</v>
       </c>
-      <c r="Q56">
+      <c r="Q56" s="3">
         <f t="shared" si="43"/>
         <v>105.59402240477635</v>
       </c>
     </row>
     <row r="57" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A57">
+      <c r="A57" s="3">
         <v>56</v>
       </c>
-      <c r="B57" s="1">
+      <c r="B57" s="3">
         <v>45774</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C57" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D57" s="4">
+      <c r="D57" s="2">
         <v>51166.85</v>
       </c>
-      <c r="E57" s="4">
+      <c r="E57" s="2">
         <v>51225</v>
       </c>
-      <c r="F57">
+      <c r="F57" s="3">
         <f t="shared" si="36"/>
         <v>58.150000000001455</v>
       </c>
-      <c r="G57" s="2">
+      <c r="G57" s="3">
         <f t="shared" si="37"/>
         <v>800.44642857142856</v>
       </c>
-      <c r="H57" s="2">
+      <c r="H57" s="3">
         <f t="shared" si="38"/>
         <v>0.11364780126195129</v>
       </c>
-      <c r="I57" s="2">
+      <c r="I57" s="3">
         <f t="shared" si="39"/>
         <v>3.7839970496518882</v>
       </c>
@@ -4631,58 +4625,58 @@
         <f t="shared" si="40"/>
         <v>7503.3469926899161</v>
       </c>
-      <c r="L57">
+      <c r="L57" s="3">
         <f t="shared" si="44"/>
         <v>-30699</v>
       </c>
-      <c r="M57" s="4">
+      <c r="M57" s="2">
         <f t="shared" si="41"/>
         <v>20526</v>
       </c>
-      <c r="N57" s="2">
+      <c r="N57" s="3">
         <f t="shared" si="42"/>
         <v>320.71875</v>
       </c>
-      <c r="O57">
+      <c r="O57" s="3">
         <v>94232</v>
       </c>
-      <c r="P57">
+      <c r="P57" s="3">
         <v>94047</v>
       </c>
-      <c r="Q57">
+      <c r="Q57" s="3">
         <f t="shared" si="43"/>
         <v>105.3867160317302</v>
       </c>
     </row>
     <row r="58" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A58">
+      <c r="A58" s="3">
         <v>57</v>
       </c>
-      <c r="B58" s="1">
+      <c r="B58" s="3">
         <v>45775</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C58" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D58" s="4">
+      <c r="D58" s="2">
         <v>51225</v>
       </c>
-      <c r="E58" s="4">
+      <c r="E58" s="2">
         <v>51915</v>
       </c>
-      <c r="F58">
+      <c r="F58" s="3">
         <f t="shared" si="36"/>
         <v>690</v>
       </c>
-      <c r="G58" s="2">
+      <c r="G58" s="3">
         <f t="shared" si="37"/>
         <v>798.50877192982455</v>
       </c>
-      <c r="H58" s="2">
+      <c r="H58" s="3">
         <f t="shared" si="38"/>
         <v>1.3469985358711467</v>
       </c>
-      <c r="I58" s="2">
+      <c r="I58" s="3">
         <f t="shared" si="39"/>
         <v>3.7407417401673415</v>
       </c>
@@ -4694,58 +4688,58 @@
         <f t="shared" si="40"/>
         <v>8024.0525035948867</v>
       </c>
-      <c r="L58">
+      <c r="L58" s="3">
         <f t="shared" si="44"/>
         <v>-30699</v>
       </c>
-      <c r="M58" s="4">
+      <c r="M58" s="2">
         <f t="shared" si="41"/>
         <v>21216</v>
       </c>
-      <c r="N58" s="2">
+      <c r="N58" s="3">
         <f t="shared" si="42"/>
         <v>331.5</v>
       </c>
-      <c r="O58">
+      <c r="O58" s="3">
         <v>94047</v>
       </c>
-      <c r="P58">
+      <c r="P58" s="3">
         <v>94415</v>
       </c>
-      <c r="Q58">
+      <c r="Q58" s="3">
         <f t="shared" si="43"/>
         <v>105.7990876278436</v>
       </c>
     </row>
     <row r="59" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A59">
+      <c r="A59" s="3">
         <v>58</v>
       </c>
-      <c r="B59" s="1">
+      <c r="B59" s="3">
         <v>45776</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C59" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D59" s="4">
+      <c r="D59" s="2">
         <v>51915</v>
       </c>
-      <c r="E59" s="4">
+      <c r="E59" s="2">
         <v>52670</v>
       </c>
-      <c r="F59">
+      <c r="F59" s="3">
         <f t="shared" si="36"/>
         <v>755</v>
       </c>
-      <c r="G59" s="2">
+      <c r="G59" s="3">
         <f t="shared" si="37"/>
         <v>797.75862068965512</v>
       </c>
-      <c r="H59" s="2">
+      <c r="H59" s="3">
         <f t="shared" si="38"/>
         <v>1.45430029856497</v>
       </c>
-      <c r="I59" s="2">
+      <c r="I59" s="3">
         <f t="shared" si="39"/>
         <v>3.7008870800216309</v>
       </c>
@@ -4757,58 +4751,58 @@
         <f t="shared" si="40"/>
         <v>8607.5571861416211</v>
       </c>
-      <c r="L59">
+      <c r="L59" s="3">
         <f t="shared" si="44"/>
         <v>-30699</v>
       </c>
-      <c r="M59" s="4">
+      <c r="M59" s="2">
         <f t="shared" si="41"/>
         <v>21971</v>
       </c>
-      <c r="N59" s="2">
+      <c r="N59" s="3">
         <f t="shared" si="42"/>
         <v>343.296875</v>
       </c>
-      <c r="O59">
+      <c r="O59" s="3">
         <v>94415</v>
       </c>
-      <c r="P59">
+      <c r="P59" s="3">
         <v>95022</v>
       </c>
-      <c r="Q59">
+      <c r="Q59" s="3">
         <f t="shared" si="43"/>
         <v>106.47927664643282</v>
       </c>
     </row>
     <row r="60" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A60">
+      <c r="A60" s="3">
         <v>59</v>
       </c>
-      <c r="B60" s="1">
+      <c r="B60" s="3">
         <v>45777</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C60" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D60" s="4">
+      <c r="D60" s="2">
         <v>52670</v>
       </c>
-      <c r="E60" s="4">
+      <c r="E60" s="2">
         <v>53561.74</v>
       </c>
-      <c r="F60">
+      <c r="F60" s="3">
         <f t="shared" si="36"/>
         <v>891.73999999999796</v>
       </c>
-      <c r="G60" s="2">
+      <c r="G60" s="3">
         <f t="shared" si="37"/>
         <v>799.35152542372873</v>
       </c>
-      <c r="H60" s="2">
+      <c r="H60" s="3">
         <f t="shared" si="38"/>
         <v>1.693070058857038</v>
       </c>
-      <c r="I60" s="2">
+      <c r="I60" s="3">
         <f t="shared" si="39"/>
         <v>3.6665282155353252</v>
       </c>
@@ -4820,58 +4814,58 @@
         <f t="shared" si="40"/>
         <v>9325.5724295614618</v>
       </c>
-      <c r="L60">
+      <c r="L60" s="3">
         <f t="shared" si="44"/>
         <v>-30699</v>
       </c>
-      <c r="M60" s="4">
+      <c r="M60" s="2">
         <f t="shared" si="41"/>
         <v>22862.739999999998</v>
       </c>
-      <c r="N60" s="2">
+      <c r="N60" s="3">
         <f t="shared" si="42"/>
         <v>357.23031249999997</v>
       </c>
-      <c r="O60">
+      <c r="O60" s="3">
         <v>95022</v>
       </c>
-      <c r="P60">
+      <c r="P60" s="3">
         <v>93681</v>
       </c>
-      <c r="Q60">
+      <c r="Q60" s="3">
         <f t="shared" si="43"/>
         <v>104.97658558559569</v>
       </c>
     </row>
     <row r="61" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A61">
+      <c r="A61" s="3">
         <v>60</v>
       </c>
-      <c r="B61" s="1">
+      <c r="B61" s="3">
         <v>45778</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C61" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D61" s="4">
+      <c r="D61" s="2">
         <v>53561.74</v>
       </c>
-      <c r="E61" s="4">
+      <c r="E61" s="2">
         <v>54386</v>
       </c>
-      <c r="F61">
+      <c r="F61" s="3">
         <f t="shared" si="36"/>
         <v>824.26000000000204</v>
       </c>
-      <c r="G61" s="2">
+      <c r="G61" s="3">
         <f t="shared" si="37"/>
         <v>799.76666666666665</v>
       </c>
-      <c r="H61" s="2">
+      <c r="H61" s="3">
         <f t="shared" si="38"/>
         <v>1.5388969813153963</v>
       </c>
-      <c r="I61" s="2">
+      <c r="I61" s="3">
         <f t="shared" si="39"/>
         <v>3.6307049367540145</v>
       </c>
@@ -4883,58 +4877,58 @@
         <f t="shared" si="40"/>
         <v>9973.8492511457644</v>
       </c>
-      <c r="L61">
+      <c r="L61" s="3">
         <f t="shared" si="44"/>
         <v>-30699</v>
       </c>
-      <c r="M61" s="4">
+      <c r="M61" s="2">
         <f t="shared" si="41"/>
         <v>23687</v>
       </c>
-      <c r="N61" s="2">
+      <c r="N61" s="3">
         <f t="shared" si="42"/>
         <v>370.109375</v>
       </c>
-      <c r="O61">
+      <c r="O61" s="3">
         <v>93681</v>
       </c>
-      <c r="P61">
+      <c r="P61" s="3">
         <v>96814</v>
       </c>
-      <c r="Q61">
+      <c r="Q61" s="3">
         <f t="shared" si="43"/>
         <v>108.48734702750676</v>
       </c>
     </row>
     <row r="62" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A62">
+      <c r="A62" s="3">
         <v>61</v>
       </c>
-      <c r="B62" s="1">
+      <c r="B62" s="3">
         <v>45779</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C62" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D62" s="4">
+      <c r="D62" s="2">
         <v>54386</v>
       </c>
-      <c r="E62" s="4">
+      <c r="E62" s="2">
         <v>55327</v>
       </c>
-      <c r="F62">
+      <c r="F62" s="3">
         <f t="shared" si="36"/>
         <v>941</v>
       </c>
-      <c r="G62" s="2">
+      <c r="G62" s="3">
         <f t="shared" si="37"/>
         <v>802.08196721311481</v>
       </c>
-      <c r="H62" s="2">
+      <c r="H62" s="3">
         <f t="shared" si="38"/>
         <v>1.7302246901776286</v>
       </c>
-      <c r="I62" s="2">
+      <c r="I62" s="3">
         <f t="shared" si="39"/>
         <v>3.5992650724708364</v>
       </c>
@@ -4946,25 +4940,25 @@
         <f t="shared" si="40"/>
         <v>10736.57829141066</v>
       </c>
-      <c r="L62">
+      <c r="L62" s="3">
         <f t="shared" si="44"/>
         <v>-30699</v>
       </c>
-      <c r="M62" s="4">
+      <c r="M62" s="2">
         <f t="shared" si="41"/>
         <v>24628</v>
       </c>
-      <c r="N62" s="2">
+      <c r="N62" s="3">
         <f t="shared" si="42"/>
         <v>384.8125</v>
       </c>
-      <c r="O62">
+      <c r="O62" s="3">
         <v>96814</v>
       </c>
-      <c r="P62">
+      <c r="P62" s="3">
         <v>97711</v>
       </c>
-      <c r="Q62">
+      <c r="Q62" s="3">
         <f t="shared" si="43"/>
         <v>109.49250279303317</v>
       </c>

</xml_diff>

<commit_message>
자동 업데이트: 2025-05-03 22:03:13
</commit_message>
<xml_diff>
--- a/data/daily_report.xlsx
+++ b/data/daily_report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c58a53286e4c1d7a/문서/GitHub/Dashboard/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="269" documentId="8_{9DD2A88B-03DA-4864-84CC-4418086E8BD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{159E1548-2E6F-4CD8-A09F-13D356E11DC7}"/>
+  <xr:revisionPtr revIDLastSave="270" documentId="8_{9DD2A88B-03DA-4864-84CC-4418086E8BD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3A47580B-B26B-49A8-98D0-45BF352A0706}"/>
   <bookViews>
-    <workbookView xWindow="4290" yWindow="4275" windowWidth="27300" windowHeight="17325" xr2:uid="{4AB8DADE-1167-4E84-9D67-55086BA93884}"/>
+    <workbookView xWindow="11070" yWindow="1695" windowWidth="27300" windowHeight="17325" xr2:uid="{4AB8DADE-1167-4E84-9D67-55086BA93884}"/>
   </bookViews>
   <sheets>
     <sheet name="daily_report" sheetId="1" r:id="rId1"/>
@@ -716,7 +716,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1102,7 +1102,7 @@
   <dimension ref="A1:Q62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1117,13 +1117,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -1132,51 +1132,51 @@
       <c r="E1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" t="s">
         <v>9</v>
       </c>
       <c r="M1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="N1" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="O1" t="s">
         <v>11</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="P1" t="s">
         <v>12</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="Q1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A2" s="3">
+      <c r="A2">
         <v>0</v>
       </c>
       <c r="B2" s="3">
         <v>45719</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" s="2">
@@ -1185,56 +1185,56 @@
       <c r="E2" s="2">
         <v>6400</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2">
         <f>E2-D2</f>
         <v>0</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2">
         <v>0</v>
       </c>
-      <c r="H2" s="3">
+      <c r="H2">
         <v>0</v>
       </c>
-      <c r="I2" s="3">
+      <c r="I2">
         <v>0</v>
       </c>
-      <c r="J2" s="3">
+      <c r="J2">
         <f>D2</f>
         <v>6400</v>
       </c>
-      <c r="K2" s="3">
+      <c r="K2">
         <f t="shared" ref="K2:K36" si="0">M2-J2</f>
         <v>0</v>
       </c>
-      <c r="L2" s="3">
+      <c r="L2">
         <v>0</v>
       </c>
       <c r="M2" s="2">
         <f>L2+E2</f>
         <v>6400</v>
       </c>
-      <c r="N2" s="3">
+      <c r="N2">
         <f>M2/$D$2*100</f>
         <v>100</v>
       </c>
-      <c r="O2" s="3">
+      <c r="O2">
         <v>89239.9</v>
       </c>
-      <c r="P2" s="3">
+      <c r="P2">
         <v>89239.9</v>
       </c>
-      <c r="Q2" s="3">
+      <c r="Q2">
         <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A3" s="3">
+      <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" s="3">
         <v>45720</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" t="s">
         <v>15</v>
       </c>
       <c r="D3" s="2">
@@ -1243,60 +1243,60 @@
       <c r="E3" s="2">
         <v>6546</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3">
         <f t="shared" ref="F3:F24" si="1">E3-D3</f>
         <v>146</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3">
         <f t="shared" ref="G3:G22" si="2">(E3-$D$2)/A3</f>
         <v>146</v>
       </c>
-      <c r="H3" s="3">
+      <c r="H3">
         <f>(E3/D3-1)*100</f>
         <v>2.2812499999999902</v>
       </c>
-      <c r="I3" s="3">
+      <c r="I3">
         <f>(POWER((E3/$D$3),1/A3)-1)*100</f>
         <v>2.2812499999999902</v>
       </c>
-      <c r="J3" s="3">
+      <c r="J3">
         <f>J2*1.013</f>
         <v>6483.1999999999989</v>
       </c>
-      <c r="K3" s="3">
+      <c r="K3">
         <f t="shared" si="0"/>
         <v>62.800000000001091</v>
       </c>
-      <c r="L3" s="3">
+      <c r="L3">
         <v>0</v>
       </c>
       <c r="M3" s="2">
         <f t="shared" ref="M3:M24" si="3">L3+E3</f>
         <v>6546</v>
       </c>
-      <c r="N3" s="3">
+      <c r="N3">
         <f t="shared" ref="N3:N41" si="4">M3/$D$2*100</f>
         <v>102.28124999999999</v>
       </c>
-      <c r="O3" s="3">
+      <c r="O3">
         <v>89239.9</v>
       </c>
-      <c r="P3" s="3">
+      <c r="P3">
         <v>83157.100000000006</v>
       </c>
-      <c r="Q3" s="3">
+      <c r="Q3">
         <f>P3/$O$2*100</f>
         <v>93.183766454243013</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A4" s="3">
+      <c r="A4">
         <v>2</v>
       </c>
       <c r="B4" s="3">
         <v>45721</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" t="s">
         <v>16</v>
       </c>
       <c r="D4" s="2">
@@ -1305,60 +1305,60 @@
       <c r="E4" s="2">
         <v>6689</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4">
         <f t="shared" si="1"/>
         <v>143</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4">
         <f t="shared" si="2"/>
         <v>144.5</v>
       </c>
-      <c r="H4" s="3">
+      <c r="H4">
         <f t="shared" ref="H4:H24" si="5">(E4/D4-1)*100</f>
         <v>2.1845401772074613</v>
       </c>
-      <c r="I4" s="3">
+      <c r="I4">
         <f t="shared" ref="I4:I24" si="6">(POWER((E4/$D$3),1/A4)-1)*100</f>
         <v>2.2328836529616813</v>
       </c>
-      <c r="J4" s="3">
+      <c r="J4">
         <f t="shared" ref="J4:J62" si="7">J3*1.013</f>
         <v>6567.4815999999983</v>
       </c>
-      <c r="K4" s="3">
+      <c r="K4">
         <f t="shared" si="0"/>
         <v>121.51840000000175</v>
       </c>
-      <c r="L4" s="3">
+      <c r="L4">
         <v>0</v>
       </c>
       <c r="M4" s="2">
         <f t="shared" si="3"/>
         <v>6689</v>
       </c>
-      <c r="N4" s="3">
+      <c r="N4">
         <f t="shared" si="4"/>
         <v>104.515625</v>
       </c>
-      <c r="O4" s="3">
+      <c r="O4">
         <v>83157.100000000006</v>
       </c>
-      <c r="P4" s="3">
+      <c r="P4">
         <v>88477.3</v>
       </c>
-      <c r="Q4" s="3">
+      <c r="Q4">
         <f t="shared" ref="Q4:Q41" si="8">P4/$O$2*100</f>
         <v>99.145449513054146</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A5" s="3">
+      <c r="A5">
         <v>3</v>
       </c>
       <c r="B5" s="3">
         <v>45722</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" t="s">
         <v>17</v>
       </c>
       <c r="D5" s="2">
@@ -1367,60 +1367,60 @@
       <c r="E5" s="2">
         <v>6846</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5">
         <f t="shared" si="1"/>
         <v>157</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5">
         <f t="shared" si="2"/>
         <v>148.66666666666666</v>
       </c>
-      <c r="H5" s="3">
+      <c r="H5">
         <f t="shared" si="5"/>
         <v>2.3471370907460098</v>
       </c>
-      <c r="I5" s="3">
+      <c r="I5">
         <f t="shared" si="6"/>
         <v>2.2709539535396894</v>
       </c>
-      <c r="J5" s="3">
+      <c r="J5">
         <f t="shared" si="7"/>
         <v>6652.8588607999973</v>
       </c>
-      <c r="K5" s="3">
+      <c r="K5">
         <f t="shared" si="0"/>
         <v>193.14113920000273</v>
       </c>
-      <c r="L5" s="3">
+      <c r="L5">
         <v>0</v>
       </c>
       <c r="M5" s="2">
         <f t="shared" si="3"/>
         <v>6846</v>
       </c>
-      <c r="N5" s="3">
+      <c r="N5">
         <f t="shared" si="4"/>
         <v>106.96874999999999</v>
       </c>
-      <c r="O5" s="3">
+      <c r="O5">
         <v>88477.3</v>
       </c>
-      <c r="P5" s="3">
+      <c r="P5">
         <v>89770.4</v>
       </c>
-      <c r="Q5" s="3">
+      <c r="Q5">
         <f t="shared" si="8"/>
         <v>100.59446503189717</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A6" s="3">
+      <c r="A6">
         <v>4</v>
       </c>
       <c r="B6" s="3">
         <v>45723</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" t="s">
         <v>18</v>
       </c>
       <c r="D6" s="2">
@@ -1429,60 +1429,60 @@
       <c r="E6" s="2">
         <v>7015</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6">
         <f t="shared" si="1"/>
         <v>169</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6">
         <f t="shared" si="2"/>
         <v>153.75</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6">
         <f t="shared" si="5"/>
         <v>2.4685947998831503</v>
       </c>
-      <c r="I6" s="3">
+      <c r="I6">
         <f t="shared" si="6"/>
         <v>2.3203283980714806</v>
       </c>
-      <c r="J6" s="3">
+      <c r="J6">
         <f t="shared" si="7"/>
         <v>6739.3460259903968</v>
       </c>
-      <c r="K6" s="3">
+      <c r="K6">
         <f t="shared" si="0"/>
         <v>275.65397400960319</v>
       </c>
-      <c r="L6" s="3">
+      <c r="L6">
         <v>0</v>
       </c>
       <c r="M6" s="2">
         <f t="shared" si="3"/>
         <v>7015</v>
       </c>
-      <c r="N6" s="3">
+      <c r="N6">
         <f t="shared" si="4"/>
         <v>109.60937500000001</v>
       </c>
-      <c r="O6" s="3">
+      <c r="O6">
         <v>89770.4</v>
       </c>
-      <c r="P6" s="3">
+      <c r="P6">
         <v>90411.6</v>
       </c>
-      <c r="Q6" s="3">
+      <c r="Q6">
         <f t="shared" si="8"/>
         <v>101.3129777151252</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A7" s="3">
+      <c r="A7">
         <v>5</v>
       </c>
       <c r="B7" s="3">
         <v>45724</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" t="s">
         <v>19</v>
       </c>
       <c r="D7" s="2">
@@ -1491,60 +1491,60 @@
       <c r="E7" s="2">
         <v>7050</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7">
         <f t="shared" si="1"/>
         <v>35</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7">
         <f t="shared" si="2"/>
         <v>130</v>
       </c>
-      <c r="H7" s="3">
+      <c r="H7">
         <f t="shared" si="5"/>
         <v>0.49893086243764095</v>
       </c>
-      <c r="I7" s="3">
+      <c r="I7">
         <f t="shared" si="6"/>
         <v>1.9534270313376956</v>
       </c>
-      <c r="J7" s="3">
+      <c r="J7">
         <f t="shared" si="7"/>
         <v>6826.9575243282716</v>
       </c>
-      <c r="K7" s="3">
+      <c r="K7">
         <f t="shared" si="0"/>
         <v>223.04247567172843</v>
       </c>
-      <c r="L7" s="3">
+      <c r="L7">
         <v>0</v>
       </c>
       <c r="M7" s="2">
         <f t="shared" si="3"/>
         <v>7050</v>
       </c>
-      <c r="N7" s="3">
+      <c r="N7">
         <f t="shared" si="4"/>
         <v>110.15625</v>
       </c>
-      <c r="O7" s="3">
+      <c r="O7">
         <v>90411.6</v>
       </c>
-      <c r="P7" s="3">
+      <c r="P7">
         <v>86323.3</v>
       </c>
-      <c r="Q7" s="3">
+      <c r="Q7">
         <f t="shared" si="8"/>
         <v>96.731730985803438</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A8" s="3">
+      <c r="A8">
         <v>6</v>
       </c>
       <c r="B8" s="3">
         <v>45725</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" t="s">
         <v>20</v>
       </c>
       <c r="D8" s="2">
@@ -1553,60 +1553,60 @@
       <c r="E8" s="2">
         <v>6979</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8">
         <f t="shared" si="1"/>
         <v>-71</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G8">
         <f t="shared" si="2"/>
         <v>96.5</v>
       </c>
-      <c r="H8" s="3">
+      <c r="H8">
         <f t="shared" si="5"/>
         <v>-1.0070921985815606</v>
       </c>
-      <c r="I8" s="3">
+      <c r="I8">
         <f t="shared" si="6"/>
         <v>1.4539290311231801</v>
       </c>
-      <c r="J8" s="3">
+      <c r="J8">
         <f t="shared" si="7"/>
         <v>6915.7079721445389</v>
       </c>
-      <c r="K8" s="3">
+      <c r="K8">
         <f t="shared" si="0"/>
         <v>63.292027855461129</v>
       </c>
-      <c r="L8" s="3">
+      <c r="L8">
         <v>0</v>
       </c>
       <c r="M8" s="2">
         <f t="shared" si="3"/>
         <v>6979</v>
       </c>
-      <c r="N8" s="3">
+      <c r="N8">
         <f t="shared" si="4"/>
         <v>109.04687500000001</v>
       </c>
-      <c r="O8" s="3">
+      <c r="O8">
         <v>86323.3</v>
       </c>
-      <c r="P8" s="3">
+      <c r="P8">
         <v>83563</v>
       </c>
-      <c r="Q8" s="3">
+      <c r="Q8">
         <f t="shared" si="8"/>
         <v>93.638607842456125</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A9" s="3">
+      <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" s="3">
         <v>45726</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" t="s">
         <v>14</v>
       </c>
       <c r="D9" s="2">
@@ -1615,60 +1615,60 @@
       <c r="E9" s="2">
         <v>7170</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9">
         <f t="shared" si="1"/>
         <v>191</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G9">
         <f t="shared" si="2"/>
         <v>96.25</v>
       </c>
-      <c r="H9" s="3">
+      <c r="H9">
         <f t="shared" si="5"/>
         <v>2.7367817738931155</v>
       </c>
-      <c r="I9" s="3">
+      <c r="I9">
         <f t="shared" si="6"/>
         <v>1.4302270645888626</v>
       </c>
-      <c r="J9" s="3">
+      <c r="J9">
         <f t="shared" si="7"/>
         <v>7005.6121757824176</v>
       </c>
-      <c r="K9" s="3">
+      <c r="K9">
         <f t="shared" si="0"/>
         <v>164.38782421758242</v>
       </c>
-      <c r="L9" s="3">
+      <c r="L9">
         <v>0</v>
       </c>
       <c r="M9" s="2">
         <f t="shared" si="3"/>
         <v>7170</v>
       </c>
-      <c r="N9" s="3">
+      <c r="N9">
         <f t="shared" si="4"/>
         <v>112.03125</v>
       </c>
-      <c r="O9" s="3">
+      <c r="O9">
         <v>83563</v>
       </c>
-      <c r="P9" s="3">
+      <c r="P9">
         <v>79813.7</v>
       </c>
-      <c r="Q9" s="3">
+      <c r="Q9">
         <f t="shared" si="8"/>
         <v>89.437236034554061</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A10" s="3">
+      <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" s="3">
         <v>45727</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" t="s">
         <v>15</v>
       </c>
       <c r="D10" s="2">
@@ -1677,60 +1677,60 @@
       <c r="E10" s="2">
         <v>7315</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10">
         <f t="shared" si="1"/>
         <v>145</v>
       </c>
-      <c r="G10" s="3">
+      <c r="G10">
         <f t="shared" si="2"/>
         <v>101.66666666666667</v>
       </c>
-      <c r="H10" s="3">
+      <c r="H10">
         <f t="shared" si="5"/>
         <v>2.0223152022315283</v>
       </c>
-      <c r="I10" s="3">
+      <c r="I10">
         <f t="shared" si="6"/>
         <v>1.4958445810377752</v>
       </c>
-      <c r="J10" s="3">
+      <c r="J10">
         <f t="shared" si="7"/>
         <v>7096.6851340675885</v>
       </c>
-      <c r="K10" s="3">
+      <c r="K10">
         <f t="shared" si="0"/>
         <v>218.31486593241152</v>
       </c>
-      <c r="L10" s="3">
+      <c r="L10">
         <v>0</v>
       </c>
       <c r="M10" s="2">
         <f t="shared" si="3"/>
         <v>7315</v>
       </c>
-      <c r="N10" s="3">
+      <c r="N10">
         <f t="shared" si="4"/>
         <v>114.29687500000001</v>
       </c>
-      <c r="O10" s="3">
+      <c r="O10">
         <v>79813.7</v>
       </c>
-      <c r="P10" s="3">
+      <c r="P10">
         <v>80615.7</v>
       </c>
-      <c r="Q10" s="3">
+      <c r="Q10">
         <f t="shared" si="8"/>
         <v>90.335937176083789</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A11" s="3">
+      <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" s="3">
         <v>45728</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" t="s">
         <v>16</v>
       </c>
       <c r="D11" s="2">
@@ -1739,60 +1739,60 @@
       <c r="E11" s="2">
         <v>6845</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11">
         <f t="shared" si="1"/>
         <v>-470</v>
       </c>
-      <c r="G11" s="3">
+      <c r="G11">
         <f t="shared" si="2"/>
         <v>44.5</v>
       </c>
-      <c r="H11" s="3">
+      <c r="H11">
         <f t="shared" si="5"/>
         <v>-6.4251537935748448</v>
       </c>
-      <c r="I11" s="3">
+      <c r="I11">
         <f t="shared" si="6"/>
         <v>0.67446905031474103</v>
       </c>
-      <c r="J11" s="3">
+      <c r="J11">
         <f t="shared" si="7"/>
         <v>7188.9420408104661</v>
       </c>
-      <c r="K11" s="3">
+      <c r="K11">
         <f t="shared" si="0"/>
         <v>-343.9420408104661</v>
       </c>
-      <c r="L11" s="3">
+      <c r="L11">
         <v>0</v>
       </c>
       <c r="M11" s="2">
         <f t="shared" si="3"/>
         <v>6845</v>
       </c>
-      <c r="N11" s="3">
+      <c r="N11">
         <f t="shared" si="4"/>
         <v>106.953125</v>
       </c>
-      <c r="O11" s="3">
+      <c r="O11">
         <v>80615.7</v>
       </c>
-      <c r="P11" s="3">
+      <c r="P11">
         <v>81500.899999999994</v>
       </c>
-      <c r="Q11" s="3">
+      <c r="Q11">
         <f t="shared" si="8"/>
         <v>91.327870156734832</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A12" s="3">
+      <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" s="3">
         <v>45729</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" t="s">
         <v>17</v>
       </c>
       <c r="D12" s="2">
@@ -1801,60 +1801,60 @@
       <c r="E12" s="2">
         <v>7567</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12">
         <f t="shared" si="1"/>
         <v>722</v>
       </c>
-      <c r="G12" s="3">
+      <c r="G12">
         <f t="shared" si="2"/>
         <v>106.09090909090909</v>
       </c>
-      <c r="H12" s="3">
+      <c r="H12">
         <f t="shared" si="5"/>
         <v>10.547845142439737</v>
       </c>
-      <c r="I12" s="3">
+      <c r="I12">
         <f t="shared" si="6"/>
         <v>1.5343678109079883</v>
       </c>
-      <c r="J12" s="3">
+      <c r="J12">
         <f t="shared" si="7"/>
         <v>7282.3982873410014</v>
       </c>
-      <c r="K12" s="3">
+      <c r="K12">
         <f t="shared" si="0"/>
         <v>284.60171265899862</v>
       </c>
-      <c r="L12" s="3">
+      <c r="L12">
         <v>0</v>
       </c>
       <c r="M12" s="2">
         <f t="shared" si="3"/>
         <v>7567</v>
       </c>
-      <c r="N12" s="3">
+      <c r="N12">
         <f t="shared" si="4"/>
         <v>118.234375</v>
       </c>
-      <c r="O12" s="3">
+      <c r="O12">
         <v>81500.899999999994</v>
       </c>
-      <c r="P12" s="3">
+      <c r="P12">
         <v>81966.600000000006</v>
       </c>
-      <c r="Q12" s="3">
+      <c r="Q12">
         <f t="shared" si="8"/>
         <v>91.849721929316388</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A13" s="3">
+      <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" s="3">
         <v>45730</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" t="s">
         <v>18</v>
       </c>
       <c r="D13" s="2">
@@ -1863,60 +1863,60 @@
       <c r="E13" s="2">
         <v>7763</v>
       </c>
-      <c r="F13" s="3">
+      <c r="F13">
         <f t="shared" si="1"/>
         <v>196</v>
       </c>
-      <c r="G13" s="3">
+      <c r="G13">
         <f t="shared" si="2"/>
         <v>113.58333333333333</v>
       </c>
-      <c r="H13" s="3">
+      <c r="H13">
         <f t="shared" si="5"/>
         <v>2.5901942645698339</v>
       </c>
-      <c r="I13" s="3">
+      <c r="I13">
         <f t="shared" si="6"/>
         <v>1.6219367680212704</v>
       </c>
-      <c r="J13" s="3">
+      <c r="J13">
         <f t="shared" si="7"/>
         <v>7377.0694650764335</v>
       </c>
-      <c r="K13" s="3">
+      <c r="K13">
         <f t="shared" si="0"/>
         <v>385.93053492356648</v>
       </c>
-      <c r="L13" s="3">
+      <c r="L13">
         <v>0</v>
       </c>
       <c r="M13" s="2">
         <f t="shared" si="3"/>
         <v>7763</v>
       </c>
-      <c r="N13" s="3">
+      <c r="N13">
         <f t="shared" si="4"/>
         <v>121.296875</v>
       </c>
-      <c r="O13" s="3">
+      <c r="O13">
         <v>81966.600000000006</v>
       </c>
-      <c r="P13" s="3">
+      <c r="P13">
         <v>83496</v>
       </c>
-      <c r="Q13" s="3">
+      <c r="Q13">
         <f t="shared" si="8"/>
         <v>93.563529318163745</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A14" s="3">
+      <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" s="3">
         <v>45731</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" t="s">
         <v>19</v>
       </c>
       <c r="D14" s="2">
@@ -1925,60 +1925,60 @@
       <c r="E14" s="2">
         <v>7845</v>
       </c>
-      <c r="F14" s="3">
+      <c r="F14">
         <f t="shared" si="1"/>
         <v>82</v>
       </c>
-      <c r="G14" s="3">
+      <c r="G14">
         <f t="shared" si="2"/>
         <v>111.15384615384616</v>
       </c>
-      <c r="H14" s="3">
+      <c r="H14">
         <f t="shared" si="5"/>
         <v>1.0562926703594044</v>
       </c>
-      <c r="I14" s="3">
+      <c r="I14">
         <f t="shared" si="6"/>
         <v>1.5783135032505946</v>
       </c>
-      <c r="J14" s="3">
+      <c r="J14">
         <f t="shared" si="7"/>
         <v>7472.9713681224266</v>
       </c>
-      <c r="K14" s="3">
+      <c r="K14">
         <f t="shared" si="0"/>
         <v>372.02863187757339</v>
       </c>
-      <c r="L14" s="3">
+      <c r="L14">
         <v>0</v>
       </c>
       <c r="M14" s="2">
         <f t="shared" si="3"/>
         <v>7845</v>
       </c>
-      <c r="N14" s="3">
+      <c r="N14">
         <f t="shared" si="4"/>
         <v>122.578125</v>
       </c>
-      <c r="O14" s="3">
+      <c r="O14">
         <v>83496</v>
       </c>
-      <c r="P14" s="3">
+      <c r="P14">
         <v>84108.4</v>
       </c>
-      <c r="Q14" s="3">
+      <c r="Q14">
         <f t="shared" si="8"/>
         <v>94.249769441695918</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A15" s="3">
+      <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" s="3">
         <v>45732</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" t="s">
         <v>20</v>
       </c>
       <c r="D15" s="2">
@@ -1987,60 +1987,60 @@
       <c r="E15" s="2">
         <v>7879</v>
       </c>
-      <c r="F15" s="3">
+      <c r="F15">
         <f t="shared" si="1"/>
         <v>34</v>
       </c>
-      <c r="G15" s="3">
+      <c r="G15">
         <f t="shared" si="2"/>
         <v>105.64285714285714</v>
       </c>
-      <c r="H15" s="3">
+      <c r="H15">
         <f t="shared" si="5"/>
         <v>0.43339706819629509</v>
       </c>
-      <c r="I15" s="3">
+      <c r="I15">
         <f t="shared" si="6"/>
         <v>1.4961026704697122</v>
       </c>
-      <c r="J15" s="3">
+      <c r="J15">
         <f t="shared" si="7"/>
         <v>7570.1199959080177</v>
       </c>
-      <c r="K15" s="3">
+      <c r="K15">
         <f t="shared" si="0"/>
         <v>308.8800040919823</v>
       </c>
-      <c r="L15" s="3">
+      <c r="L15">
         <v>0</v>
       </c>
       <c r="M15" s="2">
         <f t="shared" si="3"/>
         <v>7879</v>
       </c>
-      <c r="N15" s="3">
+      <c r="N15">
         <f t="shared" si="4"/>
         <v>123.10937500000001</v>
       </c>
-      <c r="O15" s="3">
+      <c r="O15">
         <v>84108.4</v>
       </c>
-      <c r="P15" s="3">
+      <c r="P15">
         <v>83334.2</v>
       </c>
-      <c r="Q15" s="3">
+      <c r="Q15">
         <f t="shared" si="8"/>
         <v>93.382220284872574</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A16" s="3">
+      <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" s="3">
         <v>45733</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" t="s">
         <v>14</v>
       </c>
       <c r="D16" s="2">
@@ -2049,60 +2049,60 @@
       <c r="E16" s="2">
         <v>7952</v>
       </c>
-      <c r="F16" s="3">
+      <c r="F16">
         <f t="shared" si="1"/>
         <v>73</v>
       </c>
-      <c r="G16" s="3">
+      <c r="G16">
         <f t="shared" si="2"/>
         <v>103.46666666666667</v>
       </c>
-      <c r="H16" s="3">
+      <c r="H16">
         <f t="shared" si="5"/>
         <v>0.92651351694377215</v>
       </c>
-      <c r="I16" s="3">
+      <c r="I16">
         <f t="shared" si="6"/>
         <v>1.4580302525748934</v>
       </c>
-      <c r="J16" s="3">
+      <c r="J16">
         <f t="shared" si="7"/>
         <v>7668.5315558548209</v>
       </c>
-      <c r="K16" s="3">
+      <c r="K16">
         <f t="shared" si="0"/>
         <v>283.46844414517909</v>
       </c>
-      <c r="L16" s="3">
+      <c r="L16">
         <v>0</v>
       </c>
       <c r="M16" s="2">
         <f t="shared" si="3"/>
         <v>7952</v>
       </c>
-      <c r="N16" s="3">
+      <c r="N16">
         <f t="shared" si="4"/>
         <v>124.25</v>
       </c>
-      <c r="O16" s="3">
+      <c r="O16">
         <v>83334.2</v>
       </c>
-      <c r="P16" s="3">
+      <c r="P16">
         <v>82873.100000000006</v>
       </c>
-      <c r="Q16" s="3">
+      <c r="Q16">
         <f t="shared" si="8"/>
         <v>92.865523157242464</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A17" s="3">
+      <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" s="3">
         <v>45734</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" t="s">
         <v>15</v>
       </c>
       <c r="D17" s="2">
@@ -2111,60 +2111,60 @@
       <c r="E17" s="2">
         <v>7797</v>
       </c>
-      <c r="F17" s="3">
+      <c r="F17">
         <f t="shared" si="1"/>
         <v>-155</v>
       </c>
-      <c r="G17" s="3">
+      <c r="G17">
         <f t="shared" si="2"/>
         <v>87.3125</v>
       </c>
-      <c r="H17" s="3">
+      <c r="H17">
         <f t="shared" si="5"/>
         <v>-1.9491951710261524</v>
       </c>
-      <c r="I17" s="3">
+      <c r="I17">
         <f t="shared" si="6"/>
         <v>1.2416518639221996</v>
       </c>
-      <c r="J17" s="3">
+      <c r="J17">
         <f t="shared" si="7"/>
         <v>7768.2224660809325</v>
       </c>
-      <c r="K17" s="3">
+      <c r="K17">
         <f t="shared" si="0"/>
         <v>28.777533919067537</v>
       </c>
-      <c r="L17" s="3">
+      <c r="L17">
         <v>0</v>
       </c>
       <c r="M17" s="2">
         <f t="shared" si="3"/>
         <v>7797</v>
       </c>
-      <c r="N17" s="3">
+      <c r="N17">
         <f t="shared" si="4"/>
         <v>121.828125</v>
       </c>
-      <c r="O17" s="3">
+      <c r="O17">
         <v>82873.100000000006</v>
       </c>
-      <c r="P17" s="3">
+      <c r="P17">
         <v>81809.5</v>
       </c>
-      <c r="Q17" s="3">
+      <c r="Q17">
         <f t="shared" si="8"/>
         <v>91.673679598475573</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A18" s="3">
+      <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" s="3">
         <v>45735</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" t="s">
         <v>16</v>
       </c>
       <c r="D18" s="2">
@@ -2173,60 +2173,60 @@
       <c r="E18" s="2">
         <v>8335</v>
       </c>
-      <c r="F18" s="3">
+      <c r="F18">
         <f t="shared" si="1"/>
         <v>538</v>
       </c>
-      <c r="G18" s="3">
+      <c r="G18">
         <f t="shared" si="2"/>
         <v>113.82352941176471</v>
       </c>
-      <c r="H18" s="3">
+      <c r="H18">
         <f t="shared" si="5"/>
         <v>6.9000897781198001</v>
       </c>
-      <c r="I18" s="3">
+      <c r="I18">
         <f t="shared" si="6"/>
         <v>1.5660508945335661</v>
       </c>
-      <c r="J18" s="3">
+      <c r="J18">
         <f t="shared" si="7"/>
         <v>7869.209358139984</v>
       </c>
-      <c r="K18" s="3">
+      <c r="K18">
         <f t="shared" si="0"/>
         <v>465.79064186001597</v>
       </c>
-      <c r="L18" s="3">
+      <c r="L18">
         <v>0</v>
       </c>
       <c r="M18" s="2">
         <f t="shared" si="3"/>
         <v>8335</v>
       </c>
-      <c r="N18" s="3">
+      <c r="N18">
         <f t="shared" si="4"/>
         <v>130.234375</v>
       </c>
-      <c r="O18" s="3">
+      <c r="O18">
         <v>81809.5</v>
       </c>
-      <c r="P18" s="3">
+      <c r="P18">
         <v>84267.4</v>
       </c>
-      <c r="Q18" s="3">
+      <c r="Q18">
         <f t="shared" si="8"/>
         <v>94.427940865016652</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A19" s="3">
+      <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" s="3">
         <v>45736</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" t="s">
         <v>17</v>
       </c>
       <c r="D19" s="2">
@@ -2235,60 +2235,60 @@
       <c r="E19" s="2">
         <v>8461</v>
       </c>
-      <c r="F19" s="3">
+      <c r="F19">
         <f t="shared" si="1"/>
         <v>126</v>
       </c>
-      <c r="G19" s="3">
+      <c r="G19">
         <f t="shared" si="2"/>
         <v>114.5</v>
       </c>
-      <c r="H19" s="3">
+      <c r="H19">
         <f t="shared" si="5"/>
         <v>1.5116976604679033</v>
       </c>
-      <c r="I19" s="3">
+      <c r="I19">
         <f t="shared" si="6"/>
         <v>1.5630305070633677</v>
       </c>
-      <c r="J19" s="3">
+      <c r="J19">
         <f t="shared" si="7"/>
         <v>7971.5090797958028</v>
       </c>
-      <c r="K19" s="3">
+      <c r="K19">
         <f t="shared" si="0"/>
         <v>489.49092020419721</v>
       </c>
-      <c r="L19" s="3">
+      <c r="L19">
         <v>0</v>
       </c>
       <c r="M19" s="2">
         <f t="shared" si="3"/>
         <v>8461</v>
       </c>
-      <c r="N19" s="3">
+      <c r="N19">
         <f t="shared" si="4"/>
         <v>132.203125</v>
       </c>
-      <c r="O19" s="3">
+      <c r="O19">
         <v>84267.4</v>
       </c>
-      <c r="P19" s="3">
+      <c r="P19">
         <v>86123.6</v>
       </c>
-      <c r="Q19" s="3">
+      <c r="Q19">
         <f t="shared" si="8"/>
         <v>96.507952160412572</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A20" s="3">
+      <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" s="3">
         <v>45737</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" t="s">
         <v>18</v>
       </c>
       <c r="D20" s="2">
@@ -2297,60 +2297,60 @@
       <c r="E20" s="2">
         <v>8330</v>
       </c>
-      <c r="F20" s="3">
+      <c r="F20">
         <f t="shared" si="1"/>
         <v>-131</v>
       </c>
-      <c r="G20" s="3">
+      <c r="G20">
         <f t="shared" si="2"/>
         <v>101.57894736842105</v>
       </c>
-      <c r="H20" s="3">
+      <c r="H20">
         <f t="shared" si="5"/>
         <v>-1.5482803451128735</v>
       </c>
-      <c r="I20" s="3">
+      <c r="I20">
         <f t="shared" si="6"/>
         <v>1.3968527401524877</v>
       </c>
-      <c r="J20" s="3">
+      <c r="J20">
         <f t="shared" si="7"/>
         <v>8075.1386978331475</v>
       </c>
-      <c r="K20" s="3">
+      <c r="K20">
         <f t="shared" si="0"/>
         <v>254.86130216685251</v>
       </c>
-      <c r="L20" s="3">
+      <c r="L20">
         <v>0</v>
       </c>
       <c r="M20" s="2">
         <f t="shared" si="3"/>
         <v>8330</v>
       </c>
-      <c r="N20" s="3">
+      <c r="N20">
         <f t="shared" si="4"/>
         <v>130.15625</v>
       </c>
-      <c r="O20" s="3">
+      <c r="O20">
         <v>86123.6</v>
       </c>
-      <c r="P20" s="3">
+      <c r="P20">
         <v>84200</v>
       </c>
-      <c r="Q20" s="3">
+      <c r="Q20">
         <f t="shared" si="8"/>
         <v>94.352414110728503</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A21" s="3">
+      <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" s="3">
         <v>45738</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" t="s">
         <v>19</v>
       </c>
       <c r="D21" s="2">
@@ -2359,60 +2359,60 @@
       <c r="E21" s="2">
         <v>8331</v>
       </c>
-      <c r="F21" s="3">
+      <c r="F21">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="G21" s="3">
+      <c r="G21">
         <f t="shared" si="2"/>
         <v>96.55</v>
       </c>
-      <c r="H21" s="3">
+      <c r="H21">
         <f t="shared" si="5"/>
         <v>1.2004801920761921E-2</v>
       </c>
-      <c r="I21" s="3">
+      <c r="I21">
         <f t="shared" si="6"/>
         <v>1.3271571111354463</v>
       </c>
-      <c r="J21" s="3">
+      <c r="J21">
         <f t="shared" si="7"/>
         <v>8180.115500904978</v>
       </c>
-      <c r="K21" s="3">
+      <c r="K21">
         <f t="shared" si="0"/>
         <v>150.88449909502197</v>
       </c>
-      <c r="L21" s="3">
+      <c r="L21">
         <v>0</v>
       </c>
       <c r="M21" s="2">
         <f t="shared" si="3"/>
         <v>8331</v>
       </c>
-      <c r="N21" s="3">
+      <c r="N21">
         <f t="shared" si="4"/>
         <v>130.171875</v>
       </c>
-      <c r="O21" s="3">
+      <c r="O21">
         <v>84200</v>
       </c>
-      <c r="P21" s="3">
+      <c r="P21">
         <v>83970.6</v>
       </c>
-      <c r="Q21" s="3">
+      <c r="Q21">
         <f t="shared" si="8"/>
         <v>94.095354208151292</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A22" s="3">
+      <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" s="3">
         <v>45739</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" t="s">
         <v>20</v>
       </c>
       <c r="D22" s="2">
@@ -2421,60 +2421,60 @@
       <c r="E22" s="2">
         <v>8590</v>
       </c>
-      <c r="F22" s="3">
+      <c r="F22">
         <f t="shared" si="1"/>
         <v>259</v>
       </c>
-      <c r="G22" s="3">
+      <c r="G22">
         <f t="shared" si="2"/>
         <v>104.28571428571429</v>
       </c>
-      <c r="H22" s="3">
+      <c r="H22">
         <f t="shared" si="5"/>
         <v>3.1088704837354486</v>
       </c>
-      <c r="I22" s="3">
+      <c r="I22">
         <f t="shared" si="6"/>
         <v>1.4112982170128241</v>
       </c>
-      <c r="J22" s="3">
+      <c r="J22">
         <f t="shared" si="7"/>
         <v>8286.4570024167424</v>
       </c>
-      <c r="K22" s="3">
+      <c r="K22">
         <f t="shared" si="0"/>
         <v>303.5429975832576</v>
       </c>
-      <c r="L22" s="3">
+      <c r="L22">
         <v>0</v>
       </c>
       <c r="M22" s="2">
         <f t="shared" si="3"/>
         <v>8590</v>
       </c>
-      <c r="N22" s="3">
+      <c r="N22">
         <f t="shared" si="4"/>
         <v>134.21875</v>
       </c>
-      <c r="O22" s="3">
+      <c r="O22">
         <v>83970.6</v>
       </c>
-      <c r="P22" s="3">
+      <c r="P22">
         <v>84862</v>
       </c>
-      <c r="Q22" s="3">
+      <c r="Q22">
         <f t="shared" si="8"/>
         <v>95.094234753736842</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A23" s="3">
+      <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" s="3">
         <v>45740</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" t="s">
         <v>14</v>
       </c>
       <c r="D23" s="2">
@@ -2483,60 +2483,60 @@
       <c r="E23" s="2">
         <v>8925</v>
       </c>
-      <c r="F23" s="3">
+      <c r="F23">
         <f t="shared" si="1"/>
         <v>335</v>
       </c>
-      <c r="G23" s="3">
+      <c r="G23">
         <f>(E23-$D$2)/A23</f>
         <v>114.77272727272727</v>
       </c>
-      <c r="H23" s="3">
+      <c r="H23">
         <f t="shared" si="5"/>
         <v>3.8998835855646119</v>
       </c>
-      <c r="I23" s="3">
+      <c r="I23">
         <f t="shared" si="6"/>
         <v>1.5231117007673323</v>
       </c>
-      <c r="J23" s="3">
+      <c r="J23">
         <f t="shared" si="7"/>
         <v>8394.1809434481584</v>
       </c>
-      <c r="K23" s="3">
+      <c r="K23">
         <f t="shared" si="0"/>
         <v>530.81905655184164</v>
       </c>
-      <c r="L23" s="3">
+      <c r="L23">
         <v>0</v>
       </c>
       <c r="M23" s="2">
         <f t="shared" si="3"/>
         <v>8925</v>
       </c>
-      <c r="N23" s="3">
+      <c r="N23">
         <f t="shared" si="4"/>
         <v>139.453125</v>
       </c>
-      <c r="O23" s="3">
+      <c r="O23">
         <v>84862</v>
       </c>
-      <c r="P23" s="3">
+      <c r="P23">
         <v>87921</v>
       </c>
-      <c r="Q23" s="3">
+      <c r="Q23">
         <f t="shared" si="8"/>
         <v>98.522073646429462</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A24" s="3">
+      <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" s="3">
         <v>45741</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" t="s">
         <v>15</v>
       </c>
       <c r="D24" s="2">
@@ -2545,60 +2545,60 @@
       <c r="E24" s="2">
         <v>9113</v>
       </c>
-      <c r="F24" s="3">
+      <c r="F24">
         <f t="shared" si="1"/>
         <v>188</v>
       </c>
-      <c r="G24" s="3">
+      <c r="G24">
         <f>(E24-$D$2)/A24</f>
         <v>117.95652173913044</v>
       </c>
-      <c r="H24" s="3">
+      <c r="H24">
         <f t="shared" si="5"/>
         <v>2.1064425770308093</v>
       </c>
-      <c r="I24" s="3">
+      <c r="I24">
         <f t="shared" si="6"/>
         <v>1.5484044777758443</v>
       </c>
-      <c r="J24" s="3">
+      <c r="J24">
         <f t="shared" si="7"/>
         <v>8503.3052957129839</v>
       </c>
-      <c r="K24" s="3">
+      <c r="K24">
         <f t="shared" si="0"/>
         <v>609.69470428701607</v>
       </c>
-      <c r="L24" s="3">
+      <c r="L24">
         <v>0</v>
       </c>
       <c r="M24" s="2">
         <f t="shared" si="3"/>
         <v>9113</v>
       </c>
-      <c r="N24" s="3">
+      <c r="N24">
         <f t="shared" si="4"/>
         <v>142.390625</v>
       </c>
-      <c r="O24" s="3">
+      <c r="O24">
         <v>87921</v>
       </c>
-      <c r="P24" s="3">
+      <c r="P24">
         <v>87985.1</v>
       </c>
-      <c r="Q24" s="3">
+      <c r="Q24">
         <f t="shared" si="8"/>
         <v>98.59390250325248</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A25" s="3">
+      <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" s="3">
         <v>45742</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25" t="s">
         <v>16</v>
       </c>
       <c r="D25" s="2">
@@ -2607,60 +2607,60 @@
       <c r="E25" s="2">
         <v>9163</v>
       </c>
-      <c r="F25" s="3">
+      <c r="F25">
         <f t="shared" ref="F25" si="9">E25-D25</f>
         <v>50</v>
       </c>
-      <c r="G25" s="3">
+      <c r="G25">
         <f>(E25-$D$2)/A25</f>
         <v>115.125</v>
       </c>
-      <c r="H25" s="3">
+      <c r="H25">
         <f t="shared" ref="H25" si="10">(E25/D25-1)*100</f>
         <v>0.54866673982223446</v>
       </c>
-      <c r="I25" s="3">
+      <c r="I25">
         <f t="shared" ref="I25" si="11">(POWER((E25/$D$3),1/A25)-1)*100</f>
         <v>1.5065509612034012</v>
       </c>
-      <c r="J25" s="3">
+      <c r="J25">
         <f t="shared" si="7"/>
         <v>8613.8482645572512</v>
       </c>
-      <c r="K25" s="3">
+      <c r="K25">
         <f t="shared" si="0"/>
         <v>549.15173544274876</v>
       </c>
-      <c r="L25" s="3">
+      <c r="L25">
         <v>0</v>
       </c>
       <c r="M25" s="2">
         <f t="shared" ref="M25" si="12">L25+E25</f>
         <v>9163</v>
       </c>
-      <c r="N25" s="3">
+      <c r="N25">
         <f t="shared" si="4"/>
         <v>143.171875</v>
       </c>
-      <c r="O25" s="3">
+      <c r="O25">
         <v>87985.1</v>
       </c>
-      <c r="P25" s="3">
+      <c r="P25">
         <v>86736.1</v>
       </c>
-      <c r="Q25" s="3">
+      <c r="Q25">
         <f t="shared" si="8"/>
         <v>97.194304341443697</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A26" s="3">
+      <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" s="3">
         <v>45743</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C26" t="s">
         <v>17</v>
       </c>
       <c r="D26" s="2">
@@ -2669,60 +2669,60 @@
       <c r="E26" s="2">
         <v>9353</v>
       </c>
-      <c r="F26" s="3">
+      <c r="F26">
         <f t="shared" ref="F26" si="13">E26-D26</f>
         <v>190</v>
       </c>
-      <c r="G26" s="3">
+      <c r="G26">
         <f>(E26-$D$2)/A26</f>
         <v>118.12</v>
       </c>
-      <c r="H26" s="3">
+      <c r="H26">
         <f t="shared" ref="H26" si="14">(E26/D26-1)*100</f>
         <v>2.0735566954054319</v>
       </c>
-      <c r="I26" s="3">
+      <c r="I26">
         <f t="shared" ref="I26" si="15">(POWER((E26/$D$3),1/A26)-1)*100</f>
         <v>1.5291706005972516</v>
       </c>
-      <c r="J26" s="3">
+      <c r="J26">
         <f t="shared" si="7"/>
         <v>8725.828291996495</v>
       </c>
-      <c r="K26" s="3">
+      <c r="K26">
         <f t="shared" si="0"/>
         <v>627.17170800350505</v>
       </c>
-      <c r="L26" s="3">
+      <c r="L26">
         <v>0</v>
       </c>
       <c r="M26" s="2">
         <f t="shared" ref="M26" si="16">L26+E26</f>
         <v>9353</v>
       </c>
-      <c r="N26" s="3">
+      <c r="N26">
         <f t="shared" si="4"/>
         <v>146.140625</v>
       </c>
-      <c r="O26" s="3">
+      <c r="O26">
         <v>86736.1</v>
       </c>
-      <c r="P26" s="3">
+      <c r="P26">
         <v>87249.1</v>
       </c>
-      <c r="Q26" s="3">
+      <c r="Q26">
         <f t="shared" si="8"/>
         <v>97.769159311025689</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A27" s="3">
+      <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" s="3">
         <v>45744</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C27" t="s">
         <v>18</v>
       </c>
       <c r="D27" s="2">
@@ -2731,60 +2731,60 @@
       <c r="E27" s="2">
         <v>9353</v>
       </c>
-      <c r="F27" s="3">
+      <c r="F27">
         <f t="shared" ref="F27:F32" si="17">E27-D27</f>
         <v>0</v>
       </c>
-      <c r="G27" s="3">
+      <c r="G27">
         <f t="shared" ref="G27:G31" si="18">(E27-$D$2)/A27</f>
         <v>113.57692307692308</v>
       </c>
-      <c r="H27" s="3">
+      <c r="H27">
         <f t="shared" ref="H27:H32" si="19">(E27/D27-1)*100</f>
         <v>0</v>
       </c>
-      <c r="I27" s="3">
+      <c r="I27">
         <f t="shared" ref="I27:I32" si="20">(POWER((E27/$D$3),1/A27)-1)*100</f>
         <v>1.4699262282590997</v>
       </c>
-      <c r="J27" s="3">
+      <c r="J27">
         <f t="shared" si="7"/>
         <v>8839.2640597924492</v>
       </c>
-      <c r="K27" s="3">
+      <c r="K27">
         <f t="shared" si="0"/>
         <v>513.73594020755081</v>
       </c>
-      <c r="L27" s="3">
+      <c r="L27">
         <v>0</v>
       </c>
       <c r="M27" s="2">
         <f t="shared" ref="M27:M32" si="21">L27+E27</f>
         <v>9353</v>
       </c>
-      <c r="N27" s="3">
+      <c r="N27">
         <f t="shared" si="4"/>
         <v>146.140625</v>
       </c>
-      <c r="O27" s="3">
+      <c r="O27">
         <v>87249.1</v>
       </c>
-      <c r="P27" s="3">
+      <c r="P27">
         <v>84105.3</v>
       </c>
-      <c r="Q27" s="3">
+      <c r="Q27">
         <f t="shared" si="8"/>
         <v>94.246295659228679</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A28" s="3">
+      <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" s="3">
         <v>45745</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C28" t="s">
         <v>19</v>
       </c>
       <c r="D28" s="2">
@@ -2793,60 +2793,60 @@
       <c r="E28" s="2">
         <v>9400</v>
       </c>
-      <c r="F28" s="3">
+      <c r="F28">
         <f t="shared" si="17"/>
         <v>47</v>
       </c>
-      <c r="G28" s="3">
+      <c r="G28">
         <f t="shared" si="18"/>
         <v>111.11111111111111</v>
       </c>
-      <c r="H28" s="3">
+      <c r="H28">
         <f t="shared" si="19"/>
         <v>0.50251256281406143</v>
       </c>
-      <c r="I28" s="3">
+      <c r="I28">
         <f t="shared" si="20"/>
         <v>1.433930583006493</v>
       </c>
-      <c r="J28" s="3">
+      <c r="J28">
         <f t="shared" si="7"/>
         <v>8954.1744925697494</v>
       </c>
-      <c r="K28" s="3">
+      <c r="K28">
         <f t="shared" si="0"/>
         <v>445.82550743025058</v>
       </c>
-      <c r="L28" s="3">
+      <c r="L28">
         <v>0</v>
       </c>
       <c r="M28" s="2">
         <f t="shared" si="21"/>
         <v>9400</v>
       </c>
-      <c r="N28" s="3">
+      <c r="N28">
         <f t="shared" si="4"/>
         <v>146.875</v>
       </c>
-      <c r="O28" s="3">
+      <c r="O28">
         <v>84105.3</v>
       </c>
-      <c r="P28" s="3">
+      <c r="P28">
         <v>82428.800000000003</v>
       </c>
-      <c r="Q28" s="3">
+      <c r="Q28">
         <f t="shared" si="8"/>
         <v>92.367651689434894</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A29" s="3">
+      <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" s="3">
         <v>45746</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C29" t="s">
         <v>20</v>
       </c>
       <c r="D29" s="2">
@@ -2855,60 +2855,60 @@
       <c r="E29" s="2">
         <v>9450</v>
       </c>
-      <c r="F29" s="3">
+      <c r="F29">
         <f t="shared" si="17"/>
         <v>50</v>
       </c>
-      <c r="G29" s="3">
+      <c r="G29">
         <f t="shared" si="18"/>
         <v>108.92857142857143</v>
       </c>
-      <c r="H29" s="3">
+      <c r="H29">
         <f t="shared" si="19"/>
         <v>0.53191489361701372</v>
       </c>
-      <c r="I29" s="3">
+      <c r="I29">
         <f t="shared" si="20"/>
         <v>1.4015768054668865</v>
       </c>
-      <c r="J29" s="3">
+      <c r="J29">
         <f t="shared" si="7"/>
         <v>9070.578760973156</v>
       </c>
-      <c r="K29" s="3">
+      <c r="K29">
         <f t="shared" si="0"/>
         <v>379.42123902684398</v>
       </c>
-      <c r="L29" s="3">
+      <c r="L29">
         <v>0</v>
       </c>
       <c r="M29" s="2">
         <f t="shared" si="21"/>
         <v>9450</v>
       </c>
-      <c r="N29" s="3">
+      <c r="N29">
         <f t="shared" si="4"/>
         <v>147.65625</v>
       </c>
-      <c r="O29" s="3">
+      <c r="O29">
         <v>82428.800000000003</v>
       </c>
-      <c r="P29" s="3">
+      <c r="P29">
         <v>82745.100000000006</v>
       </c>
-      <c r="Q29" s="3">
+      <c r="Q29">
         <f t="shared" si="8"/>
         <v>92.72208955859432</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A30" s="3">
+      <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" s="3">
         <v>45747</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C30" t="s">
         <v>14</v>
       </c>
       <c r="D30" s="2">
@@ -2917,60 +2917,60 @@
       <c r="E30" s="2">
         <v>9452</v>
       </c>
-      <c r="F30" s="3">
+      <c r="F30">
         <f t="shared" si="17"/>
         <v>2</v>
       </c>
-      <c r="G30" s="3">
+      <c r="G30">
         <f t="shared" si="18"/>
         <v>105.24137931034483</v>
       </c>
-      <c r="H30" s="3">
+      <c r="H30">
         <f t="shared" si="19"/>
         <v>2.1164021164010727E-2</v>
       </c>
-      <c r="I30" s="3">
+      <c r="I30">
         <f t="shared" si="20"/>
         <v>1.3536607182727423</v>
       </c>
-      <c r="J30" s="3">
+      <c r="J30">
         <f t="shared" si="7"/>
         <v>9188.496284865807</v>
       </c>
-      <c r="K30" s="3">
+      <c r="K30">
         <f t="shared" si="0"/>
         <v>263.50371513419304</v>
       </c>
-      <c r="L30" s="3">
+      <c r="L30">
         <v>0</v>
       </c>
       <c r="M30" s="2">
         <f t="shared" si="21"/>
         <v>9452</v>
       </c>
-      <c r="N30" s="3">
+      <c r="N30">
         <f t="shared" si="4"/>
         <v>147.6875</v>
       </c>
-      <c r="O30" s="3">
+      <c r="O30">
         <v>82745.100000000006</v>
       </c>
-      <c r="P30" s="3">
+      <c r="P30">
         <v>83448.100000000006</v>
       </c>
-      <c r="Q30" s="3">
+      <c r="Q30">
         <f t="shared" si="8"/>
         <v>93.509853776169635</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A31" s="3">
+      <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" s="3">
         <v>45748</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C31" t="s">
         <v>15</v>
       </c>
       <c r="D31" s="2">
@@ -2979,60 +2979,60 @@
       <c r="E31" s="2">
         <v>9512</v>
       </c>
-      <c r="F31" s="3">
+      <c r="F31">
         <f t="shared" si="17"/>
         <v>60</v>
       </c>
-      <c r="G31" s="3">
+      <c r="G31">
         <f t="shared" si="18"/>
         <v>103.73333333333333</v>
       </c>
-      <c r="H31" s="3">
+      <c r="H31">
         <f t="shared" si="19"/>
         <v>0.6347862886161737</v>
       </c>
-      <c r="I31" s="3">
+      <c r="I31">
         <f t="shared" si="20"/>
         <v>1.3296157062268277</v>
       </c>
-      <c r="J31" s="3">
+      <c r="J31">
         <f t="shared" si="7"/>
         <v>9307.9467365690616</v>
       </c>
-      <c r="K31" s="3">
+      <c r="K31">
         <f t="shared" si="0"/>
         <v>204.05326343093839</v>
       </c>
-      <c r="L31" s="3">
+      <c r="L31">
         <v>0</v>
       </c>
       <c r="M31" s="2">
         <f t="shared" si="21"/>
         <v>9512</v>
       </c>
-      <c r="N31" s="3">
+      <c r="N31">
         <f t="shared" si="4"/>
         <v>148.625</v>
       </c>
-      <c r="O31" s="3">
+      <c r="O31">
         <v>83448.100000000006</v>
       </c>
-      <c r="P31" s="3">
+      <c r="P31">
         <v>84138.9</v>
       </c>
-      <c r="Q31" s="3">
+      <c r="Q31">
         <f t="shared" si="8"/>
         <v>94.2839469788738</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A32" s="3">
+      <c r="A32">
         <v>31</v>
       </c>
       <c r="B32" s="3">
         <v>45749</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C32" t="s">
         <v>16</v>
       </c>
       <c r="D32" s="2">
@@ -3041,60 +3041,60 @@
       <c r="E32" s="2">
         <v>9666</v>
       </c>
-      <c r="F32" s="3">
+      <c r="F32">
         <f t="shared" si="17"/>
         <v>154</v>
       </c>
-      <c r="G32" s="3">
+      <c r="G32">
         <f>(E32-$D$2)/A32</f>
         <v>105.35483870967742</v>
       </c>
-      <c r="H32" s="3">
+      <c r="H32">
         <f t="shared" si="19"/>
         <v>1.619007569386044</v>
       </c>
-      <c r="I32" s="3">
+      <c r="I32">
         <f t="shared" si="20"/>
         <v>1.3389380513060933</v>
       </c>
-      <c r="J32" s="3">
+      <c r="J32">
         <f t="shared" si="7"/>
         <v>9428.9500441444579</v>
       </c>
-      <c r="K32" s="3">
+      <c r="K32">
         <f t="shared" si="0"/>
         <v>237.04995585554207</v>
       </c>
-      <c r="L32" s="3">
+      <c r="L32">
         <v>0</v>
       </c>
       <c r="M32" s="2">
         <f t="shared" si="21"/>
         <v>9666</v>
       </c>
-      <c r="N32" s="3">
+      <c r="N32">
         <f t="shared" si="4"/>
         <v>151.03125</v>
       </c>
-      <c r="O32" s="3">
+      <c r="O32">
         <v>84138.9</v>
       </c>
-      <c r="P32" s="3">
+      <c r="P32">
         <v>85827.9</v>
       </c>
-      <c r="Q32" s="3">
+      <c r="Q32">
         <f t="shared" si="8"/>
         <v>96.176598136035565</v>
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A33" s="3">
+      <c r="A33">
         <v>32</v>
       </c>
       <c r="B33" s="3">
         <v>45750</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C33" t="s">
         <v>17</v>
       </c>
       <c r="D33" s="2">
@@ -3103,60 +3103,60 @@
       <c r="E33" s="2">
         <v>9890</v>
       </c>
-      <c r="F33" s="3">
+      <c r="F33">
         <f t="shared" ref="F33:F41" si="22">E33-D33</f>
         <v>224</v>
       </c>
-      <c r="G33" s="3">
+      <c r="G33">
         <f t="shared" ref="G33:G41" si="23">(E33-$D$2)/A33</f>
         <v>109.0625</v>
       </c>
-      <c r="H33" s="3">
+      <c r="H33">
         <f t="shared" ref="H33:H41" si="24">(E33/D33-1)*100</f>
         <v>2.3174012000827693</v>
       </c>
-      <c r="I33" s="3">
+      <c r="I33">
         <f t="shared" ref="I33:I41" si="25">(POWER((E33/$D$3),1/A33)-1)*100</f>
         <v>1.3693729216394335</v>
       </c>
-      <c r="J33" s="3">
+      <c r="J33">
         <f t="shared" si="7"/>
         <v>9551.5263947183357</v>
       </c>
-      <c r="K33" s="3">
+      <c r="K33">
         <f t="shared" si="0"/>
         <v>338.47360528166428</v>
       </c>
-      <c r="L33" s="3">
+      <c r="L33">
         <v>0</v>
       </c>
       <c r="M33" s="2">
         <f t="shared" ref="M33:M41" si="26">L33+E33</f>
         <v>9890</v>
       </c>
-      <c r="N33" s="3">
+      <c r="N33">
         <f t="shared" si="4"/>
         <v>154.53125</v>
       </c>
-      <c r="O33" s="3">
+      <c r="O33">
         <v>85827.9</v>
       </c>
-      <c r="P33" s="3">
+      <c r="P33">
         <v>81465.600000000006</v>
       </c>
-      <c r="Q33" s="3">
+      <c r="Q33">
         <f t="shared" si="8"/>
         <v>91.288313859607655</v>
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A34" s="3">
+      <c r="A34">
         <v>33</v>
       </c>
       <c r="B34" s="3">
         <v>45751</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C34" t="s">
         <v>18</v>
       </c>
       <c r="D34" s="2">
@@ -3165,60 +3165,60 @@
       <c r="E34" s="2">
         <v>10200</v>
       </c>
-      <c r="F34" s="3">
+      <c r="F34">
         <f t="shared" si="22"/>
         <v>310</v>
       </c>
-      <c r="G34" s="3">
+      <c r="G34">
         <f t="shared" si="23"/>
         <v>115.15151515151516</v>
       </c>
-      <c r="H34" s="3">
+      <c r="H34">
         <f t="shared" si="24"/>
         <v>3.1344792719919079</v>
       </c>
-      <c r="I34" s="3">
+      <c r="I34">
         <f t="shared" si="25"/>
         <v>1.4224145175464553</v>
       </c>
-      <c r="J34" s="3">
+      <c r="J34">
         <f t="shared" si="7"/>
         <v>9675.6962378496737</v>
       </c>
-      <c r="K34" s="3">
+      <c r="K34">
         <f t="shared" si="0"/>
         <v>524.30376215032629</v>
       </c>
-      <c r="L34" s="3">
+      <c r="L34">
         <v>0</v>
       </c>
       <c r="M34" s="2">
         <f t="shared" si="26"/>
         <v>10200</v>
       </c>
-      <c r="N34" s="3">
+      <c r="N34">
         <f t="shared" si="4"/>
         <v>159.375</v>
       </c>
-      <c r="O34" s="3">
+      <c r="O34">
         <v>81465.600000000006</v>
       </c>
-      <c r="P34" s="3">
+      <c r="P34">
         <v>82498</v>
       </c>
-      <c r="Q34" s="3">
+      <c r="Q34">
         <f t="shared" si="8"/>
         <v>92.445195478704036</v>
       </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A35" s="3">
+      <c r="A35">
         <v>34</v>
       </c>
       <c r="B35" s="3">
         <v>45752</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C35" t="s">
         <v>19</v>
       </c>
       <c r="D35" s="2">
@@ -3227,60 +3227,60 @@
       <c r="E35" s="2">
         <v>10565</v>
       </c>
-      <c r="F35" s="3">
+      <c r="F35">
         <f t="shared" si="22"/>
         <v>365</v>
       </c>
-      <c r="G35" s="3">
+      <c r="G35">
         <f t="shared" si="23"/>
         <v>122.5</v>
       </c>
-      <c r="H35" s="3">
+      <c r="H35">
         <f t="shared" si="24"/>
         <v>3.5784313725490291</v>
       </c>
-      <c r="I35" s="3">
+      <c r="I35">
         <f t="shared" si="25"/>
         <v>1.4851815919634914</v>
       </c>
-      <c r="J35" s="3">
+      <c r="J35">
         <f t="shared" si="7"/>
         <v>9801.4802889417188</v>
       </c>
-      <c r="K35" s="3">
+      <c r="K35">
         <f t="shared" si="0"/>
         <v>763.51971105828125</v>
       </c>
-      <c r="L35" s="3">
+      <c r="L35">
         <v>0</v>
       </c>
       <c r="M35" s="2">
         <f t="shared" si="26"/>
         <v>10565</v>
       </c>
-      <c r="N35" s="3">
+      <c r="N35">
         <f t="shared" si="4"/>
         <v>165.078125</v>
       </c>
-      <c r="O35" s="3">
+      <c r="O35">
         <v>82498</v>
       </c>
-      <c r="P35" s="3">
+      <c r="P35">
         <v>82847.899999999994</v>
       </c>
-      <c r="Q35" s="3">
+      <c r="Q35">
         <f t="shared" si="8"/>
         <v>92.837284667508584</v>
       </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A36" s="3">
+      <c r="A36">
         <v>35</v>
       </c>
       <c r="B36" s="3">
         <v>45753</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="C36" t="s">
         <v>20</v>
       </c>
       <c r="D36" s="2">
@@ -3289,60 +3289,60 @@
       <c r="E36" s="2">
         <v>10845</v>
       </c>
-      <c r="F36" s="3">
+      <c r="F36">
         <f t="shared" si="22"/>
         <v>280</v>
       </c>
-      <c r="G36" s="3">
+      <c r="G36">
         <f t="shared" si="23"/>
         <v>127</v>
       </c>
-      <c r="H36" s="3">
+      <c r="H36">
         <f t="shared" si="24"/>
         <v>2.6502602934216801</v>
       </c>
-      <c r="I36" s="3">
+      <c r="I36">
         <f t="shared" si="25"/>
         <v>1.5182853250945039</v>
       </c>
-      <c r="J36" s="3">
+      <c r="J36">
         <f t="shared" si="7"/>
         <v>9928.8995326979602</v>
       </c>
-      <c r="K36" s="3">
+      <c r="K36">
         <f t="shared" si="0"/>
         <v>916.10046730203976</v>
       </c>
-      <c r="L36" s="3">
+      <c r="L36">
         <v>0</v>
       </c>
       <c r="M36" s="2">
         <f t="shared" si="26"/>
         <v>10845</v>
       </c>
-      <c r="N36" s="3">
+      <c r="N36">
         <f t="shared" si="4"/>
         <v>169.453125</v>
       </c>
-      <c r="O36" s="3">
+      <c r="O36">
         <v>82847.899999999994</v>
       </c>
-      <c r="P36" s="3">
+      <c r="P36">
         <v>82606.7</v>
       </c>
-      <c r="Q36" s="3">
+      <c r="Q36">
         <f t="shared" si="8"/>
         <v>92.567001980056006</v>
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A37" s="3">
+      <c r="A37">
         <v>36</v>
       </c>
       <c r="B37" s="3">
         <v>45754</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="C37" t="s">
         <v>14</v>
       </c>
       <c r="D37" s="2">
@@ -3351,60 +3351,60 @@
       <c r="E37" s="2">
         <v>22699</v>
       </c>
-      <c r="F37" s="3">
+      <c r="F37">
         <f t="shared" si="22"/>
         <v>1854</v>
       </c>
-      <c r="G37" s="3">
+      <c r="G37">
         <f t="shared" si="23"/>
         <v>452.75</v>
       </c>
-      <c r="H37" s="3">
+      <c r="H37">
         <f t="shared" si="24"/>
         <v>8.8942192372271514</v>
       </c>
-      <c r="I37" s="3">
+      <c r="I37">
         <f t="shared" si="25"/>
         <v>3.5792984780890658</v>
       </c>
-      <c r="J37" s="3">
+      <c r="J37">
         <f t="shared" si="7"/>
         <v>10057.975226623033</v>
       </c>
-      <c r="K37" s="3">
+      <c r="K37">
         <f>M37-J37</f>
         <v>2641.0247733769666</v>
       </c>
-      <c r="L37" s="3">
+      <c r="L37">
         <v>-10000</v>
       </c>
       <c r="M37" s="2">
         <f t="shared" si="26"/>
         <v>12699</v>
       </c>
-      <c r="N37" s="3">
+      <c r="N37">
         <f t="shared" si="4"/>
         <v>198.421875</v>
       </c>
-      <c r="O37" s="3">
+      <c r="O37">
         <v>82606.7</v>
       </c>
-      <c r="P37" s="3">
+      <c r="P37">
         <v>78951.899999999994</v>
       </c>
-      <c r="Q37" s="3">
+      <c r="Q37">
         <f t="shared" si="8"/>
         <v>88.471524508655889</v>
       </c>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A38" s="3">
+      <c r="A38">
         <v>37</v>
       </c>
       <c r="B38" s="3">
         <v>45755</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="C38" t="s">
         <v>15</v>
       </c>
       <c r="D38" s="2">
@@ -3413,60 +3413,60 @@
       <c r="E38" s="2">
         <v>22955</v>
       </c>
-      <c r="F38" s="3">
+      <c r="F38">
         <f t="shared" si="22"/>
         <v>256</v>
       </c>
-      <c r="G38" s="3">
+      <c r="G38">
         <f t="shared" si="23"/>
         <v>447.43243243243245</v>
       </c>
-      <c r="H38" s="3">
+      <c r="H38">
         <f t="shared" si="24"/>
         <v>1.1278029869157269</v>
       </c>
-      <c r="I38" s="3">
+      <c r="I38">
         <f t="shared" si="25"/>
         <v>3.5122668721563333</v>
       </c>
-      <c r="J38" s="3">
+      <c r="J38">
         <f t="shared" si="7"/>
         <v>10188.728904569132</v>
       </c>
-      <c r="K38" s="3">
+      <c r="K38">
         <f t="shared" ref="K38:K41" si="27">M38-J38</f>
         <v>2766.2710954308677</v>
       </c>
-      <c r="L38" s="3">
+      <c r="L38">
         <v>-10000</v>
       </c>
       <c r="M38" s="2">
         <f t="shared" si="26"/>
         <v>12955</v>
       </c>
-      <c r="N38" s="3">
+      <c r="N38">
         <f t="shared" si="4"/>
         <v>202.42187500000003</v>
       </c>
-      <c r="O38" s="3">
+      <c r="O38">
         <v>78951.899999999994</v>
       </c>
-      <c r="P38" s="3">
+      <c r="P38">
         <v>78410.600000000006</v>
       </c>
-      <c r="Q38" s="3">
+      <c r="Q38">
         <f t="shared" si="8"/>
         <v>87.864957266872793</v>
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A39" s="3">
+      <c r="A39">
         <v>38</v>
       </c>
       <c r="B39" s="3">
         <v>45756</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="C39" t="s">
         <v>16</v>
       </c>
       <c r="D39" s="2">
@@ -3475,60 +3475,60 @@
       <c r="E39" s="2">
         <v>24388</v>
       </c>
-      <c r="F39" s="3">
+      <c r="F39">
         <f t="shared" si="22"/>
         <v>1433</v>
       </c>
-      <c r="G39" s="3">
+      <c r="G39">
         <f t="shared" si="23"/>
         <v>473.36842105263156</v>
       </c>
-      <c r="H39" s="3">
+      <c r="H39">
         <f t="shared" si="24"/>
         <v>6.2426486604225673</v>
       </c>
-      <c r="I39" s="3">
+      <c r="I39">
         <f t="shared" si="25"/>
         <v>3.5832120312270677</v>
       </c>
-      <c r="J39" s="3">
+      <c r="J39">
         <f t="shared" si="7"/>
         <v>10321.18238032853</v>
       </c>
-      <c r="K39" s="3">
+      <c r="K39">
         <f t="shared" si="27"/>
         <v>4066.8176196714703</v>
       </c>
-      <c r="L39" s="3">
+      <c r="L39">
         <v>-10000</v>
       </c>
       <c r="M39" s="2">
         <f t="shared" si="26"/>
         <v>14388</v>
       </c>
-      <c r="N39" s="3">
+      <c r="N39">
         <f t="shared" si="4"/>
         <v>224.8125</v>
       </c>
-      <c r="O39" s="3">
+      <c r="O39">
         <v>78410.600000000006</v>
       </c>
-      <c r="P39" s="3">
+      <c r="P39">
         <v>76791.100000000006</v>
       </c>
-      <c r="Q39" s="3">
+      <c r="Q39">
         <f t="shared" si="8"/>
         <v>86.050186071477015</v>
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A40" s="3">
+      <c r="A40">
         <v>39</v>
       </c>
       <c r="B40" s="3">
         <v>45757</v>
       </c>
-      <c r="C40" s="3" t="s">
+      <c r="C40" t="s">
         <v>17</v>
       </c>
       <c r="D40" s="2">
@@ -3537,60 +3537,60 @@
       <c r="E40" s="2">
         <v>24713</v>
       </c>
-      <c r="F40" s="3">
+      <c r="F40">
         <f t="shared" si="22"/>
         <v>325</v>
       </c>
-      <c r="G40" s="3">
+      <c r="G40">
         <f t="shared" si="23"/>
         <v>469.56410256410254</v>
       </c>
-      <c r="H40" s="3">
+      <c r="H40">
         <f t="shared" si="24"/>
         <v>1.3326226012793096</v>
       </c>
-      <c r="I40" s="3">
+      <c r="I40">
         <f t="shared" si="25"/>
         <v>3.5248848916893172</v>
       </c>
-      <c r="J40" s="3">
+      <c r="J40">
         <f t="shared" si="7"/>
         <v>10455.357751272799</v>
       </c>
-      <c r="K40" s="3">
+      <c r="K40">
         <f t="shared" si="27"/>
         <v>4257.6422487272011</v>
       </c>
-      <c r="L40" s="3">
+      <c r="L40">
         <v>-10000</v>
       </c>
       <c r="M40" s="2">
         <f t="shared" si="26"/>
         <v>14713</v>
       </c>
-      <c r="N40" s="3">
+      <c r="N40">
         <f t="shared" si="4"/>
         <v>229.890625</v>
       </c>
-      <c r="O40" s="3">
+      <c r="O40">
         <v>76791.100000000006</v>
       </c>
-      <c r="P40" s="3">
+      <c r="P40">
         <v>81192.2</v>
       </c>
-      <c r="Q40" s="3">
+      <c r="Q40">
         <f t="shared" si="8"/>
         <v>90.981948657495138</v>
       </c>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A41" s="3">
+      <c r="A41">
         <v>40</v>
       </c>
       <c r="B41" s="3">
         <v>45758</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="C41" t="s">
         <v>18</v>
       </c>
       <c r="D41" s="2">
@@ -3599,60 +3599,60 @@
       <c r="E41" s="2">
         <v>25029</v>
       </c>
-      <c r="F41" s="3">
+      <c r="F41">
         <f t="shared" si="22"/>
         <v>316</v>
       </c>
-      <c r="G41" s="3">
+      <c r="G41">
         <f t="shared" si="23"/>
         <v>465.72500000000002</v>
       </c>
-      <c r="H41" s="3">
+      <c r="H41">
         <f t="shared" si="24"/>
         <v>1.2786792376481948</v>
       </c>
-      <c r="I41" s="3">
+      <c r="I41">
         <f t="shared" si="25"/>
         <v>3.4681271506401101</v>
       </c>
-      <c r="J41" s="3">
+      <c r="J41">
         <f t="shared" si="7"/>
         <v>10591.277402039344</v>
       </c>
-      <c r="K41" s="3">
+      <c r="K41">
         <f t="shared" si="27"/>
         <v>4437.7225979606555</v>
       </c>
-      <c r="L41" s="3">
+      <c r="L41">
         <v>-10000</v>
       </c>
       <c r="M41" s="2">
         <f t="shared" si="26"/>
         <v>15029</v>
       </c>
-      <c r="N41" s="3">
+      <c r="N41">
         <f t="shared" si="4"/>
         <v>234.828125</v>
       </c>
-      <c r="O41" s="3">
+      <c r="O41">
         <v>81192.2</v>
       </c>
-      <c r="P41" s="3">
+      <c r="P41">
         <v>81812</v>
       </c>
-      <c r="Q41" s="3">
+      <c r="Q41">
         <f t="shared" si="8"/>
         <v>91.67648103594918</v>
       </c>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A42" s="3">
+      <c r="A42">
         <v>41</v>
       </c>
       <c r="B42" s="3">
         <v>45759</v>
       </c>
-      <c r="C42" s="3" t="s">
+      <c r="C42" t="s">
         <v>19</v>
       </c>
       <c r="D42" s="2">
@@ -3661,60 +3661,60 @@
       <c r="E42" s="2">
         <v>25088</v>
       </c>
-      <c r="F42" s="3">
+      <c r="F42">
         <f t="shared" ref="F42:F46" si="28">E42-D42</f>
         <v>59</v>
       </c>
-      <c r="G42" s="3">
+      <c r="G42">
         <f t="shared" ref="G42:G46" si="29">(E42-$D$2)/A42</f>
         <v>455.80487804878049</v>
       </c>
-      <c r="H42" s="3">
+      <c r="H42">
         <f t="shared" ref="H42:H46" si="30">(E42/D42-1)*100</f>
         <v>0.23572655719366065</v>
       </c>
-      <c r="I42" s="3">
+      <c r="I42">
         <f t="shared" ref="I42:I46" si="31">(POWER((E42/$D$3),1/A42)-1)*100</f>
         <v>3.3880613542311755</v>
       </c>
-      <c r="J42" s="3">
+      <c r="J42">
         <f t="shared" si="7"/>
         <v>10728.964008265855</v>
       </c>
-      <c r="K42" s="3">
+      <c r="K42">
         <f t="shared" ref="K42:K46" si="32">M42-J42</f>
         <v>4359.0359917341448</v>
       </c>
-      <c r="L42" s="3">
+      <c r="L42">
         <v>-10000</v>
       </c>
       <c r="M42" s="2">
         <f t="shared" ref="M42:M46" si="33">L42+E42</f>
         <v>15088</v>
       </c>
-      <c r="N42" s="3">
+      <c r="N42">
         <f t="shared" ref="N42:N46" si="34">M42/$D$2*100</f>
         <v>235.75</v>
       </c>
-      <c r="O42" s="3">
+      <c r="O42">
         <v>81812</v>
       </c>
-      <c r="P42" s="3">
+      <c r="P42">
         <v>84763.1</v>
       </c>
-      <c r="Q42" s="3">
+      <c r="Q42">
         <f t="shared" ref="Q42:Q46" si="35">P42/$O$2*100</f>
         <v>94.983409887281383</v>
       </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A43" s="3">
+      <c r="A43">
         <v>42</v>
       </c>
       <c r="B43" s="3">
         <v>45760</v>
       </c>
-      <c r="C43" s="3" t="s">
+      <c r="C43" t="s">
         <v>20</v>
       </c>
       <c r="D43" s="2">
@@ -3723,60 +3723,60 @@
       <c r="E43" s="2">
         <v>25195</v>
       </c>
-      <c r="F43" s="3">
+      <c r="F43">
         <f t="shared" si="28"/>
         <v>107</v>
       </c>
-      <c r="G43" s="3">
+      <c r="G43">
         <f t="shared" si="29"/>
         <v>447.5</v>
       </c>
-      <c r="H43" s="3">
+      <c r="H43">
         <f t="shared" si="30"/>
         <v>0.42649872448978776</v>
       </c>
-      <c r="I43" s="3">
+      <c r="I43">
         <f t="shared" si="31"/>
         <v>3.3165430633898429</v>
       </c>
-      <c r="J43" s="3">
+      <c r="J43">
         <f t="shared" si="7"/>
         <v>10868.440540373311</v>
       </c>
-      <c r="K43" s="3">
+      <c r="K43">
         <f t="shared" si="32"/>
         <v>4326.5594596266892</v>
       </c>
-      <c r="L43" s="3">
+      <c r="L43">
         <v>-10000</v>
       </c>
       <c r="M43" s="2">
         <f t="shared" si="33"/>
         <v>15195</v>
       </c>
-      <c r="N43" s="3">
+      <c r="N43">
         <f t="shared" si="34"/>
         <v>237.42187499999997</v>
       </c>
-      <c r="O43" s="3">
+      <c r="O43">
         <v>84763.1</v>
       </c>
-      <c r="P43" s="3">
+      <c r="P43">
         <v>84024</v>
       </c>
-      <c r="Q43" s="3">
+      <c r="Q43">
         <f t="shared" si="35"/>
         <v>94.15519291258731</v>
       </c>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A44" s="3">
+      <c r="A44">
         <v>43</v>
       </c>
       <c r="B44" s="3">
         <v>45761</v>
       </c>
-      <c r="C44" s="3" t="s">
+      <c r="C44" t="s">
         <v>14</v>
       </c>
       <c r="D44" s="2">
@@ -3785,60 +3785,60 @@
       <c r="E44" s="2">
         <v>25835</v>
       </c>
-      <c r="F44" s="3">
+      <c r="F44">
         <f t="shared" si="28"/>
         <v>640</v>
       </c>
-      <c r="G44" s="3">
+      <c r="G44">
         <f t="shared" si="29"/>
         <v>451.97674418604652</v>
       </c>
-      <c r="H44" s="3">
+      <c r="H44">
         <f t="shared" si="30"/>
         <v>2.5401865449493854</v>
       </c>
-      <c r="I44" s="3">
+      <c r="I44">
         <f t="shared" si="31"/>
         <v>3.2984216732465654</v>
       </c>
-      <c r="J44" s="3">
+      <c r="J44">
         <f t="shared" si="7"/>
         <v>11009.730267398163</v>
       </c>
-      <c r="K44" s="3">
+      <c r="K44">
         <f t="shared" si="32"/>
         <v>4825.2697326018369</v>
       </c>
-      <c r="L44" s="3">
+      <c r="L44">
         <v>-10000</v>
       </c>
       <c r="M44" s="2">
         <f t="shared" si="33"/>
         <v>15835</v>
       </c>
-      <c r="N44" s="3">
+      <c r="N44">
         <f t="shared" si="34"/>
         <v>247.421875</v>
       </c>
-      <c r="O44" s="3">
+      <c r="O44">
         <v>84024</v>
       </c>
-      <c r="P44" s="3">
+      <c r="P44">
         <v>85364.7</v>
       </c>
-      <c r="Q44" s="3">
+      <c r="Q44">
         <f t="shared" si="35"/>
         <v>95.657547800927617</v>
       </c>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A45" s="3">
+      <c r="A45">
         <v>44</v>
       </c>
       <c r="B45" s="3">
         <v>45762</v>
       </c>
-      <c r="C45" s="3" t="s">
+      <c r="C45" t="s">
         <v>15</v>
       </c>
       <c r="D45" s="2">
@@ -3847,60 +3847,60 @@
       <c r="E45" s="2">
         <v>25600</v>
       </c>
-      <c r="F45" s="3">
+      <c r="F45">
         <f t="shared" si="28"/>
         <v>-235</v>
       </c>
-      <c r="G45" s="3">
+      <c r="G45">
         <f t="shared" si="29"/>
         <v>436.36363636363637</v>
       </c>
-      <c r="H45" s="3">
+      <c r="H45">
         <f t="shared" si="30"/>
         <v>-0.90961873427520823</v>
       </c>
-      <c r="I45" s="3">
+      <c r="I45">
         <f t="shared" si="31"/>
         <v>3.200827973420961</v>
       </c>
-      <c r="J45" s="3">
+      <c r="J45">
         <f t="shared" si="7"/>
         <v>11152.856760874338</v>
       </c>
-      <c r="K45" s="3">
+      <c r="K45">
         <f t="shared" si="32"/>
         <v>4447.1432391256621</v>
       </c>
-      <c r="L45" s="3">
+      <c r="L45">
         <v>-10000</v>
       </c>
       <c r="M45" s="2">
         <f t="shared" si="33"/>
         <v>15600</v>
       </c>
-      <c r="N45" s="3">
+      <c r="N45">
         <f t="shared" si="34"/>
         <v>243.75</v>
       </c>
-      <c r="O45" s="3">
+      <c r="O45">
         <v>85364.7</v>
       </c>
-      <c r="P45" s="3">
+      <c r="P45">
         <v>85100.2</v>
       </c>
-      <c r="Q45" s="3">
+      <c r="Q45">
         <f t="shared" si="35"/>
         <v>95.36115571622112</v>
       </c>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A46" s="3">
+      <c r="A46">
         <v>45</v>
       </c>
       <c r="B46" s="3">
         <v>45763</v>
       </c>
-      <c r="C46" s="3" t="s">
+      <c r="C46" t="s">
         <v>16</v>
       </c>
       <c r="D46" s="2">
@@ -3909,60 +3909,60 @@
       <c r="E46" s="2">
         <v>26102</v>
       </c>
-      <c r="F46" s="3">
+      <c r="F46">
         <f t="shared" si="28"/>
         <v>502</v>
       </c>
-      <c r="G46" s="3">
+      <c r="G46">
         <f t="shared" si="29"/>
         <v>437.82222222222219</v>
       </c>
-      <c r="H46" s="3">
+      <c r="H46">
         <f t="shared" si="30"/>
         <v>1.9609374999999929</v>
       </c>
-      <c r="I46" s="3">
+      <c r="I46">
         <f t="shared" si="31"/>
         <v>3.1731117201337034</v>
       </c>
-      <c r="J46" s="3">
+      <c r="J46">
         <f t="shared" si="7"/>
         <v>11297.843898765703</v>
       </c>
-      <c r="K46" s="3">
+      <c r="K46">
         <f t="shared" si="32"/>
         <v>4804.1561012342972</v>
       </c>
-      <c r="L46" s="3">
+      <c r="L46">
         <v>-10000</v>
       </c>
       <c r="M46" s="2">
         <f t="shared" si="33"/>
         <v>16102</v>
       </c>
-      <c r="N46" s="3">
+      <c r="N46">
         <f t="shared" si="34"/>
         <v>251.59375000000003</v>
       </c>
-      <c r="O46" s="3">
+      <c r="O46">
         <v>85100.2</v>
       </c>
-      <c r="P46" s="3">
+      <c r="P46">
         <v>84562.7</v>
       </c>
-      <c r="Q46" s="3">
+      <c r="Q46">
         <f t="shared" si="35"/>
         <v>94.758846659397875</v>
       </c>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A47" s="3">
+      <c r="A47">
         <v>46</v>
       </c>
       <c r="B47" s="3">
         <v>45764</v>
       </c>
-      <c r="C47" s="3" t="s">
+      <c r="C47" t="s">
         <v>17</v>
       </c>
       <c r="D47" s="2">
@@ -3971,31 +3971,31 @@
       <c r="E47" s="2">
         <v>47035</v>
       </c>
-      <c r="F47" s="3">
+      <c r="F47">
         <f t="shared" ref="F47:F62" si="36">E47-D47</f>
         <v>233</v>
       </c>
-      <c r="G47" s="3">
+      <c r="G47">
         <f t="shared" ref="G47:G62" si="37">(E47-$D$2)/A47</f>
         <v>883.36956521739125</v>
       </c>
-      <c r="H47" s="3">
+      <c r="H47">
         <f t="shared" ref="H47:H62" si="38">(E47/D47-1)*100</f>
         <v>0.49784197256528273</v>
       </c>
-      <c r="I47" s="3">
+      <c r="I47">
         <f t="shared" ref="I47:I62" si="39">(POWER((E47/$D$3),1/A47)-1)*100</f>
         <v>4.4314552374297156</v>
       </c>
-      <c r="J47" s="3">
+      <c r="J47">
         <f t="shared" si="7"/>
         <v>11444.715869449656</v>
       </c>
-      <c r="K47" s="3">
+      <c r="K47">
         <f t="shared" ref="K47:K62" si="40">M47-J47</f>
         <v>4891.2841305503443</v>
       </c>
-      <c r="L47" s="3">
+      <c r="L47">
         <f>-9999-20700</f>
         <v>-30699</v>
       </c>
@@ -4003,29 +4003,29 @@
         <f t="shared" ref="M47:M62" si="41">L47+E47</f>
         <v>16336</v>
       </c>
-      <c r="N47" s="3">
+      <c r="N47">
         <f t="shared" ref="N47:N62" si="42">M47/$D$2*100</f>
         <v>255.25000000000003</v>
       </c>
-      <c r="O47" s="3">
+      <c r="O47">
         <v>84562.7</v>
       </c>
-      <c r="P47" s="3">
+      <c r="P47">
         <v>84046</v>
       </c>
-      <c r="Q47" s="3">
+      <c r="Q47">
         <f t="shared" ref="Q47:Q62" si="43">P47/$O$2*100</f>
         <v>94.179845562354956</v>
       </c>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A48" s="3">
+      <c r="A48">
         <v>47</v>
       </c>
       <c r="B48" s="3">
         <v>45765</v>
       </c>
-      <c r="C48" s="3" t="s">
+      <c r="C48" t="s">
         <v>18</v>
       </c>
       <c r="D48" s="2">
@@ -4034,31 +4034,31 @@
       <c r="E48" s="2">
         <v>47070</v>
       </c>
-      <c r="F48" s="3">
+      <c r="F48">
         <f t="shared" si="36"/>
         <v>35</v>
       </c>
-      <c r="G48" s="3">
+      <c r="G48">
         <f t="shared" si="37"/>
         <v>865.31914893617022</v>
       </c>
-      <c r="H48" s="3">
+      <c r="H48">
         <f t="shared" si="38"/>
         <v>7.4412671414902931E-2</v>
       </c>
-      <c r="I48" s="3">
+      <c r="I48">
         <f t="shared" si="39"/>
         <v>4.3368057343146749</v>
       </c>
-      <c r="J48" s="3">
+      <c r="J48">
         <f t="shared" si="7"/>
         <v>11593.4971757525</v>
       </c>
-      <c r="K48" s="3">
+      <c r="K48">
         <f t="shared" si="40"/>
         <v>4777.5028242475</v>
       </c>
-      <c r="L48" s="3">
+      <c r="L48">
         <f>L47</f>
         <v>-30699</v>
       </c>
@@ -4066,29 +4066,29 @@
         <f t="shared" si="41"/>
         <v>16371</v>
       </c>
-      <c r="N48" s="3">
+      <c r="N48">
         <f t="shared" si="42"/>
         <v>255.796875</v>
       </c>
-      <c r="O48" s="3">
+      <c r="O48">
         <v>84046</v>
       </c>
-      <c r="P48" s="3">
+      <c r="P48">
         <v>84534</v>
       </c>
-      <c r="Q48" s="3">
+      <c r="Q48">
         <f t="shared" si="43"/>
         <v>94.726686157200987</v>
       </c>
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A49" s="3">
+      <c r="A49">
         <v>48</v>
       </c>
       <c r="B49" s="3">
         <v>45766</v>
       </c>
-      <c r="C49" s="3" t="s">
+      <c r="C49" t="s">
         <v>19</v>
       </c>
       <c r="D49" s="2">
@@ -4097,31 +4097,31 @@
       <c r="E49" s="2">
         <v>47160</v>
       </c>
-      <c r="F49" s="3">
+      <c r="F49">
         <f t="shared" si="36"/>
         <v>90</v>
       </c>
-      <c r="G49" s="3">
+      <c r="G49">
         <f t="shared" si="37"/>
         <v>849.16666666666663</v>
       </c>
-      <c r="H49" s="3">
+      <c r="H49">
         <f t="shared" si="38"/>
         <v>0.19120458891013214</v>
       </c>
-      <c r="I49" s="3">
+      <c r="I49">
         <f t="shared" si="39"/>
         <v>4.2487136066875042</v>
       </c>
-      <c r="J49" s="3">
+      <c r="J49">
         <f t="shared" si="7"/>
         <v>11744.212639037281</v>
       </c>
-      <c r="K49" s="3">
+      <c r="K49">
         <f t="shared" si="40"/>
         <v>4716.7873609627186</v>
       </c>
-      <c r="L49" s="3">
+      <c r="L49">
         <f t="shared" ref="L49:L62" si="44">L48</f>
         <v>-30699</v>
       </c>
@@ -4129,29 +4129,29 @@
         <f t="shared" si="41"/>
         <v>16461</v>
       </c>
-      <c r="N49" s="3">
+      <c r="N49">
         <f t="shared" si="42"/>
         <v>257.203125</v>
       </c>
-      <c r="O49" s="3">
+      <c r="O49">
         <v>84534</v>
       </c>
-      <c r="P49" s="3">
+      <c r="P49">
         <v>85355</v>
       </c>
-      <c r="Q49" s="3">
+      <c r="Q49">
         <f t="shared" si="43"/>
         <v>95.646678223530074</v>
       </c>
     </row>
     <row r="50" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A50" s="3">
+      <c r="A50">
         <v>49</v>
       </c>
       <c r="B50" s="3">
         <v>45767</v>
       </c>
-      <c r="C50" s="3" t="s">
+      <c r="C50" t="s">
         <v>20</v>
       </c>
       <c r="D50" s="2">
@@ -4160,31 +4160,31 @@
       <c r="E50" s="2">
         <v>47420</v>
       </c>
-      <c r="F50" s="3">
+      <c r="F50">
         <f t="shared" si="36"/>
         <v>260</v>
       </c>
-      <c r="G50" s="3">
+      <c r="G50">
         <f t="shared" si="37"/>
         <v>837.14285714285711</v>
       </c>
-      <c r="H50" s="3">
+      <c r="H50">
         <f t="shared" si="38"/>
         <v>0.55131467345208574</v>
       </c>
-      <c r="I50" s="3">
+      <c r="I50">
         <f t="shared" si="39"/>
         <v>4.1719141601861187</v>
       </c>
-      <c r="J50" s="3">
+      <c r="J50">
         <f t="shared" si="7"/>
         <v>11896.887403344765</v>
       </c>
-      <c r="K50" s="3">
+      <c r="K50">
         <f t="shared" si="40"/>
         <v>4824.1125966552354</v>
       </c>
-      <c r="L50" s="3">
+      <c r="L50">
         <f t="shared" si="44"/>
         <v>-30699</v>
       </c>
@@ -4192,29 +4192,29 @@
         <f t="shared" si="41"/>
         <v>16721</v>
       </c>
-      <c r="N50" s="3">
+      <c r="N50">
         <f t="shared" si="42"/>
         <v>261.265625</v>
       </c>
-      <c r="O50" s="3">
+      <c r="O50">
         <v>85355</v>
       </c>
-      <c r="P50" s="3">
+      <c r="P50">
         <v>84585</v>
       </c>
-      <c r="Q50" s="3">
+      <c r="Q50">
         <f t="shared" si="43"/>
         <v>94.783835481662365</v>
       </c>
     </row>
     <row r="51" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A51" s="3">
+      <c r="A51">
         <v>50</v>
       </c>
       <c r="B51" s="3">
         <v>45768</v>
       </c>
-      <c r="C51" s="3" t="s">
+      <c r="C51" t="s">
         <v>14</v>
       </c>
       <c r="D51" s="2">
@@ -4223,31 +4223,31 @@
       <c r="E51" s="2">
         <v>47910</v>
       </c>
-      <c r="F51" s="3">
+      <c r="F51">
         <f t="shared" si="36"/>
         <v>490</v>
       </c>
-      <c r="G51" s="3">
+      <c r="G51">
         <f t="shared" si="37"/>
         <v>830.2</v>
       </c>
-      <c r="H51" s="3">
+      <c r="H51">
         <f t="shared" si="38"/>
         <v>1.03331927456769</v>
       </c>
-      <c r="I51" s="3">
+      <c r="I51">
         <f t="shared" si="39"/>
         <v>4.1081966963260053</v>
       </c>
-      <c r="J51" s="3">
+      <c r="J51">
         <f t="shared" si="7"/>
         <v>12051.546939588245</v>
       </c>
-      <c r="K51" s="3">
+      <c r="K51">
         <f t="shared" si="40"/>
         <v>5159.4530604117554</v>
       </c>
-      <c r="L51" s="3">
+      <c r="L51">
         <f t="shared" si="44"/>
         <v>-30699</v>
       </c>
@@ -4255,29 +4255,29 @@
         <f t="shared" si="41"/>
         <v>17211</v>
       </c>
-      <c r="N51" s="3">
+      <c r="N51">
         <f t="shared" si="42"/>
         <v>268.921875</v>
       </c>
-      <c r="O51" s="3">
+      <c r="O51">
         <v>84585</v>
       </c>
-      <c r="P51" s="3">
+      <c r="P51">
         <v>88165</v>
       </c>
-      <c r="Q51" s="3">
+      <c r="Q51">
         <f t="shared" si="43"/>
         <v>98.795493943852478</v>
       </c>
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A52" s="3">
+      <c r="A52">
         <v>51</v>
       </c>
       <c r="B52" s="3">
         <v>45769</v>
       </c>
-      <c r="C52" s="3" t="s">
+      <c r="C52" t="s">
         <v>15</v>
       </c>
       <c r="D52" s="2">
@@ -4286,31 +4286,31 @@
       <c r="E52" s="2">
         <v>49488</v>
       </c>
-      <c r="F52" s="3">
+      <c r="F52">
         <f t="shared" si="36"/>
         <v>1578</v>
       </c>
-      <c r="G52" s="3">
+      <c r="G52">
         <f t="shared" si="37"/>
         <v>844.86274509803923</v>
       </c>
-      <c r="H52" s="3">
+      <c r="H52">
         <f t="shared" si="38"/>
         <v>3.2936756418284308</v>
       </c>
-      <c r="I52" s="3">
+      <c r="I52">
         <f t="shared" si="39"/>
         <v>4.0921641251811192</v>
       </c>
-      <c r="J52" s="3">
+      <c r="J52">
         <f t="shared" si="7"/>
         <v>12208.21704980289</v>
       </c>
-      <c r="K52" s="3">
+      <c r="K52">
         <f t="shared" si="40"/>
         <v>6580.78295019711</v>
       </c>
-      <c r="L52" s="3">
+      <c r="L52">
         <f t="shared" si="44"/>
         <v>-30699</v>
       </c>
@@ -4318,29 +4318,29 @@
         <f t="shared" si="41"/>
         <v>18789</v>
       </c>
-      <c r="N52" s="3">
+      <c r="N52">
         <f t="shared" si="42"/>
         <v>293.578125</v>
       </c>
-      <c r="O52" s="3">
+      <c r="O52">
         <v>88165</v>
       </c>
-      <c r="P52" s="3">
+      <c r="P52">
         <v>91407</v>
       </c>
-      <c r="Q52" s="3">
+      <c r="Q52">
         <f t="shared" si="43"/>
         <v>102.42839805961235</v>
       </c>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A53" s="3">
+      <c r="A53">
         <v>52</v>
       </c>
       <c r="B53" s="3">
         <v>45770</v>
       </c>
-      <c r="C53" s="3" t="s">
+      <c r="C53" t="s">
         <v>16</v>
       </c>
       <c r="D53" s="2">
@@ -4349,31 +4349,31 @@
       <c r="E53" s="2">
         <v>50094</v>
       </c>
-      <c r="F53" s="3">
+      <c r="F53">
         <f t="shared" si="36"/>
         <v>606</v>
       </c>
-      <c r="G53" s="3">
+      <c r="G53">
         <f t="shared" si="37"/>
         <v>840.26923076923072</v>
       </c>
-      <c r="H53" s="3">
+      <c r="H53">
         <f t="shared" si="38"/>
         <v>1.2245392822502366</v>
       </c>
-      <c r="I53" s="3">
+      <c r="I53">
         <f t="shared" si="39"/>
         <v>4.0362586513626564</v>
       </c>
-      <c r="J53" s="3">
+      <c r="J53">
         <f t="shared" si="7"/>
         <v>12366.923871450326</v>
       </c>
-      <c r="K53" s="3">
+      <c r="K53">
         <f t="shared" si="40"/>
         <v>7028.0761285496737</v>
       </c>
-      <c r="L53" s="3">
+      <c r="L53">
         <f t="shared" si="44"/>
         <v>-30699</v>
       </c>
@@ -4381,29 +4381,29 @@
         <f t="shared" si="41"/>
         <v>19395</v>
       </c>
-      <c r="N53" s="3">
+      <c r="N53">
         <f t="shared" si="42"/>
         <v>303.046875</v>
       </c>
-      <c r="O53" s="3">
+      <c r="O53">
         <v>91407</v>
       </c>
-      <c r="P53" s="3">
+      <c r="P53">
         <v>92926</v>
       </c>
-      <c r="Q53" s="3">
+      <c r="Q53">
         <f t="shared" si="43"/>
         <v>104.13055146856955</v>
       </c>
     </row>
     <row r="54" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A54" s="3">
+      <c r="A54">
         <v>53</v>
       </c>
       <c r="B54" s="3">
         <v>45771</v>
       </c>
-      <c r="C54" s="3" t="s">
+      <c r="C54" t="s">
         <v>17</v>
       </c>
       <c r="D54" s="2">
@@ -4412,31 +4412,31 @@
       <c r="E54" s="2">
         <v>50900</v>
       </c>
-      <c r="F54" s="3">
+      <c r="F54">
         <f t="shared" si="36"/>
         <v>806</v>
       </c>
-      <c r="G54" s="3">
+      <c r="G54">
         <f t="shared" si="37"/>
         <v>839.62264150943395</v>
       </c>
-      <c r="H54" s="3">
+      <c r="H54">
         <f t="shared" si="38"/>
         <v>1.6089751267616803</v>
       </c>
-      <c r="I54" s="3">
+      <c r="I54">
         <f t="shared" si="39"/>
         <v>3.9899284528173595</v>
       </c>
-      <c r="J54" s="3">
+      <c r="J54">
         <f t="shared" si="7"/>
         <v>12527.69388177918</v>
       </c>
-      <c r="K54" s="3">
+      <c r="K54">
         <f t="shared" si="40"/>
         <v>7673.3061182208203</v>
       </c>
-      <c r="L54" s="3">
+      <c r="L54">
         <f t="shared" si="44"/>
         <v>-30699</v>
       </c>
@@ -4444,29 +4444,29 @@
         <f t="shared" si="41"/>
         <v>20201</v>
       </c>
-      <c r="N54" s="3">
+      <c r="N54">
         <f t="shared" si="42"/>
         <v>315.640625</v>
       </c>
-      <c r="O54" s="3">
+      <c r="O54">
         <v>92926</v>
       </c>
-      <c r="P54" s="3">
+      <c r="P54">
         <v>93092</v>
       </c>
-      <c r="Q54" s="3">
+      <c r="Q54">
         <f t="shared" si="43"/>
         <v>104.31656691681637</v>
       </c>
     </row>
     <row r="55" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A55" s="3">
+      <c r="A55">
         <v>54</v>
       </c>
       <c r="B55" s="3">
         <v>45772</v>
       </c>
-      <c r="C55" s="3" t="s">
+      <c r="C55" t="s">
         <v>18</v>
       </c>
       <c r="D55" s="2">
@@ -4475,31 +4475,31 @@
       <c r="E55" s="2">
         <v>51087.55</v>
       </c>
-      <c r="F55" s="3">
+      <c r="F55">
         <f t="shared" si="36"/>
         <v>187.55000000000291</v>
       </c>
-      <c r="G55" s="3">
+      <c r="G55">
         <f t="shared" si="37"/>
         <v>827.54722222222233</v>
       </c>
-      <c r="H55" s="3">
+      <c r="H55">
         <f t="shared" si="38"/>
         <v>0.36846758349706743</v>
       </c>
-      <c r="I55" s="3">
+      <c r="I55">
         <f t="shared" si="39"/>
         <v>3.9216911636315688</v>
       </c>
-      <c r="J55" s="3">
+      <c r="J55">
         <f t="shared" si="7"/>
         <v>12690.553902242307</v>
       </c>
-      <c r="K55" s="3">
+      <c r="K55">
         <f t="shared" si="40"/>
         <v>7697.9960977576957</v>
       </c>
-      <c r="L55" s="3">
+      <c r="L55">
         <f t="shared" si="44"/>
         <v>-30699</v>
       </c>
@@ -4507,29 +4507,29 @@
         <f t="shared" si="41"/>
         <v>20388.550000000003</v>
       </c>
-      <c r="N55" s="3">
+      <c r="N55">
         <f t="shared" si="42"/>
         <v>318.57109375000005</v>
       </c>
-      <c r="O55" s="3">
+      <c r="O55">
         <v>93092</v>
       </c>
-      <c r="P55" s="3">
+      <c r="P55">
         <v>95419</v>
       </c>
-      <c r="Q55" s="3">
+      <c r="Q55">
         <f t="shared" si="43"/>
         <v>106.92414491723994</v>
       </c>
     </row>
     <row r="56" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A56" s="3">
+      <c r="A56">
         <v>55</v>
       </c>
       <c r="B56" s="3">
         <v>45773</v>
       </c>
-      <c r="C56" s="3" t="s">
+      <c r="C56" t="s">
         <v>19</v>
       </c>
       <c r="D56" s="2">
@@ -4538,31 +4538,31 @@
       <c r="E56" s="2">
         <v>51166.85</v>
       </c>
-      <c r="F56" s="3">
+      <c r="F56">
         <f t="shared" si="36"/>
         <v>79.299999999995634</v>
       </c>
-      <c r="G56" s="3">
+      <c r="G56">
         <f t="shared" si="37"/>
         <v>813.94272727272721</v>
       </c>
-      <c r="H56" s="3">
+      <c r="H56">
         <f t="shared" si="38"/>
         <v>0.15522372867753376</v>
       </c>
-      <c r="I56" s="3">
+      <c r="I56">
         <f t="shared" si="39"/>
         <v>3.8519615234979154</v>
       </c>
-      <c r="J56" s="3">
+      <c r="J56">
         <f t="shared" si="7"/>
         <v>12855.531102971456</v>
       </c>
-      <c r="K56" s="3">
+      <c r="K56">
         <f t="shared" si="40"/>
         <v>7612.3188970285428</v>
       </c>
-      <c r="L56" s="3">
+      <c r="L56">
         <f t="shared" si="44"/>
         <v>-30699</v>
       </c>
@@ -4570,29 +4570,29 @@
         <f t="shared" si="41"/>
         <v>20467.849999999999</v>
       </c>
-      <c r="N56" s="3">
+      <c r="N56">
         <f t="shared" si="42"/>
         <v>319.81015624999998</v>
       </c>
-      <c r="O56" s="3">
+      <c r="O56">
         <v>95419</v>
       </c>
-      <c r="P56" s="3">
+      <c r="P56">
         <v>94232</v>
       </c>
-      <c r="Q56" s="3">
+      <c r="Q56">
         <f t="shared" si="43"/>
         <v>105.59402240477635</v>
       </c>
     </row>
     <row r="57" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A57" s="3">
+      <c r="A57">
         <v>56</v>
       </c>
       <c r="B57" s="3">
         <v>45774</v>
       </c>
-      <c r="C57" s="3" t="s">
+      <c r="C57" t="s">
         <v>20</v>
       </c>
       <c r="D57" s="2">
@@ -4601,31 +4601,31 @@
       <c r="E57" s="2">
         <v>51225</v>
       </c>
-      <c r="F57" s="3">
+      <c r="F57">
         <f t="shared" si="36"/>
         <v>58.150000000001455</v>
       </c>
-      <c r="G57" s="3">
+      <c r="G57">
         <f t="shared" si="37"/>
         <v>800.44642857142856</v>
       </c>
-      <c r="H57" s="3">
+      <c r="H57">
         <f t="shared" si="38"/>
         <v>0.11364780126195129</v>
       </c>
-      <c r="I57" s="3">
+      <c r="I57">
         <f t="shared" si="39"/>
         <v>3.7839970496518882</v>
       </c>
-      <c r="J57" s="3">
+      <c r="J57">
         <f t="shared" si="7"/>
         <v>13022.653007310084</v>
       </c>
-      <c r="K57" s="3">
+      <c r="K57">
         <f t="shared" si="40"/>
         <v>7503.3469926899161</v>
       </c>
-      <c r="L57" s="3">
+      <c r="L57">
         <f t="shared" si="44"/>
         <v>-30699</v>
       </c>
@@ -4633,29 +4633,29 @@
         <f t="shared" si="41"/>
         <v>20526</v>
       </c>
-      <c r="N57" s="3">
+      <c r="N57">
         <f t="shared" si="42"/>
         <v>320.71875</v>
       </c>
-      <c r="O57" s="3">
+      <c r="O57">
         <v>94232</v>
       </c>
-      <c r="P57" s="3">
+      <c r="P57">
         <v>94047</v>
       </c>
-      <c r="Q57" s="3">
+      <c r="Q57">
         <f t="shared" si="43"/>
         <v>105.3867160317302</v>
       </c>
     </row>
     <row r="58" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A58" s="3">
+      <c r="A58">
         <v>57</v>
       </c>
       <c r="B58" s="3">
         <v>45775</v>
       </c>
-      <c r="C58" s="3" t="s">
+      <c r="C58" t="s">
         <v>14</v>
       </c>
       <c r="D58" s="2">
@@ -4664,31 +4664,31 @@
       <c r="E58" s="2">
         <v>51915</v>
       </c>
-      <c r="F58" s="3">
+      <c r="F58">
         <f t="shared" si="36"/>
         <v>690</v>
       </c>
-      <c r="G58" s="3">
+      <c r="G58">
         <f t="shared" si="37"/>
         <v>798.50877192982455</v>
       </c>
-      <c r="H58" s="3">
+      <c r="H58">
         <f t="shared" si="38"/>
         <v>1.3469985358711467</v>
       </c>
-      <c r="I58" s="3">
+      <c r="I58">
         <f t="shared" si="39"/>
         <v>3.7407417401673415</v>
       </c>
-      <c r="J58" s="3">
+      <c r="J58">
         <f t="shared" si="7"/>
         <v>13191.947496405113</v>
       </c>
-      <c r="K58" s="3">
+      <c r="K58">
         <f t="shared" si="40"/>
         <v>8024.0525035948867</v>
       </c>
-      <c r="L58" s="3">
+      <c r="L58">
         <f t="shared" si="44"/>
         <v>-30699</v>
       </c>
@@ -4696,29 +4696,29 @@
         <f t="shared" si="41"/>
         <v>21216</v>
       </c>
-      <c r="N58" s="3">
+      <c r="N58">
         <f t="shared" si="42"/>
         <v>331.5</v>
       </c>
-      <c r="O58" s="3">
+      <c r="O58">
         <v>94047</v>
       </c>
-      <c r="P58" s="3">
+      <c r="P58">
         <v>94415</v>
       </c>
-      <c r="Q58" s="3">
+      <c r="Q58">
         <f t="shared" si="43"/>
         <v>105.7990876278436</v>
       </c>
     </row>
     <row r="59" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A59" s="3">
+      <c r="A59">
         <v>58</v>
       </c>
       <c r="B59" s="3">
         <v>45776</v>
       </c>
-      <c r="C59" s="3" t="s">
+      <c r="C59" t="s">
         <v>15</v>
       </c>
       <c r="D59" s="2">
@@ -4727,31 +4727,31 @@
       <c r="E59" s="2">
         <v>52670</v>
       </c>
-      <c r="F59" s="3">
+      <c r="F59">
         <f t="shared" si="36"/>
         <v>755</v>
       </c>
-      <c r="G59" s="3">
+      <c r="G59">
         <f t="shared" si="37"/>
         <v>797.75862068965512</v>
       </c>
-      <c r="H59" s="3">
+      <c r="H59">
         <f t="shared" si="38"/>
         <v>1.45430029856497</v>
       </c>
-      <c r="I59" s="3">
+      <c r="I59">
         <f t="shared" si="39"/>
         <v>3.7008870800216309</v>
       </c>
-      <c r="J59" s="3">
+      <c r="J59">
         <f t="shared" si="7"/>
         <v>13363.442813858379</v>
       </c>
-      <c r="K59" s="3">
+      <c r="K59">
         <f t="shared" si="40"/>
         <v>8607.5571861416211</v>
       </c>
-      <c r="L59" s="3">
+      <c r="L59">
         <f t="shared" si="44"/>
         <v>-30699</v>
       </c>
@@ -4759,29 +4759,29 @@
         <f t="shared" si="41"/>
         <v>21971</v>
       </c>
-      <c r="N59" s="3">
+      <c r="N59">
         <f t="shared" si="42"/>
         <v>343.296875</v>
       </c>
-      <c r="O59" s="3">
+      <c r="O59">
         <v>94415</v>
       </c>
-      <c r="P59" s="3">
+      <c r="P59">
         <v>95022</v>
       </c>
-      <c r="Q59" s="3">
+      <c r="Q59">
         <f t="shared" si="43"/>
         <v>106.47927664643282</v>
       </c>
     </row>
     <row r="60" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A60" s="3">
+      <c r="A60">
         <v>59</v>
       </c>
       <c r="B60" s="3">
         <v>45777</v>
       </c>
-      <c r="C60" s="3" t="s">
+      <c r="C60" t="s">
         <v>16</v>
       </c>
       <c r="D60" s="2">
@@ -4790,31 +4790,31 @@
       <c r="E60" s="2">
         <v>53561.74</v>
       </c>
-      <c r="F60" s="3">
+      <c r="F60">
         <f t="shared" si="36"/>
         <v>891.73999999999796</v>
       </c>
-      <c r="G60" s="3">
+      <c r="G60">
         <f t="shared" si="37"/>
         <v>799.35152542372873</v>
       </c>
-      <c r="H60" s="3">
+      <c r="H60">
         <f t="shared" si="38"/>
         <v>1.693070058857038</v>
       </c>
-      <c r="I60" s="3">
+      <c r="I60">
         <f t="shared" si="39"/>
         <v>3.6665282155353252</v>
       </c>
-      <c r="J60" s="3">
+      <c r="J60">
         <f t="shared" si="7"/>
         <v>13537.167570438536</v>
       </c>
-      <c r="K60" s="3">
+      <c r="K60">
         <f t="shared" si="40"/>
         <v>9325.5724295614618</v>
       </c>
-      <c r="L60" s="3">
+      <c r="L60">
         <f t="shared" si="44"/>
         <v>-30699</v>
       </c>
@@ -4822,29 +4822,29 @@
         <f t="shared" si="41"/>
         <v>22862.739999999998</v>
       </c>
-      <c r="N60" s="3">
+      <c r="N60">
         <f t="shared" si="42"/>
         <v>357.23031249999997</v>
       </c>
-      <c r="O60" s="3">
+      <c r="O60">
         <v>95022</v>
       </c>
-      <c r="P60" s="3">
+      <c r="P60">
         <v>93681</v>
       </c>
-      <c r="Q60" s="3">
+      <c r="Q60">
         <f t="shared" si="43"/>
         <v>104.97658558559569</v>
       </c>
     </row>
     <row r="61" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A61" s="3">
+      <c r="A61">
         <v>60</v>
       </c>
       <c r="B61" s="3">
         <v>45778</v>
       </c>
-      <c r="C61" s="3" t="s">
+      <c r="C61" t="s">
         <v>17</v>
       </c>
       <c r="D61" s="2">
@@ -4853,31 +4853,31 @@
       <c r="E61" s="2">
         <v>54386</v>
       </c>
-      <c r="F61" s="3">
+      <c r="F61">
         <f t="shared" si="36"/>
         <v>824.26000000000204</v>
       </c>
-      <c r="G61" s="3">
+      <c r="G61">
         <f t="shared" si="37"/>
         <v>799.76666666666665</v>
       </c>
-      <c r="H61" s="3">
+      <c r="H61">
         <f t="shared" si="38"/>
         <v>1.5388969813153963</v>
       </c>
-      <c r="I61" s="3">
+      <c r="I61">
         <f t="shared" si="39"/>
         <v>3.6307049367540145</v>
       </c>
-      <c r="J61" s="3">
+      <c r="J61">
         <f t="shared" si="7"/>
         <v>13713.150748854236</v>
       </c>
-      <c r="K61" s="3">
+      <c r="K61">
         <f t="shared" si="40"/>
         <v>9973.8492511457644</v>
       </c>
-      <c r="L61" s="3">
+      <c r="L61">
         <f t="shared" si="44"/>
         <v>-30699</v>
       </c>
@@ -4885,29 +4885,29 @@
         <f t="shared" si="41"/>
         <v>23687</v>
       </c>
-      <c r="N61" s="3">
+      <c r="N61">
         <f t="shared" si="42"/>
         <v>370.109375</v>
       </c>
-      <c r="O61" s="3">
+      <c r="O61">
         <v>93681</v>
       </c>
-      <c r="P61" s="3">
+      <c r="P61">
         <v>96814</v>
       </c>
-      <c r="Q61" s="3">
+      <c r="Q61">
         <f t="shared" si="43"/>
         <v>108.48734702750676</v>
       </c>
     </row>
     <row r="62" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A62" s="3">
+      <c r="A62">
         <v>61</v>
       </c>
       <c r="B62" s="3">
         <v>45779</v>
       </c>
-      <c r="C62" s="3" t="s">
+      <c r="C62" t="s">
         <v>18</v>
       </c>
       <c r="D62" s="2">
@@ -4916,31 +4916,31 @@
       <c r="E62" s="2">
         <v>55327</v>
       </c>
-      <c r="F62" s="3">
+      <c r="F62">
         <f t="shared" si="36"/>
         <v>941</v>
       </c>
-      <c r="G62" s="3">
+      <c r="G62">
         <f t="shared" si="37"/>
         <v>802.08196721311481</v>
       </c>
-      <c r="H62" s="3">
+      <c r="H62">
         <f t="shared" si="38"/>
         <v>1.7302246901776286</v>
       </c>
-      <c r="I62" s="3">
+      <c r="I62">
         <f t="shared" si="39"/>
         <v>3.5992650724708364</v>
       </c>
-      <c r="J62" s="3">
+      <c r="J62">
         <f t="shared" si="7"/>
         <v>13891.42170858934</v>
       </c>
-      <c r="K62" s="3">
+      <c r="K62">
         <f t="shared" si="40"/>
         <v>10736.57829141066</v>
       </c>
-      <c r="L62" s="3">
+      <c r="L62">
         <f t="shared" si="44"/>
         <v>-30699</v>
       </c>
@@ -4948,17 +4948,17 @@
         <f t="shared" si="41"/>
         <v>24628</v>
       </c>
-      <c r="N62" s="3">
+      <c r="N62">
         <f t="shared" si="42"/>
         <v>384.8125</v>
       </c>
-      <c r="O62" s="3">
+      <c r="O62">
         <v>96814</v>
       </c>
-      <c r="P62" s="3">
+      <c r="P62">
         <v>97711</v>
       </c>
-      <c r="Q62" s="3">
+      <c r="Q62">
         <f t="shared" si="43"/>
         <v>109.49250279303317</v>
       </c>

</xml_diff>

<commit_message>
자동 업데이트: 2025-05-09 01:20:27
</commit_message>
<xml_diff>
--- a/data/daily_report.xlsx
+++ b/data/daily_report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c58a53286e4c1d7a/문서/GitHub/Dashboard/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="270" documentId="8_{9DD2A88B-03DA-4864-84CC-4418086E8BD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3A47580B-B26B-49A8-98D0-45BF352A0706}"/>
+  <xr:revisionPtr revIDLastSave="285" documentId="8_{9DD2A88B-03DA-4864-84CC-4418086E8BD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D1690D0C-B431-43CA-B495-A2305834B0C0}"/>
   <bookViews>
-    <workbookView xWindow="11070" yWindow="1695" windowWidth="27300" windowHeight="17325" xr2:uid="{4AB8DADE-1167-4E84-9D67-55086BA93884}"/>
+    <workbookView xWindow="3675" yWindow="2625" windowWidth="27300" windowHeight="17325" xr2:uid="{4AB8DADE-1167-4E84-9D67-55086BA93884}"/>
   </bookViews>
   <sheets>
     <sheet name="daily_report" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="24">
   <si>
     <t>Index</t>
   </si>
@@ -1099,10 +1099,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48182F73-FFD5-43FF-A3B0-19A54A277A3F}">
-  <dimension ref="A1:Q62"/>
+  <dimension ref="A1:Q68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N49" sqref="N49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1322,7 +1322,7 @@
         <v>2.2328836529616813</v>
       </c>
       <c r="J4">
-        <f t="shared" ref="J4:J62" si="7">J3*1.013</f>
+        <f t="shared" ref="J4:J67" si="7">J3*1.013</f>
         <v>6567.4815999999983</v>
       </c>
       <c r="K4">
@@ -3993,19 +3993,19 @@
       </c>
       <c r="K47">
         <f t="shared" ref="K47:K62" si="40">M47-J47</f>
-        <v>4891.2841305503443</v>
+        <v>4890.2841305503443</v>
       </c>
       <c r="L47">
-        <f>-9999-20700</f>
-        <v>-30699</v>
+        <f>-10000-20700</f>
+        <v>-30700</v>
       </c>
       <c r="M47" s="2">
         <f t="shared" ref="M47:M62" si="41">L47+E47</f>
-        <v>16336</v>
+        <v>16335</v>
       </c>
       <c r="N47">
         <f t="shared" ref="N47:N62" si="42">M47/$D$2*100</f>
-        <v>255.25000000000003</v>
+        <v>255.234375</v>
       </c>
       <c r="O47">
         <v>84562.7</v>
@@ -4056,19 +4056,19 @@
       </c>
       <c r="K48">
         <f t="shared" si="40"/>
-        <v>4777.5028242475</v>
+        <v>4776.5028242475</v>
       </c>
       <c r="L48">
         <f>L47</f>
-        <v>-30699</v>
+        <v>-30700</v>
       </c>
       <c r="M48" s="2">
         <f t="shared" si="41"/>
-        <v>16371</v>
+        <v>16370</v>
       </c>
       <c r="N48">
         <f t="shared" si="42"/>
-        <v>255.796875</v>
+        <v>255.78124999999997</v>
       </c>
       <c r="O48">
         <v>84046</v>
@@ -4119,19 +4119,19 @@
       </c>
       <c r="K49">
         <f t="shared" si="40"/>
-        <v>4716.7873609627186</v>
+        <v>4715.7873609627186</v>
       </c>
       <c r="L49">
-        <f t="shared" ref="L49:L62" si="44">L48</f>
-        <v>-30699</v>
+        <f t="shared" ref="L49:L68" si="44">L48</f>
+        <v>-30700</v>
       </c>
       <c r="M49" s="2">
         <f t="shared" si="41"/>
-        <v>16461</v>
+        <v>16460</v>
       </c>
       <c r="N49">
         <f t="shared" si="42"/>
-        <v>257.203125</v>
+        <v>257.1875</v>
       </c>
       <c r="O49">
         <v>84534</v>
@@ -4182,19 +4182,19 @@
       </c>
       <c r="K50">
         <f t="shared" si="40"/>
-        <v>4824.1125966552354</v>
+        <v>4823.1125966552354</v>
       </c>
       <c r="L50">
         <f t="shared" si="44"/>
-        <v>-30699</v>
+        <v>-30700</v>
       </c>
       <c r="M50" s="2">
         <f t="shared" si="41"/>
-        <v>16721</v>
+        <v>16720</v>
       </c>
       <c r="N50">
         <f t="shared" si="42"/>
-        <v>261.265625</v>
+        <v>261.25</v>
       </c>
       <c r="O50">
         <v>85355</v>
@@ -4245,19 +4245,19 @@
       </c>
       <c r="K51">
         <f t="shared" si="40"/>
-        <v>5159.4530604117554</v>
+        <v>5158.4530604117554</v>
       </c>
       <c r="L51">
         <f t="shared" si="44"/>
-        <v>-30699</v>
+        <v>-30700</v>
       </c>
       <c r="M51" s="2">
         <f t="shared" si="41"/>
-        <v>17211</v>
+        <v>17210</v>
       </c>
       <c r="N51">
         <f t="shared" si="42"/>
-        <v>268.921875</v>
+        <v>268.90625</v>
       </c>
       <c r="O51">
         <v>84585</v>
@@ -4308,19 +4308,19 @@
       </c>
       <c r="K52">
         <f t="shared" si="40"/>
-        <v>6580.78295019711</v>
+        <v>6579.78295019711</v>
       </c>
       <c r="L52">
         <f t="shared" si="44"/>
-        <v>-30699</v>
+        <v>-30700</v>
       </c>
       <c r="M52" s="2">
         <f t="shared" si="41"/>
-        <v>18789</v>
+        <v>18788</v>
       </c>
       <c r="N52">
         <f t="shared" si="42"/>
-        <v>293.578125</v>
+        <v>293.5625</v>
       </c>
       <c r="O52">
         <v>88165</v>
@@ -4371,19 +4371,19 @@
       </c>
       <c r="K53">
         <f t="shared" si="40"/>
-        <v>7028.0761285496737</v>
+        <v>7027.0761285496737</v>
       </c>
       <c r="L53">
         <f t="shared" si="44"/>
-        <v>-30699</v>
+        <v>-30700</v>
       </c>
       <c r="M53" s="2">
         <f t="shared" si="41"/>
-        <v>19395</v>
+        <v>19394</v>
       </c>
       <c r="N53">
         <f t="shared" si="42"/>
-        <v>303.046875</v>
+        <v>303.03125</v>
       </c>
       <c r="O53">
         <v>91407</v>
@@ -4434,19 +4434,19 @@
       </c>
       <c r="K54">
         <f t="shared" si="40"/>
-        <v>7673.3061182208203</v>
+        <v>7672.3061182208203</v>
       </c>
       <c r="L54">
         <f t="shared" si="44"/>
-        <v>-30699</v>
+        <v>-30700</v>
       </c>
       <c r="M54" s="2">
         <f t="shared" si="41"/>
-        <v>20201</v>
+        <v>20200</v>
       </c>
       <c r="N54">
         <f t="shared" si="42"/>
-        <v>315.640625</v>
+        <v>315.625</v>
       </c>
       <c r="O54">
         <v>92926</v>
@@ -4497,19 +4497,19 @@
       </c>
       <c r="K55">
         <f t="shared" si="40"/>
-        <v>7697.9960977576957</v>
+        <v>7696.9960977576957</v>
       </c>
       <c r="L55">
         <f t="shared" si="44"/>
-        <v>-30699</v>
+        <v>-30700</v>
       </c>
       <c r="M55" s="2">
         <f t="shared" si="41"/>
-        <v>20388.550000000003</v>
+        <v>20387.550000000003</v>
       </c>
       <c r="N55">
         <f t="shared" si="42"/>
-        <v>318.57109375000005</v>
+        <v>318.55546875000005</v>
       </c>
       <c r="O55">
         <v>93092</v>
@@ -4560,19 +4560,19 @@
       </c>
       <c r="K56">
         <f t="shared" si="40"/>
-        <v>7612.3188970285428</v>
+        <v>7611.3188970285428</v>
       </c>
       <c r="L56">
         <f t="shared" si="44"/>
-        <v>-30699</v>
+        <v>-30700</v>
       </c>
       <c r="M56" s="2">
         <f t="shared" si="41"/>
-        <v>20467.849999999999</v>
+        <v>20466.849999999999</v>
       </c>
       <c r="N56">
         <f t="shared" si="42"/>
-        <v>319.81015624999998</v>
+        <v>319.79453124999998</v>
       </c>
       <c r="O56">
         <v>95419</v>
@@ -4623,19 +4623,19 @@
       </c>
       <c r="K57">
         <f t="shared" si="40"/>
-        <v>7503.3469926899161</v>
+        <v>7502.3469926899161</v>
       </c>
       <c r="L57">
         <f t="shared" si="44"/>
-        <v>-30699</v>
+        <v>-30700</v>
       </c>
       <c r="M57" s="2">
         <f t="shared" si="41"/>
-        <v>20526</v>
+        <v>20525</v>
       </c>
       <c r="N57">
         <f t="shared" si="42"/>
-        <v>320.71875</v>
+        <v>320.703125</v>
       </c>
       <c r="O57">
         <v>94232</v>
@@ -4686,19 +4686,19 @@
       </c>
       <c r="K58">
         <f t="shared" si="40"/>
-        <v>8024.0525035948867</v>
+        <v>8023.0525035948867</v>
       </c>
       <c r="L58">
         <f t="shared" si="44"/>
-        <v>-30699</v>
+        <v>-30700</v>
       </c>
       <c r="M58" s="2">
         <f t="shared" si="41"/>
-        <v>21216</v>
+        <v>21215</v>
       </c>
       <c r="N58">
         <f t="shared" si="42"/>
-        <v>331.5</v>
+        <v>331.484375</v>
       </c>
       <c r="O58">
         <v>94047</v>
@@ -4749,19 +4749,19 @@
       </c>
       <c r="K59">
         <f t="shared" si="40"/>
-        <v>8607.5571861416211</v>
+        <v>8606.5571861416211</v>
       </c>
       <c r="L59">
         <f t="shared" si="44"/>
-        <v>-30699</v>
+        <v>-30700</v>
       </c>
       <c r="M59" s="2">
         <f t="shared" si="41"/>
-        <v>21971</v>
+        <v>21970</v>
       </c>
       <c r="N59">
         <f t="shared" si="42"/>
-        <v>343.296875</v>
+        <v>343.28125</v>
       </c>
       <c r="O59">
         <v>94415</v>
@@ -4812,19 +4812,19 @@
       </c>
       <c r="K60">
         <f t="shared" si="40"/>
-        <v>9325.5724295614618</v>
+        <v>9324.5724295614618</v>
       </c>
       <c r="L60">
         <f t="shared" si="44"/>
-        <v>-30699</v>
+        <v>-30700</v>
       </c>
       <c r="M60" s="2">
         <f t="shared" si="41"/>
-        <v>22862.739999999998</v>
+        <v>22861.739999999998</v>
       </c>
       <c r="N60">
         <f t="shared" si="42"/>
-        <v>357.23031249999997</v>
+        <v>357.21468749999997</v>
       </c>
       <c r="O60">
         <v>95022</v>
@@ -4875,19 +4875,19 @@
       </c>
       <c r="K61">
         <f t="shared" si="40"/>
-        <v>9973.8492511457644</v>
+        <v>9972.8492511457644</v>
       </c>
       <c r="L61">
         <f t="shared" si="44"/>
-        <v>-30699</v>
+        <v>-30700</v>
       </c>
       <c r="M61" s="2">
         <f t="shared" si="41"/>
-        <v>23687</v>
+        <v>23686</v>
       </c>
       <c r="N61">
         <f t="shared" si="42"/>
-        <v>370.109375</v>
+        <v>370.09375</v>
       </c>
       <c r="O61">
         <v>93681</v>
@@ -4938,19 +4938,19 @@
       </c>
       <c r="K62">
         <f t="shared" si="40"/>
-        <v>10736.57829141066</v>
+        <v>10735.57829141066</v>
       </c>
       <c r="L62">
         <f t="shared" si="44"/>
-        <v>-30699</v>
+        <v>-30700</v>
       </c>
       <c r="M62" s="2">
         <f t="shared" si="41"/>
-        <v>24628</v>
+        <v>24627</v>
       </c>
       <c r="N62">
         <f t="shared" si="42"/>
-        <v>384.8125</v>
+        <v>384.796875</v>
       </c>
       <c r="O62">
         <v>96814</v>
@@ -4963,8 +4963,387 @@
         <v>109.49250279303317</v>
       </c>
     </row>
+    <row r="63" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63" s="3">
+        <v>45780</v>
+      </c>
+      <c r="C63" t="s">
+        <v>19</v>
+      </c>
+      <c r="D63" s="2">
+        <v>55327</v>
+      </c>
+      <c r="E63" s="2">
+        <v>55407</v>
+      </c>
+      <c r="F63">
+        <f t="shared" ref="F63:F68" si="45">E63-D63</f>
+        <v>80</v>
+      </c>
+      <c r="G63">
+        <f t="shared" ref="G63:G68" si="46">(E63-$D$2)/A63</f>
+        <v>790.43548387096769</v>
+      </c>
+      <c r="H63">
+        <f t="shared" ref="H63:H68" si="47">(E63/D63-1)*100</f>
+        <v>0.14459486326747761</v>
+      </c>
+      <c r="I63">
+        <f t="shared" ref="I63:I68" si="48">(POWER((E63/$D$3),1/A63)-1)*100</f>
+        <v>3.5426098572639342</v>
+      </c>
+      <c r="J63">
+        <f t="shared" si="7"/>
+        <v>14072.010190801</v>
+      </c>
+      <c r="K63">
+        <f t="shared" ref="K63:K68" si="49">M63-J63</f>
+        <v>10634.989809199</v>
+      </c>
+      <c r="L63">
+        <f t="shared" si="44"/>
+        <v>-30700</v>
+      </c>
+      <c r="M63" s="2">
+        <f t="shared" ref="M63:M68" si="50">L63+E63</f>
+        <v>24707</v>
+      </c>
+      <c r="N63">
+        <f t="shared" ref="N63:N68" si="51">M63/$D$2*100</f>
+        <v>386.046875</v>
+      </c>
+      <c r="O63">
+        <v>97711</v>
+      </c>
+      <c r="P63">
+        <v>96346</v>
+      </c>
+      <c r="Q63">
+        <f t="shared" ref="Q63:Q68" si="52">P63/$O$2*100</f>
+        <v>107.9629179324495</v>
+      </c>
+    </row>
+    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64" s="3">
+        <v>45781</v>
+      </c>
+      <c r="C64" t="s">
+        <v>20</v>
+      </c>
+      <c r="D64" s="2">
+        <v>55407</v>
+      </c>
+      <c r="E64" s="2">
+        <v>55343.86</v>
+      </c>
+      <c r="F64">
+        <f t="shared" si="45"/>
+        <v>-63.139999999999418</v>
+      </c>
+      <c r="G64">
+        <f t="shared" si="46"/>
+        <v>776.88666666666666</v>
+      </c>
+      <c r="H64">
+        <f t="shared" si="47"/>
+        <v>-0.11395672027000314</v>
+      </c>
+      <c r="I64">
+        <f t="shared" si="48"/>
+        <v>3.4835363472130121</v>
+      </c>
+      <c r="J64">
+        <f t="shared" si="7"/>
+        <v>14254.946323281412</v>
+      </c>
+      <c r="K64">
+        <f t="shared" si="49"/>
+        <v>10388.913676718588</v>
+      </c>
+      <c r="L64">
+        <f t="shared" si="44"/>
+        <v>-30700</v>
+      </c>
+      <c r="M64" s="2">
+        <f t="shared" si="50"/>
+        <v>24643.86</v>
+      </c>
+      <c r="N64">
+        <f t="shared" si="51"/>
+        <v>385.06031250000001</v>
+      </c>
+      <c r="O64">
+        <v>96346</v>
+      </c>
+      <c r="P64">
+        <v>95562</v>
+      </c>
+      <c r="Q64">
+        <f t="shared" si="52"/>
+        <v>107.08438714072966</v>
+      </c>
+    </row>
+    <row r="65" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65" s="3">
+        <v>45782</v>
+      </c>
+      <c r="C65" t="s">
+        <v>14</v>
+      </c>
+      <c r="D65" s="2">
+        <v>55343.86</v>
+      </c>
+      <c r="E65" s="2">
+        <v>55587.76</v>
+      </c>
+      <c r="F65">
+        <f t="shared" si="45"/>
+        <v>243.90000000000146</v>
+      </c>
+      <c r="G65">
+        <f t="shared" si="46"/>
+        <v>768.55875000000003</v>
+      </c>
+      <c r="H65">
+        <f t="shared" si="47"/>
+        <v>0.44069929347176906</v>
+      </c>
+      <c r="I65">
+        <f t="shared" si="48"/>
+        <v>3.4352902582946987</v>
+      </c>
+      <c r="J65">
+        <f t="shared" si="7"/>
+        <v>14440.260625484068</v>
+      </c>
+      <c r="K65">
+        <f t="shared" si="49"/>
+        <v>10447.499374515934</v>
+      </c>
+      <c r="L65">
+        <f t="shared" si="44"/>
+        <v>-30700</v>
+      </c>
+      <c r="M65" s="2">
+        <f t="shared" si="50"/>
+        <v>24887.760000000002</v>
+      </c>
+      <c r="N65">
+        <f t="shared" si="51"/>
+        <v>388.87125000000003</v>
+      </c>
+      <c r="O65">
+        <v>95562</v>
+      </c>
+      <c r="P65">
+        <v>93833</v>
+      </c>
+      <c r="Q65">
+        <f t="shared" si="52"/>
+        <v>105.14691298399035</v>
+      </c>
+    </row>
+    <row r="66" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <v>65</v>
+      </c>
+      <c r="B66" s="3">
+        <v>45783</v>
+      </c>
+      <c r="C66" t="s">
+        <v>15</v>
+      </c>
+      <c r="D66" s="2">
+        <v>55587.76</v>
+      </c>
+      <c r="E66" s="2">
+        <v>56222.65</v>
+      </c>
+      <c r="F66">
+        <f t="shared" si="45"/>
+        <v>634.88999999999942</v>
+      </c>
+      <c r="G66">
+        <f t="shared" si="46"/>
+        <v>766.50230769230768</v>
+      </c>
+      <c r="H66">
+        <f t="shared" si="47"/>
+        <v>1.1421399243286556</v>
+      </c>
+      <c r="I66">
+        <f t="shared" si="48"/>
+        <v>3.399620227843414</v>
+      </c>
+      <c r="J66">
+        <f t="shared" si="7"/>
+        <v>14627.98401361536</v>
+      </c>
+      <c r="K66">
+        <f t="shared" si="49"/>
+        <v>10894.665986384642</v>
+      </c>
+      <c r="L66">
+        <f t="shared" si="44"/>
+        <v>-30700</v>
+      </c>
+      <c r="M66" s="2">
+        <f t="shared" si="50"/>
+        <v>25522.65</v>
+      </c>
+      <c r="N66">
+        <f t="shared" si="51"/>
+        <v>398.79140625000002</v>
+      </c>
+      <c r="O66">
+        <v>93833</v>
+      </c>
+      <c r="P66">
+        <v>94090</v>
+      </c>
+      <c r="Q66">
+        <f t="shared" si="52"/>
+        <v>105.43490075627606</v>
+      </c>
+    </row>
+    <row r="67" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <v>66</v>
+      </c>
+      <c r="B67" s="3">
+        <v>45784</v>
+      </c>
+      <c r="C67" t="s">
+        <v>16</v>
+      </c>
+      <c r="D67" s="2">
+        <v>56222.65</v>
+      </c>
+      <c r="E67" s="2">
+        <v>56495.43</v>
+      </c>
+      <c r="F67">
+        <f t="shared" si="45"/>
+        <v>272.77999999999884</v>
+      </c>
+      <c r="G67">
+        <f t="shared" si="46"/>
+        <v>759.02166666666665</v>
+      </c>
+      <c r="H67">
+        <f t="shared" si="47"/>
+        <v>0.48517812660910931</v>
+      </c>
+      <c r="I67">
+        <f t="shared" si="48"/>
+        <v>3.3548374418092886</v>
+      </c>
+      <c r="J67">
+        <f t="shared" si="7"/>
+        <v>14818.147805792358</v>
+      </c>
+      <c r="K67">
+        <f t="shared" si="49"/>
+        <v>10977.282194207643</v>
+      </c>
+      <c r="L67">
+        <f t="shared" si="44"/>
+        <v>-30700</v>
+      </c>
+      <c r="M67" s="2">
+        <f t="shared" si="50"/>
+        <v>25795.43</v>
+      </c>
+      <c r="N67">
+        <f t="shared" si="51"/>
+        <v>403.05359375</v>
+      </c>
+      <c r="O67">
+        <v>94090</v>
+      </c>
+      <c r="P67">
+        <v>96902</v>
+      </c>
+      <c r="Q67">
+        <f t="shared" si="52"/>
+        <v>108.58595762657737</v>
+      </c>
+    </row>
+    <row r="68" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A68">
+        <v>67</v>
+      </c>
+      <c r="B68" s="3">
+        <v>45785</v>
+      </c>
+      <c r="C68" t="s">
+        <v>17</v>
+      </c>
+      <c r="D68" s="2">
+        <v>56495.43</v>
+      </c>
+      <c r="E68" s="2">
+        <v>59105</v>
+      </c>
+      <c r="F68">
+        <f t="shared" si="45"/>
+        <v>2609.5699999999997</v>
+      </c>
+      <c r="G68">
+        <f t="shared" si="46"/>
+        <v>786.64179104477614</v>
+      </c>
+      <c r="H68">
+        <f t="shared" si="47"/>
+        <v>4.6190815788108797</v>
+      </c>
+      <c r="I68">
+        <f t="shared" si="48"/>
+        <v>3.3735939861297304</v>
+      </c>
+      <c r="J68">
+        <f t="shared" ref="J68" si="53">J67*1.013</f>
+        <v>15010.783727267657</v>
+      </c>
+      <c r="K68">
+        <f t="shared" si="49"/>
+        <v>13394.216272732343</v>
+      </c>
+      <c r="L68">
+        <f t="shared" si="44"/>
+        <v>-30700</v>
+      </c>
+      <c r="M68" s="2">
+        <f t="shared" si="50"/>
+        <v>28405</v>
+      </c>
+      <c r="N68">
+        <f>M68/$D$2*100</f>
+        <v>443.828125</v>
+      </c>
+      <c r="O68">
+        <v>96902</v>
+      </c>
+      <c r="P68">
+        <v>99342</v>
+      </c>
+      <c r="Q68">
+        <f t="shared" si="52"/>
+        <v>111.3201606008075</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>